<commit_message>
added {entry-exit} and holding time to algo
</commit_message>
<xml_diff>
--- a/algo high low.xlsx
+++ b/algo high low.xlsx
@@ -1043,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J122" sqref="J122"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,22 +1079,22 @@
         <v>6</v>
       </c>
       <c r="B2" s="8">
-        <v>536.29999999999995</v>
+        <v>569.25</v>
       </c>
       <c r="C2" s="10">
-        <v>530</v>
+        <v>556</v>
       </c>
       <c r="D2" s="13">
-        <v>530.75</v>
+        <v>562</v>
       </c>
       <c r="E2" s="5">
-        <v>531.45000000000005</v>
+        <v>562.35</v>
       </c>
       <c r="F2" s="16">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G2" s="5">
-        <v>532.45000000000005</v>
+        <v>562.25</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1102,22 +1102,22 @@
         <v>7</v>
       </c>
       <c r="B3" s="9">
-        <v>4276.45</v>
+        <v>4683</v>
       </c>
       <c r="C3" s="11">
-        <v>4224</v>
+        <v>4506</v>
       </c>
       <c r="D3" s="14">
-        <v>4253</v>
+        <v>4639</v>
       </c>
       <c r="E3" s="6">
-        <v>4262.3500000000004</v>
+        <v>4630.75</v>
       </c>
       <c r="F3" s="17">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G3" s="6">
-        <v>4254.6000000000004</v>
+        <v>4537.2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1125,22 +1125,22 @@
         <v>8</v>
       </c>
       <c r="B4" s="9">
-        <v>172</v>
+        <v>173.5</v>
       </c>
       <c r="C4" s="11">
-        <v>167.2</v>
+        <v>170.85</v>
       </c>
       <c r="D4" s="14">
-        <v>167.75</v>
+        <v>172.9</v>
       </c>
       <c r="E4" s="6">
-        <v>168.7</v>
+        <v>172.55</v>
       </c>
       <c r="F4" s="17">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G4" s="6">
-        <v>171.85</v>
+        <v>171.2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1148,22 +1148,22 @@
         <v>9</v>
       </c>
       <c r="B5" s="9">
-        <v>232.8</v>
+        <v>234.8</v>
       </c>
       <c r="C5" s="11">
-        <v>225.35</v>
+        <v>231.05</v>
       </c>
       <c r="D5" s="14">
-        <v>227.7</v>
+        <v>232.45</v>
       </c>
       <c r="E5" s="6">
-        <v>228.3</v>
+        <v>232.45</v>
       </c>
       <c r="F5" s="17">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="G5" s="6">
-        <v>226.9</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1171,22 +1171,22 @@
         <v>10</v>
       </c>
       <c r="B6" s="9">
-        <v>2251.9499999999998</v>
+        <v>2548.4</v>
       </c>
       <c r="C6" s="11">
-        <v>2160.9</v>
+        <v>2495</v>
       </c>
       <c r="D6" s="14">
-        <v>2250</v>
+        <v>2523</v>
       </c>
       <c r="E6" s="6">
-        <v>2225.4499999999998</v>
+        <v>2531.1999999999998</v>
       </c>
       <c r="F6" s="17">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="G6" s="6">
-        <v>2176.8000000000002</v>
+        <v>2514.0500000000002</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1194,22 +1194,22 @@
         <v>11</v>
       </c>
       <c r="B7" s="9">
-        <v>802.95</v>
+        <v>880</v>
       </c>
       <c r="C7" s="11">
-        <v>785</v>
+        <v>862.2</v>
       </c>
       <c r="D7" s="14">
-        <v>801</v>
+        <v>878.7</v>
       </c>
       <c r="E7" s="6">
-        <v>795.55</v>
+        <v>878.65</v>
       </c>
       <c r="F7" s="17">
-        <v>44</v>
+        <v>110</v>
       </c>
       <c r="G7" s="6">
-        <v>793.1</v>
+        <v>864.8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1217,22 +1217,22 @@
         <v>12</v>
       </c>
       <c r="B8" s="9">
-        <v>4593.45</v>
+        <v>4650</v>
       </c>
       <c r="C8" s="11">
-        <v>4543.3</v>
+        <v>4601</v>
       </c>
       <c r="D8" s="14">
-        <v>4560</v>
+        <v>4615</v>
       </c>
       <c r="E8" s="6">
-        <v>4557.8</v>
+        <v>4613.1499999999996</v>
       </c>
       <c r="F8" s="17">
         <v>1</v>
       </c>
       <c r="G8" s="6">
-        <v>4568.6000000000004</v>
+        <v>4624.05</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1240,22 +1240,22 @@
         <v>13</v>
       </c>
       <c r="B9" s="9">
-        <v>415.85</v>
+        <v>475.8</v>
       </c>
       <c r="C9" s="11">
-        <v>411.35</v>
+        <v>453.75</v>
       </c>
       <c r="D9" s="14">
-        <v>415.2</v>
+        <v>474.5</v>
       </c>
       <c r="E9" s="6">
-        <v>414.3</v>
+        <v>474.55</v>
       </c>
       <c r="F9" s="17">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="G9" s="6">
-        <v>413.35</v>
+        <v>455.65</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1263,22 +1263,22 @@
         <v>14</v>
       </c>
       <c r="B10" s="9">
-        <v>5490</v>
+        <v>5658.25</v>
       </c>
       <c r="C10" s="11">
-        <v>5395</v>
+        <v>5596.9</v>
       </c>
       <c r="D10" s="14">
-        <v>5408.7</v>
+        <v>5621.05</v>
       </c>
       <c r="E10" s="6">
-        <v>5401.3</v>
+        <v>5622.55</v>
       </c>
       <c r="F10" s="17">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G10" s="6">
-        <v>5467.15</v>
+        <v>5598.8</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1286,22 +1286,22 @@
         <v>15</v>
       </c>
       <c r="B11" s="9">
-        <v>419.75</v>
+        <v>450.75</v>
       </c>
       <c r="C11" s="11">
-        <v>413.95</v>
+        <v>442.75</v>
       </c>
       <c r="D11" s="14">
-        <v>415.55</v>
+        <v>450</v>
       </c>
       <c r="E11" s="6">
-        <v>414.6</v>
+        <v>449.95</v>
       </c>
       <c r="F11" s="17">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G11" s="6">
-        <v>418.95</v>
+        <v>444.85</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1309,22 +1309,22 @@
         <v>16</v>
       </c>
       <c r="B12" s="9">
-        <v>179.85</v>
+        <v>176.7</v>
       </c>
       <c r="C12" s="11">
-        <v>175.8</v>
+        <v>174.2</v>
       </c>
       <c r="D12" s="14">
-        <v>178.2</v>
+        <v>174.5</v>
       </c>
       <c r="E12" s="6">
-        <v>178.15</v>
+        <v>174.45</v>
       </c>
       <c r="F12" s="17">
-        <v>96</v>
+        <v>292</v>
       </c>
       <c r="G12" s="6">
-        <v>177.25</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1332,22 +1332,22 @@
         <v>17</v>
       </c>
       <c r="B13" s="9">
-        <v>1951</v>
+        <v>2006</v>
       </c>
       <c r="C13" s="11">
-        <v>1925</v>
+        <v>1963.15</v>
       </c>
       <c r="D13" s="14">
-        <v>1933</v>
+        <v>1990</v>
       </c>
       <c r="E13" s="6">
-        <v>1933.7</v>
+        <v>1991</v>
       </c>
       <c r="F13" s="17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G13" s="6">
-        <v>1945.05</v>
+        <v>2002.9</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1355,22 +1355,22 @@
         <v>18</v>
       </c>
       <c r="B14" s="9">
-        <v>6620</v>
+        <v>6836</v>
       </c>
       <c r="C14" s="11">
-        <v>6500.1</v>
+        <v>6621.15</v>
       </c>
       <c r="D14" s="14">
-        <v>6535.7</v>
+        <v>6775</v>
       </c>
       <c r="E14" s="6">
-        <v>6540.7</v>
+        <v>6747.05</v>
       </c>
       <c r="F14" s="17">
         <v>0</v>
       </c>
       <c r="G14" s="6">
-        <v>6607</v>
+        <v>6652.05</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1378,22 +1378,22 @@
         <v>19</v>
       </c>
       <c r="B15" s="9">
-        <v>723.25</v>
+        <v>755.6</v>
       </c>
       <c r="C15" s="11">
-        <v>711.55</v>
+        <v>742.85</v>
       </c>
       <c r="D15" s="14">
-        <v>722.3</v>
+        <v>754.7</v>
       </c>
       <c r="E15" s="6">
-        <v>722.2</v>
+        <v>753.75</v>
       </c>
       <c r="F15" s="17">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G15" s="6">
-        <v>716.05</v>
+        <v>748.8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1401,22 +1401,22 @@
         <v>20</v>
       </c>
       <c r="B16" s="9">
-        <v>1042.3</v>
+        <v>1045</v>
       </c>
       <c r="C16" s="11">
-        <v>1028.95</v>
+        <v>1023.25</v>
       </c>
       <c r="D16" s="14">
-        <v>1031.9000000000001</v>
+        <v>1041.3</v>
       </c>
       <c r="E16" s="6">
-        <v>1032.8</v>
+        <v>1042.6500000000001</v>
       </c>
       <c r="F16" s="17">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G16" s="6">
-        <v>1037.25</v>
+        <v>1032.25</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1424,22 +1424,22 @@
         <v>21</v>
       </c>
       <c r="B17" s="9">
-        <v>1623.4</v>
+        <v>1711.7</v>
       </c>
       <c r="C17" s="11">
-        <v>1612</v>
+        <v>1685.9</v>
       </c>
       <c r="D17" s="14">
-        <v>1615</v>
+        <v>1694</v>
       </c>
       <c r="E17" s="6">
-        <v>1617.25</v>
+        <v>1696.25</v>
       </c>
       <c r="F17" s="17">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G17" s="6">
-        <v>1621.45</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1447,22 +1447,22 @@
         <v>22</v>
       </c>
       <c r="B18" s="9">
-        <v>7089.95</v>
+        <v>7420</v>
       </c>
       <c r="C18" s="11">
-        <v>7011</v>
+        <v>7315.05</v>
       </c>
       <c r="D18" s="14">
-        <v>7035</v>
+        <v>7405</v>
       </c>
       <c r="E18" s="6">
-        <v>7020.8</v>
+        <v>7407.65</v>
       </c>
       <c r="F18" s="17">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G18" s="6">
-        <v>7076.55</v>
+        <v>7357.65</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1470,22 +1470,22 @@
         <v>23</v>
       </c>
       <c r="B19" s="9">
-        <v>2585.85</v>
+        <v>2571.25</v>
       </c>
       <c r="C19" s="11">
-        <v>2549.5</v>
+        <v>2529</v>
       </c>
       <c r="D19" s="14">
-        <v>2568</v>
+        <v>2553.1999999999998</v>
       </c>
       <c r="E19" s="6">
-        <v>2570.85</v>
+        <v>2560.8000000000002</v>
       </c>
       <c r="F19" s="17">
         <v>2</v>
       </c>
       <c r="G19" s="6">
-        <v>2551</v>
+        <v>2566.9499999999998</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1493,22 +1493,22 @@
         <v>24</v>
       </c>
       <c r="B20" s="9">
-        <v>465.9</v>
+        <v>475.5</v>
       </c>
       <c r="C20" s="11">
-        <v>455</v>
+        <v>467.7</v>
       </c>
       <c r="D20" s="14">
-        <v>461</v>
+        <v>469.95</v>
       </c>
       <c r="E20" s="6">
-        <v>460.85</v>
+        <v>468.55</v>
       </c>
       <c r="F20" s="17">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="G20" s="6">
-        <v>464.8</v>
+        <v>472.85</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1516,22 +1516,22 @@
         <v>25</v>
       </c>
       <c r="B21" s="9">
-        <v>214.95</v>
+        <v>234.85</v>
       </c>
       <c r="C21" s="11">
-        <v>212</v>
+        <v>229.25</v>
       </c>
       <c r="D21" s="14">
-        <v>212.2</v>
+        <v>234.5</v>
       </c>
       <c r="E21" s="6">
-        <v>212.35</v>
+        <v>234.3</v>
       </c>
       <c r="F21" s="17">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G21" s="6">
-        <v>212.9</v>
+        <v>230.85</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1539,22 +1539,22 @@
         <v>26</v>
       </c>
       <c r="B22" s="9">
-        <v>195.5</v>
+        <v>210</v>
       </c>
       <c r="C22" s="11">
-        <v>192.75</v>
+        <v>205.75</v>
       </c>
       <c r="D22" s="14">
-        <v>192.95</v>
+        <v>209</v>
       </c>
       <c r="E22" s="6">
-        <v>193.1</v>
+        <v>209.05</v>
       </c>
       <c r="F22" s="17">
-        <v>54</v>
+        <v>359</v>
       </c>
       <c r="G22" s="6">
-        <v>195.3</v>
+        <v>206.3</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1562,22 +1562,22 @@
         <v>27</v>
       </c>
       <c r="B23" s="9">
-        <v>1611.2</v>
+        <v>1638.65</v>
       </c>
       <c r="C23" s="11">
-        <v>1590</v>
+        <v>1603.3</v>
       </c>
       <c r="D23" s="14">
-        <v>1607</v>
+        <v>1629.5</v>
       </c>
       <c r="E23" s="6">
-        <v>1606.95</v>
+        <v>1630</v>
       </c>
       <c r="F23" s="17">
         <v>2</v>
       </c>
       <c r="G23" s="6">
-        <v>1605.25</v>
+        <v>1626.65</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1585,22 +1585,22 @@
         <v>28</v>
       </c>
       <c r="B24" s="9">
-        <v>142.15</v>
+        <v>157.5</v>
       </c>
       <c r="C24" s="11">
-        <v>137.35</v>
+        <v>151.69999999999999</v>
       </c>
       <c r="D24" s="14">
-        <v>140.4</v>
+        <v>153.75</v>
       </c>
       <c r="E24" s="6">
-        <v>140.35</v>
+        <v>153.55000000000001</v>
       </c>
       <c r="F24" s="17">
-        <v>196</v>
+        <v>514</v>
       </c>
       <c r="G24" s="6">
-        <v>140.30000000000001</v>
+        <v>152.05000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1608,22 +1608,22 @@
         <v>29</v>
       </c>
       <c r="B25" s="9">
-        <v>1120.9000000000001</v>
+        <v>1168.6500000000001</v>
       </c>
       <c r="C25" s="11">
-        <v>1096.9000000000001</v>
+        <v>1155.05</v>
       </c>
       <c r="D25" s="14">
-        <v>1115.1500000000001</v>
+        <v>1159.75</v>
       </c>
       <c r="E25" s="6">
-        <v>1115.55</v>
+        <v>1157.2</v>
       </c>
       <c r="F25" s="17">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G25" s="6">
-        <v>1097.9000000000001</v>
+        <v>1166.45</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1631,22 +1631,22 @@
         <v>30</v>
       </c>
       <c r="B26" s="9">
-        <v>238.95</v>
+        <v>241.9</v>
       </c>
       <c r="C26" s="11">
-        <v>234.9</v>
+        <v>238.9</v>
       </c>
       <c r="D26" s="14">
-        <v>235.5</v>
+        <v>240.9</v>
       </c>
       <c r="E26" s="6">
-        <v>235.35</v>
+        <v>240.65</v>
       </c>
       <c r="F26" s="17">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G26" s="6">
-        <v>237</v>
+        <v>241.4</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1654,22 +1654,22 @@
         <v>31</v>
       </c>
       <c r="B27" s="9">
-        <v>4699</v>
+        <v>4954.8500000000004</v>
       </c>
       <c r="C27" s="11">
-        <v>4640.5</v>
+        <v>4915</v>
       </c>
       <c r="D27" s="14">
-        <v>4642</v>
+        <v>4934</v>
       </c>
       <c r="E27" s="6">
-        <v>4644.1499999999996</v>
+        <v>4937.75</v>
       </c>
       <c r="F27" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G27" s="6">
-        <v>4690.55</v>
+        <v>4949</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1677,22 +1677,22 @@
         <v>32</v>
       </c>
       <c r="B28" s="9">
-        <v>623</v>
+        <v>639.54999999999995</v>
       </c>
       <c r="C28" s="11">
-        <v>612</v>
+        <v>631.4</v>
       </c>
       <c r="D28" s="14">
-        <v>614.75</v>
+        <v>635</v>
       </c>
       <c r="E28" s="6">
-        <v>613.85</v>
+        <v>635.15</v>
       </c>
       <c r="F28" s="17">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G28" s="6">
-        <v>622.29999999999995</v>
+        <v>636</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1700,22 +1700,22 @@
         <v>33</v>
       </c>
       <c r="B29" s="9">
-        <v>395.8</v>
+        <v>429</v>
       </c>
       <c r="C29" s="11">
-        <v>389</v>
+        <v>420.6</v>
       </c>
       <c r="D29" s="14">
-        <v>389.7</v>
+        <v>428</v>
       </c>
       <c r="E29" s="6">
-        <v>389.8</v>
+        <v>426.95</v>
       </c>
       <c r="F29" s="17">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="G29" s="6">
-        <v>395.15</v>
+        <v>421.85</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1723,22 +1723,22 @@
         <v>34</v>
       </c>
       <c r="B30" s="9">
-        <v>766.9</v>
+        <v>843</v>
       </c>
       <c r="C30" s="11">
-        <v>751</v>
+        <v>814.3</v>
       </c>
       <c r="D30" s="14">
-        <v>752.55</v>
+        <v>825.25</v>
       </c>
       <c r="E30" s="6">
-        <v>753.65</v>
+        <v>825.15</v>
       </c>
       <c r="F30" s="17">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G30" s="6">
-        <v>766.05</v>
+        <v>824.2</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1746,22 +1746,22 @@
         <v>35</v>
       </c>
       <c r="B31" s="9">
-        <v>312.5</v>
+        <v>327</v>
       </c>
       <c r="C31" s="11">
-        <v>307</v>
+        <v>322</v>
       </c>
       <c r="D31" s="14">
-        <v>309</v>
+        <v>324.75</v>
       </c>
       <c r="E31" s="6">
-        <v>308.64999999999998</v>
+        <v>324.95</v>
       </c>
       <c r="F31" s="17">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="G31" s="6">
-        <v>310.95</v>
+        <v>324.10000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1769,22 +1769,22 @@
         <v>36</v>
       </c>
       <c r="B32" s="9">
-        <v>1124.1500000000001</v>
+        <v>1161.95</v>
       </c>
       <c r="C32" s="11">
-        <v>1091.3</v>
+        <v>1141</v>
       </c>
       <c r="D32" s="14">
-        <v>1095.7</v>
+        <v>1150</v>
       </c>
       <c r="E32" s="6">
-        <v>1094.5</v>
+        <v>1148.75</v>
       </c>
       <c r="F32" s="17">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G32" s="6">
-        <v>1119.3499999999999</v>
+        <v>1151.2</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1792,22 +1792,22 @@
         <v>37</v>
       </c>
       <c r="B33" s="9">
-        <v>1205</v>
+        <v>1219.0999999999999</v>
       </c>
       <c r="C33" s="11">
-        <v>1178</v>
+        <v>1206.25</v>
       </c>
       <c r="D33" s="14">
-        <v>1196.25</v>
+        <v>1218.5</v>
       </c>
       <c r="E33" s="6">
-        <v>1198.6500000000001</v>
+        <v>1216.5</v>
       </c>
       <c r="F33" s="17">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="G33" s="6">
-        <v>1188.8499999999999</v>
+        <v>1212.4000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1815,22 +1815,22 @@
         <v>38</v>
       </c>
       <c r="B34" s="9">
-        <v>5625.55</v>
+        <v>5754</v>
       </c>
       <c r="C34" s="11">
-        <v>5550</v>
+        <v>5655.05</v>
       </c>
       <c r="D34" s="14">
-        <v>5603.6</v>
+        <v>5671.15</v>
       </c>
       <c r="E34" s="6">
-        <v>5618.55</v>
+        <v>5675.95</v>
       </c>
       <c r="F34" s="17">
         <v>1</v>
       </c>
       <c r="G34" s="6">
-        <v>5597.95</v>
+        <v>5716.95</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1838,22 +1838,22 @@
         <v>39</v>
       </c>
       <c r="B35" s="9">
-        <v>754.2</v>
+        <v>804</v>
       </c>
       <c r="C35" s="11">
-        <v>742</v>
+        <v>787.8</v>
       </c>
       <c r="D35" s="14">
-        <v>746.4</v>
+        <v>800</v>
       </c>
       <c r="E35" s="6">
-        <v>748.6</v>
+        <v>800.9</v>
       </c>
       <c r="F35" s="17">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="G35" s="6">
-        <v>746.75</v>
+        <v>795.2</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1861,22 +1861,22 @@
         <v>40</v>
       </c>
       <c r="B36" s="9">
-        <v>1143</v>
+        <v>1181.9000000000001</v>
       </c>
       <c r="C36" s="11">
-        <v>1127.5999999999999</v>
+        <v>1162</v>
       </c>
       <c r="D36" s="14">
-        <v>1130.4000000000001</v>
+        <v>1178</v>
       </c>
       <c r="E36" s="6">
-        <v>1135.05</v>
+        <v>1178.0999999999999</v>
       </c>
       <c r="F36" s="17">
         <v>2</v>
       </c>
       <c r="G36" s="6">
-        <v>1132.3</v>
+        <v>1165.45</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1884,22 +1884,22 @@
         <v>41</v>
       </c>
       <c r="B37" s="9">
-        <v>289.55</v>
+        <v>295.64999999999998</v>
       </c>
       <c r="C37" s="11">
-        <v>282.95</v>
+        <v>289.89999999999998</v>
       </c>
       <c r="D37" s="14">
-        <v>283</v>
+        <v>295.3</v>
       </c>
       <c r="E37" s="6">
-        <v>283.8</v>
+        <v>294.8</v>
       </c>
       <c r="F37" s="17">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G37" s="6">
-        <v>289.10000000000002</v>
+        <v>293.5</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1907,22 +1907,22 @@
         <v>42</v>
       </c>
       <c r="B38" s="9">
-        <v>1878.55</v>
+        <v>1959.9</v>
       </c>
       <c r="C38" s="11">
-        <v>1850.8</v>
+        <v>1921.5</v>
       </c>
       <c r="D38" s="14">
-        <v>1864.9</v>
+        <v>1957.8</v>
       </c>
       <c r="E38" s="6">
-        <v>1871.75</v>
+        <v>1953.9</v>
       </c>
       <c r="F38" s="17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G38" s="6">
-        <v>1868.6</v>
+        <v>1937.7</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1930,22 +1930,22 @@
         <v>43</v>
       </c>
       <c r="B39" s="9">
-        <v>540.65</v>
+        <v>548.9</v>
       </c>
       <c r="C39" s="11">
-        <v>536</v>
+        <v>541.70000000000005</v>
       </c>
       <c r="D39" s="14">
-        <v>536.5</v>
+        <v>547</v>
       </c>
       <c r="E39" s="6">
-        <v>537.35</v>
+        <v>547</v>
       </c>
       <c r="F39" s="17">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G39" s="6">
-        <v>539.04999999999995</v>
+        <v>543.6</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1953,22 +1953,22 @@
         <v>44</v>
       </c>
       <c r="B40" s="9">
-        <v>2260.4499999999998</v>
+        <v>2328.9</v>
       </c>
       <c r="C40" s="11">
-        <v>2164.0500000000002</v>
+        <v>2274.8000000000002</v>
       </c>
       <c r="D40" s="14">
-        <v>2224</v>
+        <v>2305</v>
       </c>
       <c r="E40" s="6">
-        <v>2231.1</v>
+        <v>2307.5500000000002</v>
       </c>
       <c r="F40" s="17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G40" s="6">
-        <v>2184</v>
+        <v>2294.9499999999998</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1976,22 +1976,22 @@
         <v>45</v>
       </c>
       <c r="B41" s="9">
-        <v>609.79999999999995</v>
+        <v>647.9</v>
       </c>
       <c r="C41" s="11">
-        <v>600</v>
+        <v>628.54999999999995</v>
       </c>
       <c r="D41" s="14">
-        <v>601.95000000000005</v>
+        <v>643.5</v>
       </c>
       <c r="E41" s="6">
-        <v>600.95000000000005</v>
+        <v>645.1</v>
       </c>
       <c r="F41" s="17">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G41" s="6">
-        <v>607.70000000000005</v>
+        <v>634.35</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1999,22 +1999,22 @@
         <v>46</v>
       </c>
       <c r="B42" s="9">
-        <v>2239.8000000000002</v>
+        <v>2227</v>
       </c>
       <c r="C42" s="11">
-        <v>2190</v>
+        <v>2204.6</v>
       </c>
       <c r="D42" s="14">
-        <v>2194.0500000000002</v>
+        <v>2209.9499999999998</v>
       </c>
       <c r="E42" s="6">
-        <v>2195.1999999999998</v>
+        <v>2210.35</v>
       </c>
       <c r="F42" s="17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G42" s="6">
-        <v>2222.1999999999998</v>
+        <v>2215.5</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2022,22 +2022,22 @@
         <v>47</v>
       </c>
       <c r="B43" s="9">
-        <v>140</v>
+        <v>144.85</v>
       </c>
       <c r="C43" s="11">
-        <v>136.35</v>
+        <v>139.5</v>
       </c>
       <c r="D43" s="14">
-        <v>136.5</v>
+        <v>140.44999999999999</v>
       </c>
       <c r="E43" s="6">
-        <v>136.85</v>
+        <v>140.44999999999999</v>
       </c>
       <c r="F43" s="17">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="G43" s="6">
-        <v>138.05000000000001</v>
+        <v>144.4</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2045,22 +2045,22 @@
         <v>48</v>
       </c>
       <c r="B44" s="9">
-        <v>3778.95</v>
+        <v>3835.05</v>
       </c>
       <c r="C44" s="11">
-        <v>3739.1</v>
+        <v>3790</v>
       </c>
       <c r="D44" s="14">
-        <v>3760</v>
+        <v>3800</v>
       </c>
       <c r="E44" s="6">
-        <v>3764.8</v>
+        <v>3798.1</v>
       </c>
       <c r="F44" s="17">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G44" s="6">
-        <v>3746</v>
+        <v>3820.55</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2068,22 +2068,22 @@
         <v>49</v>
       </c>
       <c r="B45" s="9">
-        <v>5363</v>
+        <v>6041.2</v>
       </c>
       <c r="C45" s="11">
-        <v>5265</v>
+        <v>5876</v>
       </c>
       <c r="D45" s="14">
-        <v>5270</v>
+        <v>6000</v>
       </c>
       <c r="E45" s="6">
-        <v>5277.85</v>
+        <v>6002.2</v>
       </c>
       <c r="F45" s="17">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G45" s="6">
-        <v>5358.55</v>
+        <v>6009.95</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2091,22 +2091,22 @@
         <v>50</v>
       </c>
       <c r="B46" s="9">
-        <v>641.1</v>
+        <v>652</v>
       </c>
       <c r="C46" s="11">
-        <v>628.35</v>
+        <v>632.79999999999995</v>
       </c>
       <c r="D46" s="14">
-        <v>630.75</v>
+        <v>649.15</v>
       </c>
       <c r="E46" s="6">
-        <v>629.35</v>
+        <v>649.25</v>
       </c>
       <c r="F46" s="17">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G46" s="6">
-        <v>636.95000000000005</v>
+        <v>636.45000000000005</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2114,22 +2114,22 @@
         <v>51</v>
       </c>
       <c r="B47" s="9">
-        <v>5756.85</v>
+        <v>5775</v>
       </c>
       <c r="C47" s="11">
-        <v>5615</v>
+        <v>5728.4</v>
       </c>
       <c r="D47" s="14">
-        <v>5625</v>
+        <v>5775</v>
       </c>
       <c r="E47" s="6">
-        <v>5646.15</v>
+        <v>5756</v>
       </c>
       <c r="F47" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G47" s="6">
-        <v>5725</v>
+        <v>5748.6</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2137,22 +2137,22 @@
         <v>52</v>
       </c>
       <c r="B48" s="9">
-        <v>3252.4</v>
+        <v>3225</v>
       </c>
       <c r="C48" s="11">
-        <v>3211.05</v>
+        <v>3174.2</v>
       </c>
       <c r="D48" s="14">
-        <v>3218</v>
+        <v>3218.45</v>
       </c>
       <c r="E48" s="6">
-        <v>3229.45</v>
+        <v>3213.5</v>
       </c>
       <c r="F48" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G48" s="6">
-        <v>3232</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2160,22 +2160,22 @@
         <v>53</v>
       </c>
       <c r="B49" s="9">
-        <v>285</v>
+        <v>298.60000000000002</v>
       </c>
       <c r="C49" s="11">
-        <v>280.85000000000002</v>
+        <v>292.3</v>
       </c>
       <c r="D49" s="14">
-        <v>281.5</v>
+        <v>293.39999999999998</v>
       </c>
       <c r="E49" s="6">
-        <v>281.5</v>
+        <v>293.85000000000002</v>
       </c>
       <c r="F49" s="17">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="G49" s="6">
-        <v>284.64999999999998</v>
+        <v>295.14999999999998</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2183,22 +2183,22 @@
         <v>54</v>
       </c>
       <c r="B50" s="9">
-        <v>799.8</v>
+        <v>802</v>
       </c>
       <c r="C50" s="11">
-        <v>785.2</v>
+        <v>774</v>
       </c>
       <c r="D50" s="14">
-        <v>786.5</v>
+        <v>779.95</v>
       </c>
       <c r="E50" s="6">
-        <v>786.9</v>
+        <v>775.75</v>
       </c>
       <c r="F50" s="17">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G50" s="6">
-        <v>789.4</v>
+        <v>798.8</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2206,22 +2206,22 @@
         <v>55</v>
       </c>
       <c r="B51" s="9">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C51" s="11">
-        <v>620.20000000000005</v>
+        <v>633.54999999999995</v>
       </c>
       <c r="D51" s="14">
-        <v>636.04999999999995</v>
+        <v>640</v>
       </c>
       <c r="E51" s="6">
-        <v>634.79999999999995</v>
+        <v>640.29999999999995</v>
       </c>
       <c r="F51" s="17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G51" s="6">
-        <v>623</v>
+        <v>637.15</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2229,22 +2229,22 @@
         <v>56</v>
       </c>
       <c r="B52" s="9">
-        <v>705.5</v>
+        <v>726.25</v>
       </c>
       <c r="C52" s="11">
-        <v>691.1</v>
+        <v>700.1</v>
       </c>
       <c r="D52" s="14">
-        <v>693.7</v>
+        <v>713.7</v>
       </c>
       <c r="E52" s="6">
-        <v>693.15</v>
+        <v>711.55</v>
       </c>
       <c r="F52" s="17">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G52" s="6">
-        <v>704.9</v>
+        <v>707.95</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2252,22 +2252,22 @@
         <v>57</v>
       </c>
       <c r="B53" s="9">
-        <v>1015.7</v>
+        <v>1044</v>
       </c>
       <c r="C53" s="11">
-        <v>1003.2</v>
+        <v>1028.0999999999999</v>
       </c>
       <c r="D53" s="14">
-        <v>1009.85</v>
+        <v>1042</v>
       </c>
       <c r="E53" s="6">
-        <v>1009.5</v>
+        <v>1041.75</v>
       </c>
       <c r="F53" s="17">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G53" s="6">
-        <v>1010.05</v>
+        <v>1032.75</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2275,22 +2275,22 @@
         <v>58</v>
       </c>
       <c r="B54" s="9">
-        <v>1859</v>
+        <v>1943</v>
       </c>
       <c r="C54" s="11">
-        <v>1832.2</v>
+        <v>1872.95</v>
       </c>
       <c r="D54" s="14">
-        <v>1838</v>
+        <v>1918</v>
       </c>
       <c r="E54" s="6">
-        <v>1841.05</v>
+        <v>1915.6</v>
       </c>
       <c r="F54" s="17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G54" s="6">
-        <v>1846.4</v>
+        <v>1883.6</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2298,22 +2298,22 @@
         <v>59</v>
       </c>
       <c r="B55" s="9">
-        <v>389.95</v>
+        <v>398.35</v>
       </c>
       <c r="C55" s="11">
-        <v>371.1</v>
+        <v>390.4</v>
       </c>
       <c r="D55" s="14">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="E55" s="6">
-        <v>387.2</v>
+        <v>391.5</v>
       </c>
       <c r="F55" s="17">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="G55" s="6">
-        <v>375.15</v>
+        <v>396.5</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2321,22 +2321,22 @@
         <v>60</v>
       </c>
       <c r="B56" s="9">
-        <v>1967.65</v>
+        <v>2059.9</v>
       </c>
       <c r="C56" s="11">
-        <v>1945.45</v>
+        <v>2028.45</v>
       </c>
       <c r="D56" s="14">
-        <v>1945.95</v>
+        <v>2051.9</v>
       </c>
       <c r="E56" s="6">
-        <v>1949.4</v>
+        <v>2052.9499999999998</v>
       </c>
       <c r="F56" s="17">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G56" s="6">
-        <v>1960.25</v>
+        <v>2042.75</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2344,22 +2344,22 @@
         <v>61</v>
       </c>
       <c r="B57" s="9">
-        <v>430.8</v>
+        <v>444.7</v>
       </c>
       <c r="C57" s="11">
-        <v>425</v>
+        <v>436.1</v>
       </c>
       <c r="D57" s="14">
-        <v>425</v>
+        <v>442</v>
       </c>
       <c r="E57" s="6">
-        <v>425.55</v>
+        <v>441.85</v>
       </c>
       <c r="F57" s="17">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="G57" s="6">
-        <v>428.35</v>
+        <v>436.45</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2367,22 +2367,22 @@
         <v>62</v>
       </c>
       <c r="B58" s="9">
-        <v>2251</v>
+        <v>2532.8000000000002</v>
       </c>
       <c r="C58" s="11">
-        <v>2145.75</v>
+        <v>2473</v>
       </c>
       <c r="D58" s="14">
-        <v>2249.6999999999998</v>
+        <v>2524.9</v>
       </c>
       <c r="E58" s="6">
-        <v>2240.3000000000002</v>
+        <v>2519.4</v>
       </c>
       <c r="F58" s="17">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G58" s="6">
-        <v>2151.9</v>
+        <v>2489.4499999999998</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2390,22 +2390,22 @@
         <v>63</v>
       </c>
       <c r="B59" s="9">
-        <v>1302.5</v>
+        <v>1320.3</v>
       </c>
       <c r="C59" s="11">
-        <v>1285.7</v>
+        <v>1308.5999999999999</v>
       </c>
       <c r="D59" s="14">
-        <v>1291.0999999999999</v>
+        <v>1314.9</v>
       </c>
       <c r="E59" s="6">
-        <v>1294.3</v>
+        <v>1313.7</v>
       </c>
       <c r="F59" s="17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G59" s="6">
-        <v>1298.45</v>
+        <v>1317.45</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2413,22 +2413,22 @@
         <v>64</v>
       </c>
       <c r="B60" s="9">
-        <v>1326.7</v>
+        <v>1344.35</v>
       </c>
       <c r="C60" s="11">
-        <v>1305.6500000000001</v>
+        <v>1331</v>
       </c>
       <c r="D60" s="14">
-        <v>1308.4000000000001</v>
+        <v>1335</v>
       </c>
       <c r="E60" s="6">
-        <v>1309.1500000000001</v>
+        <v>1337.95</v>
       </c>
       <c r="F60" s="17">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G60" s="6">
-        <v>1325.1</v>
+        <v>1339.55</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2436,22 +2436,22 @@
         <v>65</v>
       </c>
       <c r="B61" s="9">
-        <v>2895</v>
+        <v>2993.5</v>
       </c>
       <c r="C61" s="11">
-        <v>2832.7</v>
+        <v>2947.1</v>
       </c>
       <c r="D61" s="14">
-        <v>2850</v>
+        <v>2952.85</v>
       </c>
       <c r="E61" s="6">
-        <v>2841.55</v>
+        <v>2953.55</v>
       </c>
       <c r="F61" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G61" s="6">
-        <v>2870.9</v>
+        <v>2982.75</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2459,22 +2459,22 @@
         <v>66</v>
       </c>
       <c r="B62" s="9">
+        <v>686.1</v>
+      </c>
+      <c r="C62" s="11">
         <v>672.25</v>
       </c>
-      <c r="C62" s="11">
-        <v>663.05</v>
-      </c>
       <c r="D62" s="14">
-        <v>668</v>
+        <v>676.5</v>
       </c>
       <c r="E62" s="6">
-        <v>668</v>
+        <v>674.95</v>
       </c>
       <c r="F62" s="17">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="G62" s="6">
-        <v>665.45</v>
+        <v>685.05</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2482,22 +2482,22 @@
         <v>67</v>
       </c>
       <c r="B63" s="9">
-        <v>512.75</v>
+        <v>526.65</v>
       </c>
       <c r="C63" s="11">
-        <v>503.15</v>
+        <v>516.54999999999995</v>
       </c>
       <c r="D63" s="14">
-        <v>509</v>
+        <v>519.25</v>
       </c>
       <c r="E63" s="6">
-        <v>507.8</v>
+        <v>519.25</v>
       </c>
       <c r="F63" s="17">
         <v>59</v>
       </c>
       <c r="G63" s="6">
-        <v>503.4</v>
+        <v>521</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2505,22 +2505,22 @@
         <v>68</v>
       </c>
       <c r="B64" s="9">
-        <v>167.4</v>
+        <v>183.2</v>
       </c>
       <c r="C64" s="11">
-        <v>163</v>
+        <v>176.15</v>
       </c>
       <c r="D64" s="14">
-        <v>164.15</v>
+        <v>178.45</v>
       </c>
       <c r="E64" s="6">
-        <v>163.95</v>
+        <v>178.1</v>
       </c>
       <c r="F64" s="17">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="G64" s="6">
-        <v>163.19999999999999</v>
+        <v>177.45</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2528,22 +2528,22 @@
         <v>69</v>
       </c>
       <c r="B65" s="9">
-        <v>1450</v>
+        <v>1476.9</v>
       </c>
       <c r="C65" s="11">
-        <v>1426.6</v>
+        <v>1444.6</v>
       </c>
       <c r="D65" s="14">
-        <v>1434</v>
+        <v>1471.25</v>
       </c>
       <c r="E65" s="6">
-        <v>1438.5</v>
+        <v>1470.9</v>
       </c>
       <c r="F65" s="17">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G65" s="6">
-        <v>1445.05</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2551,22 +2551,22 @@
         <v>70</v>
       </c>
       <c r="B66" s="9">
-        <v>563.5</v>
+        <v>564</v>
       </c>
       <c r="C66" s="11">
-        <v>554.54999999999995</v>
+        <v>556.70000000000005</v>
       </c>
       <c r="D66" s="14">
-        <v>554.75</v>
+        <v>562.85</v>
       </c>
       <c r="E66" s="6">
-        <v>555.45000000000005</v>
+        <v>563.29999999999995</v>
       </c>
       <c r="F66" s="17">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G66" s="6">
-        <v>559.54999999999995</v>
+        <v>561.9</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2574,22 +2574,22 @@
         <v>71</v>
       </c>
       <c r="B67" s="9">
-        <v>144.75</v>
+        <v>147.4</v>
       </c>
       <c r="C67" s="11">
-        <v>141.19999999999999</v>
+        <v>143.44999999999999</v>
       </c>
       <c r="D67" s="14">
-        <v>142.25</v>
+        <v>145</v>
       </c>
       <c r="E67" s="6">
-        <v>142.05000000000001</v>
+        <v>144.94999999999999</v>
       </c>
       <c r="F67" s="17">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G67" s="6">
-        <v>144.6</v>
+        <v>144.65</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2597,22 +2597,22 @@
         <v>72</v>
       </c>
       <c r="B68" s="9">
-        <v>394.25</v>
+        <v>404.75</v>
       </c>
       <c r="C68" s="11">
-        <v>391</v>
+        <v>394.6</v>
       </c>
       <c r="D68" s="14">
-        <v>392.2</v>
+        <v>401.2</v>
       </c>
       <c r="E68" s="6">
-        <v>392</v>
+        <v>401.2</v>
       </c>
       <c r="F68" s="17">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="G68" s="6">
-        <v>392.9</v>
+        <v>396.1</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2620,22 +2620,22 @@
         <v>73</v>
       </c>
       <c r="B69" s="9">
-        <v>422.35</v>
+        <v>436.05</v>
       </c>
       <c r="C69" s="11">
-        <v>418.1</v>
+        <v>427.55</v>
       </c>
       <c r="D69" s="14">
-        <v>419.5</v>
+        <v>433.5</v>
       </c>
       <c r="E69" s="6">
-        <v>420.5</v>
+        <v>434</v>
       </c>
       <c r="F69" s="17">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G69" s="6">
-        <v>418.9</v>
+        <v>431</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2643,22 +2643,22 @@
         <v>74</v>
       </c>
       <c r="B70" s="9">
-        <v>221.8</v>
+        <v>259.89999999999998</v>
       </c>
       <c r="C70" s="11">
-        <v>216.8</v>
+        <v>252.95</v>
       </c>
       <c r="D70" s="14">
-        <v>220.25</v>
+        <v>254.45</v>
       </c>
       <c r="E70" s="6">
-        <v>220</v>
+        <v>254.05</v>
       </c>
       <c r="F70" s="17">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="G70" s="6">
-        <v>216.8</v>
+        <v>255.8</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2666,22 +2666,22 @@
         <v>75</v>
       </c>
       <c r="B71" s="9">
-        <v>2610</v>
+        <v>2612.35</v>
       </c>
       <c r="C71" s="11">
-        <v>2591.15</v>
+        <v>2586.0500000000002</v>
       </c>
       <c r="D71" s="14">
-        <v>2601</v>
+        <v>2605</v>
       </c>
       <c r="E71" s="6">
-        <v>2599.1</v>
+        <v>2604.4</v>
       </c>
       <c r="F71" s="17">
         <v>1</v>
       </c>
       <c r="G71" s="6">
-        <v>2602</v>
+        <v>2600.6999999999998</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2689,22 +2689,22 @@
         <v>76</v>
       </c>
       <c r="B72" s="9">
-        <v>2615.35</v>
+        <v>2859.9</v>
       </c>
       <c r="C72" s="11">
-        <v>2562.3000000000002</v>
+        <v>2780.8</v>
       </c>
       <c r="D72" s="14">
-        <v>2568.4499999999998</v>
+        <v>2815</v>
       </c>
       <c r="E72" s="6">
-        <v>2568.35</v>
+        <v>2820.25</v>
       </c>
       <c r="F72" s="17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G72" s="6">
-        <v>2607</v>
+        <v>2801.6</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2712,22 +2712,22 @@
         <v>77</v>
       </c>
       <c r="B73" s="9">
-        <v>1490.9</v>
+        <v>1517.55</v>
       </c>
       <c r="C73" s="11">
-        <v>1474</v>
+        <v>1479.65</v>
       </c>
       <c r="D73" s="14">
-        <v>1476</v>
+        <v>1515.55</v>
       </c>
       <c r="E73" s="6">
-        <v>1476.2</v>
+        <v>1514.65</v>
       </c>
       <c r="F73" s="17">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="G73" s="6">
-        <v>1488.7</v>
+        <v>1483.15</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2735,22 +2735,22 @@
         <v>78</v>
       </c>
       <c r="B74" s="9">
-        <v>187.1</v>
+        <v>189.7</v>
       </c>
       <c r="C74" s="11">
-        <v>184.3</v>
+        <v>186.55</v>
       </c>
       <c r="D74" s="14">
-        <v>185.2</v>
+        <v>187.75</v>
       </c>
       <c r="E74" s="6">
-        <v>185.6</v>
+        <v>187</v>
       </c>
       <c r="F74" s="17">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G74" s="6">
-        <v>186.55</v>
+        <v>188.9</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2758,22 +2758,22 @@
         <v>79</v>
       </c>
       <c r="B75" s="9">
-        <v>716.85</v>
+        <v>779.5</v>
       </c>
       <c r="C75" s="11">
-        <v>703</v>
+        <v>750.95</v>
       </c>
       <c r="D75" s="14">
-        <v>709</v>
+        <v>755</v>
       </c>
       <c r="E75" s="6">
-        <v>710.2</v>
+        <v>754.15</v>
       </c>
       <c r="F75" s="17">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G75" s="6">
-        <v>708.95</v>
+        <v>752.35</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2781,22 +2781,22 @@
         <v>80</v>
       </c>
       <c r="B76" s="9">
-        <v>1097.1500000000001</v>
+        <v>1154</v>
       </c>
       <c r="C76" s="11">
-        <v>1076.3499999999999</v>
+        <v>1134.0999999999999</v>
       </c>
       <c r="D76" s="14">
-        <v>1085.0999999999999</v>
+        <v>1144.0999999999999</v>
       </c>
       <c r="E76" s="6">
-        <v>1091.8</v>
+        <v>1142.55</v>
       </c>
       <c r="F76" s="17">
         <v>2</v>
       </c>
       <c r="G76" s="6">
-        <v>1080.3</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2804,22 +2804,22 @@
         <v>81</v>
       </c>
       <c r="B77" s="9">
-        <v>661.4</v>
+        <v>694.05</v>
       </c>
       <c r="C77" s="11">
-        <v>652.25</v>
+        <v>678.45</v>
       </c>
       <c r="D77" s="14">
-        <v>660</v>
+        <v>680.85</v>
       </c>
       <c r="E77" s="6">
-        <v>660.3</v>
+        <v>681.5</v>
       </c>
       <c r="F77" s="17">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G77" s="6">
-        <v>655.20000000000005</v>
+        <v>693.3</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2827,22 +2827,22 @@
         <v>82</v>
       </c>
       <c r="B78" s="9">
-        <v>3547.8</v>
+        <v>3692.9</v>
       </c>
       <c r="C78" s="11">
-        <v>3500.05</v>
+        <v>3630</v>
       </c>
       <c r="D78" s="14">
-        <v>3502</v>
+        <v>3669</v>
       </c>
       <c r="E78" s="6">
-        <v>3528.05</v>
+        <v>3674.05</v>
       </c>
       <c r="F78" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G78" s="6">
-        <v>3543.8</v>
+        <v>3692.5</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2850,22 +2850,22 @@
         <v>83</v>
       </c>
       <c r="B79" s="9">
-        <v>786.25</v>
+        <v>823.4</v>
       </c>
       <c r="C79" s="11">
-        <v>776.4</v>
+        <v>812.35</v>
       </c>
       <c r="D79" s="14">
-        <v>779.85</v>
+        <v>820</v>
       </c>
       <c r="E79" s="6">
-        <v>782.05</v>
+        <v>819.6</v>
       </c>
       <c r="F79" s="17">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G79" s="6">
-        <v>777</v>
+        <v>818.45</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2873,22 +2873,22 @@
         <v>84</v>
       </c>
       <c r="B80" s="9">
-        <v>546.95000000000005</v>
+        <v>574.9</v>
       </c>
       <c r="C80" s="11">
-        <v>537.20000000000005</v>
+        <v>560.79999999999995</v>
       </c>
       <c r="D80" s="14">
-        <v>544.54999999999995</v>
+        <v>561.1</v>
       </c>
       <c r="E80" s="6">
-        <v>544.85</v>
+        <v>561.45000000000005</v>
       </c>
       <c r="F80" s="17">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G80" s="6">
-        <v>537.75</v>
+        <v>573.20000000000005</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2896,22 +2896,22 @@
         <v>85</v>
       </c>
       <c r="B81" s="9">
-        <v>1749.5</v>
+        <v>1825.95</v>
       </c>
       <c r="C81" s="11">
-        <v>1734</v>
+        <v>1766.3</v>
       </c>
       <c r="D81" s="14">
-        <v>1746.9</v>
+        <v>1819.2</v>
       </c>
       <c r="E81" s="6">
-        <v>1744</v>
+        <v>1818.55</v>
       </c>
       <c r="F81" s="17">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="G81" s="6">
-        <v>1736.6</v>
+        <v>1768.95</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2919,22 +2919,22 @@
         <v>86</v>
       </c>
       <c r="B82" s="9">
-        <v>2726.95</v>
+        <v>2754.3</v>
       </c>
       <c r="C82" s="11">
-        <v>2680</v>
+        <v>2688</v>
       </c>
       <c r="D82" s="14">
-        <v>2687</v>
+        <v>2695.1</v>
       </c>
       <c r="E82" s="6">
-        <v>2687.5</v>
+        <v>2691.2</v>
       </c>
       <c r="F82" s="17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G82" s="6">
-        <v>2705.05</v>
+        <v>2746</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2942,22 +2942,22 @@
         <v>87</v>
       </c>
       <c r="B83" s="9">
-        <v>378.9</v>
+        <v>380.95</v>
       </c>
       <c r="C83" s="11">
-        <v>372.1</v>
+        <v>376.65</v>
       </c>
       <c r="D83" s="14">
-        <v>372.7</v>
+        <v>379.8</v>
       </c>
       <c r="E83" s="6">
-        <v>372.75</v>
+        <v>379.25</v>
       </c>
       <c r="F83" s="17">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G83" s="6">
-        <v>377.2</v>
+        <v>379.6</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2965,22 +2965,22 @@
         <v>88</v>
       </c>
       <c r="B84" s="9">
-        <v>460.9</v>
+        <v>510.6</v>
       </c>
       <c r="C84" s="11">
-        <v>453</v>
+        <v>497.1</v>
       </c>
       <c r="D84" s="14">
-        <v>454.5</v>
+        <v>504.95</v>
       </c>
       <c r="E84" s="6">
-        <v>454.65</v>
+        <v>507.55</v>
       </c>
       <c r="F84" s="17">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="G84" s="6">
-        <v>457</v>
+        <v>498.95</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2988,22 +2988,22 @@
         <v>89</v>
       </c>
       <c r="B85" s="9">
-        <v>5507.7</v>
+        <v>5620</v>
       </c>
       <c r="C85" s="11">
-        <v>5437.75</v>
+        <v>5550</v>
       </c>
       <c r="D85" s="14">
-        <v>5466.05</v>
+        <v>5583</v>
       </c>
       <c r="E85" s="6">
-        <v>5472.6</v>
+        <v>5577.4</v>
       </c>
       <c r="F85" s="17">
         <v>1</v>
       </c>
       <c r="G85" s="6">
-        <v>5498.75</v>
+        <v>5604.25</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3011,22 +3011,22 @@
         <v>90</v>
       </c>
       <c r="B86" s="9">
-        <v>4603</v>
+        <v>4798.95</v>
       </c>
       <c r="C86" s="11">
-        <v>4519.7</v>
+        <v>4727.6000000000004</v>
       </c>
       <c r="D86" s="14">
-        <v>4556.5</v>
+        <v>4748.8999999999996</v>
       </c>
       <c r="E86" s="6">
-        <v>4568.55</v>
+        <v>4748.1000000000004</v>
       </c>
       <c r="F86" s="17">
         <v>1</v>
       </c>
       <c r="G86" s="6">
-        <v>4534.7</v>
+        <v>4794.6000000000004</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3034,22 +3034,22 @@
         <v>91</v>
       </c>
       <c r="B87" s="9">
-        <v>1245</v>
+        <v>1293.1500000000001</v>
       </c>
       <c r="C87" s="11">
-        <v>1214</v>
+        <v>1256</v>
       </c>
       <c r="D87" s="14">
-        <v>1242.8499999999999</v>
+        <v>1262.5</v>
       </c>
       <c r="E87" s="6">
-        <v>1243.2</v>
+        <v>1260.55</v>
       </c>
       <c r="F87" s="17">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G87" s="6">
-        <v>1227.9000000000001</v>
+        <v>1287.5</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3057,22 +3057,22 @@
         <v>92</v>
       </c>
       <c r="B88" s="9">
-        <v>273.8</v>
+        <v>281.35000000000002</v>
       </c>
       <c r="C88" s="11">
-        <v>263.5</v>
+        <v>276.10000000000002</v>
       </c>
       <c r="D88" s="14">
-        <v>263.89999999999998</v>
+        <v>278.05</v>
       </c>
       <c r="E88" s="6">
-        <v>263.89999999999998</v>
+        <v>277.7</v>
       </c>
       <c r="F88" s="17">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G88" s="6">
-        <v>273.45</v>
+        <v>277.7</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3080,22 +3080,22 @@
         <v>93</v>
       </c>
       <c r="B89" s="9">
-        <v>154</v>
+        <v>170.4</v>
       </c>
       <c r="C89" s="11">
-        <v>147.15</v>
+        <v>166.75</v>
       </c>
       <c r="D89" s="14">
-        <v>148.94999999999999</v>
+        <v>167.5</v>
       </c>
       <c r="E89" s="6">
-        <v>148.15</v>
+        <v>167.35</v>
       </c>
       <c r="F89" s="17">
-        <v>104</v>
+        <v>157</v>
       </c>
       <c r="G89" s="6">
-        <v>153.6</v>
+        <v>168.3</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3103,22 +3103,22 @@
         <v>94</v>
       </c>
       <c r="B90" s="9">
-        <v>534.5</v>
+        <v>541</v>
       </c>
       <c r="C90" s="11">
-        <v>521.79999999999995</v>
+        <v>534.4</v>
       </c>
       <c r="D90" s="14">
-        <v>523.35</v>
+        <v>536.6</v>
       </c>
       <c r="E90" s="6">
-        <v>523.65</v>
+        <v>536</v>
       </c>
       <c r="F90" s="17">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G90" s="6">
-        <v>531.65</v>
+        <v>539.1</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3126,22 +3126,22 @@
         <v>95</v>
       </c>
       <c r="B91" s="9">
-        <v>1064.55</v>
+        <v>1055.95</v>
       </c>
       <c r="C91" s="11">
-        <v>1040</v>
+        <v>1046.75</v>
       </c>
       <c r="D91" s="14">
-        <v>1041</v>
+        <v>1050</v>
       </c>
       <c r="E91" s="6">
-        <v>1042.5</v>
+        <v>1050.3499999999999</v>
       </c>
       <c r="F91" s="17">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G91" s="6">
-        <v>1057.9000000000001</v>
+        <v>1053.5999999999999</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3149,22 +3149,22 @@
         <v>96</v>
       </c>
       <c r="B92" s="9">
-        <v>2979.95</v>
+        <v>3159.5</v>
       </c>
       <c r="C92" s="11">
-        <v>2913.3</v>
+        <v>3063.75</v>
       </c>
       <c r="D92" s="14">
-        <v>2920.1</v>
+        <v>3095</v>
       </c>
       <c r="E92" s="6">
-        <v>2927.35</v>
+        <v>3090.15</v>
       </c>
       <c r="F92" s="17">
         <v>10</v>
       </c>
       <c r="G92" s="6">
-        <v>2921.45</v>
+        <v>3135.65</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3172,22 +3172,22 @@
         <v>97</v>
       </c>
       <c r="B93" s="9">
-        <v>1670</v>
+        <v>1705.4</v>
       </c>
       <c r="C93" s="11">
-        <v>1640.85</v>
+        <v>1676</v>
       </c>
       <c r="D93" s="14">
-        <v>1651</v>
+        <v>1680.5</v>
       </c>
       <c r="E93" s="6">
-        <v>1658.2</v>
+        <v>1684.55</v>
       </c>
       <c r="F93" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G93" s="6">
-        <v>1654</v>
+        <v>1697.05</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3195,22 +3195,22 @@
         <v>98</v>
       </c>
       <c r="B94" s="9">
-        <v>980.9</v>
+        <v>1027.55</v>
       </c>
       <c r="C94" s="11">
-        <v>958.1</v>
+        <v>1004</v>
       </c>
       <c r="D94" s="14">
-        <v>970</v>
+        <v>1024.75</v>
       </c>
       <c r="E94" s="6">
-        <v>969.35</v>
+        <v>1023.35</v>
       </c>
       <c r="F94" s="17">
         <v>5</v>
       </c>
       <c r="G94" s="6">
-        <v>975</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3218,22 +3218,22 @@
         <v>99</v>
       </c>
       <c r="B95" s="9">
-        <v>1030.1500000000001</v>
+        <v>1112.95</v>
       </c>
       <c r="C95" s="11">
-        <v>1021.55</v>
+        <v>1065</v>
       </c>
       <c r="D95" s="14">
-        <v>1021.55</v>
+        <v>1098</v>
       </c>
       <c r="E95" s="6">
-        <v>1024.55</v>
+        <v>1098.75</v>
       </c>
       <c r="F95" s="17">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G95" s="6">
-        <v>1026.55</v>
+        <v>1066.6500000000001</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -3241,22 +3241,22 @@
         <v>100</v>
       </c>
       <c r="B96" s="9">
-        <v>2355.4499999999998</v>
+        <v>2394.9</v>
       </c>
       <c r="C96" s="11">
-        <v>2287</v>
+        <v>2361.9499999999998</v>
       </c>
       <c r="D96" s="14">
-        <v>2294.35</v>
+        <v>2378</v>
       </c>
       <c r="E96" s="6">
-        <v>2319.4</v>
+        <v>2371.3000000000002</v>
       </c>
       <c r="F96" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G96" s="6">
-        <v>2350</v>
+        <v>2381.25</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -3264,22 +3264,22 @@
         <v>101</v>
       </c>
       <c r="B97" s="9">
-        <v>1340.3</v>
+        <v>1470</v>
       </c>
       <c r="C97" s="11">
-        <v>1321</v>
+        <v>1453</v>
       </c>
       <c r="D97" s="14">
-        <v>1323</v>
+        <v>1464.15</v>
       </c>
       <c r="E97" s="6">
-        <v>1324.95</v>
+        <v>1464.85</v>
       </c>
       <c r="F97" s="17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G97" s="6">
-        <v>1338.1</v>
+        <v>1464.4</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3287,22 +3287,22 @@
         <v>102</v>
       </c>
       <c r="B98" s="9">
-        <v>420</v>
+        <v>443.85</v>
       </c>
       <c r="C98" s="11">
-        <v>404.1</v>
+        <v>433</v>
       </c>
       <c r="D98" s="14">
-        <v>406</v>
+        <v>439.45</v>
       </c>
       <c r="E98" s="6">
-        <v>407.15</v>
+        <v>441.45</v>
       </c>
       <c r="F98" s="17">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G98" s="6">
-        <v>419.9</v>
+        <v>434</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3310,22 +3310,22 @@
         <v>103</v>
       </c>
       <c r="B99" s="9">
-        <v>4624</v>
+        <v>4644.1499999999996</v>
       </c>
       <c r="C99" s="11">
-        <v>4581.1000000000004</v>
+        <v>4570.3500000000004</v>
       </c>
       <c r="D99" s="14">
-        <v>4586</v>
+        <v>4593</v>
       </c>
       <c r="E99" s="6">
-        <v>4596.8999999999996</v>
+        <v>4596.3500000000004</v>
       </c>
       <c r="F99" s="17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G99" s="6">
-        <v>4608.8999999999996</v>
+        <v>4615.25</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3333,22 +3333,22 @@
         <v>104</v>
       </c>
       <c r="B100" s="9">
-        <v>3744.45</v>
+        <v>3765.65</v>
       </c>
       <c r="C100" s="11">
-        <v>3702</v>
+        <v>3732.2</v>
       </c>
       <c r="D100" s="14">
-        <v>3730</v>
+        <v>3742</v>
       </c>
       <c r="E100" s="6">
-        <v>3732.75</v>
+        <v>3740.1</v>
       </c>
       <c r="F100" s="17">
         <v>1</v>
       </c>
       <c r="G100" s="6">
-        <v>3740.1</v>
+        <v>3755</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3356,22 +3356,22 @@
         <v>105</v>
       </c>
       <c r="B101" s="9">
-        <v>177.35</v>
+        <v>185.85</v>
       </c>
       <c r="C101" s="11">
-        <v>172.45</v>
+        <v>183.3</v>
       </c>
       <c r="D101" s="14">
-        <v>173.95</v>
+        <v>184</v>
       </c>
       <c r="E101" s="6">
-        <v>173.2</v>
+        <v>184.05</v>
       </c>
       <c r="F101" s="17">
-        <v>236</v>
+        <v>105</v>
       </c>
       <c r="G101" s="6">
-        <v>175.8</v>
+        <v>184.05</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3379,22 +3379,22 @@
         <v>106</v>
       </c>
       <c r="B102" s="9">
-        <v>256.85000000000002</v>
+        <v>277.35000000000002</v>
       </c>
       <c r="C102" s="11">
-        <v>253.55</v>
+        <v>273.25</v>
       </c>
       <c r="D102" s="14">
-        <v>253.8</v>
+        <v>274.89999999999998</v>
       </c>
       <c r="E102" s="6">
-        <v>253.9</v>
+        <v>274.8</v>
       </c>
       <c r="F102" s="17">
-        <v>71</v>
+        <v>204</v>
       </c>
       <c r="G102" s="6">
-        <v>254.35</v>
+        <v>274.35000000000002</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3402,22 +3402,22 @@
         <v>107</v>
       </c>
       <c r="B103" s="9">
-        <v>1410.5</v>
+        <v>1455.95</v>
       </c>
       <c r="C103" s="11">
-        <v>1383.45</v>
+        <v>1410</v>
       </c>
       <c r="D103" s="14">
-        <v>1390.95</v>
+        <v>1437.35</v>
       </c>
       <c r="E103" s="6">
-        <v>1389.95</v>
+        <v>1438.8</v>
       </c>
       <c r="F103" s="17">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G103" s="6">
-        <v>1400.6</v>
+        <v>1413.15</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3425,22 +3425,22 @@
         <v>108</v>
       </c>
       <c r="B104" s="9">
-        <v>907</v>
+        <v>945.95</v>
       </c>
       <c r="C104" s="11">
-        <v>889</v>
+        <v>936</v>
       </c>
       <c r="D104" s="14">
-        <v>890.6</v>
+        <v>941.5</v>
       </c>
       <c r="E104" s="6">
-        <v>890.9</v>
+        <v>940.15</v>
       </c>
       <c r="F104" s="17">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G104" s="6">
-        <v>906.85</v>
+        <v>938.25</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3448,22 +3448,22 @@
         <v>109</v>
       </c>
       <c r="B105" s="9">
-        <v>6469.9</v>
+        <v>6508</v>
       </c>
       <c r="C105" s="11">
-        <v>6326.7</v>
+        <v>6396.7</v>
       </c>
       <c r="D105" s="14">
-        <v>6360</v>
+        <v>6484</v>
       </c>
       <c r="E105" s="6">
-        <v>6390.35</v>
+        <v>6441.45</v>
       </c>
       <c r="F105" s="17">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G105" s="6">
-        <v>6444</v>
+        <v>6440.95</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3471,22 +3471,22 @@
         <v>110</v>
       </c>
       <c r="B106" s="9">
-        <v>196.3</v>
+        <v>206.95</v>
       </c>
       <c r="C106" s="11">
-        <v>195</v>
+        <v>203.95</v>
       </c>
       <c r="D106" s="14">
-        <v>195.2</v>
+        <v>205.55</v>
       </c>
       <c r="E106" s="6">
-        <v>195.3</v>
+        <v>205.15</v>
       </c>
       <c r="F106" s="17">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="G106" s="6">
-        <v>196</v>
+        <v>204.2</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3494,22 +3494,22 @@
         <v>111</v>
       </c>
       <c r="B107" s="9">
-        <v>2510</v>
+        <v>2572.0500000000002</v>
       </c>
       <c r="C107" s="11">
-        <v>2482</v>
+        <v>2546</v>
       </c>
       <c r="D107" s="14">
-        <v>2509.65</v>
+        <v>2554.9499999999998</v>
       </c>
       <c r="E107" s="6">
-        <v>2504.1</v>
+        <v>2553.4499999999998</v>
       </c>
       <c r="F107" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G107" s="6">
-        <v>2505</v>
+        <v>2567</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3517,22 +3517,22 @@
         <v>112</v>
       </c>
       <c r="B108" s="9">
-        <v>5311.45</v>
+        <v>5355.7</v>
       </c>
       <c r="C108" s="11">
-        <v>5204.55</v>
+        <v>5288</v>
       </c>
       <c r="D108" s="14">
-        <v>5265</v>
+        <v>5344</v>
       </c>
       <c r="E108" s="6">
-        <v>5280.2</v>
+        <v>5341.6</v>
       </c>
       <c r="F108" s="17">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G108" s="6">
-        <v>5255</v>
+        <v>5313</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -3540,22 +3540,22 @@
         <v>113</v>
       </c>
       <c r="B109" s="9">
-        <v>212.1</v>
+        <v>213.2</v>
       </c>
       <c r="C109" s="11">
-        <v>209.5</v>
+        <v>211.75</v>
       </c>
       <c r="D109" s="14">
-        <v>209.8</v>
+        <v>213</v>
       </c>
       <c r="E109" s="6">
-        <v>210.45</v>
+        <v>212.9</v>
       </c>
       <c r="F109" s="17">
-        <v>72</v>
+        <v>279</v>
       </c>
       <c r="G109" s="6">
-        <v>212</v>
+        <v>212.05</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -3563,22 +3563,22 @@
         <v>114</v>
       </c>
       <c r="B110" s="9">
-        <v>146.55000000000001</v>
+        <v>145.94999999999999</v>
       </c>
       <c r="C110" s="11">
-        <v>142.5</v>
+        <v>144.1</v>
       </c>
       <c r="D110" s="14">
-        <v>143.69999999999999</v>
+        <v>144.85</v>
       </c>
       <c r="E110" s="6">
-        <v>143.5</v>
+        <v>144.69999999999999</v>
       </c>
       <c r="F110" s="17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G110" s="6">
-        <v>146.4</v>
+        <v>145.15</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -3586,22 +3586,22 @@
         <v>115</v>
       </c>
       <c r="B111" s="9">
-        <v>974.45</v>
+        <v>1038.1500000000001</v>
       </c>
       <c r="C111" s="11">
-        <v>959.1</v>
+        <v>1002.25</v>
       </c>
       <c r="D111" s="14">
-        <v>960.1</v>
+        <v>1033</v>
       </c>
       <c r="E111" s="6">
-        <v>961.85</v>
+        <v>1032.4000000000001</v>
       </c>
       <c r="F111" s="17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G111" s="6">
-        <v>967.85</v>
+        <v>1011.7</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -3609,22 +3609,22 @@
         <v>116</v>
       </c>
       <c r="B112" s="9">
-        <v>239.35</v>
+        <v>244</v>
       </c>
       <c r="C112" s="11">
-        <v>233.25</v>
+        <v>237</v>
       </c>
       <c r="D112" s="14">
-        <v>235.5</v>
+        <v>243</v>
       </c>
       <c r="E112" s="6">
-        <v>234.5</v>
+        <v>242.45</v>
       </c>
       <c r="F112" s="17">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="G112" s="6">
-        <v>238.9</v>
+        <v>237.9</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3632,22 +3632,22 @@
         <v>117</v>
       </c>
       <c r="B113" s="9">
-        <v>342.2</v>
+        <v>394.8</v>
       </c>
       <c r="C113" s="11">
-        <v>337.3</v>
+        <v>376.15</v>
       </c>
       <c r="D113" s="14">
-        <v>337.7</v>
+        <v>389.45</v>
       </c>
       <c r="E113" s="6">
-        <v>337.95</v>
+        <v>389.8</v>
       </c>
       <c r="F113" s="17">
-        <v>74</v>
+        <v>260</v>
       </c>
       <c r="G113" s="6">
-        <v>341.75</v>
+        <v>377.5</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -3655,22 +3655,22 @@
         <v>118</v>
       </c>
       <c r="B114" s="9">
-        <v>744.35</v>
+        <v>756</v>
       </c>
       <c r="C114" s="11">
-        <v>735.55</v>
+        <v>748.2</v>
       </c>
       <c r="D114" s="14">
-        <v>739.1</v>
+        <v>753</v>
       </c>
       <c r="E114" s="6">
-        <v>739.15</v>
+        <v>751.7</v>
       </c>
       <c r="F114" s="17">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G114" s="6">
-        <v>741.9</v>
+        <v>750.55</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3678,22 +3678,22 @@
         <v>119</v>
       </c>
       <c r="B115" s="9">
-        <v>1412.75</v>
+        <v>1458.7</v>
       </c>
       <c r="C115" s="11">
-        <v>1401.05</v>
+        <v>1415</v>
       </c>
       <c r="D115" s="14">
-        <v>1404.75</v>
+        <v>1456.2</v>
       </c>
       <c r="E115" s="6">
-        <v>1409.7</v>
+        <v>1454</v>
       </c>
       <c r="F115" s="17">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="G115" s="6">
-        <v>1409.75</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -3701,22 +3701,22 @@
         <v>120</v>
       </c>
       <c r="B116" s="9">
-        <v>3641.85</v>
+        <v>3837.95</v>
       </c>
       <c r="C116" s="11">
-        <v>3608.05</v>
+        <v>3740.6</v>
       </c>
       <c r="D116" s="14">
-        <v>3618</v>
+        <v>3800</v>
       </c>
       <c r="E116" s="6">
-        <v>3628.6</v>
+        <v>3807.2</v>
       </c>
       <c r="F116" s="17">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G116" s="6">
-        <v>3627.4</v>
+        <v>3820.8</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -3724,22 +3724,22 @@
         <v>121</v>
       </c>
       <c r="B117" s="9">
-        <v>2383.25</v>
+        <v>2444.4</v>
       </c>
       <c r="C117" s="11">
-        <v>2350.6</v>
+        <v>2412.85</v>
       </c>
       <c r="D117" s="14">
-        <v>2354</v>
+        <v>2429</v>
       </c>
       <c r="E117" s="6">
-        <v>2359.4</v>
+        <v>2427.4499999999998</v>
       </c>
       <c r="F117" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G117" s="6">
-        <v>2366.15</v>
+        <v>2433.5</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -3747,22 +3747,22 @@
         <v>122</v>
       </c>
       <c r="B118" s="9">
-        <v>505.9</v>
+        <v>508</v>
       </c>
       <c r="C118" s="11">
-        <v>495.1</v>
+        <v>495.4</v>
       </c>
       <c r="D118" s="14">
-        <v>495.5</v>
+        <v>496</v>
       </c>
       <c r="E118" s="6">
-        <v>496.05</v>
+        <v>496.25</v>
       </c>
       <c r="F118" s="17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G118" s="6">
-        <v>497</v>
+        <v>508</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -3770,22 +3770,22 @@
         <v>123</v>
       </c>
       <c r="B119" s="9">
-        <v>1209.5999999999999</v>
+        <v>1238.9000000000001</v>
       </c>
       <c r="C119" s="11">
-        <v>1192.8</v>
+        <v>1220.5</v>
       </c>
       <c r="D119" s="14">
-        <v>1194.05</v>
+        <v>1230</v>
       </c>
       <c r="E119" s="6">
-        <v>1195.45</v>
+        <v>1231.1500000000001</v>
       </c>
       <c r="F119" s="17">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G119" s="6">
-        <v>1202</v>
+        <v>1232.7</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -3793,22 +3793,22 @@
         <v>124</v>
       </c>
       <c r="B120" s="9">
-        <v>759.5</v>
+        <v>749.5</v>
       </c>
       <c r="C120" s="11">
-        <v>744.3</v>
+        <v>735.6</v>
       </c>
       <c r="D120" s="14">
-        <v>746.4</v>
+        <v>746.55</v>
       </c>
       <c r="E120" s="6">
-        <v>745.55</v>
+        <v>745.35</v>
       </c>
       <c r="F120" s="17">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G120" s="6">
-        <v>749.95</v>
+        <v>748</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -3816,22 +3816,22 @@
         <v>125</v>
       </c>
       <c r="B121" s="9">
-        <v>1769.3</v>
+        <v>1675</v>
       </c>
       <c r="C121" s="11">
-        <v>1717.5</v>
+        <v>1656.9</v>
       </c>
       <c r="D121" s="14">
-        <v>1723</v>
+        <v>1665</v>
       </c>
       <c r="E121" s="6">
-        <v>1723.75</v>
+        <v>1662.85</v>
       </c>
       <c r="F121" s="17">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="G121" s="6">
-        <v>1727.65</v>
+        <v>1667.85</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -3839,22 +3839,22 @@
         <v>126</v>
       </c>
       <c r="B122" s="9">
-        <v>678.55</v>
+        <v>709.9</v>
       </c>
       <c r="C122" s="11">
-        <v>671.25</v>
+        <v>704.8</v>
       </c>
       <c r="D122" s="14">
-        <v>673.5</v>
+        <v>706.1</v>
       </c>
       <c r="E122" s="6">
-        <v>673.7</v>
+        <v>705.6</v>
       </c>
       <c r="F122" s="17">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="G122" s="6">
-        <v>678</v>
+        <v>707.35</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -3862,22 +3862,22 @@
         <v>127</v>
       </c>
       <c r="B123" s="9">
-        <v>1214</v>
+        <v>1235.95</v>
       </c>
       <c r="C123" s="11">
-        <v>1195.0999999999999</v>
+        <v>1218</v>
       </c>
       <c r="D123" s="14">
-        <v>1197.2</v>
+        <v>1224.9000000000001</v>
       </c>
       <c r="E123" s="6">
-        <v>1197.8499999999999</v>
+        <v>1223.9000000000001</v>
       </c>
       <c r="F123" s="17">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G123" s="6">
-        <v>1212</v>
+        <v>1231.5999999999999</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -3885,22 +3885,22 @@
         <v>128</v>
       </c>
       <c r="B124" s="9">
-        <v>2129</v>
+        <v>2160.65</v>
       </c>
       <c r="C124" s="11">
-        <v>2083.3000000000002</v>
+        <v>2112.3000000000002</v>
       </c>
       <c r="D124" s="14">
-        <v>2084.75</v>
+        <v>2131.4</v>
       </c>
       <c r="E124" s="6">
-        <v>2090.8000000000002</v>
+        <v>2133.6</v>
       </c>
       <c r="F124" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G124" s="6">
-        <v>2117.6</v>
+        <v>2148.0500000000002</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -3908,22 +3908,22 @@
         <v>129</v>
       </c>
       <c r="B125" s="9">
-        <v>827.5</v>
+        <v>971.6</v>
       </c>
       <c r="C125" s="11">
-        <v>796.9</v>
+        <v>944.05</v>
       </c>
       <c r="D125" s="14">
-        <v>815</v>
+        <v>966</v>
       </c>
       <c r="E125" s="6">
-        <v>816</v>
+        <v>967.3</v>
       </c>
       <c r="F125" s="17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G125" s="6">
-        <v>796.9</v>
+        <v>956.05</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -3931,22 +3931,22 @@
         <v>130</v>
       </c>
       <c r="B126" s="9">
-        <v>2666.35</v>
+        <v>2836.85</v>
       </c>
       <c r="C126" s="11">
-        <v>2640</v>
+        <v>2772.25</v>
       </c>
       <c r="D126" s="14">
-        <v>2644</v>
+        <v>2810</v>
       </c>
       <c r="E126" s="6">
-        <v>2649.7</v>
+        <v>2816.85</v>
       </c>
       <c r="F126" s="17">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G126" s="6">
-        <v>2660.9</v>
+        <v>2797.95</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -3954,22 +3954,22 @@
         <v>131</v>
       </c>
       <c r="B127" s="9">
-        <v>1818.4</v>
+        <v>1915</v>
       </c>
       <c r="C127" s="11">
-        <v>1786.1</v>
+        <v>1890</v>
       </c>
       <c r="D127" s="14">
-        <v>1800.05</v>
+        <v>1907</v>
       </c>
       <c r="E127" s="6">
-        <v>1799.95</v>
+        <v>1903.95</v>
       </c>
       <c r="F127" s="17">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G127" s="6">
-        <v>1786.1</v>
+        <v>1909.85</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -3977,22 +3977,22 @@
         <v>132</v>
       </c>
       <c r="B128" s="9">
-        <v>1636.5</v>
+        <v>1708.9</v>
       </c>
       <c r="C128" s="11">
-        <v>1579.6</v>
+        <v>1674.8</v>
       </c>
       <c r="D128" s="14">
-        <v>1580</v>
+        <v>1704</v>
       </c>
       <c r="E128" s="6">
-        <v>1584.1</v>
+        <v>1702</v>
       </c>
       <c r="F128" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G128" s="6">
-        <v>1622.55</v>
+        <v>1675.5</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -4000,22 +4000,22 @@
         <v>133</v>
       </c>
       <c r="B129" s="9">
-        <v>8645.85</v>
+        <v>9340.7999999999993</v>
       </c>
       <c r="C129" s="11">
-        <v>8545.0499999999993</v>
+        <v>9090</v>
       </c>
       <c r="D129" s="14">
-        <v>8570</v>
+        <v>9295</v>
       </c>
       <c r="E129" s="6">
-        <v>8556.2000000000007</v>
+        <v>9317.75</v>
       </c>
       <c r="F129" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G129" s="6">
-        <v>8627.4500000000007</v>
+        <v>9113.1</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -4023,22 +4023,22 @@
         <v>134</v>
       </c>
       <c r="B130" s="9">
-        <v>566.9</v>
+        <v>584.85</v>
       </c>
       <c r="C130" s="11">
-        <v>558.04999999999995</v>
+        <v>577</v>
       </c>
       <c r="D130" s="14">
-        <v>558.95000000000005</v>
+        <v>578.9</v>
       </c>
       <c r="E130" s="6">
-        <v>558.95000000000005</v>
+        <v>578.9</v>
       </c>
       <c r="F130" s="17">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="G130" s="6">
-        <v>565.79999999999995</v>
+        <v>579.70000000000005</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -4046,22 +4046,22 @@
         <v>135</v>
       </c>
       <c r="B131" s="9">
-        <v>235.5</v>
+        <v>243.35</v>
       </c>
       <c r="C131" s="11">
-        <v>231.1</v>
+        <v>239.5</v>
       </c>
       <c r="D131" s="14">
-        <v>232.5</v>
+        <v>242.2</v>
       </c>
       <c r="E131" s="6">
-        <v>232.2</v>
+        <v>241.9</v>
       </c>
       <c r="F131" s="17">
-        <v>38</v>
+        <v>125</v>
       </c>
       <c r="G131" s="6">
-        <v>234.1</v>
+        <v>242</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -4069,22 +4069,22 @@
         <v>136</v>
       </c>
       <c r="B132" s="9">
-        <v>835.25</v>
+        <v>842.4</v>
       </c>
       <c r="C132" s="11">
-        <v>818.8</v>
+        <v>830.55</v>
       </c>
       <c r="D132" s="14">
-        <v>821.9</v>
+        <v>839.65</v>
       </c>
       <c r="E132" s="6">
-        <v>825</v>
+        <v>837.85</v>
       </c>
       <c r="F132" s="17">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G132" s="6">
-        <v>832.25</v>
+        <v>840.75</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -4092,22 +4092,22 @@
         <v>137</v>
       </c>
       <c r="B133" s="9">
-        <v>254.8</v>
+        <v>260.7</v>
       </c>
       <c r="C133" s="11">
-        <v>250.25</v>
+        <v>254.45</v>
       </c>
       <c r="D133" s="14">
-        <v>252.8</v>
+        <v>255.5</v>
       </c>
       <c r="E133" s="6">
-        <v>252.85</v>
+        <v>255.9</v>
       </c>
       <c r="F133" s="17">
-        <v>66</v>
+        <v>440</v>
       </c>
       <c r="G133" s="6">
-        <v>250.75</v>
+        <v>256.95</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4115,22 +4115,22 @@
         <v>138</v>
       </c>
       <c r="B134" s="19">
-        <v>648</v>
+        <v>642.35</v>
       </c>
       <c r="C134" s="12">
-        <v>638.5</v>
+        <v>630</v>
       </c>
       <c r="D134" s="15">
-        <v>639</v>
+        <v>635.20000000000005</v>
       </c>
       <c r="E134" s="7">
-        <v>639.9</v>
+        <v>633.4</v>
       </c>
       <c r="F134" s="18">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G134" s="7">
-        <v>639.1</v>
+        <v>640.29999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug where weekly hcl wouldnt compute if there was a gap in data
</commit_message>
<xml_diff>
--- a/algo high low.xlsx
+++ b/algo high low.xlsx
@@ -1043,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,22 +1079,22 @@
         <v>6</v>
       </c>
       <c r="B2" s="8">
-        <v>569.25</v>
+        <v>577.4</v>
       </c>
       <c r="C2" s="10">
-        <v>556</v>
+        <v>560</v>
       </c>
       <c r="D2" s="13">
-        <v>562</v>
+        <v>570</v>
       </c>
       <c r="E2" s="5">
-        <v>562.35</v>
+        <v>569.35</v>
       </c>
       <c r="F2" s="16">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G2" s="5">
-        <v>562.25</v>
+        <v>576.35</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1102,22 +1102,22 @@
         <v>7</v>
       </c>
       <c r="B3" s="9">
-        <v>4683</v>
+        <v>4832</v>
       </c>
       <c r="C3" s="11">
-        <v>4506</v>
+        <v>4684.45</v>
       </c>
       <c r="D3" s="14">
-        <v>4639</v>
+        <v>4749</v>
       </c>
       <c r="E3" s="6">
-        <v>4630.75</v>
+        <v>4746.8</v>
       </c>
       <c r="F3" s="17">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G3" s="6">
-        <v>4537.2</v>
+        <v>4831.95</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1125,22 +1125,22 @@
         <v>8</v>
       </c>
       <c r="B4" s="9">
-        <v>173.5</v>
+        <v>167.55</v>
       </c>
       <c r="C4" s="11">
-        <v>170.85</v>
+        <v>161.94999999999999</v>
       </c>
       <c r="D4" s="14">
-        <v>172.9</v>
+        <v>163.44999999999999</v>
       </c>
       <c r="E4" s="6">
-        <v>172.55</v>
+        <v>163.19999999999999</v>
       </c>
       <c r="F4" s="17">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="G4" s="6">
-        <v>171.2</v>
+        <v>167.25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1148,22 +1148,22 @@
         <v>9</v>
       </c>
       <c r="B5" s="9">
-        <v>234.8</v>
+        <v>241.2</v>
       </c>
       <c r="C5" s="11">
-        <v>231.05</v>
+        <v>231.2</v>
       </c>
       <c r="D5" s="14">
-        <v>232.45</v>
+        <v>234.6</v>
       </c>
       <c r="E5" s="6">
-        <v>232.45</v>
+        <v>233.95</v>
       </c>
       <c r="F5" s="17">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" s="6">
-        <v>234</v>
+        <v>241.1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1171,22 +1171,22 @@
         <v>10</v>
       </c>
       <c r="B6" s="9">
-        <v>2548.4</v>
+        <v>2927</v>
       </c>
       <c r="C6" s="11">
-        <v>2495</v>
+        <v>2760</v>
       </c>
       <c r="D6" s="14">
-        <v>2523</v>
+        <v>2829.9</v>
       </c>
       <c r="E6" s="6">
-        <v>2531.1999999999998</v>
+        <v>2822.15</v>
       </c>
       <c r="F6" s="17">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="G6" s="6">
-        <v>2514.0500000000002</v>
+        <v>2890.9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1194,22 +1194,22 @@
         <v>11</v>
       </c>
       <c r="B7" s="9">
-        <v>880</v>
+        <v>1051.0999999999999</v>
       </c>
       <c r="C7" s="11">
-        <v>862.2</v>
+        <v>992.3</v>
       </c>
       <c r="D7" s="14">
-        <v>878.7</v>
+        <v>1021.1</v>
       </c>
       <c r="E7" s="6">
-        <v>878.65</v>
+        <v>1022.95</v>
       </c>
       <c r="F7" s="17">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="G7" s="6">
-        <v>864.8</v>
+        <v>1044.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1217,22 +1217,22 @@
         <v>12</v>
       </c>
       <c r="B8" s="9">
-        <v>4650</v>
+        <v>4883.25</v>
       </c>
       <c r="C8" s="11">
-        <v>4601</v>
+        <v>4750.6000000000004</v>
       </c>
       <c r="D8" s="14">
-        <v>4615</v>
+        <v>4799</v>
       </c>
       <c r="E8" s="6">
-        <v>4613.1499999999996</v>
+        <v>4796.05</v>
       </c>
       <c r="F8" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G8" s="6">
-        <v>4624.05</v>
+        <v>4874.45</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1240,22 +1240,22 @@
         <v>13</v>
       </c>
       <c r="B9" s="9">
-        <v>475.8</v>
+        <v>506.25</v>
       </c>
       <c r="C9" s="11">
-        <v>453.75</v>
+        <v>482.35</v>
       </c>
       <c r="D9" s="14">
-        <v>474.5</v>
+        <v>494.4</v>
       </c>
       <c r="E9" s="6">
-        <v>474.55</v>
+        <v>494.35</v>
       </c>
       <c r="F9" s="17">
-        <v>131</v>
+        <v>40</v>
       </c>
       <c r="G9" s="6">
-        <v>455.65</v>
+        <v>505.4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1263,22 +1263,22 @@
         <v>14</v>
       </c>
       <c r="B10" s="9">
-        <v>5658.25</v>
+        <v>5572.55</v>
       </c>
       <c r="C10" s="11">
-        <v>5596.9</v>
+        <v>5439.05</v>
       </c>
       <c r="D10" s="14">
-        <v>5621.05</v>
+        <v>5540</v>
       </c>
       <c r="E10" s="6">
-        <v>5622.55</v>
+        <v>5555.35</v>
       </c>
       <c r="F10" s="17">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G10" s="6">
-        <v>5598.8</v>
+        <v>5521.3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1286,22 +1286,22 @@
         <v>15</v>
       </c>
       <c r="B11" s="9">
-        <v>450.75</v>
+        <v>465</v>
       </c>
       <c r="C11" s="11">
-        <v>442.75</v>
+        <v>453.4</v>
       </c>
       <c r="D11" s="14">
-        <v>450</v>
+        <v>459.4</v>
       </c>
       <c r="E11" s="6">
-        <v>449.95</v>
+        <v>458.55</v>
       </c>
       <c r="F11" s="17">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G11" s="6">
-        <v>444.85</v>
+        <v>462.85</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1309,22 +1309,22 @@
         <v>16</v>
       </c>
       <c r="B12" s="9">
-        <v>176.7</v>
+        <v>177.5</v>
       </c>
       <c r="C12" s="11">
-        <v>174.2</v>
+        <v>173.85</v>
       </c>
       <c r="D12" s="14">
-        <v>174.5</v>
+        <v>175</v>
       </c>
       <c r="E12" s="6">
-        <v>174.45</v>
+        <v>174.9</v>
       </c>
       <c r="F12" s="17">
-        <v>292</v>
+        <v>130</v>
       </c>
       <c r="G12" s="6">
-        <v>176</v>
+        <v>177.45</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1332,22 +1332,22 @@
         <v>17</v>
       </c>
       <c r="B13" s="9">
-        <v>2006</v>
+        <v>1979.35</v>
       </c>
       <c r="C13" s="11">
-        <v>1963.15</v>
+        <v>1918.25</v>
       </c>
       <c r="D13" s="14">
-        <v>1990</v>
+        <v>1930.65</v>
       </c>
       <c r="E13" s="6">
-        <v>1991</v>
+        <v>1928.75</v>
       </c>
       <c r="F13" s="17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G13" s="6">
-        <v>2002.9</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1355,22 +1355,22 @@
         <v>18</v>
       </c>
       <c r="B14" s="9">
-        <v>6836</v>
+        <v>6893</v>
       </c>
       <c r="C14" s="11">
-        <v>6621.15</v>
+        <v>6703.5</v>
       </c>
       <c r="D14" s="14">
-        <v>6775</v>
+        <v>6809.95</v>
       </c>
       <c r="E14" s="6">
-        <v>6747.05</v>
+        <v>6748.7</v>
       </c>
       <c r="F14" s="17">
         <v>0</v>
       </c>
       <c r="G14" s="6">
-        <v>6652.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1378,22 +1378,22 @@
         <v>19</v>
       </c>
       <c r="B15" s="9">
-        <v>755.6</v>
+        <v>748.55</v>
       </c>
       <c r="C15" s="11">
-        <v>742.85</v>
+        <v>734.25</v>
       </c>
       <c r="D15" s="14">
-        <v>754.7</v>
+        <v>739</v>
       </c>
       <c r="E15" s="6">
-        <v>753.75</v>
+        <v>740.5</v>
       </c>
       <c r="F15" s="17">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="G15" s="6">
-        <v>748.8</v>
+        <v>748.55</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1401,22 +1401,22 @@
         <v>20</v>
       </c>
       <c r="B16" s="9">
-        <v>1045</v>
+        <v>1031.95</v>
       </c>
       <c r="C16" s="11">
-        <v>1023.25</v>
+        <v>1004.55</v>
       </c>
       <c r="D16" s="14">
-        <v>1041.3</v>
+        <v>1018</v>
       </c>
       <c r="E16" s="6">
-        <v>1042.6500000000001</v>
+        <v>1017.4</v>
       </c>
       <c r="F16" s="17">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="G16" s="6">
-        <v>1032.25</v>
+        <v>1029.3499999999999</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1424,22 +1424,22 @@
         <v>21</v>
       </c>
       <c r="B17" s="9">
-        <v>1711.7</v>
+        <v>1714.55</v>
       </c>
       <c r="C17" s="11">
-        <v>1685.9</v>
+        <v>1692.5</v>
       </c>
       <c r="D17" s="14">
-        <v>1694</v>
+        <v>1711.5</v>
       </c>
       <c r="E17" s="6">
-        <v>1696.25</v>
+        <v>1710.15</v>
       </c>
       <c r="F17" s="17">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G17" s="6">
-        <v>1701</v>
+        <v>1709.4</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1447,22 +1447,22 @@
         <v>22</v>
       </c>
       <c r="B18" s="9">
-        <v>7420</v>
+        <v>7376.7</v>
       </c>
       <c r="C18" s="11">
-        <v>7315.05</v>
+        <v>7274</v>
       </c>
       <c r="D18" s="14">
-        <v>7405</v>
+        <v>7310</v>
       </c>
       <c r="E18" s="6">
-        <v>7407.65</v>
+        <v>7307.6</v>
       </c>
       <c r="F18" s="17">
         <v>11</v>
       </c>
       <c r="G18" s="6">
-        <v>7357.65</v>
+        <v>7376.7</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1470,22 +1470,22 @@
         <v>23</v>
       </c>
       <c r="B19" s="9">
-        <v>2571.25</v>
+        <v>2642.25</v>
       </c>
       <c r="C19" s="11">
-        <v>2529</v>
+        <v>2560.1999999999998</v>
       </c>
       <c r="D19" s="14">
-        <v>2553.1999999999998</v>
+        <v>2601</v>
       </c>
       <c r="E19" s="6">
-        <v>2560.8000000000002</v>
+        <v>2605.65</v>
       </c>
       <c r="F19" s="17">
         <v>2</v>
       </c>
       <c r="G19" s="6">
-        <v>2566.9499999999998</v>
+        <v>2637.2</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1493,22 +1493,22 @@
         <v>24</v>
       </c>
       <c r="B20" s="9">
-        <v>475.5</v>
+        <v>409.35</v>
       </c>
       <c r="C20" s="11">
-        <v>467.7</v>
+        <v>384</v>
       </c>
       <c r="D20" s="14">
-        <v>469.95</v>
+        <v>392.6</v>
       </c>
       <c r="E20" s="6">
-        <v>468.55</v>
+        <v>392.7</v>
       </c>
       <c r="F20" s="17">
-        <v>9</v>
+        <v>139</v>
       </c>
       <c r="G20" s="6">
-        <v>472.85</v>
+        <v>408.5</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1516,22 +1516,22 @@
         <v>25</v>
       </c>
       <c r="B21" s="9">
-        <v>234.85</v>
+        <v>238.6</v>
       </c>
       <c r="C21" s="11">
-        <v>229.25</v>
+        <v>233.75</v>
       </c>
       <c r="D21" s="14">
-        <v>234.5</v>
+        <v>236.8</v>
       </c>
       <c r="E21" s="6">
-        <v>234.3</v>
+        <v>237.05</v>
       </c>
       <c r="F21" s="17">
-        <v>141</v>
+        <v>67</v>
       </c>
       <c r="G21" s="6">
-        <v>230.85</v>
+        <v>238.55</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1539,22 +1539,22 @@
         <v>26</v>
       </c>
       <c r="B22" s="9">
-        <v>210</v>
+        <v>215.7</v>
       </c>
       <c r="C22" s="11">
-        <v>205.75</v>
+        <v>208.5</v>
       </c>
       <c r="D22" s="14">
-        <v>209</v>
+        <v>212.15</v>
       </c>
       <c r="E22" s="6">
-        <v>209.05</v>
+        <v>212</v>
       </c>
       <c r="F22" s="17">
-        <v>359</v>
+        <v>295</v>
       </c>
       <c r="G22" s="6">
-        <v>206.3</v>
+        <v>212.5</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1562,22 +1562,22 @@
         <v>27</v>
       </c>
       <c r="B23" s="9">
-        <v>1638.65</v>
+        <v>1670</v>
       </c>
       <c r="C23" s="11">
-        <v>1603.3</v>
+        <v>1628.45</v>
       </c>
       <c r="D23" s="14">
-        <v>1629.5</v>
+        <v>1655.35</v>
       </c>
       <c r="E23" s="6">
-        <v>1630</v>
+        <v>1663.35</v>
       </c>
       <c r="F23" s="17">
         <v>2</v>
       </c>
       <c r="G23" s="6">
-        <v>1626.65</v>
+        <v>1664.5</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1585,22 +1585,22 @@
         <v>28</v>
       </c>
       <c r="B24" s="9">
-        <v>157.5</v>
+        <v>161.5</v>
       </c>
       <c r="C24" s="11">
-        <v>151.69999999999999</v>
+        <v>157.30000000000001</v>
       </c>
       <c r="D24" s="14">
-        <v>153.75</v>
+        <v>158.69999999999999</v>
       </c>
       <c r="E24" s="6">
-        <v>153.55000000000001</v>
+        <v>158.75</v>
       </c>
       <c r="F24" s="17">
-        <v>514</v>
+        <v>228</v>
       </c>
       <c r="G24" s="6">
-        <v>152.05000000000001</v>
+        <v>161.15</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1608,22 +1608,22 @@
         <v>29</v>
       </c>
       <c r="B25" s="9">
-        <v>1168.6500000000001</v>
+        <v>1180.25</v>
       </c>
       <c r="C25" s="11">
-        <v>1155.05</v>
+        <v>1164.2</v>
       </c>
       <c r="D25" s="14">
-        <v>1159.75</v>
+        <v>1176</v>
       </c>
       <c r="E25" s="6">
-        <v>1157.2</v>
+        <v>1177.1500000000001</v>
       </c>
       <c r="F25" s="17">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G25" s="6">
-        <v>1166.45</v>
+        <v>1174.8499999999999</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1631,22 +1631,22 @@
         <v>30</v>
       </c>
       <c r="B26" s="9">
-        <v>241.9</v>
+        <v>243.5</v>
       </c>
       <c r="C26" s="11">
-        <v>238.9</v>
+        <v>236.9</v>
       </c>
       <c r="D26" s="14">
-        <v>240.9</v>
+        <v>239</v>
       </c>
       <c r="E26" s="6">
-        <v>240.65</v>
+        <v>239</v>
       </c>
       <c r="F26" s="17">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G26" s="6">
-        <v>241.4</v>
+        <v>243.35</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1654,22 +1654,22 @@
         <v>31</v>
       </c>
       <c r="B27" s="9">
-        <v>4954.8500000000004</v>
+        <v>5060</v>
       </c>
       <c r="C27" s="11">
-        <v>4915</v>
+        <v>4931</v>
       </c>
       <c r="D27" s="14">
-        <v>4934</v>
+        <v>4945</v>
       </c>
       <c r="E27" s="6">
-        <v>4937.75</v>
+        <v>4942.2</v>
       </c>
       <c r="F27" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G27" s="6">
-        <v>4949</v>
+        <v>5054.25</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1677,22 +1677,22 @@
         <v>32</v>
       </c>
       <c r="B28" s="9">
-        <v>639.54999999999995</v>
+        <v>667</v>
       </c>
       <c r="C28" s="11">
-        <v>631.4</v>
+        <v>648.04999999999995</v>
       </c>
       <c r="D28" s="14">
-        <v>635</v>
+        <v>658</v>
       </c>
       <c r="E28" s="6">
-        <v>635.15</v>
+        <v>657.75</v>
       </c>
       <c r="F28" s="17">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G28" s="6">
-        <v>636</v>
+        <v>657.7</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1700,22 +1700,22 @@
         <v>33</v>
       </c>
       <c r="B29" s="9">
-        <v>429</v>
+        <v>441</v>
       </c>
       <c r="C29" s="11">
-        <v>420.6</v>
+        <v>430.25</v>
       </c>
       <c r="D29" s="14">
-        <v>428</v>
+        <v>438.65</v>
       </c>
       <c r="E29" s="6">
-        <v>426.95</v>
+        <v>438.55</v>
       </c>
       <c r="F29" s="17">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="G29" s="6">
-        <v>421.85</v>
+        <v>436.4</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1723,22 +1723,22 @@
         <v>34</v>
       </c>
       <c r="B30" s="9">
-        <v>843</v>
+        <v>803.95</v>
       </c>
       <c r="C30" s="11">
-        <v>814.3</v>
+        <v>779.5</v>
       </c>
       <c r="D30" s="14">
-        <v>825.25</v>
+        <v>790.8</v>
       </c>
       <c r="E30" s="6">
-        <v>825.15</v>
+        <v>790.45</v>
       </c>
       <c r="F30" s="17">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="G30" s="6">
-        <v>824.2</v>
+        <v>800.9</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1746,22 +1746,22 @@
         <v>35</v>
       </c>
       <c r="B31" s="9">
-        <v>327</v>
+        <v>350.4</v>
       </c>
       <c r="C31" s="11">
-        <v>322</v>
+        <v>338.45</v>
       </c>
       <c r="D31" s="14">
-        <v>324.75</v>
+        <v>341.5</v>
       </c>
       <c r="E31" s="6">
-        <v>324.95</v>
+        <v>341.9</v>
       </c>
       <c r="F31" s="17">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="G31" s="6">
-        <v>324.10000000000002</v>
+        <v>349.7</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1769,22 +1769,22 @@
         <v>36</v>
       </c>
       <c r="B32" s="9">
-        <v>1161.95</v>
+        <v>1174.95</v>
       </c>
       <c r="C32" s="11">
-        <v>1141</v>
+        <v>1128.25</v>
       </c>
       <c r="D32" s="14">
-        <v>1150</v>
+        <v>1171</v>
       </c>
       <c r="E32" s="6">
-        <v>1148.75</v>
+        <v>1166.6500000000001</v>
       </c>
       <c r="F32" s="17">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G32" s="6">
-        <v>1151.2</v>
+        <v>1136.3</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1792,22 +1792,22 @@
         <v>37</v>
       </c>
       <c r="B33" s="9">
+        <v>1228.5</v>
+      </c>
+      <c r="C33" s="11">
+        <v>1204</v>
+      </c>
+      <c r="D33" s="14">
+        <v>1219</v>
+      </c>
+      <c r="E33" s="6">
         <v>1219.0999999999999</v>
       </c>
-      <c r="C33" s="11">
-        <v>1206.25</v>
-      </c>
-      <c r="D33" s="14">
-        <v>1218.5</v>
-      </c>
-      <c r="E33" s="6">
-        <v>1216.5</v>
-      </c>
       <c r="F33" s="17">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G33" s="6">
-        <v>1212.4000000000001</v>
+        <v>1225.05</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1815,22 +1815,22 @@
         <v>38</v>
       </c>
       <c r="B34" s="9">
-        <v>5754</v>
+        <v>5919.95</v>
       </c>
       <c r="C34" s="11">
-        <v>5655.05</v>
+        <v>5690.05</v>
       </c>
       <c r="D34" s="14">
-        <v>5671.15</v>
+        <v>5785</v>
       </c>
       <c r="E34" s="6">
-        <v>5675.95</v>
+        <v>5783</v>
       </c>
       <c r="F34" s="17">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G34" s="6">
-        <v>5716.95</v>
+        <v>5712</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1838,22 +1838,22 @@
         <v>39</v>
       </c>
       <c r="B35" s="9">
-        <v>804</v>
+        <v>851.4</v>
       </c>
       <c r="C35" s="11">
-        <v>787.8</v>
+        <v>830.1</v>
       </c>
       <c r="D35" s="14">
-        <v>800</v>
+        <v>844.95</v>
       </c>
       <c r="E35" s="6">
-        <v>800.9</v>
+        <v>843.2</v>
       </c>
       <c r="F35" s="17">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G35" s="6">
-        <v>795.2</v>
+        <v>847.7</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1861,22 +1861,22 @@
         <v>40</v>
       </c>
       <c r="B36" s="9">
-        <v>1181.9000000000001</v>
+        <v>1248</v>
       </c>
       <c r="C36" s="11">
-        <v>1162</v>
+        <v>1219.55</v>
       </c>
       <c r="D36" s="14">
-        <v>1178</v>
+        <v>1225.0999999999999</v>
       </c>
       <c r="E36" s="6">
-        <v>1178.0999999999999</v>
+        <v>1224.75</v>
       </c>
       <c r="F36" s="17">
         <v>2</v>
       </c>
       <c r="G36" s="6">
-        <v>1165.45</v>
+        <v>1247.95</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1884,22 +1884,22 @@
         <v>41</v>
       </c>
       <c r="B37" s="9">
-        <v>295.64999999999998</v>
+        <v>305.89999999999998</v>
       </c>
       <c r="C37" s="11">
-        <v>289.89999999999998</v>
+        <v>297.05</v>
       </c>
       <c r="D37" s="14">
-        <v>295.3</v>
+        <v>299.3</v>
       </c>
       <c r="E37" s="6">
-        <v>294.8</v>
+        <v>299.45</v>
       </c>
       <c r="F37" s="17">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G37" s="6">
-        <v>293.5</v>
+        <v>304.2</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1907,22 +1907,22 @@
         <v>42</v>
       </c>
       <c r="B38" s="9">
-        <v>1959.9</v>
+        <v>1965.5</v>
       </c>
       <c r="C38" s="11">
-        <v>1921.5</v>
+        <v>1927.05</v>
       </c>
       <c r="D38" s="14">
-        <v>1957.8</v>
+        <v>1953</v>
       </c>
       <c r="E38" s="6">
-        <v>1953.9</v>
+        <v>1949.35</v>
       </c>
       <c r="F38" s="17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G38" s="6">
-        <v>1937.7</v>
+        <v>1961.5</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1930,22 +1930,22 @@
         <v>43</v>
       </c>
       <c r="B39" s="9">
-        <v>548.9</v>
+        <v>556.15</v>
       </c>
       <c r="C39" s="11">
-        <v>541.70000000000005</v>
+        <v>545.79999999999995</v>
       </c>
       <c r="D39" s="14">
-        <v>547</v>
+        <v>548.25</v>
       </c>
       <c r="E39" s="6">
-        <v>547</v>
+        <v>547.5</v>
       </c>
       <c r="F39" s="17">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G39" s="6">
-        <v>543.6</v>
+        <v>556</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1953,22 +1953,22 @@
         <v>44</v>
       </c>
       <c r="B40" s="9">
-        <v>2328.9</v>
+        <v>2368.4</v>
       </c>
       <c r="C40" s="11">
-        <v>2274.8000000000002</v>
+        <v>2293.65</v>
       </c>
       <c r="D40" s="14">
-        <v>2305</v>
+        <v>2340</v>
       </c>
       <c r="E40" s="6">
-        <v>2307.5500000000002</v>
+        <v>2331.1999999999998</v>
       </c>
       <c r="F40" s="17">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G40" s="6">
-        <v>2294.9499999999998</v>
+        <v>2368.35</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1976,22 +1976,22 @@
         <v>45</v>
       </c>
       <c r="B41" s="9">
+        <v>668.95</v>
+      </c>
+      <c r="C41" s="11">
+        <v>640</v>
+      </c>
+      <c r="D41" s="14">
         <v>647.9</v>
-      </c>
-      <c r="C41" s="11">
-        <v>628.54999999999995</v>
-      </c>
-      <c r="D41" s="14">
-        <v>643.5</v>
       </c>
       <c r="E41" s="6">
         <v>645.1</v>
       </c>
       <c r="F41" s="17">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G41" s="6">
-        <v>634.35</v>
+        <v>664</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1999,22 +1999,22 @@
         <v>46</v>
       </c>
       <c r="B42" s="9">
-        <v>2227</v>
+        <v>2262.9499999999998</v>
       </c>
       <c r="C42" s="11">
-        <v>2204.6</v>
+        <v>2182.1</v>
       </c>
       <c r="D42" s="14">
-        <v>2209.9499999999998</v>
+        <v>2217.9499999999998</v>
       </c>
       <c r="E42" s="6">
-        <v>2210.35</v>
+        <v>2215.25</v>
       </c>
       <c r="F42" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G42" s="6">
-        <v>2215.5</v>
+        <v>2261.9</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2022,22 +2022,22 @@
         <v>47</v>
       </c>
       <c r="B43" s="9">
-        <v>144.85</v>
+        <v>141.1</v>
       </c>
       <c r="C43" s="11">
-        <v>139.5</v>
+        <v>136.80000000000001</v>
       </c>
       <c r="D43" s="14">
-        <v>140.44999999999999</v>
+        <v>137.1</v>
       </c>
       <c r="E43" s="6">
-        <v>140.44999999999999</v>
+        <v>137.25</v>
       </c>
       <c r="F43" s="17">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="G43" s="6">
-        <v>144.4</v>
+        <v>140.94999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2045,22 +2045,22 @@
         <v>48</v>
       </c>
       <c r="B44" s="9">
-        <v>3835.05</v>
+        <v>3737</v>
       </c>
       <c r="C44" s="11">
-        <v>3790</v>
+        <v>3662.4</v>
       </c>
       <c r="D44" s="14">
-        <v>3800</v>
+        <v>3680</v>
       </c>
       <c r="E44" s="6">
-        <v>3798.1</v>
+        <v>3681.75</v>
       </c>
       <c r="F44" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G44" s="6">
-        <v>3820.55</v>
+        <v>3725.2</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2068,22 +2068,22 @@
         <v>49</v>
       </c>
       <c r="B45" s="9">
-        <v>6041.2</v>
+        <v>6025</v>
       </c>
       <c r="C45" s="11">
-        <v>5876</v>
+        <v>5893.4</v>
       </c>
       <c r="D45" s="14">
-        <v>6000</v>
+        <v>5970</v>
       </c>
       <c r="E45" s="6">
-        <v>6002.2</v>
+        <v>5964.9</v>
       </c>
       <c r="F45" s="17">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G45" s="6">
-        <v>6009.95</v>
+        <v>6005.95</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2091,22 +2091,22 @@
         <v>50</v>
       </c>
       <c r="B46" s="9">
-        <v>652</v>
+        <v>663.9</v>
       </c>
       <c r="C46" s="11">
-        <v>632.79999999999995</v>
+        <v>641.45000000000005</v>
       </c>
       <c r="D46" s="14">
-        <v>649.15</v>
+        <v>649.25</v>
       </c>
       <c r="E46" s="6">
-        <v>649.25</v>
+        <v>649.9</v>
       </c>
       <c r="F46" s="17">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G46" s="6">
-        <v>636.45000000000005</v>
+        <v>662.3</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2114,22 +2114,22 @@
         <v>51</v>
       </c>
       <c r="B47" s="9">
-        <v>5775</v>
+        <v>5778.15</v>
       </c>
       <c r="C47" s="11">
-        <v>5728.4</v>
+        <v>5712</v>
       </c>
       <c r="D47" s="14">
-        <v>5775</v>
+        <v>5768</v>
       </c>
       <c r="E47" s="6">
-        <v>5756</v>
+        <v>5763.9</v>
       </c>
       <c r="F47" s="17">
         <v>2</v>
       </c>
       <c r="G47" s="6">
-        <v>5748.6</v>
+        <v>5755.6</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2137,22 +2137,22 @@
         <v>52</v>
       </c>
       <c r="B48" s="9">
-        <v>3225</v>
+        <v>3259.05</v>
       </c>
       <c r="C48" s="11">
-        <v>3174.2</v>
+        <v>3110.65</v>
       </c>
       <c r="D48" s="14">
-        <v>3218.45</v>
+        <v>3146</v>
       </c>
       <c r="E48" s="6">
-        <v>3213.5</v>
+        <v>3145.3</v>
       </c>
       <c r="F48" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G48" s="6">
-        <v>3200</v>
+        <v>3259</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2160,22 +2160,22 @@
         <v>53</v>
       </c>
       <c r="B49" s="9">
-        <v>298.60000000000002</v>
+        <v>297</v>
       </c>
       <c r="C49" s="11">
-        <v>292.3</v>
+        <v>287.25</v>
       </c>
       <c r="D49" s="14">
-        <v>293.39999999999998</v>
+        <v>290.05</v>
       </c>
       <c r="E49" s="6">
-        <v>293.85000000000002</v>
+        <v>289.89999999999998</v>
       </c>
       <c r="F49" s="17">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="G49" s="6">
-        <v>295.14999999999998</v>
+        <v>296.45</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2183,22 +2183,22 @@
         <v>54</v>
       </c>
       <c r="B50" s="9">
-        <v>802</v>
+        <v>815.95</v>
       </c>
       <c r="C50" s="11">
-        <v>774</v>
+        <v>787.1</v>
       </c>
       <c r="D50" s="14">
-        <v>779.95</v>
+        <v>797.1</v>
       </c>
       <c r="E50" s="6">
-        <v>775.75</v>
+        <v>795.95</v>
       </c>
       <c r="F50" s="17">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G50" s="6">
-        <v>798.8</v>
+        <v>814.55</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2206,22 +2206,22 @@
         <v>55</v>
       </c>
       <c r="B51" s="9">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="C51" s="11">
-        <v>633.54999999999995</v>
+        <v>633.6</v>
       </c>
       <c r="D51" s="14">
-        <v>640</v>
+        <v>635.20000000000005</v>
       </c>
       <c r="E51" s="6">
-        <v>640.29999999999995</v>
+        <v>635</v>
       </c>
       <c r="F51" s="17">
         <v>0</v>
       </c>
       <c r="G51" s="6">
-        <v>637.15</v>
+        <v>633.6</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2229,22 +2229,22 @@
         <v>56</v>
       </c>
       <c r="B52" s="9">
-        <v>726.25</v>
+        <v>742.65</v>
       </c>
       <c r="C52" s="11">
-        <v>700.1</v>
+        <v>710.15</v>
       </c>
       <c r="D52" s="14">
-        <v>713.7</v>
+        <v>718.1</v>
       </c>
       <c r="E52" s="6">
-        <v>711.55</v>
+        <v>718.55</v>
       </c>
       <c r="F52" s="17">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G52" s="6">
-        <v>707.95</v>
+        <v>741.7</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2252,22 +2252,22 @@
         <v>57</v>
       </c>
       <c r="B53" s="9">
-        <v>1044</v>
+        <v>1026.95</v>
       </c>
       <c r="C53" s="11">
-        <v>1028.0999999999999</v>
+        <v>1015.7</v>
       </c>
       <c r="D53" s="14">
-        <v>1042</v>
+        <v>1025.95</v>
       </c>
       <c r="E53" s="6">
-        <v>1041.75</v>
+        <v>1021.55</v>
       </c>
       <c r="F53" s="17">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G53" s="6">
-        <v>1032.75</v>
+        <v>1024.5</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2275,22 +2275,22 @@
         <v>58</v>
       </c>
       <c r="B54" s="9">
-        <v>1943</v>
+        <v>1953.75</v>
       </c>
       <c r="C54" s="11">
-        <v>1872.95</v>
+        <v>1903.4</v>
       </c>
       <c r="D54" s="14">
-        <v>1918</v>
+        <v>1930</v>
       </c>
       <c r="E54" s="6">
-        <v>1915.6</v>
+        <v>1930.15</v>
       </c>
       <c r="F54" s="17">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G54" s="6">
-        <v>1883.6</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2298,22 +2298,22 @@
         <v>59</v>
       </c>
       <c r="B55" s="9">
-        <v>398.35</v>
+        <v>396.65</v>
       </c>
       <c r="C55" s="11">
-        <v>390.4</v>
+        <v>384.5</v>
       </c>
       <c r="D55" s="14">
-        <v>393</v>
+        <v>387.65</v>
       </c>
       <c r="E55" s="6">
-        <v>391.5</v>
+        <v>388.45</v>
       </c>
       <c r="F55" s="17">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G55" s="6">
-        <v>396.5</v>
+        <v>395.7</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2321,22 +2321,22 @@
         <v>60</v>
       </c>
       <c r="B56" s="9">
-        <v>2059.9</v>
+        <v>2099.3000000000002</v>
       </c>
       <c r="C56" s="11">
-        <v>2028.45</v>
+        <v>2042.65</v>
       </c>
       <c r="D56" s="14">
-        <v>2051.9</v>
+        <v>2070</v>
       </c>
       <c r="E56" s="6">
-        <v>2052.9499999999998</v>
+        <v>2070.0500000000002</v>
       </c>
       <c r="F56" s="17">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G56" s="6">
-        <v>2042.75</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2344,22 +2344,22 @@
         <v>61</v>
       </c>
       <c r="B57" s="9">
-        <v>444.7</v>
+        <v>446</v>
       </c>
       <c r="C57" s="11">
-        <v>436.1</v>
+        <v>439.45</v>
       </c>
       <c r="D57" s="14">
-        <v>442</v>
+        <v>441.9</v>
       </c>
       <c r="E57" s="6">
-        <v>441.85</v>
+        <v>440.3</v>
       </c>
       <c r="F57" s="17">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G57" s="6">
-        <v>436.45</v>
+        <v>444.05</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2367,22 +2367,22 @@
         <v>62</v>
       </c>
       <c r="B58" s="9">
-        <v>2532.8000000000002</v>
+        <v>2765</v>
       </c>
       <c r="C58" s="11">
-        <v>2473</v>
+        <v>2690.05</v>
       </c>
       <c r="D58" s="14">
-        <v>2524.9</v>
+        <v>2738</v>
       </c>
       <c r="E58" s="6">
-        <v>2519.4</v>
+        <v>2733.65</v>
       </c>
       <c r="F58" s="17">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G58" s="6">
-        <v>2489.4499999999998</v>
+        <v>2760.05</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2390,22 +2390,22 @@
         <v>63</v>
       </c>
       <c r="B59" s="9">
-        <v>1320.3</v>
+        <v>1354.5</v>
       </c>
       <c r="C59" s="11">
-        <v>1308.5999999999999</v>
+        <v>1332</v>
       </c>
       <c r="D59" s="14">
-        <v>1314.9</v>
+        <v>1343</v>
       </c>
       <c r="E59" s="6">
-        <v>1313.7</v>
+        <v>1343</v>
       </c>
       <c r="F59" s="17">
         <v>5</v>
       </c>
       <c r="G59" s="6">
-        <v>1317.45</v>
+        <v>1353.4</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2413,22 +2413,22 @@
         <v>64</v>
       </c>
       <c r="B60" s="9">
-        <v>1344.35</v>
+        <v>1369.95</v>
       </c>
       <c r="C60" s="11">
-        <v>1331</v>
+        <v>1340.15</v>
       </c>
       <c r="D60" s="14">
-        <v>1335</v>
+        <v>1365.9</v>
       </c>
       <c r="E60" s="6">
-        <v>1337.95</v>
+        <v>1364.1</v>
       </c>
       <c r="F60" s="17">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="G60" s="6">
-        <v>1339.55</v>
+        <v>1349.95</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2436,22 +2436,22 @@
         <v>65</v>
       </c>
       <c r="B61" s="9">
-        <v>2993.5</v>
+        <v>3010</v>
       </c>
       <c r="C61" s="11">
-        <v>2947.1</v>
+        <v>2972.9</v>
       </c>
       <c r="D61" s="14">
-        <v>2952.85</v>
+        <v>2993</v>
       </c>
       <c r="E61" s="6">
-        <v>2953.55</v>
+        <v>2987.05</v>
       </c>
       <c r="F61" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G61" s="6">
-        <v>2982.75</v>
+        <v>3009.05</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2459,22 +2459,22 @@
         <v>66</v>
       </c>
       <c r="B62" s="9">
-        <v>686.1</v>
+        <v>680.2</v>
       </c>
       <c r="C62" s="11">
-        <v>672.25</v>
+        <v>667</v>
       </c>
       <c r="D62" s="14">
-        <v>676.5</v>
+        <v>672.4</v>
       </c>
       <c r="E62" s="6">
-        <v>674.95</v>
+        <v>671.25</v>
       </c>
       <c r="F62" s="17">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="G62" s="6">
-        <v>685.05</v>
+        <v>679.25</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2482,22 +2482,22 @@
         <v>67</v>
       </c>
       <c r="B63" s="9">
-        <v>526.65</v>
+        <v>525.04999999999995</v>
       </c>
       <c r="C63" s="11">
-        <v>516.54999999999995</v>
+        <v>514</v>
       </c>
       <c r="D63" s="14">
-        <v>519.25</v>
+        <v>520.15</v>
       </c>
       <c r="E63" s="6">
-        <v>519.25</v>
+        <v>520.35</v>
       </c>
       <c r="F63" s="17">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="G63" s="6">
-        <v>521</v>
+        <v>521.35</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2505,22 +2505,22 @@
         <v>68</v>
       </c>
       <c r="B64" s="9">
-        <v>183.2</v>
+        <v>192</v>
       </c>
       <c r="C64" s="11">
-        <v>176.15</v>
+        <v>184.25</v>
       </c>
       <c r="D64" s="14">
-        <v>178.45</v>
+        <v>184.8</v>
       </c>
       <c r="E64" s="6">
-        <v>178.1</v>
+        <v>186.2</v>
       </c>
       <c r="F64" s="17">
-        <v>138</v>
+        <v>265</v>
       </c>
       <c r="G64" s="6">
-        <v>177.45</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2528,22 +2528,22 @@
         <v>69</v>
       </c>
       <c r="B65" s="9">
-        <v>1476.9</v>
+        <v>1450.9</v>
       </c>
       <c r="C65" s="11">
-        <v>1444.6</v>
+        <v>1440.05</v>
       </c>
       <c r="D65" s="14">
-        <v>1471.25</v>
+        <v>1447.25</v>
       </c>
       <c r="E65" s="6">
-        <v>1470.9</v>
+        <v>1449.4</v>
       </c>
       <c r="F65" s="17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G65" s="6">
-        <v>1464</v>
+        <v>1449.05</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2551,22 +2551,22 @@
         <v>70</v>
       </c>
       <c r="B66" s="9">
-        <v>564</v>
+        <v>548.85</v>
       </c>
       <c r="C66" s="11">
-        <v>556.70000000000005</v>
+        <v>539.65</v>
       </c>
       <c r="D66" s="14">
-        <v>562.85</v>
+        <v>543.9</v>
       </c>
       <c r="E66" s="6">
-        <v>563.29999999999995</v>
+        <v>543.54999999999995</v>
       </c>
       <c r="F66" s="17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G66" s="6">
-        <v>561.9</v>
+        <v>548.04999999999995</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2574,22 +2574,22 @@
         <v>71</v>
       </c>
       <c r="B67" s="9">
-        <v>147.4</v>
+        <v>159.44999999999999</v>
       </c>
       <c r="C67" s="11">
-        <v>143.44999999999999</v>
+        <v>150.44999999999999</v>
       </c>
       <c r="D67" s="14">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E67" s="6">
-        <v>144.94999999999999</v>
+        <v>152.69999999999999</v>
       </c>
       <c r="F67" s="17">
-        <v>102</v>
+        <v>222</v>
       </c>
       <c r="G67" s="6">
-        <v>144.65</v>
+        <v>158.94999999999999</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2597,22 +2597,22 @@
         <v>72</v>
       </c>
       <c r="B68" s="9">
-        <v>404.75</v>
+        <v>409.8</v>
       </c>
       <c r="C68" s="11">
-        <v>394.6</v>
+        <v>398.3</v>
       </c>
       <c r="D68" s="14">
-        <v>401.2</v>
+        <v>401.9</v>
       </c>
       <c r="E68" s="6">
-        <v>401.2</v>
+        <v>401.1</v>
       </c>
       <c r="F68" s="17">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G68" s="6">
-        <v>396.1</v>
+        <v>408.2</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2620,22 +2620,22 @@
         <v>73</v>
       </c>
       <c r="B69" s="9">
-        <v>436.05</v>
+        <v>440.95</v>
       </c>
       <c r="C69" s="11">
-        <v>427.55</v>
+        <v>432.35</v>
       </c>
       <c r="D69" s="14">
-        <v>433.5</v>
+        <v>434.1</v>
       </c>
       <c r="E69" s="6">
-        <v>434</v>
+        <v>435.5</v>
       </c>
       <c r="F69" s="17">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="G69" s="6">
-        <v>431</v>
+        <v>440.45</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2643,22 +2643,22 @@
         <v>74</v>
       </c>
       <c r="B70" s="9">
-        <v>259.89999999999998</v>
+        <v>272.89999999999998</v>
       </c>
       <c r="C70" s="11">
-        <v>252.95</v>
+        <v>255.5</v>
       </c>
       <c r="D70" s="14">
-        <v>254.45</v>
+        <v>272.5</v>
       </c>
       <c r="E70" s="6">
-        <v>254.05</v>
+        <v>271.10000000000002</v>
       </c>
       <c r="F70" s="17">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="G70" s="6">
-        <v>255.8</v>
+        <v>265.45</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2666,22 +2666,22 @@
         <v>75</v>
       </c>
       <c r="B71" s="9">
-        <v>2612.35</v>
+        <v>2712.3</v>
       </c>
       <c r="C71" s="11">
-        <v>2586.0500000000002</v>
+        <v>2645.05</v>
       </c>
       <c r="D71" s="14">
-        <v>2605</v>
+        <v>2675</v>
       </c>
       <c r="E71" s="6">
-        <v>2604.4</v>
+        <v>2677.3</v>
       </c>
       <c r="F71" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G71" s="6">
-        <v>2600.6999999999998</v>
+        <v>2711.95</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2689,22 +2689,22 @@
         <v>76</v>
       </c>
       <c r="B72" s="9">
-        <v>2859.9</v>
+        <v>2938.8</v>
       </c>
       <c r="C72" s="11">
-        <v>2780.8</v>
+        <v>2873.65</v>
       </c>
       <c r="D72" s="14">
-        <v>2815</v>
+        <v>2900</v>
       </c>
       <c r="E72" s="6">
-        <v>2820.25</v>
+        <v>2897.95</v>
       </c>
       <c r="F72" s="17">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G72" s="6">
-        <v>2801.6</v>
+        <v>2904</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2712,22 +2712,22 @@
         <v>77</v>
       </c>
       <c r="B73" s="9">
-        <v>1517.55</v>
+        <v>1520.95</v>
       </c>
       <c r="C73" s="11">
-        <v>1479.65</v>
+        <v>1494.05</v>
       </c>
       <c r="D73" s="14">
-        <v>1515.55</v>
+        <v>1509.5</v>
       </c>
       <c r="E73" s="6">
-        <v>1514.65</v>
+        <v>1508.95</v>
       </c>
       <c r="F73" s="17">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="G73" s="6">
-        <v>1483.15</v>
+        <v>1515.6</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2735,22 +2735,22 @@
         <v>78</v>
       </c>
       <c r="B74" s="9">
-        <v>189.7</v>
+        <v>194.35</v>
       </c>
       <c r="C74" s="11">
-        <v>186.55</v>
+        <v>187.5</v>
       </c>
       <c r="D74" s="14">
-        <v>187.75</v>
+        <v>190.75</v>
       </c>
       <c r="E74" s="6">
-        <v>187</v>
+        <v>190.45</v>
       </c>
       <c r="F74" s="17">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="G74" s="6">
-        <v>188.9</v>
+        <v>193.85</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2758,22 +2758,22 @@
         <v>79</v>
       </c>
       <c r="B75" s="9">
-        <v>779.5</v>
+        <v>760</v>
       </c>
       <c r="C75" s="11">
-        <v>750.95</v>
+        <v>737.05</v>
       </c>
       <c r="D75" s="14">
-        <v>755</v>
+        <v>747.25</v>
       </c>
       <c r="E75" s="6">
-        <v>754.15</v>
+        <v>748.55</v>
       </c>
       <c r="F75" s="17">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G75" s="6">
-        <v>752.35</v>
+        <v>745.45</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2781,22 +2781,22 @@
         <v>80</v>
       </c>
       <c r="B76" s="9">
-        <v>1154</v>
+        <v>1135</v>
       </c>
       <c r="C76" s="11">
-        <v>1134.0999999999999</v>
+        <v>1108.2</v>
       </c>
       <c r="D76" s="14">
-        <v>1144.0999999999999</v>
+        <v>1117.95</v>
       </c>
       <c r="E76" s="6">
-        <v>1142.55</v>
+        <v>1119.3</v>
       </c>
       <c r="F76" s="17">
         <v>2</v>
       </c>
       <c r="G76" s="6">
-        <v>1142</v>
+        <v>1131.9000000000001</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2804,22 +2804,22 @@
         <v>81</v>
       </c>
       <c r="B77" s="9">
-        <v>694.05</v>
+        <v>697.45</v>
       </c>
       <c r="C77" s="11">
-        <v>678.45</v>
+        <v>676.4</v>
       </c>
       <c r="D77" s="14">
-        <v>680.85</v>
+        <v>685.1</v>
       </c>
       <c r="E77" s="6">
-        <v>681.5</v>
+        <v>686.25</v>
       </c>
       <c r="F77" s="17">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G77" s="6">
-        <v>693.3</v>
+        <v>690.2</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2827,22 +2827,22 @@
         <v>82</v>
       </c>
       <c r="B78" s="9">
-        <v>3692.9</v>
+        <v>3833.8</v>
       </c>
       <c r="C78" s="11">
-        <v>3630</v>
+        <v>3730</v>
       </c>
       <c r="D78" s="14">
-        <v>3669</v>
+        <v>3791</v>
       </c>
       <c r="E78" s="6">
-        <v>3674.05</v>
+        <v>3798.05</v>
       </c>
       <c r="F78" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G78" s="6">
-        <v>3692.5</v>
+        <v>3790</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2850,22 +2850,22 @@
         <v>83</v>
       </c>
       <c r="B79" s="9">
-        <v>823.4</v>
+        <v>853.45</v>
       </c>
       <c r="C79" s="11">
-        <v>812.35</v>
+        <v>831.55</v>
       </c>
       <c r="D79" s="14">
-        <v>820</v>
+        <v>839.35</v>
       </c>
       <c r="E79" s="6">
-        <v>819.6</v>
+        <v>839.35</v>
       </c>
       <c r="F79" s="17">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="G79" s="6">
-        <v>818.45</v>
+        <v>840.45</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2873,22 +2873,22 @@
         <v>84</v>
       </c>
       <c r="B80" s="9">
-        <v>574.9</v>
+        <v>563.20000000000005</v>
       </c>
       <c r="C80" s="11">
-        <v>560.79999999999995</v>
+        <v>556</v>
       </c>
       <c r="D80" s="14">
-        <v>561.1</v>
+        <v>557</v>
       </c>
       <c r="E80" s="6">
-        <v>561.45000000000005</v>
+        <v>559.75</v>
       </c>
       <c r="F80" s="17">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="G80" s="6">
-        <v>573.20000000000005</v>
+        <v>563</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2896,22 +2896,22 @@
         <v>85</v>
       </c>
       <c r="B81" s="9">
-        <v>1825.95</v>
+        <v>1843</v>
       </c>
       <c r="C81" s="11">
-        <v>1766.3</v>
+        <v>1821.2</v>
       </c>
       <c r="D81" s="14">
-        <v>1819.2</v>
+        <v>1842.6</v>
       </c>
       <c r="E81" s="6">
-        <v>1818.55</v>
+        <v>1838.45</v>
       </c>
       <c r="F81" s="17">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="G81" s="6">
-        <v>1768.95</v>
+        <v>1828.2</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2919,22 +2919,22 @@
         <v>86</v>
       </c>
       <c r="B82" s="9">
-        <v>2754.3</v>
+        <v>2700.65</v>
       </c>
       <c r="C82" s="11">
-        <v>2688</v>
+        <v>2607.0500000000002</v>
       </c>
       <c r="D82" s="14">
-        <v>2695.1</v>
+        <v>2634</v>
       </c>
       <c r="E82" s="6">
-        <v>2691.2</v>
+        <v>2638.55</v>
       </c>
       <c r="F82" s="17">
         <v>1</v>
       </c>
       <c r="G82" s="6">
-        <v>2746</v>
+        <v>2690.45</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2942,22 +2942,22 @@
         <v>87</v>
       </c>
       <c r="B83" s="9">
-        <v>380.95</v>
+        <v>396.1</v>
       </c>
       <c r="C83" s="11">
-        <v>376.65</v>
+        <v>381.5</v>
       </c>
       <c r="D83" s="14">
-        <v>379.8</v>
+        <v>384.95</v>
       </c>
       <c r="E83" s="6">
-        <v>379.25</v>
+        <v>383.65</v>
       </c>
       <c r="F83" s="17">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="G83" s="6">
-        <v>379.6</v>
+        <v>394.8</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2965,22 +2965,22 @@
         <v>88</v>
       </c>
       <c r="B84" s="9">
-        <v>510.6</v>
+        <v>543.9</v>
       </c>
       <c r="C84" s="11">
-        <v>497.1</v>
+        <v>526.65</v>
       </c>
       <c r="D84" s="14">
-        <v>504.95</v>
+        <v>531.79999999999995</v>
       </c>
       <c r="E84" s="6">
-        <v>507.55</v>
+        <v>532.29999999999995</v>
       </c>
       <c r="F84" s="17">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="G84" s="6">
-        <v>498.95</v>
+        <v>529.79999999999995</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2988,22 +2988,22 @@
         <v>89</v>
       </c>
       <c r="B85" s="9">
-        <v>5620</v>
+        <v>5754</v>
       </c>
       <c r="C85" s="11">
-        <v>5550</v>
+        <v>5600</v>
       </c>
       <c r="D85" s="14">
-        <v>5583</v>
+        <v>5710</v>
       </c>
       <c r="E85" s="6">
-        <v>5577.4</v>
+        <v>5708.7</v>
       </c>
       <c r="F85" s="17">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G85" s="6">
-        <v>5604.25</v>
+        <v>5632</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3011,22 +3011,22 @@
         <v>90</v>
       </c>
       <c r="B86" s="9">
-        <v>4798.95</v>
+        <v>4988.6499999999996</v>
       </c>
       <c r="C86" s="11">
-        <v>4727.6000000000004</v>
+        <v>4891</v>
       </c>
       <c r="D86" s="14">
-        <v>4748.8999999999996</v>
+        <v>4938.2</v>
       </c>
       <c r="E86" s="6">
-        <v>4748.1000000000004</v>
+        <v>4939.05</v>
       </c>
       <c r="F86" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G86" s="6">
-        <v>4794.6000000000004</v>
+        <v>4956.7</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3034,22 +3034,22 @@
         <v>91</v>
       </c>
       <c r="B87" s="9">
-        <v>1293.1500000000001</v>
+        <v>1253.6500000000001</v>
       </c>
       <c r="C87" s="11">
-        <v>1256</v>
+        <v>1230.5999999999999</v>
       </c>
       <c r="D87" s="14">
-        <v>1262.5</v>
+        <v>1239.5</v>
       </c>
       <c r="E87" s="6">
-        <v>1260.55</v>
+        <v>1239.3499999999999</v>
       </c>
       <c r="F87" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G87" s="6">
-        <v>1287.5</v>
+        <v>1250.05</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3057,22 +3057,22 @@
         <v>92</v>
       </c>
       <c r="B88" s="9">
-        <v>281.35000000000002</v>
+        <v>276.64999999999998</v>
       </c>
       <c r="C88" s="11">
-        <v>276.10000000000002</v>
+        <v>270.55</v>
       </c>
       <c r="D88" s="14">
-        <v>278.05</v>
+        <v>273.5</v>
       </c>
       <c r="E88" s="6">
-        <v>277.7</v>
+        <v>273.25</v>
       </c>
       <c r="F88" s="17">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G88" s="6">
-        <v>277.7</v>
+        <v>275.64999999999998</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3080,22 +3080,22 @@
         <v>93</v>
       </c>
       <c r="B89" s="9">
-        <v>170.4</v>
+        <v>168.6</v>
       </c>
       <c r="C89" s="11">
-        <v>166.75</v>
+        <v>162.05000000000001</v>
       </c>
       <c r="D89" s="14">
-        <v>167.5</v>
+        <v>163.80000000000001</v>
       </c>
       <c r="E89" s="6">
-        <v>167.35</v>
+        <v>163.85</v>
       </c>
       <c r="F89" s="17">
-        <v>157</v>
+        <v>65</v>
       </c>
       <c r="G89" s="6">
-        <v>168.3</v>
+        <v>166.25</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3103,22 +3103,22 @@
         <v>94</v>
       </c>
       <c r="B90" s="9">
-        <v>541</v>
+        <v>535.79999999999995</v>
       </c>
       <c r="C90" s="11">
-        <v>534.4</v>
+        <v>527.5</v>
       </c>
       <c r="D90" s="14">
-        <v>536.6</v>
+        <v>531.29999999999995</v>
       </c>
       <c r="E90" s="6">
-        <v>536</v>
+        <v>530.5</v>
       </c>
       <c r="F90" s="17">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G90" s="6">
-        <v>539.1</v>
+        <v>535.70000000000005</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3126,22 +3126,22 @@
         <v>95</v>
       </c>
       <c r="B91" s="9">
-        <v>1055.95</v>
+        <v>1073</v>
       </c>
       <c r="C91" s="11">
-        <v>1046.75</v>
+        <v>1032.75</v>
       </c>
       <c r="D91" s="14">
-        <v>1050</v>
+        <v>1045.25</v>
       </c>
       <c r="E91" s="6">
-        <v>1050.3499999999999</v>
+        <v>1045.25</v>
       </c>
       <c r="F91" s="17">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G91" s="6">
-        <v>1053.5999999999999</v>
+        <v>1072.25</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3149,22 +3149,22 @@
         <v>96</v>
       </c>
       <c r="B92" s="9">
-        <v>3159.5</v>
+        <v>3344</v>
       </c>
       <c r="C92" s="11">
-        <v>3063.75</v>
+        <v>3168.75</v>
       </c>
       <c r="D92" s="14">
-        <v>3095</v>
+        <v>3192</v>
       </c>
       <c r="E92" s="6">
-        <v>3090.15</v>
+        <v>3181.55</v>
       </c>
       <c r="F92" s="17">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G92" s="6">
-        <v>3135.65</v>
+        <v>3303.05</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3172,22 +3172,22 @@
         <v>97</v>
       </c>
       <c r="B93" s="9">
-        <v>1705.4</v>
+        <v>1674.1</v>
       </c>
       <c r="C93" s="11">
-        <v>1676</v>
+        <v>1642</v>
       </c>
       <c r="D93" s="14">
-        <v>1680.5</v>
+        <v>1654.4</v>
       </c>
       <c r="E93" s="6">
-        <v>1684.55</v>
+        <v>1653.7</v>
       </c>
       <c r="F93" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G93" s="6">
-        <v>1697.05</v>
+        <v>1672.2</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3195,22 +3195,22 @@
         <v>98</v>
       </c>
       <c r="B94" s="9">
-        <v>1027.55</v>
+        <v>1039.95</v>
       </c>
       <c r="C94" s="11">
-        <v>1004</v>
+        <v>1026.05</v>
       </c>
       <c r="D94" s="14">
-        <v>1024.75</v>
+        <v>1031</v>
       </c>
       <c r="E94" s="6">
-        <v>1023.35</v>
+        <v>1035.8</v>
       </c>
       <c r="F94" s="17">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G94" s="6">
-        <v>1023</v>
+        <v>1032.3499999999999</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3218,22 +3218,22 @@
         <v>99</v>
       </c>
       <c r="B95" s="9">
-        <v>1112.95</v>
+        <v>1164.0999999999999</v>
       </c>
       <c r="C95" s="11">
-        <v>1065</v>
+        <v>1140.5999999999999</v>
       </c>
       <c r="D95" s="14">
-        <v>1098</v>
+        <v>1155.75</v>
       </c>
       <c r="E95" s="6">
-        <v>1098.75</v>
+        <v>1155.75</v>
       </c>
       <c r="F95" s="17">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G95" s="6">
-        <v>1066.6500000000001</v>
+        <v>1158.05</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -3241,22 +3241,22 @@
         <v>100</v>
       </c>
       <c r="B96" s="9">
-        <v>2394.9</v>
+        <v>2455</v>
       </c>
       <c r="C96" s="11">
-        <v>2361.9499999999998</v>
+        <v>2402.65</v>
       </c>
       <c r="D96" s="14">
-        <v>2378</v>
+        <v>2418.4499999999998</v>
       </c>
       <c r="E96" s="6">
-        <v>2371.3000000000002</v>
+        <v>2427.0500000000002</v>
       </c>
       <c r="F96" s="17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G96" s="6">
-        <v>2381.25</v>
+        <v>2411.4</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -3264,22 +3264,22 @@
         <v>101</v>
       </c>
       <c r="B97" s="9">
-        <v>1470</v>
+        <v>1453.1</v>
       </c>
       <c r="C97" s="11">
-        <v>1453</v>
+        <v>1422.35</v>
       </c>
       <c r="D97" s="14">
-        <v>1464.15</v>
+        <v>1441</v>
       </c>
       <c r="E97" s="6">
-        <v>1464.85</v>
+        <v>1440.65</v>
       </c>
       <c r="F97" s="17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G97" s="6">
-        <v>1464.4</v>
+        <v>1452.15</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3287,22 +3287,22 @@
         <v>102</v>
       </c>
       <c r="B98" s="9">
-        <v>443.85</v>
+        <v>447.6</v>
       </c>
       <c r="C98" s="11">
-        <v>433</v>
+        <v>432.05</v>
       </c>
       <c r="D98" s="14">
-        <v>439.45</v>
+        <v>435</v>
       </c>
       <c r="E98" s="6">
-        <v>441.45</v>
+        <v>433.55</v>
       </c>
       <c r="F98" s="17">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G98" s="6">
-        <v>434</v>
+        <v>447.6</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3310,22 +3310,22 @@
         <v>103</v>
       </c>
       <c r="B99" s="9">
-        <v>4644.1499999999996</v>
+        <v>4807.7</v>
       </c>
       <c r="C99" s="11">
-        <v>4570.3500000000004</v>
+        <v>4681.5</v>
       </c>
       <c r="D99" s="14">
-        <v>4593</v>
+        <v>4759</v>
       </c>
       <c r="E99" s="6">
-        <v>4596.3500000000004</v>
+        <v>4745.6499999999996</v>
       </c>
       <c r="F99" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G99" s="6">
-        <v>4615.25</v>
+        <v>4796.1000000000004</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3333,22 +3333,22 @@
         <v>104</v>
       </c>
       <c r="B100" s="9">
-        <v>3765.65</v>
+        <v>3812.9</v>
       </c>
       <c r="C100" s="11">
-        <v>3732.2</v>
+        <v>3755</v>
       </c>
       <c r="D100" s="14">
-        <v>3742</v>
+        <v>3787.4</v>
       </c>
       <c r="E100" s="6">
-        <v>3740.1</v>
+        <v>3802.9</v>
       </c>
       <c r="F100" s="17">
         <v>1</v>
       </c>
       <c r="G100" s="6">
-        <v>3755</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3356,22 +3356,22 @@
         <v>105</v>
       </c>
       <c r="B101" s="9">
-        <v>185.85</v>
+        <v>189</v>
       </c>
       <c r="C101" s="11">
-        <v>183.3</v>
+        <v>180.9</v>
       </c>
       <c r="D101" s="14">
-        <v>184</v>
+        <v>183.15</v>
       </c>
       <c r="E101" s="6">
-        <v>184.05</v>
+        <v>183.6</v>
       </c>
       <c r="F101" s="17">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="G101" s="6">
-        <v>184.05</v>
+        <v>186.4</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3379,22 +3379,22 @@
         <v>106</v>
       </c>
       <c r="B102" s="9">
-        <v>277.35000000000002</v>
+        <v>291.89999999999998</v>
       </c>
       <c r="C102" s="11">
-        <v>273.25</v>
+        <v>281</v>
       </c>
       <c r="D102" s="14">
-        <v>274.89999999999998</v>
+        <v>284.55</v>
       </c>
       <c r="E102" s="6">
-        <v>274.8</v>
+        <v>285.05</v>
       </c>
       <c r="F102" s="17">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="G102" s="6">
-        <v>274.35000000000002</v>
+        <v>285.10000000000002</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3402,22 +3402,22 @@
         <v>107</v>
       </c>
       <c r="B103" s="9">
-        <v>1455.95</v>
+        <v>1479.8</v>
       </c>
       <c r="C103" s="11">
-        <v>1410</v>
+        <v>1437.65</v>
       </c>
       <c r="D103" s="14">
-        <v>1437.35</v>
+        <v>1447</v>
       </c>
       <c r="E103" s="6">
-        <v>1438.8</v>
+        <v>1447.35</v>
       </c>
       <c r="F103" s="17">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G103" s="6">
-        <v>1413.15</v>
+        <v>1477.55</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3425,22 +3425,22 @@
         <v>108</v>
       </c>
       <c r="B104" s="9">
-        <v>945.95</v>
+        <v>930.45</v>
       </c>
       <c r="C104" s="11">
-        <v>936</v>
+        <v>911.5</v>
       </c>
       <c r="D104" s="14">
-        <v>941.5</v>
+        <v>918</v>
       </c>
       <c r="E104" s="6">
-        <v>940.15</v>
+        <v>918.9</v>
       </c>
       <c r="F104" s="17">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G104" s="6">
-        <v>938.25</v>
+        <v>929.9</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3448,22 +3448,22 @@
         <v>109</v>
       </c>
       <c r="B105" s="9">
-        <v>6508</v>
+        <v>6536</v>
       </c>
       <c r="C105" s="11">
-        <v>6396.7</v>
+        <v>6314.35</v>
       </c>
       <c r="D105" s="14">
-        <v>6484</v>
+        <v>6467</v>
       </c>
       <c r="E105" s="6">
-        <v>6441.45</v>
+        <v>6464.5</v>
       </c>
       <c r="F105" s="17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G105" s="6">
-        <v>6440.95</v>
+        <v>6360</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3471,22 +3471,22 @@
         <v>110</v>
       </c>
       <c r="B106" s="9">
-        <v>206.95</v>
+        <v>213.1</v>
       </c>
       <c r="C106" s="11">
-        <v>203.95</v>
+        <v>206.9</v>
       </c>
       <c r="D106" s="14">
-        <v>205.55</v>
+        <v>210.2</v>
       </c>
       <c r="E106" s="6">
-        <v>205.15</v>
+        <v>210</v>
       </c>
       <c r="F106" s="17">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="G106" s="6">
-        <v>204.2</v>
+        <v>212.95</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3494,22 +3494,22 @@
         <v>111</v>
       </c>
       <c r="B107" s="9">
-        <v>2572.0500000000002</v>
+        <v>2603.9499999999998</v>
       </c>
       <c r="C107" s="11">
-        <v>2546</v>
+        <v>2545</v>
       </c>
       <c r="D107" s="14">
-        <v>2554.9499999999998</v>
+        <v>2562</v>
       </c>
       <c r="E107" s="6">
-        <v>2553.4499999999998</v>
+        <v>2561.65</v>
       </c>
       <c r="F107" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G107" s="6">
-        <v>2567</v>
+        <v>2602.75</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3517,22 +3517,22 @@
         <v>112</v>
       </c>
       <c r="B108" s="9">
-        <v>5355.7</v>
+        <v>5495</v>
       </c>
       <c r="C108" s="11">
-        <v>5288</v>
+        <v>5392.5</v>
       </c>
       <c r="D108" s="14">
-        <v>5344</v>
+        <v>5435</v>
       </c>
       <c r="E108" s="6">
-        <v>5341.6</v>
+        <v>5446.65</v>
       </c>
       <c r="F108" s="17">
         <v>4</v>
       </c>
       <c r="G108" s="6">
-        <v>5313</v>
+        <v>5485.75</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -3540,22 +3540,22 @@
         <v>113</v>
       </c>
       <c r="B109" s="9">
-        <v>213.2</v>
+        <v>233.4</v>
       </c>
       <c r="C109" s="11">
-        <v>211.75</v>
+        <v>226.45</v>
       </c>
       <c r="D109" s="14">
-        <v>213</v>
+        <v>228.35</v>
       </c>
       <c r="E109" s="6">
-        <v>212.9</v>
+        <v>228.6</v>
       </c>
       <c r="F109" s="17">
-        <v>279</v>
+        <v>222</v>
       </c>
       <c r="G109" s="6">
-        <v>212.05</v>
+        <v>230</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -3563,22 +3563,22 @@
         <v>114</v>
       </c>
       <c r="B110" s="9">
-        <v>145.94999999999999</v>
+        <v>151.05000000000001</v>
       </c>
       <c r="C110" s="11">
-        <v>144.1</v>
+        <v>146.6</v>
       </c>
       <c r="D110" s="14">
-        <v>144.85</v>
+        <v>148.1</v>
       </c>
       <c r="E110" s="6">
-        <v>144.69999999999999</v>
+        <v>148.1</v>
       </c>
       <c r="F110" s="17">
         <v>16</v>
       </c>
       <c r="G110" s="6">
-        <v>145.15</v>
+        <v>150.85</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -3586,22 +3586,22 @@
         <v>115</v>
       </c>
       <c r="B111" s="9">
-        <v>1038.1500000000001</v>
+        <v>1027.8499999999999</v>
       </c>
       <c r="C111" s="11">
-        <v>1002.25</v>
+        <v>1003.2</v>
       </c>
       <c r="D111" s="14">
-        <v>1033</v>
+        <v>1020.75</v>
       </c>
       <c r="E111" s="6">
-        <v>1032.4000000000001</v>
+        <v>1019</v>
       </c>
       <c r="F111" s="17">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G111" s="6">
-        <v>1011.7</v>
+        <v>1024.55</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -3609,22 +3609,22 @@
         <v>116</v>
       </c>
       <c r="B112" s="9">
-        <v>244</v>
+        <v>276.5</v>
       </c>
       <c r="C112" s="11">
-        <v>237</v>
+        <v>258.55</v>
       </c>
       <c r="D112" s="14">
-        <v>243</v>
+        <v>268.60000000000002</v>
       </c>
       <c r="E112" s="6">
-        <v>242.45</v>
+        <v>267.7</v>
       </c>
       <c r="F112" s="17">
-        <v>122</v>
+        <v>404</v>
       </c>
       <c r="G112" s="6">
-        <v>237.9</v>
+        <v>259.14999999999998</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3632,22 +3632,22 @@
         <v>117</v>
       </c>
       <c r="B113" s="9">
-        <v>394.8</v>
+        <v>409.2</v>
       </c>
       <c r="C113" s="11">
-        <v>376.15</v>
+        <v>396.35</v>
       </c>
       <c r="D113" s="14">
-        <v>389.45</v>
+        <v>407.2</v>
       </c>
       <c r="E113" s="6">
-        <v>389.8</v>
+        <v>405.45</v>
       </c>
       <c r="F113" s="17">
-        <v>260</v>
+        <v>157</v>
       </c>
       <c r="G113" s="6">
-        <v>377.5</v>
+        <v>397.55</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -3655,22 +3655,22 @@
         <v>118</v>
       </c>
       <c r="B114" s="9">
-        <v>756</v>
+        <v>775.4</v>
       </c>
       <c r="C114" s="11">
-        <v>748.2</v>
+        <v>752.55</v>
       </c>
       <c r="D114" s="14">
-        <v>753</v>
+        <v>759.9</v>
       </c>
       <c r="E114" s="6">
-        <v>751.7</v>
+        <v>759.95</v>
       </c>
       <c r="F114" s="17">
         <v>26</v>
       </c>
       <c r="G114" s="6">
-        <v>750.55</v>
+        <v>774.35</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3678,22 +3678,22 @@
         <v>119</v>
       </c>
       <c r="B115" s="9">
-        <v>1458.7</v>
+        <v>1469.55</v>
       </c>
       <c r="C115" s="11">
-        <v>1415</v>
+        <v>1451.55</v>
       </c>
       <c r="D115" s="14">
-        <v>1456.2</v>
+        <v>1465.85</v>
       </c>
       <c r="E115" s="6">
-        <v>1454</v>
+        <v>1465.2</v>
       </c>
       <c r="F115" s="17">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G115" s="6">
-        <v>1435</v>
+        <v>1464.4</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -3701,22 +3701,22 @@
         <v>120</v>
       </c>
       <c r="B116" s="9">
-        <v>3837.95</v>
+        <v>3882.45</v>
       </c>
       <c r="C116" s="11">
-        <v>3740.6</v>
+        <v>3785.05</v>
       </c>
       <c r="D116" s="14">
-        <v>3800</v>
+        <v>3827</v>
       </c>
       <c r="E116" s="6">
-        <v>3807.2</v>
+        <v>3827.2</v>
       </c>
       <c r="F116" s="17">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G116" s="6">
-        <v>3820.8</v>
+        <v>3862.5</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -3724,22 +3724,22 @@
         <v>121</v>
       </c>
       <c r="B117" s="9">
-        <v>2444.4</v>
+        <v>2456.3000000000002</v>
       </c>
       <c r="C117" s="11">
-        <v>2412.85</v>
+        <v>2396.25</v>
       </c>
       <c r="D117" s="14">
-        <v>2429</v>
+        <v>2418</v>
       </c>
       <c r="E117" s="6">
-        <v>2427.4499999999998</v>
+        <v>2423.1</v>
       </c>
       <c r="F117" s="17">
         <v>3</v>
       </c>
       <c r="G117" s="6">
-        <v>2433.5</v>
+        <v>2452.4499999999998</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -3747,22 +3747,22 @@
         <v>122</v>
       </c>
       <c r="B118" s="9">
-        <v>508</v>
+        <v>514.75</v>
       </c>
       <c r="C118" s="11">
-        <v>495.4</v>
+        <v>488.35</v>
       </c>
       <c r="D118" s="14">
-        <v>496</v>
+        <v>514</v>
       </c>
       <c r="E118" s="6">
-        <v>496.25</v>
+        <v>512.25</v>
       </c>
       <c r="F118" s="17">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G118" s="6">
-        <v>508</v>
+        <v>493.45</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -3770,22 +3770,22 @@
         <v>123</v>
       </c>
       <c r="B119" s="9">
-        <v>1238.9000000000001</v>
+        <v>1246</v>
       </c>
       <c r="C119" s="11">
-        <v>1220.5</v>
+        <v>1230.6500000000001</v>
       </c>
       <c r="D119" s="14">
-        <v>1230</v>
+        <v>1234.9000000000001</v>
       </c>
       <c r="E119" s="6">
-        <v>1231.1500000000001</v>
+        <v>1235.8</v>
       </c>
       <c r="F119" s="17">
         <v>16</v>
       </c>
       <c r="G119" s="6">
-        <v>1232.7</v>
+        <v>1244.6500000000001</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -3793,22 +3793,22 @@
         <v>124</v>
       </c>
       <c r="B120" s="9">
-        <v>749.5</v>
+        <v>735.95</v>
       </c>
       <c r="C120" s="11">
-        <v>735.6</v>
+        <v>716.7</v>
       </c>
       <c r="D120" s="14">
-        <v>746.55</v>
+        <v>722.4</v>
       </c>
       <c r="E120" s="6">
-        <v>745.35</v>
+        <v>723.1</v>
       </c>
       <c r="F120" s="17">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G120" s="6">
-        <v>748</v>
+        <v>735.2</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -3816,22 +3816,22 @@
         <v>125</v>
       </c>
       <c r="B121" s="9">
-        <v>1675</v>
+        <v>1715.9</v>
       </c>
       <c r="C121" s="11">
-        <v>1656.9</v>
+        <v>1677</v>
       </c>
       <c r="D121" s="14">
-        <v>1665</v>
+        <v>1692.65</v>
       </c>
       <c r="E121" s="6">
-        <v>1662.85</v>
+        <v>1694.85</v>
       </c>
       <c r="F121" s="17">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G121" s="6">
-        <v>1667.85</v>
+        <v>1713.3</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -3839,22 +3839,22 @@
         <v>126</v>
       </c>
       <c r="B122" s="9">
-        <v>709.9</v>
+        <v>727.6</v>
       </c>
       <c r="C122" s="11">
-        <v>704.8</v>
+        <v>707.5</v>
       </c>
       <c r="D122" s="14">
-        <v>706.1</v>
+        <v>714.5</v>
       </c>
       <c r="E122" s="6">
-        <v>705.6</v>
+        <v>714.55</v>
       </c>
       <c r="F122" s="17">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="G122" s="6">
-        <v>707.35</v>
+        <v>723.3</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -3862,22 +3862,22 @@
         <v>127</v>
       </c>
       <c r="B123" s="9">
-        <v>1235.95</v>
+        <v>1237.95</v>
       </c>
       <c r="C123" s="11">
-        <v>1218</v>
+        <v>1217.25</v>
       </c>
       <c r="D123" s="14">
-        <v>1224.9000000000001</v>
+        <v>1224.0999999999999</v>
       </c>
       <c r="E123" s="6">
-        <v>1223.9000000000001</v>
+        <v>1225.3</v>
       </c>
       <c r="F123" s="17">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="G123" s="6">
-        <v>1231.5999999999999</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -3885,22 +3885,22 @@
         <v>128</v>
       </c>
       <c r="B124" s="9">
-        <v>2160.65</v>
+        <v>2091.9499999999998</v>
       </c>
       <c r="C124" s="11">
-        <v>2112.3000000000002</v>
+        <v>2044.15</v>
       </c>
       <c r="D124" s="14">
-        <v>2131.4</v>
+        <v>2059</v>
       </c>
       <c r="E124" s="6">
-        <v>2133.6</v>
+        <v>2053.4499999999998</v>
       </c>
       <c r="F124" s="17">
         <v>2</v>
       </c>
       <c r="G124" s="6">
-        <v>2148.0500000000002</v>
+        <v>2090.1999999999998</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -3908,22 +3908,22 @@
         <v>129</v>
       </c>
       <c r="B125" s="9">
-        <v>971.6</v>
+        <v>1005</v>
       </c>
       <c r="C125" s="11">
-        <v>944.05</v>
+        <v>955</v>
       </c>
       <c r="D125" s="14">
-        <v>966</v>
+        <v>969</v>
       </c>
       <c r="E125" s="6">
-        <v>967.3</v>
+        <v>966.65</v>
       </c>
       <c r="F125" s="17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G125" s="6">
-        <v>956.05</v>
+        <v>1001.95</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -3931,22 +3931,22 @@
         <v>130</v>
       </c>
       <c r="B126" s="9">
-        <v>2836.85</v>
+        <v>2885.95</v>
       </c>
       <c r="C126" s="11">
-        <v>2772.25</v>
+        <v>2800.2</v>
       </c>
       <c r="D126" s="14">
-        <v>2810</v>
+        <v>2844.45</v>
       </c>
       <c r="E126" s="6">
-        <v>2816.85</v>
+        <v>2841.3</v>
       </c>
       <c r="F126" s="17">
         <v>6</v>
       </c>
       <c r="G126" s="6">
-        <v>2797.95</v>
+        <v>2878.9</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -3954,22 +3954,22 @@
         <v>131</v>
       </c>
       <c r="B127" s="9">
-        <v>1915</v>
+        <v>1929</v>
       </c>
       <c r="C127" s="11">
-        <v>1890</v>
+        <v>1886.6</v>
       </c>
       <c r="D127" s="14">
-        <v>1907</v>
+        <v>1903</v>
       </c>
       <c r="E127" s="6">
-        <v>1903.95</v>
+        <v>1902.7</v>
       </c>
       <c r="F127" s="17">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G127" s="6">
-        <v>1909.85</v>
+        <v>1924.55</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -3977,22 +3977,22 @@
         <v>132</v>
       </c>
       <c r="B128" s="9">
-        <v>1708.9</v>
+        <v>1737.9</v>
       </c>
       <c r="C128" s="11">
-        <v>1674.8</v>
+        <v>1711</v>
       </c>
       <c r="D128" s="14">
-        <v>1704</v>
+        <v>1723.8</v>
       </c>
       <c r="E128" s="6">
-        <v>1702</v>
+        <v>1724.65</v>
       </c>
       <c r="F128" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G128" s="6">
-        <v>1675.5</v>
+        <v>1734.1</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -4000,22 +4000,22 @@
         <v>133</v>
       </c>
       <c r="B129" s="9">
-        <v>9340.7999999999993</v>
+        <v>9431.65</v>
       </c>
       <c r="C129" s="11">
-        <v>9090</v>
+        <v>9341.15</v>
       </c>
       <c r="D129" s="14">
-        <v>9295</v>
+        <v>9422</v>
       </c>
       <c r="E129" s="6">
-        <v>9317.75</v>
+        <v>9413.5499999999993</v>
       </c>
       <c r="F129" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G129" s="6">
-        <v>9113.1</v>
+        <v>9370.75</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -4023,22 +4023,22 @@
         <v>134</v>
       </c>
       <c r="B130" s="9">
-        <v>584.85</v>
+        <v>595.70000000000005</v>
       </c>
       <c r="C130" s="11">
-        <v>577</v>
+        <v>580.25</v>
       </c>
       <c r="D130" s="14">
-        <v>578.9</v>
+        <v>585.6</v>
       </c>
       <c r="E130" s="6">
-        <v>578.9</v>
+        <v>585.20000000000005</v>
       </c>
       <c r="F130" s="17">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G130" s="6">
-        <v>579.70000000000005</v>
+        <v>595.20000000000005</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -4046,22 +4046,22 @@
         <v>135</v>
       </c>
       <c r="B131" s="9">
-        <v>243.35</v>
+        <v>254</v>
       </c>
       <c r="C131" s="11">
-        <v>239.5</v>
+        <v>241.5</v>
       </c>
       <c r="D131" s="14">
-        <v>242.2</v>
+        <v>244.95</v>
       </c>
       <c r="E131" s="6">
-        <v>241.9</v>
+        <v>244.8</v>
       </c>
       <c r="F131" s="17">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="G131" s="6">
-        <v>242</v>
+        <v>249.4</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -4069,22 +4069,22 @@
         <v>136</v>
       </c>
       <c r="B132" s="9">
-        <v>842.4</v>
+        <v>878.6</v>
       </c>
       <c r="C132" s="11">
-        <v>830.55</v>
+        <v>844.85</v>
       </c>
       <c r="D132" s="14">
-        <v>839.65</v>
+        <v>855.6</v>
       </c>
       <c r="E132" s="6">
-        <v>837.85</v>
+        <v>855.45</v>
       </c>
       <c r="F132" s="17">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G132" s="6">
-        <v>840.75</v>
+        <v>872.8</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -4092,22 +4092,22 @@
         <v>137</v>
       </c>
       <c r="B133" s="9">
-        <v>260.7</v>
+        <v>282.3</v>
       </c>
       <c r="C133" s="11">
-        <v>254.45</v>
+        <v>271.7</v>
       </c>
       <c r="D133" s="14">
-        <v>255.5</v>
+        <v>279.3</v>
       </c>
       <c r="E133" s="6">
-        <v>255.9</v>
+        <v>278.95</v>
       </c>
       <c r="F133" s="17">
-        <v>440</v>
+        <v>427</v>
       </c>
       <c r="G133" s="6">
-        <v>256.95</v>
+        <v>277.89999999999998</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4115,22 +4115,22 @@
         <v>138</v>
       </c>
       <c r="B134" s="19">
-        <v>642.35</v>
+        <v>662.7</v>
       </c>
       <c r="C134" s="12">
-        <v>630</v>
+        <v>630.85</v>
       </c>
       <c r="D134" s="15">
-        <v>635.20000000000005</v>
+        <v>639.79999999999995</v>
       </c>
       <c r="E134" s="7">
-        <v>633.4</v>
+        <v>638.54999999999995</v>
       </c>
       <c r="F134" s="18">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="G134" s="7">
-        <v>640.29999999999995</v>
+        <v>659.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified according to samco, changed coordinates in nest trader auto, changed vol calc in fo
</commit_message>
<xml_diff>
--- a/algo high low.xlsx
+++ b/algo high low.xlsx
@@ -1043,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,22 +1080,22 @@
         <v>6</v>
       </c>
       <c r="B2" s="8">
-        <v>685.9</v>
+        <v>673.1</v>
       </c>
       <c r="C2" s="10">
-        <v>671</v>
+        <v>660.55</v>
       </c>
       <c r="D2" s="13">
-        <v>673</v>
+        <v>661.8</v>
       </c>
       <c r="E2" s="5">
-        <v>674.3</v>
+        <v>662.1</v>
       </c>
       <c r="F2" s="16">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G2" s="5">
-        <v>684.05</v>
+        <v>672.5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1103,22 +1103,22 @@
         <v>7</v>
       </c>
       <c r="B3" s="9">
-        <v>5518.1</v>
+        <v>5665</v>
       </c>
       <c r="C3" s="11">
-        <v>5362.2</v>
+        <v>5528.8</v>
       </c>
       <c r="D3" s="14">
-        <v>5383.95</v>
+        <v>5623</v>
       </c>
       <c r="E3" s="6">
-        <v>5392.05</v>
+        <v>5631.55</v>
       </c>
       <c r="F3" s="17">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G3" s="6">
-        <v>5377.5</v>
+        <v>5536.4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1126,22 +1126,22 @@
         <v>8</v>
       </c>
       <c r="B4" s="9">
-        <v>188.35</v>
+        <v>194.4</v>
       </c>
       <c r="C4" s="11">
-        <v>182.85</v>
+        <v>187.6</v>
       </c>
       <c r="D4" s="14">
-        <v>187.25</v>
+        <v>191.3</v>
       </c>
       <c r="E4" s="6">
-        <v>187.35</v>
+        <v>190.95</v>
       </c>
       <c r="F4" s="17">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="G4" s="6">
-        <v>185.05</v>
+        <v>187.7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1149,22 +1149,22 @@
         <v>9</v>
       </c>
       <c r="B5" s="9">
-        <v>228.75</v>
+        <v>235.8</v>
       </c>
       <c r="C5" s="11">
-        <v>225.1</v>
+        <v>229.25</v>
       </c>
       <c r="D5" s="14">
-        <v>226.3</v>
+        <v>230.3</v>
       </c>
       <c r="E5" s="6">
-        <v>226.2</v>
+        <v>230</v>
       </c>
       <c r="F5" s="17">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="G5" s="6">
-        <v>227.2</v>
+        <v>233.95</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1172,22 +1172,22 @@
         <v>10</v>
       </c>
       <c r="B6" s="9">
-        <v>3319.95</v>
+        <v>3348</v>
       </c>
       <c r="C6" s="11">
-        <v>3225.1</v>
+        <v>3310.05</v>
       </c>
       <c r="D6" s="14">
-        <v>3273.05</v>
+        <v>3320.95</v>
       </c>
       <c r="E6" s="6">
-        <v>3273.3</v>
+        <v>3317.15</v>
       </c>
       <c r="F6" s="17">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G6" s="6">
-        <v>3263.2</v>
+        <v>3344.9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1195,22 +1195,22 @@
         <v>11</v>
       </c>
       <c r="B7" s="9">
-        <v>1332</v>
+        <v>1353.8</v>
       </c>
       <c r="C7" s="11">
-        <v>1298</v>
+        <v>1336.4</v>
       </c>
       <c r="D7" s="14">
-        <v>1320.7</v>
+        <v>1342</v>
       </c>
       <c r="E7" s="6">
-        <v>1320.7</v>
+        <v>1342.6</v>
       </c>
       <c r="F7" s="17">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G7" s="6">
-        <v>1311.65</v>
+        <v>1349.45</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1218,22 +1218,22 @@
         <v>12</v>
       </c>
       <c r="B8" s="9">
-        <v>5472.1</v>
+        <v>5169.5</v>
       </c>
       <c r="C8" s="11">
-        <v>5355</v>
+        <v>5110</v>
       </c>
       <c r="D8" s="14">
-        <v>5382</v>
+        <v>5121</v>
       </c>
       <c r="E8" s="6">
-        <v>5421.15</v>
+        <v>5124.8999999999996</v>
       </c>
       <c r="F8" s="17">
         <v>1</v>
       </c>
       <c r="G8" s="6">
-        <v>5439.95</v>
+        <v>5128</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1241,22 +1241,22 @@
         <v>13</v>
       </c>
       <c r="B9" s="9">
-        <v>608.70000000000005</v>
+        <v>618.9</v>
       </c>
       <c r="C9" s="11">
-        <v>587.25</v>
+        <v>612.54999999999995</v>
       </c>
       <c r="D9" s="14">
-        <v>602</v>
+        <v>618</v>
       </c>
       <c r="E9" s="6">
-        <v>602.95000000000005</v>
+        <v>617.15</v>
       </c>
       <c r="F9" s="17">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="G9" s="6">
-        <v>592.25</v>
+        <v>617.25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1264,22 +1264,22 @@
         <v>14</v>
       </c>
       <c r="B10" s="9">
-        <v>6786.8</v>
+        <v>6166.75</v>
       </c>
       <c r="C10" s="11">
-        <v>6723.1</v>
+        <v>6022.85</v>
       </c>
       <c r="D10" s="14">
-        <v>6751</v>
+        <v>6050</v>
       </c>
       <c r="E10" s="6">
-        <v>6774.05</v>
+        <v>6033.3</v>
       </c>
       <c r="F10" s="17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G10" s="6">
-        <v>6757</v>
+        <v>6101.05</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1287,22 +1287,22 @@
         <v>15</v>
       </c>
       <c r="B11" s="9">
-        <v>528.04999999999995</v>
+        <v>537.85</v>
       </c>
       <c r="C11" s="11">
-        <v>520.75</v>
+        <v>521.70000000000005</v>
       </c>
       <c r="D11" s="14">
-        <v>522.20000000000005</v>
+        <v>535.5</v>
       </c>
       <c r="E11" s="6">
-        <v>523.75</v>
+        <v>535.1</v>
       </c>
       <c r="F11" s="17">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G11" s="6">
-        <v>525.29999999999995</v>
+        <v>530.35</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1310,22 +1310,22 @@
         <v>16</v>
       </c>
       <c r="B12" s="9">
-        <v>174.5</v>
+        <v>173.95</v>
       </c>
       <c r="C12" s="11">
-        <v>171.85</v>
+        <v>171.3</v>
       </c>
       <c r="D12" s="14">
-        <v>173.9</v>
+        <v>172</v>
       </c>
       <c r="E12" s="6">
-        <v>174</v>
+        <v>172.05</v>
       </c>
       <c r="F12" s="17">
-        <v>109</v>
+        <v>177</v>
       </c>
       <c r="G12" s="6">
-        <v>172.15</v>
+        <v>171.8</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1333,22 +1333,22 @@
         <v>17</v>
       </c>
       <c r="B13" s="9">
+        <v>2104.6999999999998</v>
+      </c>
+      <c r="C13" s="11">
+        <v>2071.5500000000002</v>
+      </c>
+      <c r="D13" s="14">
         <v>2095</v>
       </c>
-      <c r="C13" s="11">
-        <v>1970</v>
-      </c>
-      <c r="D13" s="14">
-        <v>2077</v>
-      </c>
       <c r="E13" s="6">
-        <v>2075.9</v>
+        <v>2097.1</v>
       </c>
       <c r="F13" s="17">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="G13" s="6">
-        <v>2001.1</v>
+        <v>2091.15</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1356,22 +1356,22 @@
         <v>18</v>
       </c>
       <c r="B14" s="9">
-        <v>6349.95</v>
+        <v>6167.95</v>
       </c>
       <c r="C14" s="11">
-        <v>6280</v>
+        <v>6070.05</v>
       </c>
       <c r="D14" s="14">
-        <v>6291.05</v>
+        <v>6077.5</v>
       </c>
       <c r="E14" s="6">
-        <v>6292.05</v>
+        <v>6080.25</v>
       </c>
       <c r="F14" s="17">
         <v>0</v>
       </c>
       <c r="G14" s="6">
-        <v>6343.7</v>
+        <v>6150.7</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1379,22 +1379,22 @@
         <v>19</v>
       </c>
       <c r="B15" s="9">
-        <v>606.95000000000005</v>
+        <v>582.29999999999995</v>
       </c>
       <c r="C15" s="11">
-        <v>594.15</v>
+        <v>575.95000000000005</v>
       </c>
       <c r="D15" s="14">
-        <v>598</v>
+        <v>579.5</v>
       </c>
       <c r="E15" s="6">
-        <v>599.95000000000005</v>
+        <v>580.1</v>
       </c>
       <c r="F15" s="17">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G15" s="6">
-        <v>594.79999999999995</v>
+        <v>581.35</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1402,22 +1402,22 @@
         <v>20</v>
       </c>
       <c r="B16" s="9">
-        <v>1054.25</v>
+        <v>1114</v>
       </c>
       <c r="C16" s="11">
-        <v>1039.0999999999999</v>
+        <v>1085</v>
       </c>
       <c r="D16" s="14">
-        <v>1045</v>
+        <v>1088.05</v>
       </c>
       <c r="E16" s="6">
-        <v>1043.8</v>
+        <v>1090.9000000000001</v>
       </c>
       <c r="F16" s="17">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="G16" s="6">
-        <v>1041.95</v>
+        <v>1091.8</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1425,22 +1425,22 @@
         <v>21</v>
       </c>
       <c r="B17" s="9">
-        <v>1620.9</v>
+        <v>1625</v>
       </c>
       <c r="C17" s="11">
-        <v>1598.45</v>
+        <v>1603.3</v>
       </c>
       <c r="D17" s="14">
-        <v>1616</v>
+        <v>1622.7</v>
       </c>
       <c r="E17" s="6">
-        <v>1616.55</v>
+        <v>1619.3</v>
       </c>
       <c r="F17" s="17">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G17" s="6">
-        <v>1602</v>
+        <v>1610.7</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1448,22 +1448,22 @@
         <v>22</v>
       </c>
       <c r="B18" s="9">
-        <v>6719</v>
+        <v>6639.95</v>
       </c>
       <c r="C18" s="11">
-        <v>6632.6</v>
+        <v>6557.45</v>
       </c>
       <c r="D18" s="14">
-        <v>6690</v>
+        <v>6604</v>
       </c>
       <c r="E18" s="6">
-        <v>6697.85</v>
+        <v>6602.45</v>
       </c>
       <c r="F18" s="17">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G18" s="6">
-        <v>6674.3</v>
+        <v>6631</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1471,22 +1471,22 @@
         <v>23</v>
       </c>
       <c r="B19" s="9">
-        <v>2353.1999999999998</v>
+        <v>2262.6999999999998</v>
       </c>
       <c r="C19" s="11">
-        <v>2294.85</v>
+        <v>2233.1</v>
       </c>
       <c r="D19" s="14">
-        <v>2335.5500000000002</v>
+        <v>2239</v>
       </c>
       <c r="E19" s="6">
-        <v>2333.5</v>
+        <v>2238.35</v>
       </c>
       <c r="F19" s="17">
         <v>3</v>
       </c>
       <c r="G19" s="6">
-        <v>2312</v>
+        <v>2259.5500000000002</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1494,22 +1494,22 @@
         <v>24</v>
       </c>
       <c r="B20" s="9">
-        <v>383.85</v>
+        <v>386.1</v>
       </c>
       <c r="C20" s="11">
-        <v>378</v>
+        <v>375.45</v>
       </c>
       <c r="D20" s="14">
-        <v>378.25</v>
+        <v>381.3</v>
       </c>
       <c r="E20" s="6">
-        <v>379.7</v>
+        <v>380.35</v>
       </c>
       <c r="F20" s="17">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G20" s="6">
-        <v>382.4</v>
+        <v>376.05</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1517,22 +1517,22 @@
         <v>25</v>
       </c>
       <c r="B21" s="9">
-        <v>209.35</v>
+        <v>201.15</v>
       </c>
       <c r="C21" s="11">
-        <v>205.05</v>
+        <v>198.45</v>
       </c>
       <c r="D21" s="14">
-        <v>209.25</v>
+        <v>198.65</v>
       </c>
       <c r="E21" s="6">
-        <v>208.25</v>
+        <v>199</v>
       </c>
       <c r="F21" s="17">
-        <v>136</v>
+        <v>75</v>
       </c>
       <c r="G21" s="6">
-        <v>206.35</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1540,22 +1540,22 @@
         <v>26</v>
       </c>
       <c r="B22" s="9">
-        <v>280.14999999999998</v>
+        <v>276.25</v>
       </c>
       <c r="C22" s="11">
-        <v>265.3</v>
+        <v>272.25</v>
       </c>
       <c r="D22" s="14">
-        <v>269</v>
+        <v>273.14999999999998</v>
       </c>
       <c r="E22" s="6">
-        <v>268.85000000000002</v>
+        <v>273.2</v>
       </c>
       <c r="F22" s="17">
-        <v>232</v>
+        <v>117</v>
       </c>
       <c r="G22" s="6">
-        <v>278.89999999999998</v>
+        <v>274.10000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1563,22 +1563,22 @@
         <v>27</v>
       </c>
       <c r="B23" s="9">
-        <v>1433</v>
+        <v>1430</v>
       </c>
       <c r="C23" s="11">
-        <v>1420.3</v>
+        <v>1416</v>
       </c>
       <c r="D23" s="14">
         <v>1428</v>
       </c>
       <c r="E23" s="6">
-        <v>1426.5</v>
+        <v>1425.25</v>
       </c>
       <c r="F23" s="17">
         <v>2</v>
       </c>
       <c r="G23" s="6">
-        <v>1426.45</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1586,22 +1586,22 @@
         <v>28</v>
       </c>
       <c r="B24" s="9">
-        <v>207</v>
+        <v>212.95</v>
       </c>
       <c r="C24" s="11">
-        <v>197</v>
+        <v>206.35</v>
       </c>
       <c r="D24" s="14">
-        <v>204.6</v>
+        <v>209.85</v>
       </c>
       <c r="E24" s="6">
-        <v>205.3</v>
+        <v>209.6</v>
       </c>
       <c r="F24" s="17">
-        <v>761</v>
+        <v>342</v>
       </c>
       <c r="G24" s="6">
-        <v>198.8</v>
+        <v>207.45</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1609,22 +1609,22 @@
         <v>29</v>
       </c>
       <c r="B25" s="9">
-        <v>1145.55</v>
+        <v>1193.7</v>
       </c>
       <c r="C25" s="11">
-        <v>1125</v>
+        <v>1170</v>
       </c>
       <c r="D25" s="14">
-        <v>1130</v>
+        <v>1191</v>
       </c>
       <c r="E25" s="6">
-        <v>1132.0999999999999</v>
+        <v>1189.1500000000001</v>
       </c>
       <c r="F25" s="17">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G25" s="6">
-        <v>1137.2</v>
+        <v>1181.6500000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1632,22 +1632,22 @@
         <v>30</v>
       </c>
       <c r="B26" s="9">
-        <v>275</v>
+        <v>287.2</v>
       </c>
       <c r="C26" s="11">
-        <v>270.85000000000002</v>
+        <v>275.7</v>
       </c>
       <c r="D26" s="14">
-        <v>273.14999999999998</v>
+        <v>278.60000000000002</v>
       </c>
       <c r="E26" s="6">
-        <v>273.05</v>
+        <v>278.89999999999998</v>
       </c>
       <c r="F26" s="17">
-        <v>47</v>
+        <v>177</v>
       </c>
       <c r="G26" s="6">
-        <v>271.14999999999998</v>
+        <v>281.89999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1655,22 +1655,22 @@
         <v>31</v>
       </c>
       <c r="B27" s="9">
-        <v>4970.3999999999996</v>
+        <v>4898.55</v>
       </c>
       <c r="C27" s="11">
-        <v>4920</v>
+        <v>4833.5</v>
       </c>
       <c r="D27" s="14">
-        <v>4932.95</v>
+        <v>4840</v>
       </c>
       <c r="E27" s="6">
-        <v>4936.3500000000004</v>
+        <v>4838.8999999999996</v>
       </c>
       <c r="F27" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G27" s="6">
-        <v>4928.55</v>
+        <v>4893.75</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1678,22 +1678,22 @@
         <v>32</v>
       </c>
       <c r="B28" s="9">
-        <v>835.85</v>
+        <v>794</v>
       </c>
       <c r="C28" s="11">
-        <v>807.25</v>
+        <v>782.25</v>
       </c>
       <c r="D28" s="14">
-        <v>810</v>
+        <v>783</v>
       </c>
       <c r="E28" s="6">
-        <v>810.15</v>
+        <v>783.65</v>
       </c>
       <c r="F28" s="17">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G28" s="6">
-        <v>831.05</v>
+        <v>787.5</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1701,22 +1701,22 @@
         <v>33</v>
       </c>
       <c r="B29" s="9">
-        <v>598.79999999999995</v>
+        <v>594.45000000000005</v>
       </c>
       <c r="C29" s="11">
-        <v>578.15</v>
+        <v>584</v>
       </c>
       <c r="D29" s="14">
-        <v>579.65</v>
+        <v>591.4</v>
       </c>
       <c r="E29" s="6">
-        <v>580.45000000000005</v>
+        <v>591.9</v>
       </c>
       <c r="F29" s="17">
-        <v>164</v>
+        <v>69</v>
       </c>
       <c r="G29" s="6">
-        <v>594.29999999999995</v>
+        <v>589.6</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1724,22 +1724,22 @@
         <v>34</v>
       </c>
       <c r="B30" s="9">
-        <v>811.85</v>
+        <v>797</v>
       </c>
       <c r="C30" s="11">
-        <v>797</v>
+        <v>787.05</v>
       </c>
       <c r="D30" s="14">
-        <v>797.75</v>
+        <v>787.55</v>
       </c>
       <c r="E30" s="6">
-        <v>799.65</v>
+        <v>790.8</v>
       </c>
       <c r="F30" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G30" s="6">
-        <v>801.8</v>
+        <v>788.3</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1747,22 +1747,22 @@
         <v>35</v>
       </c>
       <c r="B31" s="9">
-        <v>372.2</v>
+        <v>356.7</v>
       </c>
       <c r="C31" s="11">
-        <v>366.35</v>
+        <v>352.5</v>
       </c>
       <c r="D31" s="14">
-        <v>367</v>
+        <v>354.7</v>
       </c>
       <c r="E31" s="6">
-        <v>367.6</v>
+        <v>354.6</v>
       </c>
       <c r="F31" s="17">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G31" s="6">
-        <v>372.2</v>
+        <v>355.2</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1770,22 +1770,22 @@
         <v>36</v>
       </c>
       <c r="B32" s="9">
-        <v>1109.7</v>
+        <v>1093.75</v>
       </c>
       <c r="C32" s="11">
-        <v>1079.0999999999999</v>
+        <v>1071</v>
       </c>
       <c r="D32" s="14">
-        <v>1104.8499999999999</v>
+        <v>1073.2</v>
       </c>
       <c r="E32" s="6">
-        <v>1105.4000000000001</v>
+        <v>1075.55</v>
       </c>
       <c r="F32" s="17">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G32" s="6">
-        <v>1082.5</v>
+        <v>1091.75</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1793,22 +1793,22 @@
         <v>37</v>
       </c>
       <c r="B33" s="9">
-        <v>1482.35</v>
+        <v>1495.3</v>
       </c>
       <c r="C33" s="11">
-        <v>1459</v>
+        <v>1469.75</v>
       </c>
       <c r="D33" s="14">
-        <v>1464.95</v>
+        <v>1472</v>
       </c>
       <c r="E33" s="6">
-        <v>1466.4</v>
+        <v>1471.5</v>
       </c>
       <c r="F33" s="17">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G33" s="6">
-        <v>1461.25</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1816,22 +1816,22 @@
         <v>38</v>
       </c>
       <c r="B34" s="9">
-        <v>6722.95</v>
+        <v>6496.45</v>
       </c>
       <c r="C34" s="11">
-        <v>6590.15</v>
+        <v>6406</v>
       </c>
       <c r="D34" s="14">
-        <v>6599</v>
+        <v>6440</v>
       </c>
       <c r="E34" s="6">
-        <v>6606</v>
+        <v>6442.7</v>
       </c>
       <c r="F34" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G34" s="6">
-        <v>6685.65</v>
+        <v>6489</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1839,22 +1839,22 @@
         <v>39</v>
       </c>
       <c r="B35" s="9">
-        <v>1020</v>
+        <v>990.75</v>
       </c>
       <c r="C35" s="11">
-        <v>1001.25</v>
+        <v>972</v>
       </c>
       <c r="D35" s="14">
-        <v>1001.9</v>
+        <v>985.1</v>
       </c>
       <c r="E35" s="6">
-        <v>1004.95</v>
+        <v>986.15</v>
       </c>
       <c r="F35" s="17">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G35" s="6">
-        <v>1016.85</v>
+        <v>984.05</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1862,22 +1862,22 @@
         <v>40</v>
       </c>
       <c r="B36" s="9">
-        <v>1099.3</v>
+        <v>1097.7</v>
       </c>
       <c r="C36" s="11">
-        <v>1076.0999999999999</v>
+        <v>1076.05</v>
       </c>
       <c r="D36" s="14">
-        <v>1078</v>
+        <v>1093</v>
       </c>
       <c r="E36" s="6">
-        <v>1081.25</v>
+        <v>1092.25</v>
       </c>
       <c r="F36" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G36" s="6">
-        <v>1099.0999999999999</v>
+        <v>1090.0999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1885,22 +1885,22 @@
         <v>41</v>
       </c>
       <c r="B37" s="9">
-        <v>297</v>
+        <v>302.85000000000002</v>
       </c>
       <c r="C37" s="11">
-        <v>291.64999999999998</v>
+        <v>297.39999999999998</v>
       </c>
       <c r="D37" s="14">
-        <v>292.5</v>
+        <v>299.85000000000002</v>
       </c>
       <c r="E37" s="6">
-        <v>293.3</v>
+        <v>299.39999999999998</v>
       </c>
       <c r="F37" s="17">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="G37" s="6">
-        <v>294.10000000000002</v>
+        <v>298.95</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1908,22 +1908,22 @@
         <v>42</v>
       </c>
       <c r="B38" s="9">
-        <v>2828</v>
+        <v>2809</v>
       </c>
       <c r="C38" s="11">
-        <v>2753.8</v>
+        <v>2703</v>
       </c>
       <c r="D38" s="14">
-        <v>2793.5</v>
+        <v>2777.75</v>
       </c>
       <c r="E38" s="6">
-        <v>2810.95</v>
+        <v>2782.9</v>
       </c>
       <c r="F38" s="17">
         <v>9</v>
       </c>
       <c r="G38" s="6">
-        <v>2765.25</v>
+        <v>2726.85</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1931,22 +1931,22 @@
         <v>43</v>
       </c>
       <c r="B39" s="9">
-        <v>544.54999999999995</v>
+        <v>539</v>
       </c>
       <c r="C39" s="11">
-        <v>534.25</v>
+        <v>531.79999999999995</v>
       </c>
       <c r="D39" s="14">
-        <v>536</v>
+        <v>537.04999999999995</v>
       </c>
       <c r="E39" s="6">
-        <v>535.29999999999995</v>
+        <v>537.29999999999995</v>
       </c>
       <c r="F39" s="17">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G39" s="6">
-        <v>543.4</v>
+        <v>536.70000000000005</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1954,22 +1954,22 @@
         <v>44</v>
       </c>
       <c r="B40" s="9">
-        <v>2116.5500000000002</v>
+        <v>2093.5500000000002</v>
       </c>
       <c r="C40" s="11">
-        <v>2080.25</v>
+        <v>2021.75</v>
       </c>
       <c r="D40" s="14">
-        <v>2090</v>
+        <v>2027</v>
       </c>
       <c r="E40" s="6">
-        <v>2089.6999999999998</v>
+        <v>2027.05</v>
       </c>
       <c r="F40" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G40" s="6">
-        <v>2097.5</v>
+        <v>2092.4</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1977,22 +1977,22 @@
         <v>45</v>
       </c>
       <c r="B41" s="9">
-        <v>525</v>
+        <v>512</v>
       </c>
       <c r="C41" s="11">
-        <v>517</v>
+        <v>504.95</v>
       </c>
       <c r="D41" s="14">
-        <v>521.5</v>
+        <v>506</v>
       </c>
       <c r="E41" s="6">
-        <v>520.25</v>
+        <v>505.85</v>
       </c>
       <c r="F41" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G41" s="6">
-        <v>519.79999999999995</v>
+        <v>510.2</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2000,22 +2000,22 @@
         <v>46</v>
       </c>
       <c r="B42" s="9">
-        <v>2352.4499999999998</v>
+        <v>2220</v>
       </c>
       <c r="C42" s="11">
-        <v>2300</v>
+        <v>2184.1</v>
       </c>
       <c r="D42" s="14">
-        <v>2306</v>
+        <v>2187.5</v>
       </c>
       <c r="E42" s="6">
-        <v>2305.5500000000002</v>
+        <v>2187.5</v>
       </c>
       <c r="F42" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" s="6">
-        <v>2347.1999999999998</v>
+        <v>2217.5</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2023,22 +2023,22 @@
         <v>47</v>
       </c>
       <c r="B43" s="9">
-        <v>147.15</v>
+        <v>140.30000000000001</v>
       </c>
       <c r="C43" s="11">
-        <v>143.6</v>
+        <v>137.1</v>
       </c>
       <c r="D43" s="14">
-        <v>146.44999999999999</v>
+        <v>137.69999999999999</v>
       </c>
       <c r="E43" s="6">
-        <v>146.69999999999999</v>
+        <v>137.65</v>
       </c>
       <c r="F43" s="17">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="G43" s="6">
-        <v>143.94999999999999</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2046,22 +2046,22 @@
         <v>48</v>
       </c>
       <c r="B44" s="9">
-        <v>3669.05</v>
+        <v>3542</v>
       </c>
       <c r="C44" s="11">
-        <v>3626.85</v>
+        <v>3478</v>
       </c>
       <c r="D44" s="14">
-        <v>3640</v>
+        <v>3481</v>
       </c>
       <c r="E44" s="6">
-        <v>3648.1</v>
+        <v>3482.3</v>
       </c>
       <c r="F44" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G44" s="6">
-        <v>3651.15</v>
+        <v>3508.15</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2069,22 +2069,22 @@
         <v>49</v>
       </c>
       <c r="B45" s="9">
-        <v>6926.7</v>
+        <v>7180.8</v>
       </c>
       <c r="C45" s="11">
-        <v>6730.05</v>
+        <v>7012</v>
       </c>
       <c r="D45" s="14">
-        <v>6854</v>
+        <v>7155.15</v>
       </c>
       <c r="E45" s="6">
-        <v>6867.5</v>
+        <v>7162.5</v>
       </c>
       <c r="F45" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G45" s="6">
-        <v>6796.4</v>
+        <v>7060.95</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2092,22 +2092,22 @@
         <v>50</v>
       </c>
       <c r="B46" s="9">
-        <v>905</v>
+        <v>941.9</v>
       </c>
       <c r="C46" s="11">
-        <v>892.35</v>
+        <v>925.25</v>
       </c>
       <c r="D46" s="14">
-        <v>897</v>
+        <v>932</v>
       </c>
       <c r="E46" s="6">
-        <v>899.25</v>
+        <v>931.8</v>
       </c>
       <c r="F46" s="17">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G46" s="6">
-        <v>899</v>
+        <v>927.2</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2115,22 +2115,22 @@
         <v>51</v>
       </c>
       <c r="B47" s="9">
-        <v>6494.05</v>
+        <v>6439.35</v>
       </c>
       <c r="C47" s="11">
-        <v>6385.95</v>
+        <v>6291.45</v>
       </c>
       <c r="D47" s="14">
-        <v>6425</v>
+        <v>6334.9</v>
       </c>
       <c r="E47" s="6">
-        <v>6442.15</v>
+        <v>6335.1</v>
       </c>
       <c r="F47" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G47" s="6">
-        <v>6396.7</v>
+        <v>6308</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2138,22 +2138,22 @@
         <v>52</v>
       </c>
       <c r="B48" s="9">
-        <v>2962.35</v>
+        <v>2936.95</v>
       </c>
       <c r="C48" s="11">
-        <v>2900</v>
+        <v>2871.05</v>
       </c>
       <c r="D48" s="14">
-        <v>2909</v>
+        <v>2919</v>
       </c>
       <c r="E48" s="6">
-        <v>2911</v>
+        <v>2918.85</v>
       </c>
       <c r="F48" s="17">
         <v>1</v>
       </c>
       <c r="G48" s="6">
-        <v>2959.55</v>
+        <v>2877</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2161,22 +2161,22 @@
         <v>53</v>
       </c>
       <c r="B49" s="9">
-        <v>334.3</v>
+        <v>332.05</v>
       </c>
       <c r="C49" s="11">
-        <v>329</v>
+        <v>324.64999999999998</v>
       </c>
       <c r="D49" s="14">
-        <v>329.65</v>
+        <v>328</v>
       </c>
       <c r="E49" s="6">
-        <v>330</v>
+        <v>328.75</v>
       </c>
       <c r="F49" s="17">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G49" s="6">
-        <v>333.9</v>
+        <v>326.89999999999998</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2184,22 +2184,22 @@
         <v>54</v>
       </c>
       <c r="B50" s="9">
-        <v>910.7</v>
+        <v>945.95</v>
       </c>
       <c r="C50" s="11">
-        <v>894.5</v>
+        <v>919.25</v>
       </c>
       <c r="D50" s="14">
-        <v>900</v>
+        <v>920.9</v>
       </c>
       <c r="E50" s="6">
-        <v>900.1</v>
+        <v>921.7</v>
       </c>
       <c r="F50" s="17">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G50" s="6">
-        <v>909.45</v>
+        <v>939.5</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2207,22 +2207,22 @@
         <v>55</v>
       </c>
       <c r="B51" s="9">
-        <v>884.05</v>
+        <v>840</v>
       </c>
       <c r="C51" s="11">
-        <v>871.25</v>
+        <v>795.35</v>
       </c>
       <c r="D51" s="14">
-        <v>879</v>
+        <v>799</v>
       </c>
       <c r="E51" s="6">
-        <v>874.8</v>
+        <v>807.35</v>
       </c>
       <c r="F51" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G51" s="6">
-        <v>878</v>
+        <v>836.55</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2230,22 +2230,22 @@
         <v>56</v>
       </c>
       <c r="B52" s="9">
-        <v>676.3</v>
+        <v>638.70000000000005</v>
       </c>
       <c r="C52" s="11">
-        <v>672.55</v>
+        <v>626.54999999999995</v>
       </c>
       <c r="D52" s="14">
-        <v>675.6</v>
+        <v>634.5</v>
       </c>
       <c r="E52" s="6">
-        <v>675.05</v>
+        <v>633.95000000000005</v>
       </c>
       <c r="F52" s="17">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G52" s="6">
-        <v>673.5</v>
+        <v>636.79999999999995</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2253,22 +2253,22 @@
         <v>57</v>
       </c>
       <c r="B53" s="9">
-        <v>1265</v>
+        <v>1261.8</v>
       </c>
       <c r="C53" s="11">
-        <v>1236.75</v>
+        <v>1242.2</v>
       </c>
       <c r="D53" s="14">
-        <v>1253.95</v>
+        <v>1254.9000000000001</v>
       </c>
       <c r="E53" s="6">
-        <v>1250.95</v>
+        <v>1253.45</v>
       </c>
       <c r="F53" s="17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G53" s="6">
-        <v>1250.6500000000001</v>
+        <v>1257.05</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2276,22 +2276,22 @@
         <v>58</v>
       </c>
       <c r="B54" s="9">
-        <v>2483.6</v>
+        <v>2541.3000000000002</v>
       </c>
       <c r="C54" s="11">
-        <v>2396.5500000000002</v>
+        <v>2467.0500000000002</v>
       </c>
       <c r="D54" s="14">
-        <v>2455</v>
+        <v>2492.4</v>
       </c>
       <c r="E54" s="6">
-        <v>2468.85</v>
+        <v>2492.0500000000002</v>
       </c>
       <c r="F54" s="17">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G54" s="6">
-        <v>2412.1999999999998</v>
+        <v>2514.3000000000002</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2299,22 +2299,22 @@
         <v>59</v>
       </c>
       <c r="B55" s="9">
-        <v>471</v>
+        <v>474.85</v>
       </c>
       <c r="C55" s="11">
-        <v>459.65</v>
+        <v>465.05</v>
       </c>
       <c r="D55" s="14">
+        <v>468.5</v>
+      </c>
+      <c r="E55" s="6">
         <v>467</v>
       </c>
-      <c r="E55" s="6">
-        <v>466.65</v>
-      </c>
       <c r="F55" s="17">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="G55" s="6">
-        <v>461.75</v>
+        <v>467.8</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2322,22 +2322,22 @@
         <v>60</v>
       </c>
       <c r="B56" s="9">
-        <v>2231</v>
+        <v>2252.8000000000002</v>
       </c>
       <c r="C56" s="11">
-        <v>2182.6</v>
+        <v>2226.3000000000002</v>
       </c>
       <c r="D56" s="14">
-        <v>2190</v>
+        <v>2236.8000000000002</v>
       </c>
       <c r="E56" s="6">
-        <v>2194.4</v>
+        <v>2234.15</v>
       </c>
       <c r="F56" s="17">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G56" s="6">
-        <v>2228.9</v>
+        <v>2250.5</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2345,22 +2345,22 @@
         <v>61</v>
       </c>
       <c r="B57" s="9">
-        <v>580.5</v>
+        <v>595.75</v>
       </c>
       <c r="C57" s="11">
-        <v>563.9</v>
+        <v>581.1</v>
       </c>
       <c r="D57" s="14">
-        <v>580.5</v>
+        <v>590.4</v>
       </c>
       <c r="E57" s="6">
-        <v>577.29999999999995</v>
+        <v>590</v>
       </c>
       <c r="F57" s="17">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G57" s="6">
-        <v>567</v>
+        <v>589</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2368,22 +2368,22 @@
         <v>62</v>
       </c>
       <c r="B58" s="9">
-        <v>3065.5</v>
+        <v>3226.85</v>
       </c>
       <c r="C58" s="11">
-        <v>3008.5</v>
+        <v>3133</v>
       </c>
       <c r="D58" s="14">
-        <v>3047</v>
+        <v>3218</v>
       </c>
       <c r="E58" s="6">
-        <v>3045.5</v>
+        <v>3214.95</v>
       </c>
       <c r="F58" s="17">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G58" s="6">
-        <v>3027.3</v>
+        <v>3153.1</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2391,22 +2391,22 @@
         <v>63</v>
       </c>
       <c r="B59" s="9">
-        <v>1438.8</v>
+        <v>1564.95</v>
       </c>
       <c r="C59" s="11">
-        <v>1422.4</v>
+        <v>1534.8</v>
       </c>
       <c r="D59" s="14">
-        <v>1424</v>
+        <v>1555</v>
       </c>
       <c r="E59" s="6">
-        <v>1429.5</v>
+        <v>1553.95</v>
       </c>
       <c r="F59" s="17">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G59" s="6">
-        <v>1427.75</v>
+        <v>1535.4</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2414,22 +2414,22 @@
         <v>64</v>
       </c>
       <c r="B60" s="9">
-        <v>1694</v>
+        <v>1648</v>
       </c>
       <c r="C60" s="11">
-        <v>1663.45</v>
+        <v>1635</v>
       </c>
       <c r="D60" s="14">
-        <v>1664.4</v>
+        <v>1638.25</v>
       </c>
       <c r="E60" s="6">
-        <v>1665.75</v>
+        <v>1637.95</v>
       </c>
       <c r="F60" s="17">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G60" s="6">
-        <v>1685.9</v>
+        <v>1643.9</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2437,22 +2437,22 @@
         <v>65</v>
       </c>
       <c r="B61" s="9">
-        <v>3838.3</v>
+        <v>3876.3</v>
       </c>
       <c r="C61" s="11">
-        <v>3776</v>
+        <v>3788.15</v>
       </c>
       <c r="D61" s="14">
-        <v>3807.8</v>
+        <v>3844</v>
       </c>
       <c r="E61" s="6">
-        <v>3817.85</v>
+        <v>3856.5</v>
       </c>
       <c r="F61" s="17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G61" s="6">
-        <v>3814.75</v>
+        <v>3803.9</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2460,22 +2460,22 @@
         <v>66</v>
       </c>
       <c r="B62" s="9">
-        <v>583.35</v>
+        <v>620.5</v>
       </c>
       <c r="C62" s="11">
-        <v>578.70000000000005</v>
+        <v>587.6</v>
       </c>
       <c r="D62" s="14">
-        <v>580.79999999999995</v>
+        <v>609</v>
       </c>
       <c r="E62" s="6">
-        <v>580.70000000000005</v>
+        <v>610.29999999999995</v>
       </c>
       <c r="F62" s="17">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="G62" s="6">
-        <v>579.79999999999995</v>
+        <v>589.45000000000005</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2483,22 +2483,22 @@
         <v>67</v>
       </c>
       <c r="B63" s="9">
-        <v>524.45000000000005</v>
+        <v>529.85</v>
       </c>
       <c r="C63" s="11">
-        <v>517</v>
+        <v>520.04999999999995</v>
       </c>
       <c r="D63" s="14">
-        <v>518.04999999999995</v>
+        <v>525.20000000000005</v>
       </c>
       <c r="E63" s="6">
-        <v>518.35</v>
+        <v>524.95000000000005</v>
       </c>
       <c r="F63" s="17">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G63" s="6">
-        <v>520.1</v>
+        <v>523.20000000000005</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2506,22 +2506,22 @@
         <v>68</v>
       </c>
       <c r="B64" s="9">
-        <v>265.5</v>
+        <v>290</v>
       </c>
       <c r="C64" s="11">
-        <v>260.3</v>
+        <v>281.60000000000002</v>
       </c>
       <c r="D64" s="14">
-        <v>263.85000000000002</v>
+        <v>284.35000000000002</v>
       </c>
       <c r="E64" s="6">
-        <v>263.05</v>
+        <v>284</v>
       </c>
       <c r="F64" s="17">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="G64" s="6">
-        <v>263</v>
+        <v>283</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2529,22 +2529,22 @@
         <v>69</v>
       </c>
       <c r="B65" s="9">
+        <v>1654.9</v>
+      </c>
+      <c r="C65" s="11">
+        <v>1625.1</v>
+      </c>
+      <c r="D65" s="14">
         <v>1650</v>
       </c>
-      <c r="C65" s="11">
-        <v>1621.15</v>
-      </c>
-      <c r="D65" s="14">
-        <v>1640</v>
-      </c>
       <c r="E65" s="6">
-        <v>1639.25</v>
+        <v>1650.1</v>
       </c>
       <c r="F65" s="17">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G65" s="6">
-        <v>1640.8</v>
+        <v>1633.4</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2552,22 +2552,22 @@
         <v>70</v>
       </c>
       <c r="B66" s="9">
-        <v>525</v>
+        <v>558.70000000000005</v>
       </c>
       <c r="C66" s="11">
-        <v>519.85</v>
+        <v>533.95000000000005</v>
       </c>
       <c r="D66" s="14">
-        <v>522.70000000000005</v>
+        <v>546.20000000000005</v>
       </c>
       <c r="E66" s="6">
-        <v>522.85</v>
+        <v>546.95000000000005</v>
       </c>
       <c r="F66" s="17">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G66" s="6">
-        <v>521.5</v>
+        <v>536.45000000000005</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2575,22 +2575,22 @@
         <v>71</v>
       </c>
       <c r="B67" s="9">
-        <v>148.19999999999999</v>
+        <v>158</v>
       </c>
       <c r="C67" s="11">
-        <v>146.1</v>
+        <v>152.75</v>
       </c>
       <c r="D67" s="14">
-        <v>147.1</v>
+        <v>153.65</v>
       </c>
       <c r="E67" s="6">
-        <v>147</v>
+        <v>153.55000000000001</v>
       </c>
       <c r="F67" s="17">
-        <v>79</v>
+        <v>354</v>
       </c>
       <c r="G67" s="6">
-        <v>146.25</v>
+        <v>156.35</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2598,22 +2598,22 @@
         <v>72</v>
       </c>
       <c r="B68" s="9">
-        <v>443.85</v>
+        <v>455.3</v>
       </c>
       <c r="C68" s="11">
-        <v>436.35</v>
+        <v>438.85</v>
       </c>
       <c r="D68" s="14">
-        <v>437.15</v>
+        <v>446.9</v>
       </c>
       <c r="E68" s="6">
-        <v>437.8</v>
+        <v>446.6</v>
       </c>
       <c r="F68" s="17">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="G68" s="6">
-        <v>441.2</v>
+        <v>440</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2621,22 +2621,22 @@
         <v>73</v>
       </c>
       <c r="B69" s="9">
-        <v>602.75</v>
+        <v>591.95000000000005</v>
       </c>
       <c r="C69" s="11">
-        <v>587.6</v>
+        <v>583.6</v>
       </c>
       <c r="D69" s="14">
-        <v>595.54999999999995</v>
+        <v>588.6</v>
       </c>
       <c r="E69" s="6">
-        <v>594.5</v>
+        <v>588.35</v>
       </c>
       <c r="F69" s="17">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="G69" s="6">
-        <v>589.15</v>
+        <v>587.4</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2644,22 +2644,22 @@
         <v>74</v>
       </c>
       <c r="B70" s="9">
-        <v>249.7</v>
+        <v>234.95</v>
       </c>
       <c r="C70" s="11">
-        <v>243.05</v>
+        <v>231</v>
       </c>
       <c r="D70" s="14">
-        <v>245</v>
+        <v>232.75</v>
       </c>
       <c r="E70" s="6">
-        <v>245.15</v>
+        <v>232.2</v>
       </c>
       <c r="F70" s="17">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="G70" s="6">
-        <v>248.9</v>
+        <v>233.65</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2667,22 +2667,22 @@
         <v>75</v>
       </c>
       <c r="B71" s="9">
-        <v>2718.45</v>
+        <v>2670.95</v>
       </c>
       <c r="C71" s="11">
-        <v>2660.1</v>
+        <v>2621.0500000000002</v>
       </c>
       <c r="D71" s="14">
-        <v>2664</v>
+        <v>2625</v>
       </c>
       <c r="E71" s="6">
-        <v>2670.95</v>
+        <v>2624.65</v>
       </c>
       <c r="F71" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G71" s="6">
-        <v>2716.5</v>
+        <v>2641.15</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2690,22 +2690,22 @@
         <v>76</v>
       </c>
       <c r="B72" s="9">
-        <v>3215.35</v>
+        <v>3202.8</v>
       </c>
       <c r="C72" s="11">
-        <v>3143.35</v>
+        <v>3153.3</v>
       </c>
       <c r="D72" s="14">
-        <v>3182</v>
+        <v>3171.4</v>
       </c>
       <c r="E72" s="6">
-        <v>3179</v>
+        <v>3171.1</v>
       </c>
       <c r="F72" s="17">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G72" s="6">
-        <v>3151.7</v>
+        <v>3162.4</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2713,22 +2713,22 @@
         <v>77</v>
       </c>
       <c r="B73" s="9">
-        <v>1504.9</v>
+        <v>1538.95</v>
       </c>
       <c r="C73" s="11">
-        <v>1475.05</v>
+        <v>1520.35</v>
       </c>
       <c r="D73" s="14">
-        <v>1478.95</v>
+        <v>1531.55</v>
       </c>
       <c r="E73" s="6">
-        <v>1480.3</v>
+        <v>1531.3</v>
       </c>
       <c r="F73" s="17">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G73" s="6">
-        <v>1496.15</v>
+        <v>1537.6</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2736,22 +2736,22 @@
         <v>78</v>
       </c>
       <c r="B74" s="9">
-        <v>245.5</v>
+        <v>269.8</v>
       </c>
       <c r="C74" s="11">
-        <v>231.7</v>
+        <v>263.60000000000002</v>
       </c>
       <c r="D74" s="14">
-        <v>240.5</v>
+        <v>268.3</v>
       </c>
       <c r="E74" s="6">
-        <v>241.15</v>
+        <v>268.10000000000002</v>
       </c>
       <c r="F74" s="17">
-        <v>778</v>
+        <v>122</v>
       </c>
       <c r="G74" s="6">
-        <v>233.7</v>
+        <v>265.89999999999998</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2759,22 +2759,22 @@
         <v>79</v>
       </c>
       <c r="B75" s="9">
-        <v>960</v>
+        <v>1134.5999999999999</v>
       </c>
       <c r="C75" s="11">
-        <v>916.15</v>
+        <v>1098.3499999999999</v>
       </c>
       <c r="D75" s="14">
-        <v>960</v>
+        <v>1121.6500000000001</v>
       </c>
       <c r="E75" s="6">
-        <v>952.8</v>
+        <v>1112.7</v>
       </c>
       <c r="F75" s="17">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G75" s="6">
-        <v>920.7</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2782,22 +2782,22 @@
         <v>80</v>
       </c>
       <c r="B76" s="9">
-        <v>1230.95</v>
+        <v>1220</v>
       </c>
       <c r="C76" s="11">
-        <v>1214.4000000000001</v>
+        <v>1198.3</v>
       </c>
       <c r="D76" s="14">
-        <v>1218</v>
+        <v>1205.8</v>
       </c>
       <c r="E76" s="6">
-        <v>1217.7</v>
+        <v>1201.8</v>
       </c>
       <c r="F76" s="17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G76" s="6">
-        <v>1228.4000000000001</v>
+        <v>1206.8499999999999</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2805,22 +2805,22 @@
         <v>81</v>
       </c>
       <c r="B77" s="9">
-        <v>795.8</v>
+        <v>849.5</v>
       </c>
       <c r="C77" s="11">
-        <v>784.1</v>
+        <v>827.6</v>
       </c>
       <c r="D77" s="14">
-        <v>786.1</v>
+        <v>840.6</v>
       </c>
       <c r="E77" s="6">
-        <v>786.55</v>
+        <v>839.45</v>
       </c>
       <c r="F77" s="17">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G77" s="6">
-        <v>791</v>
+        <v>828.45</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2828,22 +2828,22 @@
         <v>82</v>
       </c>
       <c r="B78" s="9">
-        <v>4354.8</v>
+        <v>4513.45</v>
       </c>
       <c r="C78" s="11">
-        <v>4280</v>
+        <v>4445.1000000000004</v>
       </c>
       <c r="D78" s="14">
-        <v>4340</v>
+        <v>4455</v>
       </c>
       <c r="E78" s="6">
-        <v>4343.6499999999996</v>
+        <v>4463.8999999999996</v>
       </c>
       <c r="F78" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G78" s="6">
-        <v>4303.7</v>
+        <v>4505.1000000000004</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2851,22 +2851,22 @@
         <v>83</v>
       </c>
       <c r="B79" s="9">
-        <v>835</v>
+        <v>830.7</v>
       </c>
       <c r="C79" s="11">
-        <v>819.25</v>
+        <v>818.5</v>
       </c>
       <c r="D79" s="14">
-        <v>822.5</v>
+        <v>826</v>
       </c>
       <c r="E79" s="6">
-        <v>821</v>
+        <v>824.3</v>
       </c>
       <c r="F79" s="17">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="G79" s="6">
-        <v>832.7</v>
+        <v>829.6</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2874,22 +2874,22 @@
         <v>84</v>
       </c>
       <c r="B80" s="9">
-        <v>501.5</v>
+        <v>468.3</v>
       </c>
       <c r="C80" s="11">
-        <v>490.3</v>
+        <v>462.55</v>
       </c>
       <c r="D80" s="14">
-        <v>493.4</v>
+        <v>463.25</v>
       </c>
       <c r="E80" s="6">
-        <v>493.5</v>
+        <v>463.65</v>
       </c>
       <c r="F80" s="17">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G80" s="6">
-        <v>492.35</v>
+        <v>465.4</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2897,22 +2897,22 @@
         <v>85</v>
       </c>
       <c r="B81" s="9">
-        <v>1732.75</v>
+        <v>1741.5</v>
       </c>
       <c r="C81" s="11">
-        <v>1715.4</v>
+        <v>1718.5</v>
       </c>
       <c r="D81" s="14">
-        <v>1720</v>
+        <v>1726.95</v>
       </c>
       <c r="E81" s="6">
-        <v>1724</v>
+        <v>1727.2</v>
       </c>
       <c r="F81" s="17">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G81" s="6">
-        <v>1729.75</v>
+        <v>1734.9</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2920,22 +2920,22 @@
         <v>86</v>
       </c>
       <c r="B82" s="9">
-        <v>2478.6999999999998</v>
+        <v>2347.85</v>
       </c>
       <c r="C82" s="11">
-        <v>2443.75</v>
+        <v>2269.8000000000002</v>
       </c>
       <c r="D82" s="14">
-        <v>2451.6999999999998</v>
+        <v>2278.9</v>
       </c>
       <c r="E82" s="6">
-        <v>2448</v>
+        <v>2275.25</v>
       </c>
       <c r="F82" s="17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G82" s="6">
-        <v>2453.9</v>
+        <v>2340.8000000000002</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2943,22 +2943,22 @@
         <v>87</v>
       </c>
       <c r="B83" s="9">
-        <v>402.6</v>
+        <v>418.65</v>
       </c>
       <c r="C83" s="11">
-        <v>397</v>
+        <v>410.5</v>
       </c>
       <c r="D83" s="14">
-        <v>398.45</v>
+        <v>418.1</v>
       </c>
       <c r="E83" s="6">
-        <v>398.55</v>
+        <v>417.55</v>
       </c>
       <c r="F83" s="17">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G83" s="6">
-        <v>402.3</v>
+        <v>412.2</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2966,22 +2966,22 @@
         <v>88</v>
       </c>
       <c r="B84" s="9">
-        <v>647.54999999999995</v>
+        <v>661.15</v>
       </c>
       <c r="C84" s="11">
-        <v>637.95000000000005</v>
+        <v>648.75</v>
       </c>
       <c r="D84" s="14">
-        <v>641.29999999999995</v>
+        <v>658</v>
       </c>
       <c r="E84" s="6">
-        <v>642.29999999999995</v>
+        <v>657.75</v>
       </c>
       <c r="F84" s="17">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G84" s="6">
-        <v>646.9</v>
+        <v>652.15</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2989,22 +2989,22 @@
         <v>89</v>
       </c>
       <c r="B85" s="9">
-        <v>5553</v>
+        <v>5285.8</v>
       </c>
       <c r="C85" s="11">
-        <v>5510</v>
+        <v>5209.55</v>
       </c>
       <c r="D85" s="14">
-        <v>5539.95</v>
+        <v>5214</v>
       </c>
       <c r="E85" s="6">
-        <v>5542.65</v>
+        <v>5216.8500000000004</v>
       </c>
       <c r="F85" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G85" s="6">
-        <v>5523.5</v>
+        <v>5280</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3012,22 +3012,22 @@
         <v>90</v>
       </c>
       <c r="B86" s="9">
-        <v>5524.8</v>
+        <v>5295.6</v>
       </c>
       <c r="C86" s="11">
-        <v>5429.85</v>
+        <v>5235.1000000000004</v>
       </c>
       <c r="D86" s="14">
-        <v>5430.6</v>
+        <v>5260</v>
       </c>
       <c r="E86" s="6">
-        <v>5441.65</v>
+        <v>5258.45</v>
       </c>
       <c r="F86" s="17">
         <v>1</v>
       </c>
       <c r="G86" s="6">
-        <v>5456.75</v>
+        <v>5295.35</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3035,22 +3035,22 @@
         <v>91</v>
       </c>
       <c r="B87" s="9">
-        <v>1625</v>
+        <v>1700</v>
       </c>
       <c r="C87" s="11">
-        <v>1597.75</v>
+        <v>1650</v>
       </c>
       <c r="D87" s="14">
-        <v>1614</v>
+        <v>1667</v>
       </c>
       <c r="E87" s="6">
-        <v>1614.95</v>
+        <v>1669.85</v>
       </c>
       <c r="F87" s="17">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G87" s="6">
-        <v>1602.9</v>
+        <v>1651.8</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3058,22 +3058,22 @@
         <v>92</v>
       </c>
       <c r="B88" s="9">
-        <v>294.39999999999998</v>
+        <v>290</v>
       </c>
       <c r="C88" s="11">
-        <v>288.60000000000002</v>
+        <v>286.25</v>
       </c>
       <c r="D88" s="14">
-        <v>292.5</v>
+        <v>287.75</v>
       </c>
       <c r="E88" s="6">
-        <v>292.95</v>
+        <v>287.5</v>
       </c>
       <c r="F88" s="17">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="G88" s="6">
-        <v>292.3</v>
+        <v>288.55</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3081,22 +3081,22 @@
         <v>93</v>
       </c>
       <c r="B89" s="9">
-        <v>184.45</v>
+        <v>184.95</v>
       </c>
       <c r="C89" s="11">
-        <v>181.15</v>
+        <v>181.45</v>
       </c>
       <c r="D89" s="14">
-        <v>183</v>
+        <v>183.7</v>
       </c>
       <c r="E89" s="6">
-        <v>183.3</v>
+        <v>183.95</v>
       </c>
       <c r="F89" s="17">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G89" s="6">
-        <v>182.95</v>
+        <v>181.7</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3104,22 +3104,22 @@
         <v>94</v>
       </c>
       <c r="B90" s="9">
-        <v>537.25</v>
+        <v>526.25</v>
       </c>
       <c r="C90" s="11">
-        <v>528.75</v>
+        <v>522</v>
       </c>
       <c r="D90" s="14">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="E90" s="6">
-        <v>530.15</v>
+        <v>524.04999999999995</v>
       </c>
       <c r="F90" s="17">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G90" s="6">
-        <v>536.75</v>
+        <v>523.65</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3127,22 +3127,22 @@
         <v>95</v>
       </c>
       <c r="B91" s="9">
-        <v>1180</v>
+        <v>1170.4000000000001</v>
       </c>
       <c r="C91" s="11">
-        <v>1160.7</v>
+        <v>1151.6500000000001</v>
       </c>
       <c r="D91" s="14">
-        <v>1164.05</v>
+        <v>1167.5</v>
       </c>
       <c r="E91" s="6">
-        <v>1166.05</v>
+        <v>1165.8</v>
       </c>
       <c r="F91" s="17">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G91" s="6">
-        <v>1168.8</v>
+        <v>1161.75</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3150,22 +3150,22 @@
         <v>96</v>
       </c>
       <c r="B92" s="9">
+        <v>3817.9</v>
+      </c>
+      <c r="C92" s="11">
+        <v>3691.05</v>
+      </c>
+      <c r="D92" s="14">
         <v>3715</v>
       </c>
-      <c r="C92" s="11">
-        <v>3636</v>
-      </c>
-      <c r="D92" s="14">
-        <v>3664</v>
-      </c>
       <c r="E92" s="6">
-        <v>3676.95</v>
+        <v>3707.7</v>
       </c>
       <c r="F92" s="17">
         <v>2</v>
       </c>
       <c r="G92" s="6">
-        <v>3685.1</v>
+        <v>3815.3</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3173,22 +3173,22 @@
         <v>97</v>
       </c>
       <c r="B93" s="9">
-        <v>1763.55</v>
+        <v>1697.5</v>
       </c>
       <c r="C93" s="11">
-        <v>1730.95</v>
+        <v>1640</v>
       </c>
       <c r="D93" s="14">
-        <v>1740.95</v>
+        <v>1677.05</v>
       </c>
       <c r="E93" s="6">
-        <v>1748.3</v>
+        <v>1674</v>
       </c>
       <c r="F93" s="17">
         <v>2</v>
       </c>
       <c r="G93" s="6">
-        <v>1740.1</v>
+        <v>1689.55</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3196,22 +3196,22 @@
         <v>98</v>
       </c>
       <c r="B94" s="9">
-        <v>947.35</v>
+        <v>1005.1</v>
       </c>
       <c r="C94" s="11">
-        <v>920.7</v>
+        <v>959.25</v>
       </c>
       <c r="D94" s="14">
-        <v>931.4</v>
+        <v>997</v>
       </c>
       <c r="E94" s="6">
-        <v>930.2</v>
+        <v>1000.6</v>
       </c>
       <c r="F94" s="17">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G94" s="6">
-        <v>944.2</v>
+        <v>967.6</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3219,22 +3219,22 @@
         <v>99</v>
       </c>
       <c r="B95" s="9">
-        <v>1538.3</v>
+        <v>1552</v>
       </c>
       <c r="C95" s="11">
-        <v>1514.3</v>
+        <v>1506.9</v>
       </c>
       <c r="D95" s="14">
-        <v>1528</v>
+        <v>1552</v>
       </c>
       <c r="E95" s="6">
-        <v>1523.6</v>
+        <v>1541.65</v>
       </c>
       <c r="F95" s="17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G95" s="6">
-        <v>1535.8</v>
+        <v>1511.7</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -3242,22 +3242,22 @@
         <v>100</v>
       </c>
       <c r="B96" s="9">
-        <v>2785</v>
+        <v>2649.9</v>
       </c>
       <c r="C96" s="11">
-        <v>2720</v>
+        <v>2590.9</v>
       </c>
       <c r="D96" s="14">
-        <v>2722</v>
+        <v>2600</v>
       </c>
       <c r="E96" s="6">
-        <v>2727.6</v>
+        <v>2600.6</v>
       </c>
       <c r="F96" s="17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G96" s="6">
-        <v>2732.5</v>
+        <v>2642.85</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -3265,22 +3265,22 @@
         <v>101</v>
       </c>
       <c r="B97" s="9">
-        <v>1343.4</v>
+        <v>1350</v>
       </c>
       <c r="C97" s="11">
-        <v>1307.8499999999999</v>
+        <v>1329</v>
       </c>
       <c r="D97" s="14">
-        <v>1318</v>
+        <v>1335.7</v>
       </c>
       <c r="E97" s="6">
-        <v>1320.15</v>
+        <v>1337.9</v>
       </c>
       <c r="F97" s="17">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G97" s="6">
-        <v>1339.45</v>
+        <v>1338.3</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3288,22 +3288,22 @@
         <v>102</v>
       </c>
       <c r="B98" s="9">
-        <v>507.5</v>
+        <v>520.1</v>
       </c>
       <c r="C98" s="11">
-        <v>495.2</v>
+        <v>511.6</v>
       </c>
       <c r="D98" s="14">
-        <v>502.4</v>
+        <v>513.75</v>
       </c>
       <c r="E98" s="6">
-        <v>504.15</v>
+        <v>513.65</v>
       </c>
       <c r="F98" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G98" s="6">
-        <v>504</v>
+        <v>520</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3311,22 +3311,22 @@
         <v>103</v>
       </c>
       <c r="B99" s="9">
-        <v>5437.95</v>
+        <v>5331</v>
       </c>
       <c r="C99" s="11">
-        <v>5317.35</v>
+        <v>5145.6000000000004</v>
       </c>
       <c r="D99" s="14">
-        <v>5328.8</v>
+        <v>5151.05</v>
       </c>
       <c r="E99" s="6">
-        <v>5337.15</v>
+        <v>5157.6000000000004</v>
       </c>
       <c r="F99" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G99" s="6">
-        <v>5347.5</v>
+        <v>5294.45</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3334,22 +3334,22 @@
         <v>104</v>
       </c>
       <c r="B100" s="9">
-        <v>3199.25</v>
+        <v>3070.95</v>
       </c>
       <c r="C100" s="11">
-        <v>3142.7</v>
+        <v>3036.85</v>
       </c>
       <c r="D100" s="14">
-        <v>3143.6</v>
+        <v>3050</v>
       </c>
       <c r="E100" s="6">
-        <v>3150.7</v>
+        <v>3050.2</v>
       </c>
       <c r="F100" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G100" s="6">
-        <v>3196.15</v>
+        <v>3067.95</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3357,22 +3357,22 @@
         <v>105</v>
       </c>
       <c r="B101" s="9">
-        <v>240.8</v>
+        <v>241.9</v>
       </c>
       <c r="C101" s="11">
-        <v>236</v>
+        <v>233.85</v>
       </c>
       <c r="D101" s="14">
-        <v>238.7</v>
+        <v>240.1</v>
       </c>
       <c r="E101" s="6">
-        <v>238.3</v>
+        <v>240.05</v>
       </c>
       <c r="F101" s="17">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="G101" s="6">
-        <v>239.85</v>
+        <v>236.7</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3380,22 +3380,22 @@
         <v>106</v>
       </c>
       <c r="B102" s="9">
-        <v>339.1</v>
+        <v>358.3</v>
       </c>
       <c r="C102" s="11">
-        <v>334.85</v>
+        <v>348</v>
       </c>
       <c r="D102" s="14">
-        <v>336.95</v>
+        <v>354.35</v>
       </c>
       <c r="E102" s="6">
-        <v>337.75</v>
+        <v>353.85</v>
       </c>
       <c r="F102" s="17">
-        <v>96</v>
+        <v>380</v>
       </c>
       <c r="G102" s="6">
-        <v>338.1</v>
+        <v>352.8</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3403,22 +3403,22 @@
         <v>107</v>
       </c>
       <c r="B103" s="9">
-        <v>1406.55</v>
+        <v>1398.8</v>
       </c>
       <c r="C103" s="11">
-        <v>1360.25</v>
+        <v>1374.35</v>
       </c>
       <c r="D103" s="14">
-        <v>1365</v>
+        <v>1386.75</v>
       </c>
       <c r="E103" s="6">
-        <v>1366.1</v>
+        <v>1386.7</v>
       </c>
       <c r="F103" s="17">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="G103" s="6">
-        <v>1393.85</v>
+        <v>1382.75</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3426,22 +3426,22 @@
         <v>108</v>
       </c>
       <c r="B104" s="9">
-        <v>944.35</v>
+        <v>974.7</v>
       </c>
       <c r="C104" s="11">
-        <v>930</v>
+        <v>940.65</v>
       </c>
       <c r="D104" s="14">
-        <v>930.95</v>
+        <v>968</v>
       </c>
       <c r="E104" s="6">
-        <v>933.55</v>
+        <v>966.85</v>
       </c>
       <c r="F104" s="17">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G104" s="6">
-        <v>944</v>
+        <v>942.4</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3449,22 +3449,22 @@
         <v>109</v>
       </c>
       <c r="B105" s="9">
-        <v>8744</v>
+        <v>8590</v>
       </c>
       <c r="C105" s="11">
-        <v>8620</v>
+        <v>8435</v>
       </c>
       <c r="D105" s="14">
-        <v>8620.0499999999993</v>
+        <v>8444.4</v>
       </c>
       <c r="E105" s="6">
-        <v>8652.2999999999993</v>
+        <v>8471.15</v>
       </c>
       <c r="F105" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G105" s="6">
-        <v>8639</v>
+        <v>8582.85</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3472,22 +3472,22 @@
         <v>110</v>
       </c>
       <c r="B106" s="9">
-        <v>287.7</v>
+        <v>292.39999999999998</v>
       </c>
       <c r="C106" s="11">
-        <v>281.2</v>
+        <v>282.45</v>
       </c>
       <c r="D106" s="14">
-        <v>284</v>
+        <v>292.10000000000002</v>
       </c>
       <c r="E106" s="6">
-        <v>284.7</v>
+        <v>291.2</v>
       </c>
       <c r="F106" s="17">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="G106" s="6">
-        <v>282.64999999999998</v>
+        <v>282.75</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3495,22 +3495,22 @@
         <v>111</v>
       </c>
       <c r="B107" s="9">
-        <v>2759</v>
+        <v>2737.15</v>
       </c>
       <c r="C107" s="11">
-        <v>2708.25</v>
+        <v>2696.5</v>
       </c>
       <c r="D107" s="14">
-        <v>2739.1</v>
+        <v>2699</v>
       </c>
       <c r="E107" s="6">
-        <v>2740.15</v>
+        <v>2702.05</v>
       </c>
       <c r="F107" s="17">
         <v>2</v>
       </c>
       <c r="G107" s="6">
-        <v>2721.5</v>
+        <v>2732.65</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3518,22 +3518,22 @@
         <v>112</v>
       </c>
       <c r="B108" s="9">
-        <v>4830</v>
+        <v>4805</v>
       </c>
       <c r="C108" s="11">
-        <v>4740.6000000000004</v>
+        <v>4730.95</v>
       </c>
       <c r="D108" s="14">
-        <v>4795</v>
+        <v>4750</v>
       </c>
       <c r="E108" s="6">
-        <v>4801.8</v>
+        <v>4792.2</v>
       </c>
       <c r="F108" s="17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G108" s="6">
-        <v>4743.55</v>
+        <v>4786.7</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -3541,22 +3541,22 @@
         <v>113</v>
       </c>
       <c r="B109" s="9">
-        <v>285.2</v>
+        <v>297</v>
       </c>
       <c r="C109" s="11">
-        <v>279</v>
+        <v>291.3</v>
       </c>
       <c r="D109" s="14">
-        <v>281.89999999999998</v>
+        <v>294.60000000000002</v>
       </c>
       <c r="E109" s="6">
-        <v>281.95</v>
+        <v>294.64999999999998</v>
       </c>
       <c r="F109" s="17">
-        <v>143</v>
+        <v>231</v>
       </c>
       <c r="G109" s="6">
-        <v>281</v>
+        <v>294.2</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -3564,22 +3564,22 @@
         <v>114</v>
       </c>
       <c r="B110" s="9">
-        <v>210.95</v>
+        <v>182.2</v>
       </c>
       <c r="C110" s="11">
-        <v>203.55</v>
+        <v>175.15</v>
       </c>
       <c r="D110" s="14">
-        <v>206</v>
+        <v>176.8</v>
       </c>
       <c r="E110" s="6">
-        <v>206.3</v>
+        <v>176.7</v>
       </c>
       <c r="F110" s="17">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="G110" s="6">
-        <v>210.95</v>
+        <v>181.7</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -3587,22 +3587,22 @@
         <v>115</v>
       </c>
       <c r="B111" s="9">
-        <v>876.2</v>
+        <v>850.85</v>
       </c>
       <c r="C111" s="11">
-        <v>865.8</v>
+        <v>841.75</v>
       </c>
       <c r="D111" s="14">
-        <v>867.6</v>
+        <v>847</v>
       </c>
       <c r="E111" s="6">
-        <v>867.35</v>
+        <v>848.2</v>
       </c>
       <c r="F111" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G111" s="6">
-        <v>875.5</v>
+        <v>841.8</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -3610,22 +3610,22 @@
         <v>116</v>
       </c>
       <c r="B112" s="9">
-        <v>273.2</v>
+        <v>277.25</v>
       </c>
       <c r="C112" s="11">
-        <v>266.05</v>
+        <v>271.35000000000002</v>
       </c>
       <c r="D112" s="14">
-        <v>267</v>
+        <v>272.95</v>
       </c>
       <c r="E112" s="6">
-        <v>268.60000000000002</v>
+        <v>273.5</v>
       </c>
       <c r="F112" s="17">
-        <v>132</v>
+        <v>84</v>
       </c>
       <c r="G112" s="6">
-        <v>270.45</v>
+        <v>274.25</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3633,22 +3633,22 @@
         <v>117</v>
       </c>
       <c r="B113" s="9">
-        <v>468.65</v>
+        <v>469</v>
       </c>
       <c r="C113" s="11">
-        <v>459.05</v>
+        <v>453</v>
       </c>
       <c r="D113" s="14">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="E113" s="6">
-        <v>463.95</v>
+        <v>464.95</v>
       </c>
       <c r="F113" s="17">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="G113" s="6">
-        <v>461.25</v>
+        <v>458.75</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -3656,22 +3656,22 @@
         <v>118</v>
       </c>
       <c r="B114" s="9">
-        <v>751.6</v>
+        <v>723.85</v>
       </c>
       <c r="C114" s="11">
-        <v>736.6</v>
+        <v>715</v>
       </c>
       <c r="D114" s="14">
-        <v>739</v>
+        <v>717.4</v>
       </c>
       <c r="E114" s="6">
-        <v>739.05</v>
+        <v>716.9</v>
       </c>
       <c r="F114" s="17">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G114" s="6">
-        <v>740.4</v>
+        <v>721.9</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3679,22 +3679,22 @@
         <v>119</v>
       </c>
       <c r="B115" s="9">
-        <v>1536.25</v>
+        <v>1540.95</v>
       </c>
       <c r="C115" s="11">
-        <v>1502.5</v>
+        <v>1508.25</v>
       </c>
       <c r="D115" s="14">
-        <v>1530</v>
+        <v>1515</v>
       </c>
       <c r="E115" s="6">
-        <v>1529.15</v>
+        <v>1517.95</v>
       </c>
       <c r="F115" s="17">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G115" s="6">
-        <v>1503.1</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -3702,22 +3702,22 @@
         <v>120</v>
       </c>
       <c r="B116" s="9">
-        <v>4592.25</v>
+        <v>4735</v>
       </c>
       <c r="C116" s="11">
-        <v>4518.6000000000004</v>
+        <v>4672.2</v>
       </c>
       <c r="D116" s="14">
-        <v>4534.95</v>
+        <v>4677.2</v>
       </c>
       <c r="E116" s="6">
-        <v>4536.5</v>
+        <v>4689.2</v>
       </c>
       <c r="F116" s="17">
         <v>1</v>
       </c>
       <c r="G116" s="6">
-        <v>4558.45</v>
+        <v>4704</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -3725,22 +3725,22 @@
         <v>121</v>
       </c>
       <c r="B117" s="9">
-        <v>2413.3000000000002</v>
+        <v>2388.65</v>
       </c>
       <c r="C117" s="11">
-        <v>2381.75</v>
+        <v>2367.1999999999998</v>
       </c>
       <c r="D117" s="14">
-        <v>2382.9</v>
+        <v>2376</v>
       </c>
       <c r="E117" s="6">
-        <v>2385.8000000000002</v>
+        <v>2376</v>
       </c>
       <c r="F117" s="17">
         <v>1</v>
       </c>
       <c r="G117" s="6">
-        <v>2411.35</v>
+        <v>2386.25</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -3748,22 +3748,22 @@
         <v>122</v>
       </c>
       <c r="B118" s="9">
-        <v>822.4</v>
+        <v>825</v>
       </c>
       <c r="C118" s="11">
-        <v>795.85</v>
+        <v>793</v>
       </c>
       <c r="D118" s="14">
-        <v>803</v>
+        <v>798.55</v>
       </c>
       <c r="E118" s="6">
-        <v>808.4</v>
+        <v>796.5</v>
       </c>
       <c r="F118" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G118" s="6">
-        <v>813.2</v>
+        <v>805.7</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -3771,22 +3771,22 @@
         <v>123</v>
       </c>
       <c r="B119" s="9">
-        <v>1568.45</v>
+        <v>1569.1</v>
       </c>
       <c r="C119" s="11">
+        <v>1548.9</v>
+      </c>
+      <c r="D119" s="14">
         <v>1555</v>
       </c>
-      <c r="D119" s="14">
-        <v>1562</v>
-      </c>
       <c r="E119" s="6">
-        <v>1561.25</v>
+        <v>1552.1</v>
       </c>
       <c r="F119" s="17">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="G119" s="6">
-        <v>1560.2</v>
+        <v>1560.55</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -3794,22 +3794,22 @@
         <v>124</v>
       </c>
       <c r="B120" s="9">
-        <v>751</v>
+        <v>710.5</v>
       </c>
       <c r="C120" s="11">
-        <v>738.95</v>
+        <v>696</v>
       </c>
       <c r="D120" s="14">
-        <v>740.2</v>
+        <v>698.6</v>
       </c>
       <c r="E120" s="6">
-        <v>744.5</v>
+        <v>697.1</v>
       </c>
       <c r="F120" s="17">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G120" s="6">
-        <v>748.4</v>
+        <v>708.4</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -3817,22 +3817,22 @@
         <v>125</v>
       </c>
       <c r="B121" s="9">
-        <v>1848.7</v>
+        <v>2014</v>
       </c>
       <c r="C121" s="11">
-        <v>1818.55</v>
+        <v>1950.2</v>
       </c>
       <c r="D121" s="14">
-        <v>1821</v>
+        <v>1985</v>
       </c>
       <c r="E121" s="6">
-        <v>1824.55</v>
+        <v>1984.55</v>
       </c>
       <c r="F121" s="17">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G121" s="6">
-        <v>1840.7</v>
+        <v>1958.5</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -3840,22 +3840,22 @@
         <v>126</v>
       </c>
       <c r="B122" s="9">
-        <v>939.8</v>
+        <v>992.2</v>
       </c>
       <c r="C122" s="11">
-        <v>929.4</v>
+        <v>980.1</v>
       </c>
       <c r="D122" s="14">
-        <v>935.05</v>
+        <v>988.9</v>
       </c>
       <c r="E122" s="6">
-        <v>937.4</v>
+        <v>987.2</v>
       </c>
       <c r="F122" s="17">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G122" s="6">
-        <v>934.95</v>
+        <v>991.75</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -3863,22 +3863,22 @@
         <v>127</v>
       </c>
       <c r="B123" s="9">
-        <v>1341.35</v>
+        <v>1285.5</v>
       </c>
       <c r="C123" s="11">
-        <v>1316.3</v>
+        <v>1272.5</v>
       </c>
       <c r="D123" s="14">
-        <v>1319.9</v>
+        <v>1280.8</v>
       </c>
       <c r="E123" s="6">
-        <v>1322.25</v>
+        <v>1280.05</v>
       </c>
       <c r="F123" s="17">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G123" s="6">
-        <v>1336.2</v>
+        <v>1277.5999999999999</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -3886,22 +3886,22 @@
         <v>128</v>
       </c>
       <c r="B124" s="9">
-        <v>2638.6</v>
+        <v>2733</v>
       </c>
       <c r="C124" s="11">
-        <v>2598.1</v>
+        <v>2681.55</v>
       </c>
       <c r="D124" s="14">
-        <v>2620</v>
+        <v>2692</v>
       </c>
       <c r="E124" s="6">
-        <v>2626.95</v>
+        <v>2690.85</v>
       </c>
       <c r="F124" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G124" s="6">
-        <v>2602.9499999999998</v>
+        <v>2699.65</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -3909,22 +3909,22 @@
         <v>129</v>
       </c>
       <c r="B125" s="9">
-        <v>1153</v>
+        <v>1164.5</v>
       </c>
       <c r="C125" s="11">
-        <v>1114.8499999999999</v>
+        <v>1138</v>
       </c>
       <c r="D125" s="14">
-        <v>1138.5999999999999</v>
+        <v>1151</v>
       </c>
       <c r="E125" s="6">
-        <v>1125.9000000000001</v>
+        <v>1145.7</v>
       </c>
       <c r="F125" s="17">
         <v>12</v>
       </c>
       <c r="G125" s="6">
-        <v>1143.8499999999999</v>
+        <v>1158.25</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -3932,22 +3932,22 @@
         <v>130</v>
       </c>
       <c r="B126" s="9">
-        <v>3938.35</v>
+        <v>3935</v>
       </c>
       <c r="C126" s="11">
-        <v>3868.45</v>
+        <v>3842.5</v>
       </c>
       <c r="D126" s="14">
-        <v>3878</v>
+        <v>3915.5</v>
       </c>
       <c r="E126" s="6">
-        <v>3885.8</v>
+        <v>3919.8</v>
       </c>
       <c r="F126" s="17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G126" s="6">
-        <v>3935</v>
+        <v>3884.1</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -3955,22 +3955,22 @@
         <v>131</v>
       </c>
       <c r="B127" s="9">
-        <v>2138</v>
+        <v>2267.6999999999998</v>
       </c>
       <c r="C127" s="11">
-        <v>2104.35</v>
+        <v>2220</v>
       </c>
       <c r="D127" s="14">
-        <v>2108.9</v>
+        <v>2239</v>
       </c>
       <c r="E127" s="6">
-        <v>2115.9499999999998</v>
+        <v>2232.35</v>
       </c>
       <c r="F127" s="17">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G127" s="6">
-        <v>2135</v>
+        <v>2244.85</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -3978,22 +3978,22 @@
         <v>132</v>
       </c>
       <c r="B128" s="9">
-        <v>1736.9</v>
+        <v>1717.35</v>
       </c>
       <c r="C128" s="11">
-        <v>1708</v>
+        <v>1693</v>
       </c>
       <c r="D128" s="14">
-        <v>1724</v>
+        <v>1716</v>
       </c>
       <c r="E128" s="6">
-        <v>1714.9</v>
+        <v>1713.15</v>
       </c>
       <c r="F128" s="17">
         <v>1</v>
       </c>
       <c r="G128" s="6">
-        <v>1734.8</v>
+        <v>1696.4</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -4001,22 +4001,22 @@
         <v>133</v>
       </c>
       <c r="B129" s="9">
-        <v>10028</v>
+        <v>10138.450000000001</v>
       </c>
       <c r="C129" s="11">
-        <v>9894.0499999999993</v>
+        <v>9966.2000000000007</v>
       </c>
       <c r="D129" s="14">
-        <v>10023</v>
+        <v>9986</v>
       </c>
       <c r="E129" s="6">
-        <v>10000.9</v>
+        <v>9978.4</v>
       </c>
       <c r="F129" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G129" s="6">
-        <v>9974.15</v>
+        <v>10131.450000000001</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -4024,22 +4024,22 @@
         <v>134</v>
       </c>
       <c r="B130" s="9">
-        <v>496.6</v>
+        <v>479.9</v>
       </c>
       <c r="C130" s="11">
-        <v>487.9</v>
+        <v>470</v>
       </c>
       <c r="D130" s="14">
-        <v>488.8</v>
+        <v>474.55</v>
       </c>
       <c r="E130" s="6">
-        <v>488.7</v>
+        <v>474.25</v>
       </c>
       <c r="F130" s="17">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G130" s="6">
-        <v>493</v>
+        <v>478.8</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -4047,22 +4047,22 @@
         <v>135</v>
       </c>
       <c r="B131" s="9">
-        <v>271.55</v>
+        <v>279</v>
       </c>
       <c r="C131" s="11">
-        <v>268</v>
+        <v>272.75</v>
       </c>
       <c r="D131" s="14">
-        <v>268.35000000000002</v>
+        <v>275.8</v>
       </c>
       <c r="E131" s="6">
-        <v>268.35000000000002</v>
+        <v>276.35000000000002</v>
       </c>
       <c r="F131" s="17">
-        <v>59</v>
+        <v>104</v>
       </c>
       <c r="G131" s="6">
-        <v>271.05</v>
+        <v>274.85000000000002</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -4070,22 +4070,22 @@
         <v>136</v>
       </c>
       <c r="B132" s="9">
-        <v>1107.0999999999999</v>
+        <v>1127</v>
       </c>
       <c r="C132" s="11">
-        <v>1091</v>
+        <v>1106</v>
       </c>
       <c r="D132" s="14">
-        <v>1092</v>
+        <v>1107</v>
       </c>
       <c r="E132" s="6">
-        <v>1095.05</v>
+        <v>1110.8499999999999</v>
       </c>
       <c r="F132" s="17">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G132" s="6">
-        <v>1096.4000000000001</v>
+        <v>1113.5</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -4093,22 +4093,22 @@
         <v>137</v>
       </c>
       <c r="B133" s="9">
-        <v>177.2</v>
+        <v>157.15</v>
       </c>
       <c r="C133" s="11">
-        <v>169.35</v>
+        <v>153.80000000000001</v>
       </c>
       <c r="D133" s="14">
-        <v>174.1</v>
+        <v>154.94999999999999</v>
       </c>
       <c r="E133" s="6">
-        <v>173.45</v>
+        <v>154.9</v>
       </c>
       <c r="F133" s="17">
-        <v>272</v>
+        <v>137</v>
       </c>
       <c r="G133" s="6">
-        <v>171.05</v>
+        <v>157.05000000000001</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4116,22 +4116,22 @@
         <v>138</v>
       </c>
       <c r="B134" s="19">
-        <v>937</v>
+        <v>952.05</v>
       </c>
       <c r="C134" s="12">
-        <v>903.55</v>
+        <v>934</v>
       </c>
       <c r="D134" s="15">
-        <v>919.6</v>
+        <v>949</v>
       </c>
       <c r="E134" s="7">
-        <v>923.25</v>
+        <v>946.25</v>
       </c>
       <c r="F134" s="18">
         <v>15</v>
       </c>
       <c r="G134" s="7">
-        <v>905.6</v>
+        <v>934.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added fix for close scraping from NSE
</commit_message>
<xml_diff>
--- a/algo high low.xlsx
+++ b/algo high low.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -1043,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J107" sqref="J107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,22 +1080,22 @@
         <v>6</v>
       </c>
       <c r="B2" s="8">
-        <v>673.1</v>
+        <v>650.95000000000005</v>
       </c>
       <c r="C2" s="10">
-        <v>660.55</v>
+        <v>620.1</v>
       </c>
       <c r="D2" s="13">
-        <v>661.8</v>
+        <v>621.45000000000005</v>
       </c>
       <c r="E2" s="5">
-        <v>662.1</v>
+        <v>621.9</v>
       </c>
       <c r="F2" s="16">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="G2" s="5">
-        <v>672.5</v>
+        <v>648.5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1103,22 +1103,22 @@
         <v>7</v>
       </c>
       <c r="B3" s="9">
-        <v>5665</v>
+        <v>8109.25</v>
       </c>
       <c r="C3" s="11">
-        <v>5528.8</v>
+        <v>7965.2</v>
       </c>
       <c r="D3" s="14">
-        <v>5623</v>
+        <v>8064</v>
       </c>
       <c r="E3" s="6">
-        <v>5631.55</v>
+        <v>8084.3</v>
       </c>
       <c r="F3" s="17">
         <v>4</v>
       </c>
       <c r="G3" s="6">
-        <v>5536.4</v>
+        <v>8051.9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1126,22 +1126,22 @@
         <v>8</v>
       </c>
       <c r="B4" s="9">
-        <v>194.4</v>
+        <v>224.85</v>
       </c>
       <c r="C4" s="11">
-        <v>187.6</v>
+        <v>219.65</v>
       </c>
       <c r="D4" s="14">
-        <v>191.3</v>
+        <v>220.2</v>
       </c>
       <c r="E4" s="6">
-        <v>190.95</v>
+        <v>220.45</v>
       </c>
       <c r="F4" s="17">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="G4" s="6">
-        <v>187.7</v>
+        <v>222.85</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1149,22 +1149,22 @@
         <v>9</v>
       </c>
       <c r="B5" s="9">
-        <v>235.8</v>
+        <v>267.10000000000002</v>
       </c>
       <c r="C5" s="11">
-        <v>229.25</v>
+        <v>260.10000000000002</v>
       </c>
       <c r="D5" s="14">
-        <v>230.3</v>
+        <v>262.95</v>
       </c>
       <c r="E5" s="6">
-        <v>230</v>
+        <v>263.05</v>
       </c>
       <c r="F5" s="17">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="G5" s="6">
-        <v>233.95</v>
+        <v>261.89999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1172,22 +1172,22 @@
         <v>10</v>
       </c>
       <c r="B6" s="9">
-        <v>3348</v>
+        <v>3118.85</v>
       </c>
       <c r="C6" s="11">
-        <v>3310.05</v>
+        <v>3044.85</v>
       </c>
       <c r="D6" s="14">
-        <v>3320.95</v>
+        <v>3047</v>
       </c>
       <c r="E6" s="6">
-        <v>3317.15</v>
+        <v>3049.75</v>
       </c>
       <c r="F6" s="17">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G6" s="6">
-        <v>3344.9</v>
+        <v>3066.65</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1195,22 +1195,22 @@
         <v>11</v>
       </c>
       <c r="B7" s="9">
-        <v>1353.8</v>
+        <v>1353.95</v>
       </c>
       <c r="C7" s="11">
-        <v>1336.4</v>
+        <v>1333</v>
       </c>
       <c r="D7" s="14">
-        <v>1342</v>
+        <v>1337.6</v>
       </c>
       <c r="E7" s="6">
-        <v>1342.6</v>
+        <v>1337.85</v>
       </c>
       <c r="F7" s="17">
         <v>21</v>
       </c>
       <c r="G7" s="6">
-        <v>1349.45</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1218,22 +1218,22 @@
         <v>12</v>
       </c>
       <c r="B8" s="9">
-        <v>5169.5</v>
+        <v>5310</v>
       </c>
       <c r="C8" s="11">
-        <v>5110</v>
+        <v>5191.1000000000004</v>
       </c>
       <c r="D8" s="14">
-        <v>5121</v>
+        <v>5229.2</v>
       </c>
       <c r="E8" s="6">
-        <v>5124.8999999999996</v>
+        <v>5246.95</v>
       </c>
       <c r="F8" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="6">
-        <v>5128</v>
+        <v>5255.7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1241,22 +1241,22 @@
         <v>13</v>
       </c>
       <c r="B9" s="9">
-        <v>618.9</v>
+        <v>618.25</v>
       </c>
       <c r="C9" s="11">
-        <v>612.54999999999995</v>
+        <v>609.9</v>
       </c>
       <c r="D9" s="14">
-        <v>618</v>
+        <v>611.70000000000005</v>
       </c>
       <c r="E9" s="6">
-        <v>617.15</v>
+        <v>613.25</v>
       </c>
       <c r="F9" s="17">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G9" s="6">
-        <v>617.25</v>
+        <v>615.20000000000005</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1264,22 +1264,22 @@
         <v>14</v>
       </c>
       <c r="B10" s="9">
-        <v>6166.75</v>
+        <v>5880</v>
       </c>
       <c r="C10" s="11">
-        <v>6022.85</v>
+        <v>5820</v>
       </c>
       <c r="D10" s="14">
-        <v>6050</v>
+        <v>5854.8</v>
       </c>
       <c r="E10" s="6">
-        <v>6033.3</v>
+        <v>5848.8</v>
       </c>
       <c r="F10" s="17">
         <v>5</v>
       </c>
       <c r="G10" s="6">
-        <v>6101.05</v>
+        <v>5862.1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1287,22 +1287,22 @@
         <v>15</v>
       </c>
       <c r="B11" s="9">
-        <v>537.85</v>
+        <v>481.8</v>
       </c>
       <c r="C11" s="11">
-        <v>521.70000000000005</v>
+        <v>463.5</v>
       </c>
       <c r="D11" s="14">
-        <v>535.5</v>
+        <v>473</v>
       </c>
       <c r="E11" s="6">
-        <v>535.1</v>
+        <v>474.1</v>
       </c>
       <c r="F11" s="17">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="G11" s="6">
-        <v>530.35</v>
+        <v>473.2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1310,22 +1310,22 @@
         <v>16</v>
       </c>
       <c r="B12" s="9">
-        <v>173.95</v>
+        <v>204.3</v>
       </c>
       <c r="C12" s="11">
-        <v>171.3</v>
+        <v>200.5</v>
       </c>
       <c r="D12" s="14">
-        <v>172</v>
+        <v>201.55</v>
       </c>
       <c r="E12" s="6">
-        <v>172.05</v>
+        <v>201.4</v>
       </c>
       <c r="F12" s="17">
-        <v>177</v>
+        <v>105</v>
       </c>
       <c r="G12" s="6">
-        <v>171.8</v>
+        <v>203.95</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1333,22 +1333,22 @@
         <v>17</v>
       </c>
       <c r="B13" s="9">
-        <v>2104.6999999999998</v>
+        <v>2224.9499999999998</v>
       </c>
       <c r="C13" s="11">
-        <v>2071.5500000000002</v>
+        <v>2181.6</v>
       </c>
       <c r="D13" s="14">
-        <v>2095</v>
+        <v>2213.15</v>
       </c>
       <c r="E13" s="6">
-        <v>2097.1</v>
+        <v>2212.5</v>
       </c>
       <c r="F13" s="17">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G13" s="6">
-        <v>2091.15</v>
+        <v>2218.4</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1356,22 +1356,22 @@
         <v>18</v>
       </c>
       <c r="B14" s="9">
-        <v>6167.95</v>
+        <v>5973.95</v>
       </c>
       <c r="C14" s="11">
-        <v>6070.05</v>
+        <v>5870</v>
       </c>
       <c r="D14" s="14">
-        <v>6077.5</v>
+        <v>5874</v>
       </c>
       <c r="E14" s="6">
-        <v>6080.25</v>
+        <v>5876.6</v>
       </c>
       <c r="F14" s="17">
         <v>0</v>
       </c>
       <c r="G14" s="6">
-        <v>6150.7</v>
+        <v>5955.3</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1379,22 +1379,22 @@
         <v>19</v>
       </c>
       <c r="B15" s="9">
-        <v>582.29999999999995</v>
+        <v>648.9</v>
       </c>
       <c r="C15" s="11">
-        <v>575.95000000000005</v>
+        <v>616.85</v>
       </c>
       <c r="D15" s="14">
-        <v>579.5</v>
+        <v>621.9</v>
       </c>
       <c r="E15" s="6">
-        <v>580.1</v>
+        <v>622.95000000000005</v>
       </c>
       <c r="F15" s="17">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="G15" s="6">
-        <v>581.35</v>
+        <v>647.20000000000005</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1402,22 +1402,22 @@
         <v>20</v>
       </c>
       <c r="B16" s="9">
-        <v>1114</v>
+        <v>1172.6500000000001</v>
       </c>
       <c r="C16" s="11">
-        <v>1085</v>
+        <v>1152</v>
       </c>
       <c r="D16" s="14">
-        <v>1088.05</v>
+        <v>1157.05</v>
       </c>
       <c r="E16" s="6">
-        <v>1090.9000000000001</v>
+        <v>1158.4000000000001</v>
       </c>
       <c r="F16" s="17">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="G16" s="6">
-        <v>1091.8</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1425,22 +1425,22 @@
         <v>21</v>
       </c>
       <c r="B17" s="9">
-        <v>1625</v>
+        <v>1589.65</v>
       </c>
       <c r="C17" s="11">
-        <v>1603.3</v>
+        <v>1566.6</v>
       </c>
       <c r="D17" s="14">
-        <v>1622.7</v>
+        <v>1570.75</v>
       </c>
       <c r="E17" s="6">
-        <v>1619.3</v>
+        <v>1569.05</v>
       </c>
       <c r="F17" s="17">
         <v>5</v>
       </c>
       <c r="G17" s="6">
-        <v>1610.7</v>
+        <v>1581.75</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1448,22 +1448,22 @@
         <v>22</v>
       </c>
       <c r="B18" s="9">
-        <v>6639.95</v>
+        <v>6731.95</v>
       </c>
       <c r="C18" s="11">
-        <v>6557.45</v>
+        <v>6645.05</v>
       </c>
       <c r="D18" s="14">
-        <v>6604</v>
+        <v>6681</v>
       </c>
       <c r="E18" s="6">
-        <v>6602.45</v>
+        <v>6680</v>
       </c>
       <c r="F18" s="17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G18" s="6">
-        <v>6631</v>
+        <v>6685</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1471,22 +1471,22 @@
         <v>23</v>
       </c>
       <c r="B19" s="9">
-        <v>2262.6999999999998</v>
+        <v>2528</v>
       </c>
       <c r="C19" s="11">
-        <v>2233.1</v>
+        <v>2475.5</v>
       </c>
       <c r="D19" s="14">
-        <v>2239</v>
+        <v>2507</v>
       </c>
       <c r="E19" s="6">
-        <v>2238.35</v>
+        <v>2516.6</v>
       </c>
       <c r="F19" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G19" s="6">
-        <v>2259.5500000000002</v>
+        <v>2498.6999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1494,22 +1494,22 @@
         <v>24</v>
       </c>
       <c r="B20" s="9">
-        <v>386.1</v>
+        <v>381.5</v>
       </c>
       <c r="C20" s="11">
-        <v>375.45</v>
+        <v>376.25</v>
       </c>
       <c r="D20" s="14">
-        <v>381.3</v>
+        <v>377.5</v>
       </c>
       <c r="E20" s="6">
-        <v>380.35</v>
+        <v>377.25</v>
       </c>
       <c r="F20" s="17">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="G20" s="6">
-        <v>376.05</v>
+        <v>381.1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1517,22 +1517,22 @@
         <v>25</v>
       </c>
       <c r="B21" s="9">
-        <v>201.15</v>
+        <v>191.4</v>
       </c>
       <c r="C21" s="11">
-        <v>198.45</v>
+        <v>188.15</v>
       </c>
       <c r="D21" s="14">
-        <v>198.65</v>
+        <v>189.1</v>
       </c>
       <c r="E21" s="6">
-        <v>199</v>
+        <v>189.9</v>
       </c>
       <c r="F21" s="17">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="G21" s="6">
-        <v>201</v>
+        <v>190.4</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1540,22 +1540,22 @@
         <v>26</v>
       </c>
       <c r="B22" s="9">
-        <v>276.25</v>
+        <v>267.7</v>
       </c>
       <c r="C22" s="11">
-        <v>272.25</v>
+        <v>262.60000000000002</v>
       </c>
       <c r="D22" s="14">
-        <v>273.14999999999998</v>
+        <v>263.89999999999998</v>
       </c>
       <c r="E22" s="6">
-        <v>273.2</v>
+        <v>263.89999999999998</v>
       </c>
       <c r="F22" s="17">
-        <v>117</v>
+        <v>192</v>
       </c>
       <c r="G22" s="6">
-        <v>274.10000000000002</v>
+        <v>263.89999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1563,22 +1563,22 @@
         <v>27</v>
       </c>
       <c r="B23" s="9">
-        <v>1430</v>
+        <v>1336</v>
       </c>
       <c r="C23" s="11">
-        <v>1416</v>
+        <v>1321</v>
       </c>
       <c r="D23" s="14">
-        <v>1428</v>
+        <v>1326.2</v>
       </c>
       <c r="E23" s="6">
-        <v>1425.25</v>
+        <v>1327.15</v>
       </c>
       <c r="F23" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G23" s="6">
-        <v>1424</v>
+        <v>1334.7</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1586,22 +1586,22 @@
         <v>28</v>
       </c>
       <c r="B24" s="9">
-        <v>212.95</v>
+        <v>234.5</v>
       </c>
       <c r="C24" s="11">
-        <v>206.35</v>
+        <v>229.55</v>
       </c>
       <c r="D24" s="14">
-        <v>209.85</v>
+        <v>233.25</v>
       </c>
       <c r="E24" s="6">
-        <v>209.6</v>
+        <v>232.85</v>
       </c>
       <c r="F24" s="17">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="G24" s="6">
-        <v>207.45</v>
+        <v>232.1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1609,22 +1609,22 @@
         <v>29</v>
       </c>
       <c r="B25" s="9">
-        <v>1193.7</v>
+        <v>1467.45</v>
       </c>
       <c r="C25" s="11">
-        <v>1170</v>
+        <v>1433.75</v>
       </c>
       <c r="D25" s="14">
-        <v>1191</v>
+        <v>1459.25</v>
       </c>
       <c r="E25" s="6">
-        <v>1189.1500000000001</v>
+        <v>1462.7</v>
       </c>
       <c r="F25" s="17">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="G25" s="6">
-        <v>1181.6500000000001</v>
+        <v>1441.8</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1632,22 +1632,22 @@
         <v>30</v>
       </c>
       <c r="B26" s="9">
-        <v>287.2</v>
+        <v>321.2</v>
       </c>
       <c r="C26" s="11">
-        <v>275.7</v>
+        <v>309.10000000000002</v>
       </c>
       <c r="D26" s="14">
-        <v>278.60000000000002</v>
+        <v>311.5</v>
       </c>
       <c r="E26" s="6">
-        <v>278.89999999999998</v>
+        <v>311.89999999999998</v>
       </c>
       <c r="F26" s="17">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="G26" s="6">
-        <v>281.89999999999998</v>
+        <v>313.85000000000002</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1655,22 +1655,22 @@
         <v>31</v>
       </c>
       <c r="B27" s="9">
-        <v>4898.55</v>
+        <v>5144.3500000000004</v>
       </c>
       <c r="C27" s="11">
-        <v>4833.5</v>
+        <v>5053.45</v>
       </c>
       <c r="D27" s="14">
-        <v>4840</v>
+        <v>5062.05</v>
       </c>
       <c r="E27" s="6">
-        <v>4838.8999999999996</v>
+        <v>5064</v>
       </c>
       <c r="F27" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G27" s="6">
-        <v>4893.75</v>
+        <v>5129</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1678,22 +1678,22 @@
         <v>32</v>
       </c>
       <c r="B28" s="9">
-        <v>794</v>
+        <v>614.95000000000005</v>
       </c>
       <c r="C28" s="11">
-        <v>782.25</v>
+        <v>600.04999999999995</v>
       </c>
       <c r="D28" s="14">
-        <v>783</v>
+        <v>611.85</v>
       </c>
       <c r="E28" s="6">
-        <v>783.65</v>
+        <v>612.45000000000005</v>
       </c>
       <c r="F28" s="17">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="G28" s="6">
-        <v>787.5</v>
+        <v>602.5</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1701,22 +1701,22 @@
         <v>33</v>
       </c>
       <c r="B29" s="9">
-        <v>594.45000000000005</v>
+        <v>119.6</v>
       </c>
       <c r="C29" s="11">
-        <v>584</v>
+        <v>116.9</v>
       </c>
       <c r="D29" s="14">
-        <v>591.4</v>
+        <v>119.1</v>
       </c>
       <c r="E29" s="6">
-        <v>591.9</v>
+        <v>119</v>
       </c>
       <c r="F29" s="17">
-        <v>69</v>
+        <v>581</v>
       </c>
       <c r="G29" s="6">
-        <v>589.6</v>
+        <v>117.15</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1724,22 +1724,22 @@
         <v>34</v>
       </c>
       <c r="B30" s="9">
-        <v>797</v>
+        <v>757.2</v>
       </c>
       <c r="C30" s="11">
-        <v>787.05</v>
+        <v>746.45</v>
       </c>
       <c r="D30" s="14">
-        <v>787.55</v>
+        <v>753.45</v>
       </c>
       <c r="E30" s="6">
-        <v>790.8</v>
+        <v>753</v>
       </c>
       <c r="F30" s="17">
         <v>2</v>
       </c>
       <c r="G30" s="6">
-        <v>788.3</v>
+        <v>750.85</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1747,22 +1747,22 @@
         <v>35</v>
       </c>
       <c r="B31" s="9">
-        <v>356.7</v>
+        <v>408</v>
       </c>
       <c r="C31" s="11">
-        <v>352.5</v>
+        <v>398.55</v>
       </c>
       <c r="D31" s="14">
-        <v>354.7</v>
+        <v>400.2</v>
       </c>
       <c r="E31" s="6">
-        <v>354.6</v>
+        <v>400.2</v>
       </c>
       <c r="F31" s="17">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G31" s="6">
-        <v>355.2</v>
+        <v>403.45</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1770,22 +1770,22 @@
         <v>36</v>
       </c>
       <c r="B32" s="9">
-        <v>1093.75</v>
+        <v>1254</v>
       </c>
       <c r="C32" s="11">
-        <v>1071</v>
+        <v>1224</v>
       </c>
       <c r="D32" s="14">
-        <v>1073.2</v>
+        <v>1232.3499999999999</v>
       </c>
       <c r="E32" s="6">
-        <v>1075.55</v>
+        <v>1231.3499999999999</v>
       </c>
       <c r="F32" s="17">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G32" s="6">
-        <v>1091.75</v>
+        <v>1243.3499999999999</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1793,22 +1793,22 @@
         <v>37</v>
       </c>
       <c r="B33" s="9">
-        <v>1495.3</v>
+        <v>1428.45</v>
       </c>
       <c r="C33" s="11">
-        <v>1469.75</v>
+        <v>1386.7</v>
       </c>
       <c r="D33" s="14">
-        <v>1472</v>
+        <v>1405.5</v>
       </c>
       <c r="E33" s="6">
-        <v>1471.5</v>
+        <v>1406.7</v>
       </c>
       <c r="F33" s="17">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="G33" s="6">
-        <v>1487</v>
+        <v>1403.75</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1816,22 +1816,22 @@
         <v>38</v>
       </c>
       <c r="B34" s="9">
-        <v>6496.45</v>
+        <v>4625</v>
       </c>
       <c r="C34" s="11">
-        <v>6406</v>
+        <v>4541.8500000000004</v>
       </c>
       <c r="D34" s="14">
-        <v>6440</v>
+        <v>4619.5</v>
       </c>
       <c r="E34" s="6">
-        <v>6442.7</v>
+        <v>4614.95</v>
       </c>
       <c r="F34" s="17">
         <v>4</v>
       </c>
       <c r="G34" s="6">
-        <v>6489</v>
+        <v>4545.8999999999996</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1839,22 +1839,22 @@
         <v>39</v>
       </c>
       <c r="B35" s="9">
-        <v>990.75</v>
+        <v>1038.5999999999999</v>
       </c>
       <c r="C35" s="11">
-        <v>972</v>
+        <v>1021.3</v>
       </c>
       <c r="D35" s="14">
-        <v>985.1</v>
+        <v>1026.8499999999999</v>
       </c>
       <c r="E35" s="6">
-        <v>986.15</v>
+        <v>1027.2</v>
       </c>
       <c r="F35" s="17">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G35" s="6">
-        <v>984.05</v>
+        <v>1027.5</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1862,22 +1862,22 @@
         <v>40</v>
       </c>
       <c r="B36" s="9">
-        <v>1097.7</v>
+        <v>1242.8499999999999</v>
       </c>
       <c r="C36" s="11">
-        <v>1076.05</v>
+        <v>1223.2</v>
       </c>
       <c r="D36" s="14">
-        <v>1093</v>
+        <v>1232.6500000000001</v>
       </c>
       <c r="E36" s="6">
-        <v>1092.25</v>
+        <v>1235.45</v>
       </c>
       <c r="F36" s="17">
         <v>2</v>
       </c>
       <c r="G36" s="6">
-        <v>1090.0999999999999</v>
+        <v>1234.9000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1885,22 +1885,22 @@
         <v>41</v>
       </c>
       <c r="B37" s="9">
-        <v>302.85000000000002</v>
+        <v>339.9</v>
       </c>
       <c r="C37" s="11">
-        <v>297.39999999999998</v>
+        <v>331.15</v>
       </c>
       <c r="D37" s="14">
-        <v>299.85000000000002</v>
+        <v>337.4</v>
       </c>
       <c r="E37" s="6">
-        <v>299.39999999999998</v>
+        <v>338.1</v>
       </c>
       <c r="F37" s="17">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="G37" s="6">
-        <v>298.95</v>
+        <v>332.5</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1908,22 +1908,22 @@
         <v>42</v>
       </c>
       <c r="B38" s="9">
-        <v>2809</v>
+        <v>3704</v>
       </c>
       <c r="C38" s="11">
-        <v>2703</v>
+        <v>3591.75</v>
       </c>
       <c r="D38" s="14">
-        <v>2777.75</v>
+        <v>3682.9</v>
       </c>
       <c r="E38" s="6">
-        <v>2782.9</v>
+        <v>3683.2</v>
       </c>
       <c r="F38" s="17">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G38" s="6">
-        <v>2726.85</v>
+        <v>3605</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1931,22 +1931,22 @@
         <v>43</v>
       </c>
       <c r="B39" s="9">
-        <v>539</v>
+        <v>552.4</v>
       </c>
       <c r="C39" s="11">
-        <v>531.79999999999995</v>
+        <v>543</v>
       </c>
       <c r="D39" s="14">
-        <v>537.04999999999995</v>
+        <v>546.6</v>
       </c>
       <c r="E39" s="6">
-        <v>537.29999999999995</v>
+        <v>545.85</v>
       </c>
       <c r="F39" s="17">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G39" s="6">
-        <v>536.70000000000005</v>
+        <v>550.79999999999995</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1954,22 +1954,22 @@
         <v>44</v>
       </c>
       <c r="B40" s="9">
-        <v>2093.5500000000002</v>
+        <v>1764.35</v>
       </c>
       <c r="C40" s="11">
-        <v>2021.75</v>
+        <v>1733.15</v>
       </c>
       <c r="D40" s="14">
-        <v>2027</v>
+        <v>1763</v>
       </c>
       <c r="E40" s="6">
-        <v>2027.05</v>
+        <v>1760.95</v>
       </c>
       <c r="F40" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G40" s="6">
-        <v>2092.4</v>
+        <v>1750.25</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1977,22 +1977,22 @@
         <v>45</v>
       </c>
       <c r="B41" s="9">
-        <v>512</v>
+        <v>567.4</v>
       </c>
       <c r="C41" s="11">
-        <v>504.95</v>
+        <v>540.75</v>
       </c>
       <c r="D41" s="14">
-        <v>506</v>
+        <v>554</v>
       </c>
       <c r="E41" s="6">
-        <v>505.85</v>
+        <v>552.75</v>
       </c>
       <c r="F41" s="17">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G41" s="6">
-        <v>510.2</v>
+        <v>544.29999999999995</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2000,22 +2000,22 @@
         <v>46</v>
       </c>
       <c r="B42" s="9">
-        <v>2220</v>
+        <v>2478</v>
       </c>
       <c r="C42" s="11">
-        <v>2184.1</v>
+        <v>2417</v>
       </c>
       <c r="D42" s="14">
-        <v>2187.5</v>
+        <v>2428</v>
       </c>
       <c r="E42" s="6">
-        <v>2187.5</v>
+        <v>2424.25</v>
       </c>
       <c r="F42" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" s="6">
-        <v>2217.5</v>
+        <v>2471.9499999999998</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2023,22 +2023,22 @@
         <v>47</v>
       </c>
       <c r="B43" s="9">
-        <v>140.30000000000001</v>
+        <v>119.7</v>
       </c>
       <c r="C43" s="11">
-        <v>137.1</v>
+        <v>116.55</v>
       </c>
       <c r="D43" s="14">
-        <v>137.69999999999999</v>
+        <v>116.8</v>
       </c>
       <c r="E43" s="6">
-        <v>137.65</v>
+        <v>116.9</v>
       </c>
       <c r="F43" s="17">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G43" s="6">
-        <v>139</v>
+        <v>119.2</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2046,22 +2046,22 @@
         <v>48</v>
       </c>
       <c r="B44" s="9">
-        <v>3542</v>
+        <v>3914.35</v>
       </c>
       <c r="C44" s="11">
-        <v>3478</v>
+        <v>3867.55</v>
       </c>
       <c r="D44" s="14">
-        <v>3481</v>
+        <v>3888</v>
       </c>
       <c r="E44" s="6">
-        <v>3482.3</v>
+        <v>3892.55</v>
       </c>
       <c r="F44" s="17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G44" s="6">
-        <v>3508.15</v>
+        <v>3887.5</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2069,22 +2069,22 @@
         <v>49</v>
       </c>
       <c r="B45" s="9">
-        <v>7180.8</v>
+        <v>8146</v>
       </c>
       <c r="C45" s="11">
-        <v>7012</v>
+        <v>7932.55</v>
       </c>
       <c r="D45" s="14">
-        <v>7155.15</v>
+        <v>8066.35</v>
       </c>
       <c r="E45" s="6">
-        <v>7162.5</v>
+        <v>8102.85</v>
       </c>
       <c r="F45" s="17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G45" s="6">
-        <v>7060.95</v>
+        <v>8033.6</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2092,22 +2092,22 @@
         <v>50</v>
       </c>
       <c r="B46" s="9">
-        <v>941.9</v>
+        <v>848</v>
       </c>
       <c r="C46" s="11">
-        <v>925.25</v>
+        <v>823.7</v>
       </c>
       <c r="D46" s="14">
-        <v>932</v>
+        <v>825.05</v>
       </c>
       <c r="E46" s="6">
-        <v>931.8</v>
+        <v>825.65</v>
       </c>
       <c r="F46" s="17">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="G46" s="6">
-        <v>927.2</v>
+        <v>829.35</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2115,22 +2115,22 @@
         <v>51</v>
       </c>
       <c r="B47" s="9">
-        <v>6439.35</v>
+        <v>5966.95</v>
       </c>
       <c r="C47" s="11">
-        <v>6291.45</v>
+        <v>5864.85</v>
       </c>
       <c r="D47" s="14">
-        <v>6334.9</v>
+        <v>5882</v>
       </c>
       <c r="E47" s="6">
-        <v>6335.1</v>
+        <v>5875</v>
       </c>
       <c r="F47" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G47" s="6">
-        <v>6308</v>
+        <v>5883.85</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2138,22 +2138,22 @@
         <v>52</v>
       </c>
       <c r="B48" s="9">
-        <v>2936.95</v>
+        <v>3654</v>
       </c>
       <c r="C48" s="11">
-        <v>2871.05</v>
+        <v>3594.05</v>
       </c>
       <c r="D48" s="14">
-        <v>2919</v>
+        <v>3650</v>
       </c>
       <c r="E48" s="6">
-        <v>2918.85</v>
+        <v>3649.7</v>
       </c>
       <c r="F48" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G48" s="6">
-        <v>2877</v>
+        <v>3635.05</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2161,22 +2161,22 @@
         <v>53</v>
       </c>
       <c r="B49" s="9">
-        <v>332.05</v>
+        <v>468.15</v>
       </c>
       <c r="C49" s="11">
-        <v>324.64999999999998</v>
+        <v>453.65</v>
       </c>
       <c r="D49" s="14">
-        <v>328</v>
+        <v>463</v>
       </c>
       <c r="E49" s="6">
-        <v>328.75</v>
+        <v>463.1</v>
       </c>
       <c r="F49" s="17">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G49" s="6">
-        <v>326.89999999999998</v>
+        <v>460.3</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2184,22 +2184,22 @@
         <v>54</v>
       </c>
       <c r="B50" s="9">
-        <v>945.95</v>
+        <v>1012.25</v>
       </c>
       <c r="C50" s="11">
-        <v>919.25</v>
+        <v>986.4</v>
       </c>
       <c r="D50" s="14">
-        <v>920.9</v>
+        <v>1002.6</v>
       </c>
       <c r="E50" s="6">
-        <v>921.7</v>
+        <v>1002.4</v>
       </c>
       <c r="F50" s="17">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G50" s="6">
-        <v>939.5</v>
+        <v>1010.2</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2207,22 +2207,22 @@
         <v>55</v>
       </c>
       <c r="B51" s="9">
-        <v>840</v>
+        <v>830</v>
       </c>
       <c r="C51" s="11">
-        <v>795.35</v>
+        <v>817.8</v>
       </c>
       <c r="D51" s="14">
-        <v>799</v>
+        <v>827.4</v>
       </c>
       <c r="E51" s="6">
-        <v>807.35</v>
+        <v>821.25</v>
       </c>
       <c r="F51" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51" s="6">
-        <v>836.55</v>
+        <v>822.35</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2230,22 +2230,22 @@
         <v>56</v>
       </c>
       <c r="B52" s="9">
-        <v>638.70000000000005</v>
+        <v>672.9</v>
       </c>
       <c r="C52" s="11">
-        <v>626.54999999999995</v>
+        <v>658.3</v>
       </c>
       <c r="D52" s="14">
-        <v>634.5</v>
+        <v>660</v>
       </c>
       <c r="E52" s="6">
-        <v>633.95000000000005</v>
+        <v>660.55</v>
       </c>
       <c r="F52" s="17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G52" s="6">
-        <v>636.79999999999995</v>
+        <v>665</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2253,22 +2253,22 @@
         <v>57</v>
       </c>
       <c r="B53" s="9">
-        <v>1261.8</v>
+        <v>1317.1</v>
       </c>
       <c r="C53" s="11">
-        <v>1242.2</v>
+        <v>1287.4000000000001</v>
       </c>
       <c r="D53" s="14">
-        <v>1254.9000000000001</v>
+        <v>1295</v>
       </c>
       <c r="E53" s="6">
-        <v>1253.45</v>
+        <v>1291.5999999999999</v>
       </c>
       <c r="F53" s="17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G53" s="6">
-        <v>1257.05</v>
+        <v>1307.25</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2276,22 +2276,22 @@
         <v>58</v>
       </c>
       <c r="B54" s="9">
-        <v>2541.3000000000002</v>
+        <v>2871.9</v>
       </c>
       <c r="C54" s="11">
-        <v>2467.0500000000002</v>
+        <v>2776.65</v>
       </c>
       <c r="D54" s="14">
-        <v>2492.4</v>
+        <v>2820</v>
       </c>
       <c r="E54" s="6">
-        <v>2492.0500000000002</v>
+        <v>2821.25</v>
       </c>
       <c r="F54" s="17">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G54" s="6">
-        <v>2514.3000000000002</v>
+        <v>2814.95</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2299,22 +2299,22 @@
         <v>59</v>
       </c>
       <c r="B55" s="9">
-        <v>474.85</v>
+        <v>409.9</v>
       </c>
       <c r="C55" s="11">
-        <v>465.05</v>
+        <v>389.35</v>
       </c>
       <c r="D55" s="14">
-        <v>468.5</v>
+        <v>396</v>
       </c>
       <c r="E55" s="6">
-        <v>467</v>
+        <v>396.8</v>
       </c>
       <c r="F55" s="17">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G55" s="6">
-        <v>467.8</v>
+        <v>398.7</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2322,22 +2322,22 @@
         <v>60</v>
       </c>
       <c r="B56" s="9">
-        <v>2252.8000000000002</v>
+        <v>2403.9499999999998</v>
       </c>
       <c r="C56" s="11">
-        <v>2226.3000000000002</v>
+        <v>2366.1999999999998</v>
       </c>
       <c r="D56" s="14">
-        <v>2236.8000000000002</v>
+        <v>2370</v>
       </c>
       <c r="E56" s="6">
-        <v>2234.15</v>
+        <v>2369.6999999999998</v>
       </c>
       <c r="F56" s="17">
         <v>4</v>
       </c>
       <c r="G56" s="6">
-        <v>2250.5</v>
+        <v>2396.3000000000002</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2345,22 +2345,22 @@
         <v>61</v>
       </c>
       <c r="B57" s="9">
-        <v>595.75</v>
+        <v>549.9</v>
       </c>
       <c r="C57" s="11">
-        <v>581.1</v>
+        <v>541.45000000000005</v>
       </c>
       <c r="D57" s="14">
-        <v>590.4</v>
+        <v>542.5</v>
       </c>
       <c r="E57" s="6">
-        <v>590</v>
+        <v>542.54999999999995</v>
       </c>
       <c r="F57" s="17">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="G57" s="6">
-        <v>589</v>
+        <v>548.6</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2368,22 +2368,22 @@
         <v>62</v>
       </c>
       <c r="B58" s="9">
-        <v>3226.85</v>
+        <v>4193.6000000000004</v>
       </c>
       <c r="C58" s="11">
-        <v>3133</v>
+        <v>4051</v>
       </c>
       <c r="D58" s="14">
-        <v>3218</v>
+        <v>4185</v>
       </c>
       <c r="E58" s="6">
-        <v>3214.95</v>
+        <v>4182.3500000000004</v>
       </c>
       <c r="F58" s="17">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G58" s="6">
-        <v>3153.1</v>
+        <v>4095.15</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2391,22 +2391,22 @@
         <v>63</v>
       </c>
       <c r="B59" s="9">
-        <v>1564.95</v>
+        <v>1757.2</v>
       </c>
       <c r="C59" s="11">
-        <v>1534.8</v>
+        <v>1731</v>
       </c>
       <c r="D59" s="14">
-        <v>1555</v>
+        <v>1753</v>
       </c>
       <c r="E59" s="6">
-        <v>1553.95</v>
+        <v>1754.15</v>
       </c>
       <c r="F59" s="17">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G59" s="6">
-        <v>1535.4</v>
+        <v>1731.4</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2414,22 +2414,22 @@
         <v>64</v>
       </c>
       <c r="B60" s="9">
-        <v>1648</v>
+        <v>1340.3</v>
       </c>
       <c r="C60" s="11">
-        <v>1635</v>
+        <v>1318.25</v>
       </c>
       <c r="D60" s="14">
-        <v>1638.25</v>
+        <v>1335</v>
       </c>
       <c r="E60" s="6">
-        <v>1637.95</v>
+        <v>1332.9</v>
       </c>
       <c r="F60" s="17">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="G60" s="6">
-        <v>1643.9</v>
+        <v>1322.2</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2437,22 +2437,22 @@
         <v>65</v>
       </c>
       <c r="B61" s="9">
-        <v>3876.3</v>
+        <v>3768.45</v>
       </c>
       <c r="C61" s="11">
-        <v>3788.15</v>
+        <v>3685.05</v>
       </c>
       <c r="D61" s="14">
-        <v>3844</v>
+        <v>3754.8</v>
       </c>
       <c r="E61" s="6">
-        <v>3856.5</v>
+        <v>3762.05</v>
       </c>
       <c r="F61" s="17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G61" s="6">
-        <v>3803.9</v>
+        <v>3694</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2460,22 +2460,22 @@
         <v>66</v>
       </c>
       <c r="B62" s="9">
-        <v>620.5</v>
+        <v>561.54999999999995</v>
       </c>
       <c r="C62" s="11">
-        <v>587.6</v>
+        <v>555</v>
       </c>
       <c r="D62" s="14">
-        <v>609</v>
+        <v>555.95000000000005</v>
       </c>
       <c r="E62" s="6">
-        <v>610.29999999999995</v>
+        <v>555.95000000000005</v>
       </c>
       <c r="F62" s="17">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="G62" s="6">
-        <v>589.45000000000005</v>
+        <v>558.20000000000005</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2483,22 +2483,22 @@
         <v>67</v>
       </c>
       <c r="B63" s="9">
-        <v>529.85</v>
+        <v>659</v>
       </c>
       <c r="C63" s="11">
-        <v>520.04999999999995</v>
+        <v>650.45000000000005</v>
       </c>
       <c r="D63" s="14">
-        <v>525.20000000000005</v>
+        <v>653.1</v>
       </c>
       <c r="E63" s="6">
-        <v>524.95000000000005</v>
+        <v>653.70000000000005</v>
       </c>
       <c r="F63" s="17">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="G63" s="6">
-        <v>523.20000000000005</v>
+        <v>656.3</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2506,22 +2506,22 @@
         <v>68</v>
       </c>
       <c r="B64" s="9">
-        <v>290</v>
+        <v>388.4</v>
       </c>
       <c r="C64" s="11">
-        <v>281.60000000000002</v>
+        <v>377.65</v>
       </c>
       <c r="D64" s="14">
-        <v>284.35000000000002</v>
+        <v>382.5</v>
       </c>
       <c r="E64" s="6">
-        <v>284</v>
+        <v>383.6</v>
       </c>
       <c r="F64" s="17">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="G64" s="6">
-        <v>283</v>
+        <v>386.85</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2529,22 +2529,22 @@
         <v>69</v>
       </c>
       <c r="B65" s="9">
-        <v>1654.9</v>
+        <v>1671.25</v>
       </c>
       <c r="C65" s="11">
-        <v>1625.1</v>
+        <v>1649.95</v>
       </c>
       <c r="D65" s="14">
-        <v>1650</v>
+        <v>1657.45</v>
       </c>
       <c r="E65" s="6">
-        <v>1650.1</v>
+        <v>1652.9</v>
       </c>
       <c r="F65" s="17">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G65" s="6">
-        <v>1633.4</v>
+        <v>1667.1</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2552,22 +2552,22 @@
         <v>70</v>
       </c>
       <c r="B66" s="9">
-        <v>558.70000000000005</v>
+        <v>595.95000000000005</v>
       </c>
       <c r="C66" s="11">
-        <v>533.95000000000005</v>
+        <v>574.45000000000005</v>
       </c>
       <c r="D66" s="14">
-        <v>546.20000000000005</v>
+        <v>580.35</v>
       </c>
       <c r="E66" s="6">
-        <v>546.95000000000005</v>
+        <v>577.04999999999995</v>
       </c>
       <c r="F66" s="17">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G66" s="6">
-        <v>536.45000000000005</v>
+        <v>595.15</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2575,22 +2575,22 @@
         <v>71</v>
       </c>
       <c r="B67" s="9">
-        <v>158</v>
+        <v>147.85</v>
       </c>
       <c r="C67" s="11">
-        <v>152.75</v>
+        <v>144.6</v>
       </c>
       <c r="D67" s="14">
-        <v>153.65</v>
+        <v>145.94999999999999</v>
       </c>
       <c r="E67" s="6">
-        <v>153.55000000000001</v>
+        <v>145.55000000000001</v>
       </c>
       <c r="F67" s="17">
-        <v>354</v>
+        <v>126</v>
       </c>
       <c r="G67" s="6">
-        <v>156.35</v>
+        <v>146.94999999999999</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2598,22 +2598,22 @@
         <v>72</v>
       </c>
       <c r="B68" s="9">
-        <v>455.3</v>
+        <v>448.2</v>
       </c>
       <c r="C68" s="11">
-        <v>438.85</v>
+        <v>433.4</v>
       </c>
       <c r="D68" s="14">
-        <v>446.9</v>
+        <v>439.8</v>
       </c>
       <c r="E68" s="6">
-        <v>446.6</v>
+        <v>439.8</v>
       </c>
       <c r="F68" s="17">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="G68" s="6">
-        <v>440</v>
+        <v>443.65</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2621,22 +2621,22 @@
         <v>73</v>
       </c>
       <c r="B69" s="9">
-        <v>591.95000000000005</v>
+        <v>569.85</v>
       </c>
       <c r="C69" s="11">
-        <v>583.6</v>
+        <v>558.6</v>
       </c>
       <c r="D69" s="14">
-        <v>588.6</v>
+        <v>561</v>
       </c>
       <c r="E69" s="6">
-        <v>588.35</v>
+        <v>560.9</v>
       </c>
       <c r="F69" s="17">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="G69" s="6">
-        <v>587.4</v>
+        <v>566.85</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2644,22 +2644,22 @@
         <v>74</v>
       </c>
       <c r="B70" s="9">
-        <v>234.95</v>
+        <v>212.85</v>
       </c>
       <c r="C70" s="11">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="D70" s="14">
-        <v>232.75</v>
+        <v>208.65</v>
       </c>
       <c r="E70" s="6">
-        <v>232.2</v>
+        <v>208.6</v>
       </c>
       <c r="F70" s="17">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G70" s="6">
-        <v>233.65</v>
+        <v>211.95</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2667,22 +2667,22 @@
         <v>75</v>
       </c>
       <c r="B71" s="9">
-        <v>2670.95</v>
+        <v>2652.8</v>
       </c>
       <c r="C71" s="11">
-        <v>2621.0500000000002</v>
+        <v>2620</v>
       </c>
       <c r="D71" s="14">
-        <v>2625</v>
+        <v>2629.45</v>
       </c>
       <c r="E71" s="6">
-        <v>2624.65</v>
+        <v>2627.75</v>
       </c>
       <c r="F71" s="17">
         <v>0</v>
       </c>
       <c r="G71" s="6">
-        <v>2641.15</v>
+        <v>2634.95</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2690,22 +2690,22 @@
         <v>76</v>
       </c>
       <c r="B72" s="9">
-        <v>3202.8</v>
+        <v>4314.3999999999996</v>
       </c>
       <c r="C72" s="11">
-        <v>3153.3</v>
+        <v>4134.6000000000004</v>
       </c>
       <c r="D72" s="14">
-        <v>3171.4</v>
+        <v>4275</v>
       </c>
       <c r="E72" s="6">
-        <v>3171.1</v>
+        <v>4295.5</v>
       </c>
       <c r="F72" s="17">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G72" s="6">
-        <v>3162.4</v>
+        <v>4161</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2713,22 +2713,22 @@
         <v>77</v>
       </c>
       <c r="B73" s="9">
-        <v>1538.95</v>
+        <v>1427.7</v>
       </c>
       <c r="C73" s="11">
-        <v>1520.35</v>
+        <v>1407.4</v>
       </c>
       <c r="D73" s="14">
-        <v>1531.55</v>
+        <v>1418</v>
       </c>
       <c r="E73" s="6">
-        <v>1531.3</v>
+        <v>1417.1</v>
       </c>
       <c r="F73" s="17">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G73" s="6">
-        <v>1537.6</v>
+        <v>1425.4</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2736,22 +2736,22 @@
         <v>78</v>
       </c>
       <c r="B74" s="9">
-        <v>269.8</v>
+        <v>347.5</v>
       </c>
       <c r="C74" s="11">
-        <v>263.60000000000002</v>
+        <v>340</v>
       </c>
       <c r="D74" s="14">
-        <v>268.3</v>
+        <v>341.5</v>
       </c>
       <c r="E74" s="6">
-        <v>268.10000000000002</v>
+        <v>341.8</v>
       </c>
       <c r="F74" s="17">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="G74" s="6">
-        <v>265.89999999999998</v>
+        <v>345.85</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2759,22 +2759,22 @@
         <v>79</v>
       </c>
       <c r="B75" s="9">
-        <v>1134.5999999999999</v>
+        <v>892.5</v>
       </c>
       <c r="C75" s="11">
-        <v>1098.3499999999999</v>
+        <v>875.25</v>
       </c>
       <c r="D75" s="14">
-        <v>1121.6500000000001</v>
+        <v>882</v>
       </c>
       <c r="E75" s="6">
-        <v>1112.7</v>
+        <v>880.2</v>
       </c>
       <c r="F75" s="17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G75" s="6">
-        <v>1106</v>
+        <v>881.7</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2782,22 +2782,22 @@
         <v>80</v>
       </c>
       <c r="B76" s="9">
-        <v>1220</v>
+        <v>1292.6500000000001</v>
       </c>
       <c r="C76" s="11">
-        <v>1198.3</v>
+        <v>1266.5</v>
       </c>
       <c r="D76" s="14">
-        <v>1205.8</v>
+        <v>1274.0999999999999</v>
       </c>
       <c r="E76" s="6">
-        <v>1201.8</v>
+        <v>1276.3</v>
       </c>
       <c r="F76" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G76" s="6">
-        <v>1206.8499999999999</v>
+        <v>1289.95</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2805,22 +2805,22 @@
         <v>81</v>
       </c>
       <c r="B77" s="9">
-        <v>849.5</v>
+        <v>998.7</v>
       </c>
       <c r="C77" s="11">
-        <v>827.6</v>
+        <v>975.45</v>
       </c>
       <c r="D77" s="14">
-        <v>840.6</v>
+        <v>996</v>
       </c>
       <c r="E77" s="6">
-        <v>839.45</v>
+        <v>993.55</v>
       </c>
       <c r="F77" s="17">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G77" s="6">
-        <v>828.45</v>
+        <v>988.55</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2828,22 +2828,22 @@
         <v>82</v>
       </c>
       <c r="B78" s="9">
-        <v>4513.45</v>
+        <v>3931.15</v>
       </c>
       <c r="C78" s="11">
-        <v>4445.1000000000004</v>
+        <v>3790.1</v>
       </c>
       <c r="D78" s="14">
-        <v>4455</v>
+        <v>3870</v>
       </c>
       <c r="E78" s="6">
-        <v>4463.8999999999996</v>
+        <v>3889.85</v>
       </c>
       <c r="F78" s="17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G78" s="6">
-        <v>4505.1000000000004</v>
+        <v>3834.85</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2851,22 +2851,22 @@
         <v>83</v>
       </c>
       <c r="B79" s="9">
-        <v>830.7</v>
+        <v>880.8</v>
       </c>
       <c r="C79" s="11">
-        <v>818.5</v>
+        <v>863.4</v>
       </c>
       <c r="D79" s="14">
-        <v>826</v>
+        <v>870.55</v>
       </c>
       <c r="E79" s="6">
-        <v>824.3</v>
+        <v>870.95</v>
       </c>
       <c r="F79" s="17">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="G79" s="6">
-        <v>829.6</v>
+        <v>875.35</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2874,22 +2874,22 @@
         <v>84</v>
       </c>
       <c r="B80" s="9">
-        <v>468.3</v>
+        <v>479.95</v>
       </c>
       <c r="C80" s="11">
-        <v>462.55</v>
+        <v>466.95</v>
       </c>
       <c r="D80" s="14">
-        <v>463.25</v>
+        <v>468</v>
       </c>
       <c r="E80" s="6">
-        <v>463.65</v>
+        <v>468.05</v>
       </c>
       <c r="F80" s="17">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="G80" s="6">
-        <v>465.4</v>
+        <v>475.8</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2897,22 +2897,22 @@
         <v>85</v>
       </c>
       <c r="B81" s="9">
-        <v>1741.5</v>
+        <v>1653.7</v>
       </c>
       <c r="C81" s="11">
-        <v>1718.5</v>
+        <v>1637.05</v>
       </c>
       <c r="D81" s="14">
-        <v>1726.95</v>
+        <v>1649</v>
       </c>
       <c r="E81" s="6">
-        <v>1727.2</v>
+        <v>1650.8</v>
       </c>
       <c r="F81" s="17">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="G81" s="6">
-        <v>1734.9</v>
+        <v>1648.7</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2920,22 +2920,22 @@
         <v>86</v>
       </c>
       <c r="B82" s="9">
-        <v>2347.85</v>
+        <v>2536.6999999999998</v>
       </c>
       <c r="C82" s="11">
-        <v>2269.8000000000002</v>
+        <v>2466.9499999999998</v>
       </c>
       <c r="D82" s="14">
-        <v>2278.9</v>
+        <v>2475</v>
       </c>
       <c r="E82" s="6">
-        <v>2275.25</v>
+        <v>2473.6999999999998</v>
       </c>
       <c r="F82" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G82" s="6">
-        <v>2340.8000000000002</v>
+        <v>2529</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2943,22 +2943,22 @@
         <v>87</v>
       </c>
       <c r="B83" s="9">
-        <v>418.65</v>
+        <v>440.75</v>
       </c>
       <c r="C83" s="11">
-        <v>410.5</v>
+        <v>430.2</v>
       </c>
       <c r="D83" s="14">
-        <v>418.1</v>
+        <v>436</v>
       </c>
       <c r="E83" s="6">
-        <v>417.55</v>
+        <v>437.45</v>
       </c>
       <c r="F83" s="17">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G83" s="6">
-        <v>412.2</v>
+        <v>433.75</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2966,22 +2966,22 @@
         <v>88</v>
       </c>
       <c r="B84" s="9">
-        <v>661.15</v>
+        <v>640.65</v>
       </c>
       <c r="C84" s="11">
-        <v>648.75</v>
+        <v>623.04999999999995</v>
       </c>
       <c r="D84" s="14">
-        <v>658</v>
+        <v>625.65</v>
       </c>
       <c r="E84" s="6">
-        <v>657.75</v>
+        <v>631</v>
       </c>
       <c r="F84" s="17">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G84" s="6">
-        <v>652.15</v>
+        <v>636.75</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2989,22 +2989,22 @@
         <v>89</v>
       </c>
       <c r="B85" s="9">
-        <v>5285.8</v>
+        <v>4675.95</v>
       </c>
       <c r="C85" s="11">
-        <v>5209.55</v>
+        <v>4633</v>
       </c>
       <c r="D85" s="14">
-        <v>5214</v>
+        <v>4648.95</v>
       </c>
       <c r="E85" s="6">
-        <v>5216.8500000000004</v>
+        <v>4649.3</v>
       </c>
       <c r="F85" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G85" s="6">
-        <v>5280</v>
+        <v>4643.7</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3012,22 +3012,22 @@
         <v>90</v>
       </c>
       <c r="B86" s="9">
-        <v>5295.6</v>
+        <v>4543.55</v>
       </c>
       <c r="C86" s="11">
-        <v>5235.1000000000004</v>
+        <v>4436.55</v>
       </c>
       <c r="D86" s="14">
-        <v>5260</v>
+        <v>4443</v>
       </c>
       <c r="E86" s="6">
-        <v>5258.45</v>
+        <v>4456.6499999999996</v>
       </c>
       <c r="F86" s="17">
         <v>1</v>
       </c>
       <c r="G86" s="6">
-        <v>5295.35</v>
+        <v>4504.5</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3035,22 +3035,22 @@
         <v>91</v>
       </c>
       <c r="B87" s="9">
-        <v>1700</v>
+        <v>1652</v>
       </c>
       <c r="C87" s="11">
-        <v>1650</v>
+        <v>1628.7</v>
       </c>
       <c r="D87" s="14">
-        <v>1667</v>
+        <v>1640</v>
       </c>
       <c r="E87" s="6">
-        <v>1669.85</v>
+        <v>1639.1</v>
       </c>
       <c r="F87" s="17">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G87" s="6">
-        <v>1651.8</v>
+        <v>1641.7</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3058,22 +3058,22 @@
         <v>92</v>
       </c>
       <c r="B88" s="9">
-        <v>290</v>
+        <v>267.75</v>
       </c>
       <c r="C88" s="11">
-        <v>286.25</v>
+        <v>263.7</v>
       </c>
       <c r="D88" s="14">
-        <v>287.75</v>
+        <v>265.2</v>
       </c>
       <c r="E88" s="6">
-        <v>287.5</v>
+        <v>266.89999999999998</v>
       </c>
       <c r="F88" s="17">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="G88" s="6">
-        <v>288.55</v>
+        <v>264.2</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3081,22 +3081,22 @@
         <v>93</v>
       </c>
       <c r="B89" s="9">
-        <v>184.95</v>
+        <v>181.5</v>
       </c>
       <c r="C89" s="11">
-        <v>181.45</v>
+        <v>177.35</v>
       </c>
       <c r="D89" s="14">
-        <v>183.7</v>
+        <v>179.3</v>
       </c>
       <c r="E89" s="6">
-        <v>183.95</v>
+        <v>179.55</v>
       </c>
       <c r="F89" s="17">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="G89" s="6">
-        <v>181.7</v>
+        <v>178.2</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3104,22 +3104,22 @@
         <v>94</v>
       </c>
       <c r="B90" s="9">
-        <v>526.25</v>
+        <v>602.15</v>
       </c>
       <c r="C90" s="11">
-        <v>522</v>
+        <v>586.15</v>
       </c>
       <c r="D90" s="14">
-        <v>524</v>
+        <v>590.79999999999995</v>
       </c>
       <c r="E90" s="6">
-        <v>524.04999999999995</v>
+        <v>591.6</v>
       </c>
       <c r="F90" s="17">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G90" s="6">
-        <v>523.65</v>
+        <v>598.29999999999995</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3127,22 +3127,22 @@
         <v>95</v>
       </c>
       <c r="B91" s="9">
-        <v>1170.4000000000001</v>
+        <v>1179.8499999999999</v>
       </c>
       <c r="C91" s="11">
-        <v>1151.6500000000001</v>
+        <v>1165.3</v>
       </c>
       <c r="D91" s="14">
-        <v>1167.5</v>
+        <v>1174.5</v>
       </c>
       <c r="E91" s="6">
-        <v>1165.8</v>
+        <v>1174.25</v>
       </c>
       <c r="F91" s="17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G91" s="6">
-        <v>1161.75</v>
+        <v>1168.75</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3150,22 +3150,22 @@
         <v>96</v>
       </c>
       <c r="B92" s="9">
-        <v>3817.9</v>
+        <v>3963.8</v>
       </c>
       <c r="C92" s="11">
-        <v>3691.05</v>
+        <v>3884</v>
       </c>
       <c r="D92" s="14">
-        <v>3715</v>
+        <v>3904.8</v>
       </c>
       <c r="E92" s="6">
-        <v>3707.7</v>
+        <v>3900.45</v>
       </c>
       <c r="F92" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G92" s="6">
-        <v>3815.3</v>
+        <v>3921.95</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3173,22 +3173,22 @@
         <v>97</v>
       </c>
       <c r="B93" s="9">
-        <v>1697.5</v>
+        <v>1860.1</v>
       </c>
       <c r="C93" s="11">
-        <v>1640</v>
+        <v>1805.05</v>
       </c>
       <c r="D93" s="14">
-        <v>1677.05</v>
+        <v>1858</v>
       </c>
       <c r="E93" s="6">
-        <v>1674</v>
+        <v>1850.25</v>
       </c>
       <c r="F93" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G93" s="6">
-        <v>1689.55</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3196,22 +3196,22 @@
         <v>98</v>
       </c>
       <c r="B94" s="9">
-        <v>1005.1</v>
+        <v>1002.7</v>
       </c>
       <c r="C94" s="11">
-        <v>959.25</v>
+        <v>978.95</v>
       </c>
       <c r="D94" s="14">
-        <v>997</v>
+        <v>1000.45</v>
       </c>
       <c r="E94" s="6">
-        <v>1000.6</v>
+        <v>1000.5</v>
       </c>
       <c r="F94" s="17">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G94" s="6">
-        <v>967.6</v>
+        <v>978.95</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3219,22 +3219,22 @@
         <v>99</v>
       </c>
       <c r="B95" s="9">
-        <v>1552</v>
+        <v>1321.95</v>
       </c>
       <c r="C95" s="11">
-        <v>1506.9</v>
+        <v>1280</v>
       </c>
       <c r="D95" s="14">
-        <v>1552</v>
+        <v>1285.45</v>
       </c>
       <c r="E95" s="6">
-        <v>1541.65</v>
+        <v>1285.0999999999999</v>
       </c>
       <c r="F95" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G95" s="6">
-        <v>1511.7</v>
+        <v>1321.15</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -3242,22 +3242,22 @@
         <v>100</v>
       </c>
       <c r="B96" s="9">
-        <v>2649.9</v>
+        <v>2302</v>
       </c>
       <c r="C96" s="11">
-        <v>2590.9</v>
+        <v>2270.0500000000002</v>
       </c>
       <c r="D96" s="14">
-        <v>2600</v>
+        <v>2275.8000000000002</v>
       </c>
       <c r="E96" s="6">
-        <v>2600.6</v>
+        <v>2274.35</v>
       </c>
       <c r="F96" s="17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G96" s="6">
-        <v>2642.85</v>
+        <v>2296.5500000000002</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -3265,22 +3265,22 @@
         <v>101</v>
       </c>
       <c r="B97" s="9">
-        <v>1350</v>
+        <v>1689.15</v>
       </c>
       <c r="C97" s="11">
-        <v>1329</v>
+        <v>1662.5</v>
       </c>
       <c r="D97" s="14">
-        <v>1335.7</v>
+        <v>1676.1</v>
       </c>
       <c r="E97" s="6">
-        <v>1337.9</v>
+        <v>1671.5</v>
       </c>
       <c r="F97" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G97" s="6">
-        <v>1338.3</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3288,22 +3288,22 @@
         <v>102</v>
       </c>
       <c r="B98" s="9">
-        <v>520.1</v>
+        <v>567.45000000000005</v>
       </c>
       <c r="C98" s="11">
-        <v>511.6</v>
+        <v>558.29999999999995</v>
       </c>
       <c r="D98" s="14">
-        <v>513.75</v>
+        <v>562</v>
       </c>
       <c r="E98" s="6">
-        <v>513.65</v>
+        <v>562.15</v>
       </c>
       <c r="F98" s="17">
         <v>3</v>
       </c>
       <c r="G98" s="6">
-        <v>520</v>
+        <v>564.95000000000005</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3311,22 +3311,22 @@
         <v>103</v>
       </c>
       <c r="B99" s="9">
-        <v>5331</v>
+        <v>6027.3</v>
       </c>
       <c r="C99" s="11">
-        <v>5145.6000000000004</v>
+        <v>5867.15</v>
       </c>
       <c r="D99" s="14">
-        <v>5151.05</v>
+        <v>5921.5</v>
       </c>
       <c r="E99" s="6">
-        <v>5157.6000000000004</v>
+        <v>5941.6</v>
       </c>
       <c r="F99" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G99" s="6">
-        <v>5294.45</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3334,22 +3334,22 @@
         <v>104</v>
       </c>
       <c r="B100" s="9">
-        <v>3070.95</v>
+        <v>3413.1</v>
       </c>
       <c r="C100" s="11">
-        <v>3036.85</v>
+        <v>3301</v>
       </c>
       <c r="D100" s="14">
-        <v>3050</v>
+        <v>3337.4</v>
       </c>
       <c r="E100" s="6">
-        <v>3050.2</v>
+        <v>3324.2</v>
       </c>
       <c r="F100" s="17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G100" s="6">
-        <v>3067.95</v>
+        <v>3400</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3357,22 +3357,22 @@
         <v>105</v>
       </c>
       <c r="B101" s="9">
-        <v>241.9</v>
+        <v>269.45</v>
       </c>
       <c r="C101" s="11">
-        <v>233.85</v>
+        <v>265.7</v>
       </c>
       <c r="D101" s="14">
-        <v>240.1</v>
+        <v>267.75</v>
       </c>
       <c r="E101" s="6">
-        <v>240.05</v>
+        <v>267.3</v>
       </c>
       <c r="F101" s="17">
-        <v>165</v>
+        <v>85</v>
       </c>
       <c r="G101" s="6">
-        <v>236.7</v>
+        <v>267.39999999999998</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3380,22 +3380,22 @@
         <v>106</v>
       </c>
       <c r="B102" s="9">
-        <v>358.3</v>
+        <v>363.5</v>
       </c>
       <c r="C102" s="11">
-        <v>348</v>
+        <v>357.5</v>
       </c>
       <c r="D102" s="14">
-        <v>354.35</v>
+        <v>361.5</v>
       </c>
       <c r="E102" s="6">
-        <v>353.85</v>
+        <v>361.35</v>
       </c>
       <c r="F102" s="17">
-        <v>380</v>
+        <v>85</v>
       </c>
       <c r="G102" s="6">
-        <v>352.8</v>
+        <v>363.1</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3403,22 +3403,22 @@
         <v>107</v>
       </c>
       <c r="B103" s="9">
-        <v>1398.8</v>
+        <v>1629.05</v>
       </c>
       <c r="C103" s="11">
-        <v>1374.35</v>
+        <v>1550.5</v>
       </c>
       <c r="D103" s="14">
-        <v>1386.75</v>
+        <v>1574.25</v>
       </c>
       <c r="E103" s="6">
-        <v>1386.7</v>
+        <v>1574.15</v>
       </c>
       <c r="F103" s="17">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="G103" s="6">
-        <v>1382.75</v>
+        <v>1591.6</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3426,22 +3426,22 @@
         <v>108</v>
       </c>
       <c r="B104" s="9">
-        <v>974.7</v>
+        <v>839.9</v>
       </c>
       <c r="C104" s="11">
-        <v>940.65</v>
+        <v>822</v>
       </c>
       <c r="D104" s="14">
-        <v>968</v>
+        <v>823.4</v>
       </c>
       <c r="E104" s="6">
-        <v>966.85</v>
+        <v>825.2</v>
       </c>
       <c r="F104" s="17">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="G104" s="6">
-        <v>942.4</v>
+        <v>835.75</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3449,22 +3449,22 @@
         <v>109</v>
       </c>
       <c r="B105" s="9">
-        <v>8590</v>
+        <v>3490</v>
       </c>
       <c r="C105" s="11">
-        <v>8435</v>
+        <v>3425</v>
       </c>
       <c r="D105" s="14">
-        <v>8444.4</v>
+        <v>3470</v>
       </c>
       <c r="E105" s="6">
-        <v>8471.15</v>
+        <v>3481.45</v>
       </c>
       <c r="F105" s="17">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G105" s="6">
-        <v>8582.85</v>
+        <v>3440.05</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3472,22 +3472,22 @@
         <v>110</v>
       </c>
       <c r="B106" s="9">
-        <v>292.39999999999998</v>
+        <v>308.55</v>
       </c>
       <c r="C106" s="11">
-        <v>282.45</v>
+        <v>303.10000000000002</v>
       </c>
       <c r="D106" s="14">
-        <v>292.10000000000002</v>
+        <v>306.95</v>
       </c>
       <c r="E106" s="6">
-        <v>291.2</v>
+        <v>307.2</v>
       </c>
       <c r="F106" s="17">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="G106" s="6">
-        <v>282.75</v>
+        <v>306.75</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3495,22 +3495,22 @@
         <v>111</v>
       </c>
       <c r="B107" s="9">
-        <v>2737.15</v>
+        <v>3001</v>
       </c>
       <c r="C107" s="11">
-        <v>2696.5</v>
+        <v>2955</v>
       </c>
       <c r="D107" s="14">
-        <v>2699</v>
+        <v>2986</v>
       </c>
       <c r="E107" s="6">
-        <v>2702.05</v>
+        <v>2987.45</v>
       </c>
       <c r="F107" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G107" s="6">
-        <v>2732.65</v>
+        <v>2986.15</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3518,22 +3518,22 @@
         <v>112</v>
       </c>
       <c r="B108" s="9">
-        <v>4805</v>
+        <v>6534.7</v>
       </c>
       <c r="C108" s="11">
-        <v>4730.95</v>
+        <v>6302.3</v>
       </c>
       <c r="D108" s="14">
-        <v>4750</v>
+        <v>6460</v>
       </c>
       <c r="E108" s="6">
-        <v>4792.2</v>
+        <v>6466.9</v>
       </c>
       <c r="F108" s="17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G108" s="6">
-        <v>4786.7</v>
+        <v>6341.65</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -3541,22 +3541,22 @@
         <v>113</v>
       </c>
       <c r="B109" s="9">
-        <v>297</v>
+        <v>316.3</v>
       </c>
       <c r="C109" s="11">
-        <v>291.3</v>
+        <v>308.85000000000002</v>
       </c>
       <c r="D109" s="14">
-        <v>294.60000000000002</v>
+        <v>314.35000000000002</v>
       </c>
       <c r="E109" s="6">
-        <v>294.64999999999998</v>
+        <v>314.85000000000002</v>
       </c>
       <c r="F109" s="17">
-        <v>231</v>
+        <v>113</v>
       </c>
       <c r="G109" s="6">
-        <v>294.2</v>
+        <v>311.35000000000002</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -3564,22 +3564,22 @@
         <v>114</v>
       </c>
       <c r="B110" s="9">
-        <v>182.2</v>
+        <v>166</v>
       </c>
       <c r="C110" s="11">
-        <v>175.15</v>
+        <v>161</v>
       </c>
       <c r="D110" s="14">
-        <v>176.8</v>
+        <v>161.44999999999999</v>
       </c>
       <c r="E110" s="6">
-        <v>176.7</v>
+        <v>161.65</v>
       </c>
       <c r="F110" s="17">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="G110" s="6">
-        <v>181.7</v>
+        <v>165.8</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -3587,22 +3587,22 @@
         <v>115</v>
       </c>
       <c r="B111" s="9">
-        <v>850.85</v>
+        <v>772.1</v>
       </c>
       <c r="C111" s="11">
-        <v>841.75</v>
+        <v>760</v>
       </c>
       <c r="D111" s="14">
-        <v>847</v>
+        <v>762</v>
       </c>
       <c r="E111" s="6">
-        <v>848.2</v>
+        <v>763.4</v>
       </c>
       <c r="F111" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G111" s="6">
-        <v>841.8</v>
+        <v>772.05</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -3610,22 +3610,22 @@
         <v>116</v>
       </c>
       <c r="B112" s="9">
-        <v>277.25</v>
+        <v>252.25</v>
       </c>
       <c r="C112" s="11">
-        <v>271.35000000000002</v>
+        <v>249</v>
       </c>
       <c r="D112" s="14">
-        <v>272.95</v>
+        <v>249.2</v>
       </c>
       <c r="E112" s="6">
-        <v>273.5</v>
+        <v>249.7</v>
       </c>
       <c r="F112" s="17">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="G112" s="6">
-        <v>274.25</v>
+        <v>250.65</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3633,22 +3633,22 @@
         <v>117</v>
       </c>
       <c r="B113" s="9">
-        <v>469</v>
+        <v>535.70000000000005</v>
       </c>
       <c r="C113" s="11">
-        <v>453</v>
+        <v>526.20000000000005</v>
       </c>
       <c r="D113" s="14">
-        <v>464</v>
+        <v>527.5</v>
       </c>
       <c r="E113" s="6">
-        <v>464.95</v>
+        <v>528.70000000000005</v>
       </c>
       <c r="F113" s="17">
-        <v>85</v>
+        <v>143</v>
       </c>
       <c r="G113" s="6">
-        <v>458.75</v>
+        <v>528.29999999999995</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -3656,22 +3656,22 @@
         <v>118</v>
       </c>
       <c r="B114" s="9">
-        <v>723.85</v>
+        <v>721</v>
       </c>
       <c r="C114" s="11">
-        <v>715</v>
+        <v>712.6</v>
       </c>
       <c r="D114" s="14">
-        <v>717.4</v>
+        <v>713.9</v>
       </c>
       <c r="E114" s="6">
-        <v>716.9</v>
+        <v>713.45</v>
       </c>
       <c r="F114" s="17">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G114" s="6">
-        <v>721.9</v>
+        <v>718.8</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3679,22 +3679,22 @@
         <v>119</v>
       </c>
       <c r="B115" s="9">
-        <v>1540.95</v>
+        <v>1443.85</v>
       </c>
       <c r="C115" s="11">
-        <v>1508.25</v>
+        <v>1425.75</v>
       </c>
       <c r="D115" s="14">
-        <v>1515</v>
+        <v>1428.8</v>
       </c>
       <c r="E115" s="6">
-        <v>1517.95</v>
+        <v>1430.1</v>
       </c>
       <c r="F115" s="17">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="G115" s="6">
-        <v>1539</v>
+        <v>1433.65</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -3702,22 +3702,22 @@
         <v>120</v>
       </c>
       <c r="B116" s="9">
-        <v>4735</v>
+        <v>7197.55</v>
       </c>
       <c r="C116" s="11">
-        <v>4672.2</v>
+        <v>6926</v>
       </c>
       <c r="D116" s="14">
-        <v>4677.2</v>
+        <v>7082</v>
       </c>
       <c r="E116" s="6">
-        <v>4689.2</v>
+        <v>7119.3</v>
       </c>
       <c r="F116" s="17">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="G116" s="6">
-        <v>4704</v>
+        <v>7151</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -3725,22 +3725,22 @@
         <v>121</v>
       </c>
       <c r="B117" s="9">
-        <v>2388.65</v>
+        <v>2319</v>
       </c>
       <c r="C117" s="11">
-        <v>2367.1999999999998</v>
+        <v>2282.65</v>
       </c>
       <c r="D117" s="14">
-        <v>2376</v>
+        <v>2290</v>
       </c>
       <c r="E117" s="6">
-        <v>2376</v>
+        <v>2288.1999999999998</v>
       </c>
       <c r="F117" s="17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G117" s="6">
-        <v>2386.25</v>
+        <v>2290.0500000000002</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -3748,22 +3748,22 @@
         <v>122</v>
       </c>
       <c r="B118" s="9">
-        <v>825</v>
+        <v>887.5</v>
       </c>
       <c r="C118" s="11">
-        <v>793</v>
+        <v>840.5</v>
       </c>
       <c r="D118" s="14">
-        <v>798.55</v>
+        <v>874</v>
       </c>
       <c r="E118" s="6">
-        <v>796.5</v>
+        <v>875.2</v>
       </c>
       <c r="F118" s="17">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G118" s="6">
-        <v>805.7</v>
+        <v>844</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -3771,22 +3771,22 @@
         <v>123</v>
       </c>
       <c r="B119" s="9">
-        <v>1569.1</v>
+        <v>1544.6</v>
       </c>
       <c r="C119" s="11">
-        <v>1548.9</v>
+        <v>1520.35</v>
       </c>
       <c r="D119" s="14">
-        <v>1555</v>
+        <v>1527</v>
       </c>
       <c r="E119" s="6">
-        <v>1552.1</v>
+        <v>1527.4</v>
       </c>
       <c r="F119" s="17">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G119" s="6">
-        <v>1560.55</v>
+        <v>1543.75</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -3794,22 +3794,22 @@
         <v>124</v>
       </c>
       <c r="B120" s="9">
-        <v>710.5</v>
+        <v>676.4</v>
       </c>
       <c r="C120" s="11">
-        <v>696</v>
+        <v>668.1</v>
       </c>
       <c r="D120" s="14">
-        <v>698.6</v>
+        <v>672.5</v>
       </c>
       <c r="E120" s="6">
-        <v>697.1</v>
+        <v>673.5</v>
       </c>
       <c r="F120" s="17">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G120" s="6">
-        <v>708.4</v>
+        <v>669.6</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -3817,22 +3817,22 @@
         <v>125</v>
       </c>
       <c r="B121" s="9">
-        <v>2014</v>
+        <v>1775.95</v>
       </c>
       <c r="C121" s="11">
-        <v>1950.2</v>
+        <v>1752</v>
       </c>
       <c r="D121" s="14">
-        <v>1985</v>
+        <v>1768.95</v>
       </c>
       <c r="E121" s="6">
-        <v>1984.55</v>
+        <v>1768.85</v>
       </c>
       <c r="F121" s="17">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="G121" s="6">
-        <v>1958.5</v>
+        <v>1770.15</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -3840,22 +3840,22 @@
         <v>126</v>
       </c>
       <c r="B122" s="9">
-        <v>992.2</v>
+        <v>972.95</v>
       </c>
       <c r="C122" s="11">
-        <v>980.1</v>
+        <v>945.1</v>
       </c>
       <c r="D122" s="14">
-        <v>988.9</v>
+        <v>946</v>
       </c>
       <c r="E122" s="6">
-        <v>987.2</v>
+        <v>947.3</v>
       </c>
       <c r="F122" s="17">
-        <v>60</v>
+        <v>196</v>
       </c>
       <c r="G122" s="6">
-        <v>991.75</v>
+        <v>970.4</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -3863,22 +3863,22 @@
         <v>127</v>
       </c>
       <c r="B123" s="9">
-        <v>1285.5</v>
+        <v>1282.95</v>
       </c>
       <c r="C123" s="11">
-        <v>1272.5</v>
+        <v>1265</v>
       </c>
       <c r="D123" s="14">
-        <v>1280.8</v>
+        <v>1276.9000000000001</v>
       </c>
       <c r="E123" s="6">
-        <v>1280.05</v>
+        <v>1274.5</v>
       </c>
       <c r="F123" s="17">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="G123" s="6">
-        <v>1277.5999999999999</v>
+        <v>1278.75</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -3886,22 +3886,22 @@
         <v>128</v>
       </c>
       <c r="B124" s="9">
-        <v>2733</v>
+        <v>2655.2</v>
       </c>
       <c r="C124" s="11">
-        <v>2681.55</v>
+        <v>2619.3000000000002</v>
       </c>
       <c r="D124" s="14">
-        <v>2692</v>
+        <v>2652.35</v>
       </c>
       <c r="E124" s="6">
-        <v>2690.85</v>
+        <v>2648.95</v>
       </c>
       <c r="F124" s="17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G124" s="6">
-        <v>2699.65</v>
+        <v>2635.25</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -3909,22 +3909,22 @@
         <v>129</v>
       </c>
       <c r="B125" s="9">
-        <v>1164.5</v>
+        <v>1383</v>
       </c>
       <c r="C125" s="11">
-        <v>1138</v>
+        <v>1357.15</v>
       </c>
       <c r="D125" s="14">
-        <v>1151</v>
+        <v>1360.5</v>
       </c>
       <c r="E125" s="6">
-        <v>1145.7</v>
+        <v>1365.8</v>
       </c>
       <c r="F125" s="17">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G125" s="6">
-        <v>1158.25</v>
+        <v>1375.25</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -3932,22 +3932,22 @@
         <v>130</v>
       </c>
       <c r="B126" s="9">
-        <v>3935</v>
+        <v>4579.5</v>
       </c>
       <c r="C126" s="11">
-        <v>3842.5</v>
+        <v>4509.2</v>
       </c>
       <c r="D126" s="14">
-        <v>3915.5</v>
+        <v>4522</v>
       </c>
       <c r="E126" s="6">
-        <v>3919.8</v>
+        <v>4527</v>
       </c>
       <c r="F126" s="17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G126" s="6">
-        <v>3884.1</v>
+        <v>4554.1499999999996</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -3955,22 +3955,22 @@
         <v>131</v>
       </c>
       <c r="B127" s="9">
-        <v>2267.6999999999998</v>
+        <v>2148</v>
       </c>
       <c r="C127" s="11">
-        <v>2220</v>
+        <v>2085</v>
       </c>
       <c r="D127" s="14">
-        <v>2239</v>
+        <v>2102</v>
       </c>
       <c r="E127" s="6">
-        <v>2232.35</v>
+        <v>2099.9499999999998</v>
       </c>
       <c r="F127" s="17">
         <v>7</v>
       </c>
       <c r="G127" s="6">
-        <v>2244.85</v>
+        <v>2135.1</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -3978,22 +3978,22 @@
         <v>132</v>
       </c>
       <c r="B128" s="9">
-        <v>1717.35</v>
+        <v>1917.95</v>
       </c>
       <c r="C128" s="11">
-        <v>1693</v>
+        <v>1880.7</v>
       </c>
       <c r="D128" s="14">
-        <v>1716</v>
+        <v>1895</v>
       </c>
       <c r="E128" s="6">
-        <v>1713.15</v>
+        <v>1887.2</v>
       </c>
       <c r="F128" s="17">
         <v>1</v>
       </c>
       <c r="G128" s="6">
-        <v>1696.4</v>
+        <v>1916.95</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -4001,22 +4001,22 @@
         <v>133</v>
       </c>
       <c r="B129" s="9">
-        <v>10138.450000000001</v>
+        <v>9663.85</v>
       </c>
       <c r="C129" s="11">
-        <v>9966.2000000000007</v>
+        <v>9560</v>
       </c>
       <c r="D129" s="14">
-        <v>9986</v>
+        <v>9606.2000000000007</v>
       </c>
       <c r="E129" s="6">
-        <v>9978.4</v>
+        <v>9614.1</v>
       </c>
       <c r="F129" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G129" s="6">
-        <v>10131.450000000001</v>
+        <v>9663.85</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -4024,22 +4024,22 @@
         <v>134</v>
       </c>
       <c r="B130" s="9">
-        <v>479.9</v>
+        <v>521.29999999999995</v>
       </c>
       <c r="C130" s="11">
-        <v>470</v>
+        <v>510.6</v>
       </c>
       <c r="D130" s="14">
-        <v>474.55</v>
+        <v>514.20000000000005</v>
       </c>
       <c r="E130" s="6">
-        <v>474.25</v>
+        <v>514.79999999999995</v>
       </c>
       <c r="F130" s="17">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="G130" s="6">
-        <v>478.8</v>
+        <v>517.15</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -4047,22 +4047,22 @@
         <v>135</v>
       </c>
       <c r="B131" s="9">
-        <v>279</v>
+        <v>449</v>
       </c>
       <c r="C131" s="11">
-        <v>272.75</v>
+        <v>435.55</v>
       </c>
       <c r="D131" s="14">
-        <v>275.8</v>
+        <v>438</v>
       </c>
       <c r="E131" s="6">
-        <v>276.35000000000002</v>
+        <v>437.4</v>
       </c>
       <c r="F131" s="17">
-        <v>104</v>
+        <v>201</v>
       </c>
       <c r="G131" s="6">
-        <v>274.85000000000002</v>
+        <v>438.6</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -4070,22 +4070,22 @@
         <v>136</v>
       </c>
       <c r="B132" s="9">
-        <v>1127</v>
+        <v>1317.3</v>
       </c>
       <c r="C132" s="11">
-        <v>1106</v>
+        <v>1299.6500000000001</v>
       </c>
       <c r="D132" s="14">
-        <v>1107</v>
+        <v>1300</v>
       </c>
       <c r="E132" s="6">
-        <v>1110.8499999999999</v>
+        <v>1303.45</v>
       </c>
       <c r="F132" s="17">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G132" s="6">
-        <v>1113.5</v>
+        <v>1307.25</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -4093,22 +4093,22 @@
         <v>137</v>
       </c>
       <c r="B133" s="9">
-        <v>157.15</v>
+        <v>133.55000000000001</v>
       </c>
       <c r="C133" s="11">
-        <v>153.80000000000001</v>
+        <v>130</v>
       </c>
       <c r="D133" s="14">
-        <v>154.94999999999999</v>
+        <v>130.44999999999999</v>
       </c>
       <c r="E133" s="6">
-        <v>154.9</v>
+        <v>130.80000000000001</v>
       </c>
       <c r="F133" s="17">
-        <v>137</v>
+        <v>78</v>
       </c>
       <c r="G133" s="6">
-        <v>157.05000000000001</v>
+        <v>132.80000000000001</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4116,22 +4116,22 @@
         <v>138</v>
       </c>
       <c r="B134" s="19">
-        <v>952.05</v>
+        <v>1005</v>
       </c>
       <c r="C134" s="12">
-        <v>934</v>
+        <v>990.45</v>
       </c>
       <c r="D134" s="15">
-        <v>949</v>
+        <v>999.25</v>
       </c>
       <c r="E134" s="7">
-        <v>946.25</v>
+        <v>997.05</v>
       </c>
       <c r="F134" s="18">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G134" s="7">
-        <v>934.6</v>
+        <v>991.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed MCDOWELL-N to UNITDSPRS
</commit_message>
<xml_diff>
--- a/algo high low.xlsx
+++ b/algo high low.xlsx
@@ -610,8 +610,8 @@
   </sheetPr>
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K94" sqref="K94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -661,22 +661,22 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>633.65</v>
+        <v>679.4</v>
       </c>
       <c r="C2" s="10" t="n">
-        <v>624.65</v>
+        <v>671.45</v>
       </c>
       <c r="D2" s="13" t="n">
-        <v>627.3</v>
+        <v>675.5</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>628</v>
+        <v>675.75</v>
       </c>
       <c r="F2" s="16" t="n">
         <v>10</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>625</v>
+        <v>673.95</v>
       </c>
     </row>
     <row r="3">
@@ -686,22 +686,22 @@
         </is>
       </c>
       <c r="B3" s="9" t="n">
-        <v>8248.450000000001</v>
+        <v>9145</v>
       </c>
       <c r="C3" s="11" t="n">
-        <v>8142.2</v>
+        <v>8491.049999999999</v>
       </c>
       <c r="D3" s="14" t="n">
-        <v>8185</v>
+        <v>9031</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>8198.35</v>
+        <v>9020</v>
       </c>
       <c r="F3" s="17" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G3" s="6" t="n">
-        <v>8178.45</v>
+        <v>8496.950000000001</v>
       </c>
     </row>
     <row r="4">
@@ -711,22 +711,22 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>228.8</v>
+        <v>243.3</v>
       </c>
       <c r="C4" s="11" t="n">
-        <v>225.3</v>
+        <v>238.69</v>
       </c>
       <c r="D4" s="14" t="n">
-        <v>226.6</v>
+        <v>239.55</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>225.85</v>
+        <v>239.96</v>
       </c>
       <c r="F4" s="17" t="n">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="G4" s="6" t="n">
-        <v>225.8</v>
+        <v>239.9</v>
       </c>
     </row>
     <row r="5">
@@ -736,22 +736,22 @@
         </is>
       </c>
       <c r="B5" s="9" t="n">
-        <v>301</v>
+        <v>332.85</v>
       </c>
       <c r="C5" s="11" t="n">
-        <v>280.4</v>
+        <v>326.75</v>
       </c>
       <c r="D5" s="14" t="n">
-        <v>300</v>
+        <v>328.95</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>299.3</v>
+        <v>328.6</v>
       </c>
       <c r="F5" s="17" t="n">
-        <v>168</v>
+        <v>29</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>284.5</v>
+        <v>327.2</v>
       </c>
     </row>
     <row r="6">
@@ -761,22 +761,22 @@
         </is>
       </c>
       <c r="B6" s="9" t="n">
-        <v>3322.9</v>
+        <v>3275</v>
       </c>
       <c r="C6" s="11" t="n">
         <v>3225</v>
       </c>
       <c r="D6" s="14" t="n">
-        <v>3255</v>
+        <v>3269</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>3258.8</v>
+        <v>3261.75</v>
       </c>
       <c r="F6" s="17" t="n">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>3234.85</v>
+        <v>3227.8</v>
       </c>
     </row>
     <row r="7">
@@ -786,22 +786,22 @@
         </is>
       </c>
       <c r="B7" s="9" t="n">
-        <v>1427.85</v>
+        <v>1442</v>
       </c>
       <c r="C7" s="11" t="n">
-        <v>1390</v>
+        <v>1395.45</v>
       </c>
       <c r="D7" s="14" t="n">
-        <v>1409</v>
+        <v>1429.7</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>1410</v>
+        <v>1430.7</v>
       </c>
       <c r="F7" s="17" t="n">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>1395</v>
+        <v>1397.45</v>
       </c>
     </row>
     <row r="8">
@@ -811,22 +811,22 @@
         </is>
       </c>
       <c r="B8" s="9" t="n">
-        <v>5382.9</v>
+        <v>5114.95</v>
       </c>
       <c r="C8" s="11" t="n">
-        <v>5183.3</v>
+        <v>5056.75</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>5280</v>
+        <v>5095.1</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>5262.45</v>
+        <v>5101.95</v>
       </c>
       <c r="F8" s="17" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v>5338.2</v>
+        <v>5077.95</v>
       </c>
     </row>
     <row r="9">
@@ -836,22 +836,22 @@
         </is>
       </c>
       <c r="B9" s="9" t="n">
-        <v>633.5</v>
+        <v>681.7</v>
       </c>
       <c r="C9" s="11" t="n">
-        <v>624.2</v>
+        <v>672.2</v>
       </c>
       <c r="D9" s="14" t="n">
-        <v>631.3</v>
+        <v>673.6</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>630.1</v>
+        <v>677.2</v>
       </c>
       <c r="F9" s="17" t="n">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="G9" s="6" t="n">
-        <v>627.9</v>
+        <v>675.4</v>
       </c>
     </row>
     <row r="10">
@@ -861,22 +861,22 @@
         </is>
       </c>
       <c r="B10" s="9" t="n">
-        <v>5945</v>
+        <v>6218</v>
       </c>
       <c r="C10" s="11" t="n">
-        <v>5895.5</v>
+        <v>6175</v>
       </c>
       <c r="D10" s="14" t="n">
-        <v>5898</v>
+        <v>6181.3</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>5903.45</v>
+        <v>6207.6</v>
       </c>
       <c r="F10" s="17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G10" s="6" t="n">
-        <v>5915.9</v>
+        <v>6183.9</v>
       </c>
     </row>
     <row r="11">
@@ -886,22 +886,22 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>471.85</v>
+        <v>478</v>
       </c>
       <c r="C11" s="11" t="n">
-        <v>467.1</v>
+        <v>472.1</v>
       </c>
       <c r="D11" s="14" t="n">
-        <v>471.35</v>
+        <v>476.6</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>471.05</v>
+        <v>476.45</v>
       </c>
       <c r="F11" s="17" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G11" s="6" t="n">
-        <v>468.2</v>
+        <v>474.4</v>
       </c>
     </row>
     <row r="12">
@@ -911,22 +911,22 @@
         </is>
       </c>
       <c r="B12" s="9" t="n">
-        <v>229</v>
+        <v>242.69</v>
       </c>
       <c r="C12" s="11" t="n">
-        <v>221.1</v>
+        <v>235.89</v>
       </c>
       <c r="D12" s="14" t="n">
-        <v>222.35</v>
+        <v>239.05</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>221.65</v>
+        <v>239.84</v>
       </c>
       <c r="F12" s="17" t="n">
-        <v>208</v>
+        <v>170</v>
       </c>
       <c r="G12" s="6" t="n">
-        <v>226.55</v>
+        <v>237.69</v>
       </c>
     </row>
     <row r="13">
@@ -936,22 +936,22 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>2145</v>
+        <v>2291.95</v>
       </c>
       <c r="C13" s="11" t="n">
-        <v>2106.5</v>
+        <v>2252.95</v>
       </c>
       <c r="D13" s="14" t="n">
-        <v>2110.1</v>
+        <v>2271</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>2114.05</v>
+        <v>2269.45</v>
       </c>
       <c r="F13" s="17" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G13" s="6" t="n">
-        <v>2138.55</v>
+        <v>2254.15</v>
       </c>
     </row>
     <row r="14">
@@ -961,22 +961,22 @@
         </is>
       </c>
       <c r="B14" s="9" t="n">
-        <v>5912.8</v>
+        <v>6280.95</v>
       </c>
       <c r="C14" s="11" t="n">
-        <v>5842.1</v>
+        <v>6200</v>
       </c>
       <c r="D14" s="14" t="n">
-        <v>5887.95</v>
+        <v>6225.05</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>5866.25</v>
+        <v>6261.65</v>
       </c>
       <c r="F14" s="17" t="n">
         <v>0</v>
       </c>
       <c r="G14" s="6" t="n">
-        <v>5842.7</v>
+        <v>6213.8</v>
       </c>
     </row>
     <row r="15">
@@ -986,22 +986,22 @@
         </is>
       </c>
       <c r="B15" s="9" t="n">
-        <v>652.8</v>
+        <v>669.95</v>
       </c>
       <c r="C15" s="11" t="n">
-        <v>639.1</v>
+        <v>658</v>
       </c>
       <c r="D15" s="14" t="n">
-        <v>646</v>
+        <v>661.2</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>648.3</v>
+        <v>661.25</v>
       </c>
       <c r="F15" s="17" t="n">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="G15" s="6" t="n">
-        <v>641.05</v>
+        <v>669.7</v>
       </c>
     </row>
     <row r="16">
@@ -1011,22 +1011,22 @@
         </is>
       </c>
       <c r="B16" s="9" t="n">
-        <v>1230</v>
+        <v>1264.65</v>
       </c>
       <c r="C16" s="11" t="n">
-        <v>1203.1</v>
+        <v>1238.1</v>
       </c>
       <c r="D16" s="14" t="n">
-        <v>1214.45</v>
+        <v>1258.4</v>
       </c>
       <c r="E16" s="6" t="n">
-        <v>1218.9</v>
+        <v>1259</v>
       </c>
       <c r="F16" s="17" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G16" s="6" t="n">
-        <v>1209.55</v>
+        <v>1241.9</v>
       </c>
     </row>
     <row r="17">
@@ -1036,22 +1036,22 @@
         </is>
       </c>
       <c r="B17" s="9" t="n">
-        <v>1595.75</v>
+        <v>1596</v>
       </c>
       <c r="C17" s="11" t="n">
-        <v>1565.1</v>
+        <v>1575.35</v>
       </c>
       <c r="D17" s="14" t="n">
-        <v>1567.05</v>
+        <v>1587.05</v>
       </c>
       <c r="E17" s="6" t="n">
-        <v>1569.9</v>
+        <v>1591.75</v>
       </c>
       <c r="F17" s="17" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="G17" s="6" t="n">
-        <v>1595.7</v>
+        <v>1582.6</v>
       </c>
     </row>
     <row r="18">
@@ -1061,22 +1061,22 @@
         </is>
       </c>
       <c r="B18" s="9" t="n">
-        <v>6894</v>
+        <v>7370</v>
       </c>
       <c r="C18" s="11" t="n">
-        <v>6785.35</v>
+        <v>7247</v>
       </c>
       <c r="D18" s="14" t="n">
-        <v>6791.65</v>
+        <v>7340.5</v>
       </c>
       <c r="E18" s="6" t="n">
-        <v>6806.7</v>
+        <v>7341.55</v>
       </c>
       <c r="F18" s="17" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G18" s="6" t="n">
-        <v>6870.1</v>
+        <v>7300</v>
       </c>
     </row>
     <row r="19">
@@ -1086,22 +1086,22 @@
         </is>
       </c>
       <c r="B19" s="9" t="n">
-        <v>3120</v>
+        <v>3256.65</v>
       </c>
       <c r="C19" s="11" t="n">
-        <v>3066.6</v>
+        <v>3178</v>
       </c>
       <c r="D19" s="14" t="n">
-        <v>3103</v>
+        <v>3245</v>
       </c>
       <c r="E19" s="6" t="n">
-        <v>3099.25</v>
+        <v>3240.6</v>
       </c>
       <c r="F19" s="17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19" s="6" t="n">
-        <v>3093</v>
+        <v>3183.55</v>
       </c>
     </row>
     <row r="20">
@@ -1111,22 +1111,22 @@
         </is>
       </c>
       <c r="B20" s="9" t="n">
-        <v>385</v>
+        <v>443.05</v>
       </c>
       <c r="C20" s="11" t="n">
-        <v>379</v>
+        <v>427</v>
       </c>
       <c r="D20" s="14" t="n">
-        <v>384</v>
+        <v>430</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>383.65</v>
+        <v>430.2</v>
       </c>
       <c r="F20" s="17" t="n">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="G20" s="6" t="n">
-        <v>379.25</v>
+        <v>442.95</v>
       </c>
     </row>
     <row r="21">
@@ -1136,22 +1136,22 @@
         </is>
       </c>
       <c r="B21" s="9" t="n">
-        <v>194.1</v>
+        <v>195.9</v>
       </c>
       <c r="C21" s="11" t="n">
-        <v>189.5</v>
+        <v>193.53</v>
       </c>
       <c r="D21" s="14" t="n">
-        <v>191.6</v>
+        <v>194.15</v>
       </c>
       <c r="E21" s="6" t="n">
-        <v>191.7</v>
+        <v>194.34</v>
       </c>
       <c r="F21" s="17" t="n">
-        <v>113</v>
+        <v>51</v>
       </c>
       <c r="G21" s="6" t="n">
-        <v>189.7</v>
+        <v>195.6</v>
       </c>
     </row>
     <row r="22">
@@ -1161,22 +1161,22 @@
         </is>
       </c>
       <c r="B22" s="9" t="n">
-        <v>266.2</v>
+        <v>287.5</v>
       </c>
       <c r="C22" s="11" t="n">
-        <v>262.55</v>
+        <v>281.75</v>
       </c>
       <c r="D22" s="14" t="n">
-        <v>263.5</v>
+        <v>286</v>
       </c>
       <c r="E22" s="6" t="n">
-        <v>263.4</v>
+        <v>286.25</v>
       </c>
       <c r="F22" s="17" t="n">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="G22" s="6" t="n">
-        <v>263.75</v>
+        <v>282.35</v>
       </c>
     </row>
     <row r="23">
@@ -1186,22 +1186,22 @@
         </is>
       </c>
       <c r="B23" s="9" t="n">
-        <v>1377</v>
+        <v>1466.1</v>
       </c>
       <c r="C23" s="11" t="n">
-        <v>1351.7</v>
+        <v>1448</v>
       </c>
       <c r="D23" s="14" t="n">
-        <v>1376.6</v>
+        <v>1452.7</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>1373.95</v>
+        <v>1451.8</v>
       </c>
       <c r="F23" s="17" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G23" s="6" t="n">
-        <v>1353.8</v>
+        <v>1463.75</v>
       </c>
     </row>
     <row r="24">
@@ -1211,22 +1211,22 @@
         </is>
       </c>
       <c r="B24" s="9" t="n">
-        <v>293.95</v>
+        <v>310.5</v>
       </c>
       <c r="C24" s="11" t="n">
-        <v>287.9</v>
+        <v>301.5</v>
       </c>
       <c r="D24" s="14" t="n">
-        <v>292.55</v>
+        <v>309.7</v>
       </c>
       <c r="E24" s="6" t="n">
-        <v>292.15</v>
+        <v>309.6</v>
       </c>
       <c r="F24" s="17" t="n">
-        <v>316</v>
+        <v>673</v>
       </c>
       <c r="G24" s="6" t="n">
-        <v>288.8</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25">
@@ -1236,22 +1236,22 @@
         </is>
       </c>
       <c r="B25" s="9" t="n">
-        <v>1573</v>
+        <v>1739.45</v>
       </c>
       <c r="C25" s="11" t="n">
-        <v>1545.1</v>
+        <v>1627</v>
       </c>
       <c r="D25" s="14" t="n">
-        <v>1564</v>
+        <v>1714.2</v>
       </c>
       <c r="E25" s="6" t="n">
-        <v>1568.65</v>
+        <v>1717.3</v>
       </c>
       <c r="F25" s="17" t="n">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="G25" s="6" t="n">
-        <v>1557.4</v>
+        <v>1629.25</v>
       </c>
     </row>
     <row r="26">
@@ -1261,22 +1261,22 @@
         </is>
       </c>
       <c r="B26" s="9" t="n">
-        <v>324.8</v>
+        <v>339.7</v>
       </c>
       <c r="C26" s="11" t="n">
-        <v>313.05</v>
+        <v>334.15</v>
       </c>
       <c r="D26" s="14" t="n">
-        <v>323.45</v>
+        <v>334.25</v>
       </c>
       <c r="E26" s="6" t="n">
-        <v>323.6</v>
+        <v>334.8</v>
       </c>
       <c r="F26" s="17" t="n">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="G26" s="6" t="n">
-        <v>314.65</v>
+        <v>334.65</v>
       </c>
     </row>
     <row r="27">
@@ -1286,22 +1286,22 @@
         </is>
       </c>
       <c r="B27" s="9" t="n">
-        <v>5268</v>
+        <v>5432.3</v>
       </c>
       <c r="C27" s="11" t="n">
-        <v>5211.25</v>
+        <v>5375.6</v>
       </c>
       <c r="D27" s="14" t="n">
-        <v>5217</v>
+        <v>5391.8</v>
       </c>
       <c r="E27" s="6" t="n">
-        <v>5229.8</v>
+        <v>5393.65</v>
       </c>
       <c r="F27" s="17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27" s="6" t="n">
-        <v>5217.15</v>
+        <v>5421.85</v>
       </c>
     </row>
     <row r="28">
@@ -1311,22 +1311,22 @@
         </is>
       </c>
       <c r="B28" s="9" t="n">
-        <v>622.2</v>
+        <v>685</v>
       </c>
       <c r="C28" s="11" t="n">
-        <v>614.5</v>
+        <v>670.2</v>
       </c>
       <c r="D28" s="14" t="n">
-        <v>620.9</v>
+        <v>678</v>
       </c>
       <c r="E28" s="6" t="n">
-        <v>620.45</v>
+        <v>677.95</v>
       </c>
       <c r="F28" s="17" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G28" s="6" t="n">
-        <v>615.5</v>
+        <v>671.2</v>
       </c>
     </row>
     <row r="29">
@@ -1336,22 +1336,22 @@
         </is>
       </c>
       <c r="B29" s="9" t="n">
-        <v>118.45</v>
+        <v>120.99</v>
       </c>
       <c r="C29" s="11" t="n">
-        <v>116</v>
+        <v>119.3</v>
       </c>
       <c r="D29" s="14" t="n">
-        <v>116.4</v>
+        <v>120.9</v>
       </c>
       <c r="E29" s="6" t="n">
-        <v>116.55</v>
+        <v>120.81</v>
       </c>
       <c r="F29" s="17" t="n">
-        <v>397</v>
+        <v>325</v>
       </c>
       <c r="G29" s="6" t="n">
-        <v>116.45</v>
+        <v>119.57</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -1361,22 +1361,22 @@
         </is>
       </c>
       <c r="B30" s="9" t="n">
-        <v>742.45</v>
+        <v>837.45</v>
       </c>
       <c r="C30" s="11" t="n">
-        <v>720.3</v>
+        <v>816.5</v>
       </c>
       <c r="D30" s="14" t="n">
-        <v>723</v>
+        <v>832.55</v>
       </c>
       <c r="E30" s="6" t="n">
-        <v>722.2</v>
+        <v>834.9</v>
       </c>
       <c r="F30" s="17" t="n">
         <v>10</v>
       </c>
       <c r="G30" s="6" t="n">
-        <v>741.45</v>
+        <v>816.75</v>
       </c>
     </row>
     <row r="31">
@@ -1386,22 +1386,22 @@
         </is>
       </c>
       <c r="B31" s="9" t="n">
-        <v>408.8</v>
+        <v>436</v>
       </c>
       <c r="C31" s="11" t="n">
-        <v>401.5</v>
+        <v>426</v>
       </c>
       <c r="D31" s="14" t="n">
-        <v>404.6</v>
+        <v>427</v>
       </c>
       <c r="E31" s="6" t="n">
-        <v>403.9</v>
+        <v>426.7</v>
       </c>
       <c r="F31" s="17" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G31" s="6" t="n">
-        <v>406.6</v>
+        <v>431.75</v>
       </c>
     </row>
     <row r="32">
@@ -1411,22 +1411,22 @@
         </is>
       </c>
       <c r="B32" s="9" t="n">
-        <v>1269.8</v>
+        <v>1455.85</v>
       </c>
       <c r="C32" s="11" t="n">
-        <v>1235</v>
+        <v>1438.3</v>
       </c>
       <c r="D32" s="14" t="n">
-        <v>1241.25</v>
+        <v>1442.5</v>
       </c>
       <c r="E32" s="6" t="n">
-        <v>1240.4</v>
+        <v>1447</v>
       </c>
       <c r="F32" s="17" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G32" s="6" t="n">
-        <v>1254.75</v>
+        <v>1446.45</v>
       </c>
     </row>
     <row r="33">
@@ -1436,22 +1436,22 @@
         </is>
       </c>
       <c r="B33" s="9" t="n">
-        <v>1497.6</v>
+        <v>1567</v>
       </c>
       <c r="C33" s="11" t="n">
-        <v>1477</v>
+        <v>1549.05</v>
       </c>
       <c r="D33" s="14" t="n">
-        <v>1493.45</v>
+        <v>1566</v>
       </c>
       <c r="E33" s="6" t="n">
-        <v>1493.55</v>
+        <v>1564.75</v>
       </c>
       <c r="F33" s="17" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G33" s="6" t="n">
-        <v>1478</v>
+        <v>1551.3</v>
       </c>
     </row>
     <row r="34">
@@ -1461,22 +1461,22 @@
         </is>
       </c>
       <c r="B34" s="9" t="n">
-        <v>5198</v>
+        <v>5230.45</v>
       </c>
       <c r="C34" s="11" t="n">
-        <v>5121</v>
+        <v>5178.7</v>
       </c>
       <c r="D34" s="14" t="n">
-        <v>5140.25</v>
+        <v>5192.9</v>
       </c>
       <c r="E34" s="6" t="n">
-        <v>5141.55</v>
+        <v>5201.75</v>
       </c>
       <c r="F34" s="17" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G34" s="6" t="n">
-        <v>5168</v>
+        <v>5200.7</v>
       </c>
     </row>
     <row r="35">
@@ -1486,22 +1486,22 @@
         </is>
       </c>
       <c r="B35" s="9" t="n">
-        <v>1097.2</v>
+        <v>1146.65</v>
       </c>
       <c r="C35" s="11" t="n">
-        <v>1074.4</v>
+        <v>1124.5</v>
       </c>
       <c r="D35" s="14" t="n">
-        <v>1081</v>
+        <v>1134.8</v>
       </c>
       <c r="E35" s="6" t="n">
-        <v>1084.8</v>
+        <v>1139.85</v>
       </c>
       <c r="F35" s="17" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G35" s="6" t="n">
-        <v>1078.55</v>
+        <v>1134.05</v>
       </c>
     </row>
     <row r="36">
@@ -1511,22 +1511,22 @@
         </is>
       </c>
       <c r="B36" s="9" t="n">
-        <v>1294.45</v>
+        <v>1534.75</v>
       </c>
       <c r="C36" s="11" t="n">
-        <v>1274.05</v>
+        <v>1482.1</v>
       </c>
       <c r="D36" s="14" t="n">
-        <v>1283</v>
+        <v>1505.5</v>
       </c>
       <c r="E36" s="6" t="n">
-        <v>1287.85</v>
+        <v>1508.8</v>
       </c>
       <c r="F36" s="17" t="n">
         <v>5</v>
       </c>
       <c r="G36" s="6" t="n">
-        <v>1281</v>
+        <v>1485.7</v>
       </c>
     </row>
     <row r="37">
@@ -1536,22 +1536,22 @@
         </is>
       </c>
       <c r="B37" s="9" t="n">
-        <v>401.8</v>
+        <v>429</v>
       </c>
       <c r="C37" s="11" t="n">
-        <v>388.85</v>
+        <v>421.2</v>
       </c>
       <c r="D37" s="14" t="n">
-        <v>394.15</v>
+        <v>425.1</v>
       </c>
       <c r="E37" s="6" t="n">
-        <v>393.9</v>
+        <v>426.55</v>
       </c>
       <c r="F37" s="17" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G37" s="6" t="n">
-        <v>389.65</v>
+        <v>421.75</v>
       </c>
     </row>
     <row r="38">
@@ -1561,22 +1561,22 @@
         </is>
       </c>
       <c r="B38" s="9" t="n">
-        <v>3859.9</v>
+        <v>3871.8</v>
       </c>
       <c r="C38" s="11" t="n">
-        <v>3785.55</v>
+        <v>3723.9</v>
       </c>
       <c r="D38" s="14" t="n">
-        <v>3827.25</v>
+        <v>3817</v>
       </c>
       <c r="E38" s="6" t="n">
-        <v>3834.65</v>
+        <v>3825.6</v>
       </c>
       <c r="F38" s="17" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G38" s="6" t="n">
-        <v>3830</v>
+        <v>3734.35</v>
       </c>
     </row>
     <row r="39">
@@ -1586,22 +1586,22 @@
         </is>
       </c>
       <c r="B39" s="9" t="n">
-        <v>567.65</v>
+        <v>616</v>
       </c>
       <c r="C39" s="11" t="n">
-        <v>553.05</v>
+        <v>607.5</v>
       </c>
       <c r="D39" s="14" t="n">
-        <v>555</v>
+        <v>609</v>
       </c>
       <c r="E39" s="6" t="n">
-        <v>555.45</v>
+        <v>608.65</v>
       </c>
       <c r="F39" s="17" t="n">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G39" s="6" t="n">
-        <v>567.5</v>
+        <v>614.05</v>
       </c>
     </row>
     <row r="40">
@@ -1611,22 +1611,22 @@
         </is>
       </c>
       <c r="B40" s="9" t="n">
-        <v>1810.95</v>
+        <v>1888.5</v>
       </c>
       <c r="C40" s="11" t="n">
-        <v>1772.05</v>
+        <v>1863.55</v>
       </c>
       <c r="D40" s="14" t="n">
-        <v>1774.1</v>
+        <v>1886.9</v>
       </c>
       <c r="E40" s="6" t="n">
-        <v>1775.45</v>
+        <v>1882.35</v>
       </c>
       <c r="F40" s="17" t="n">
         <v>3</v>
       </c>
       <c r="G40" s="6" t="n">
-        <v>1796.25</v>
+        <v>1870.95</v>
       </c>
     </row>
     <row r="41">
@@ -1636,22 +1636,22 @@
         </is>
       </c>
       <c r="B41" s="9" t="n">
-        <v>578</v>
+        <v>609.8</v>
       </c>
       <c r="C41" s="11" t="n">
-        <v>540</v>
+        <v>579.3</v>
       </c>
       <c r="D41" s="14" t="n">
-        <v>568</v>
+        <v>595</v>
       </c>
       <c r="E41" s="6" t="n">
-        <v>569.9</v>
+        <v>593.6</v>
       </c>
       <c r="F41" s="17" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G41" s="6" t="n">
-        <v>542.9</v>
+        <v>597.3</v>
       </c>
     </row>
     <row r="42">
@@ -1661,22 +1661,22 @@
         </is>
       </c>
       <c r="B42" s="9" t="n">
-        <v>2298</v>
+        <v>2441.4</v>
       </c>
       <c r="C42" s="11" t="n">
-        <v>2263.7</v>
+        <v>2400.35</v>
       </c>
       <c r="D42" s="14" t="n">
-        <v>2266.5</v>
+        <v>2416.6</v>
       </c>
       <c r="E42" s="6" t="n">
-        <v>2267.65</v>
+        <v>2413.7</v>
       </c>
       <c r="F42" s="17" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G42" s="6" t="n">
-        <v>2290.45</v>
+        <v>2406.9</v>
       </c>
     </row>
     <row r="43">
@@ -1686,22 +1686,22 @@
         </is>
       </c>
       <c r="B43" s="9" t="n">
-        <v>116.6</v>
+        <v>138.8</v>
       </c>
       <c r="C43" s="11" t="n">
-        <v>114.65</v>
+        <v>134.32</v>
       </c>
       <c r="D43" s="14" t="n">
-        <v>114.95</v>
+        <v>136</v>
       </c>
       <c r="E43" s="6" t="n">
-        <v>114.9</v>
+        <v>136.16</v>
       </c>
       <c r="F43" s="17" t="n">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="G43" s="6" t="n">
-        <v>116.25</v>
+        <v>134.33</v>
       </c>
     </row>
     <row r="44">
@@ -1711,22 +1711,22 @@
         </is>
       </c>
       <c r="B44" s="9" t="n">
-        <v>4467.5</v>
+        <v>4609.65</v>
       </c>
       <c r="C44" s="11" t="n">
-        <v>4380</v>
+        <v>4559.1</v>
       </c>
       <c r="D44" s="14" t="n">
-        <v>4467.5</v>
+        <v>4585</v>
       </c>
       <c r="E44" s="6" t="n">
-        <v>4448</v>
+        <v>4588.6</v>
       </c>
       <c r="F44" s="17" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G44" s="6" t="n">
-        <v>4397.1</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="45">
@@ -1736,22 +1736,22 @@
         </is>
       </c>
       <c r="B45" s="9" t="n">
-        <v>9255</v>
+        <v>11458.9</v>
       </c>
       <c r="C45" s="11" t="n">
-        <v>9054.950000000001</v>
+        <v>10864.85</v>
       </c>
       <c r="D45" s="14" t="n">
-        <v>9253</v>
+        <v>11240</v>
       </c>
       <c r="E45" s="6" t="n">
-        <v>9238.700000000001</v>
+        <v>11242.85</v>
       </c>
       <c r="F45" s="17" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G45" s="6" t="n">
-        <v>9081.549999999999</v>
+        <v>10896</v>
       </c>
     </row>
     <row r="46">
@@ -1761,22 +1761,22 @@
         </is>
       </c>
       <c r="B46" s="9" t="n">
-        <v>825.9</v>
+        <v>883.65</v>
       </c>
       <c r="C46" s="11" t="n">
-        <v>816.55</v>
+        <v>871.9</v>
       </c>
       <c r="D46" s="14" t="n">
-        <v>819</v>
+        <v>877.25</v>
       </c>
       <c r="E46" s="6" t="n">
-        <v>818.3</v>
+        <v>878.6</v>
       </c>
       <c r="F46" s="17" t="n">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="G46" s="6" t="n">
-        <v>817.95</v>
+        <v>872.85</v>
       </c>
     </row>
     <row r="47">
@@ -1786,22 +1786,22 @@
         </is>
       </c>
       <c r="B47" s="9" t="n">
-        <v>6017.95</v>
+        <v>6090.5</v>
       </c>
       <c r="C47" s="11" t="n">
-        <v>5914.6</v>
+        <v>6035.1</v>
       </c>
       <c r="D47" s="14" t="n">
-        <v>5995</v>
+        <v>6085</v>
       </c>
       <c r="E47" s="6" t="n">
-        <v>6000.75</v>
+        <v>6085.25</v>
       </c>
       <c r="F47" s="17" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G47" s="6" t="n">
-        <v>5935.2</v>
+        <v>6062.5</v>
       </c>
     </row>
     <row r="48">
@@ -1811,22 +1811,22 @@
         </is>
       </c>
       <c r="B48" s="9" t="n">
-        <v>3888</v>
+        <v>4309.95</v>
       </c>
       <c r="C48" s="11" t="n">
-        <v>3783.3</v>
+        <v>4209</v>
       </c>
       <c r="D48" s="14" t="n">
-        <v>3845</v>
+        <v>4290</v>
       </c>
       <c r="E48" s="6" t="n">
-        <v>3853.4</v>
+        <v>4292.1</v>
       </c>
       <c r="F48" s="17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G48" s="6" t="n">
-        <v>3798.05</v>
+        <v>4224.95</v>
       </c>
     </row>
     <row r="49">
@@ -1836,22 +1836,22 @@
         </is>
       </c>
       <c r="B49" s="9" t="n">
-        <v>514.8</v>
+        <v>547.9</v>
       </c>
       <c r="C49" s="11" t="n">
-        <v>504</v>
+        <v>539.2</v>
       </c>
       <c r="D49" s="14" t="n">
-        <v>506</v>
+        <v>542.2</v>
       </c>
       <c r="E49" s="6" t="n">
-        <v>506.8</v>
+        <v>542.25</v>
       </c>
       <c r="F49" s="17" t="n">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="G49" s="6" t="n">
-        <v>511.5</v>
+        <v>540.85</v>
       </c>
     </row>
     <row r="50">
@@ -1861,22 +1861,22 @@
         </is>
       </c>
       <c r="B50" s="9" t="n">
-        <v>1183.9</v>
+        <v>1240.75</v>
       </c>
       <c r="C50" s="11" t="n">
-        <v>1150</v>
+        <v>1221.8</v>
       </c>
       <c r="D50" s="14" t="n">
-        <v>1180</v>
+        <v>1236</v>
       </c>
       <c r="E50" s="6" t="n">
-        <v>1180.4</v>
+        <v>1237.15</v>
       </c>
       <c r="F50" s="17" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G50" s="6" t="n">
-        <v>1151.5</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="51">
@@ -1886,22 +1886,22 @@
         </is>
       </c>
       <c r="B51" s="9" t="n">
-        <v>837</v>
+        <v>871</v>
       </c>
       <c r="C51" s="11" t="n">
-        <v>812.6</v>
+        <v>850</v>
       </c>
       <c r="D51" s="14" t="n">
-        <v>826.2</v>
+        <v>854.3</v>
       </c>
       <c r="E51" s="6" t="n">
-        <v>831</v>
+        <v>853.35</v>
       </c>
       <c r="F51" s="17" t="n">
         <v>0</v>
       </c>
       <c r="G51" s="6" t="n">
-        <v>823.4</v>
+        <v>856.05</v>
       </c>
     </row>
     <row r="52">
@@ -1911,22 +1911,22 @@
         </is>
       </c>
       <c r="B52" s="9" t="n">
-        <v>673.55</v>
+        <v>688.15</v>
       </c>
       <c r="C52" s="11" t="n">
-        <v>655</v>
+        <v>680.8</v>
       </c>
       <c r="D52" s="14" t="n">
-        <v>666.95</v>
+        <v>683.05</v>
       </c>
       <c r="E52" s="6" t="n">
-        <v>668.95</v>
+        <v>683.8</v>
       </c>
       <c r="F52" s="17" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G52" s="6" t="n">
-        <v>656.85</v>
+        <v>685.05</v>
       </c>
     </row>
     <row r="53">
@@ -1936,22 +1936,22 @@
         </is>
       </c>
       <c r="B53" s="9" t="n">
-        <v>1321.35</v>
+        <v>1412</v>
       </c>
       <c r="C53" s="11" t="n">
-        <v>1293.55</v>
+        <v>1389.8</v>
       </c>
       <c r="D53" s="14" t="n">
-        <v>1302.95</v>
+        <v>1391.5</v>
       </c>
       <c r="E53" s="6" t="n">
-        <v>1299.6</v>
+        <v>1392.95</v>
       </c>
       <c r="F53" s="17" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G53" s="6" t="n">
-        <v>1321.15</v>
+        <v>1410.3</v>
       </c>
     </row>
     <row r="54">
@@ -1961,22 +1961,22 @@
         </is>
       </c>
       <c r="B54" s="9" t="n">
-        <v>2768.05</v>
+        <v>3052</v>
       </c>
       <c r="C54" s="11" t="n">
-        <v>2712.15</v>
+        <v>2975.65</v>
       </c>
       <c r="D54" s="14" t="n">
-        <v>2760</v>
+        <v>3005</v>
       </c>
       <c r="E54" s="6" t="n">
-        <v>2758.35</v>
+        <v>2998.5</v>
       </c>
       <c r="F54" s="17" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G54" s="6" t="n">
-        <v>2765</v>
+        <v>3030.6</v>
       </c>
     </row>
     <row r="55">
@@ -1986,22 +1986,22 @@
         </is>
       </c>
       <c r="B55" s="9" t="n">
-        <v>433.8</v>
+        <v>465.9</v>
       </c>
       <c r="C55" s="11" t="n">
-        <v>429</v>
+        <v>460.15</v>
       </c>
       <c r="D55" s="14" t="n">
-        <v>429</v>
+        <v>461</v>
       </c>
       <c r="E55" s="6" t="n">
-        <v>429.95</v>
+        <v>461.75</v>
       </c>
       <c r="F55" s="17" t="n">
         <v>5</v>
       </c>
       <c r="G55" s="6" t="n">
-        <v>433</v>
+        <v>461.35</v>
       </c>
     </row>
     <row r="56">
@@ -2011,22 +2011,22 @@
         </is>
       </c>
       <c r="B56" s="9" t="n">
-        <v>2460</v>
+        <v>2523.7</v>
       </c>
       <c r="C56" s="11" t="n">
-        <v>2393.25</v>
+        <v>2463.4</v>
       </c>
       <c r="D56" s="14" t="n">
-        <v>2399</v>
+        <v>2469</v>
       </c>
       <c r="E56" s="6" t="n">
-        <v>2400.6</v>
+        <v>2471.2</v>
       </c>
       <c r="F56" s="17" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G56" s="6" t="n">
-        <v>2434.15</v>
+        <v>2486.95</v>
       </c>
     </row>
     <row r="57">
@@ -2036,22 +2036,22 @@
         </is>
       </c>
       <c r="B57" s="9" t="n">
-        <v>557.55</v>
+        <v>640.65</v>
       </c>
       <c r="C57" s="11" t="n">
-        <v>545.6</v>
+        <v>626.85</v>
       </c>
       <c r="D57" s="14" t="n">
-        <v>555</v>
+        <v>629.95</v>
       </c>
       <c r="E57" s="6" t="n">
-        <v>555.05</v>
+        <v>632.05</v>
       </c>
       <c r="F57" s="17" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="G57" s="6" t="n">
-        <v>546.15</v>
+        <v>636.5</v>
       </c>
     </row>
     <row r="58">
@@ -2061,22 +2061,22 @@
         </is>
       </c>
       <c r="B58" s="9" t="n">
-        <v>5152</v>
+        <v>5260</v>
       </c>
       <c r="C58" s="11" t="n">
-        <v>5035.65</v>
+        <v>5103.75</v>
       </c>
       <c r="D58" s="14" t="n">
-        <v>5062</v>
+        <v>5188</v>
       </c>
       <c r="E58" s="6" t="n">
-        <v>5051.75</v>
+        <v>5200.55</v>
       </c>
       <c r="F58" s="17" t="n">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="G58" s="6" t="n">
-        <v>5057.7</v>
+        <v>5125</v>
       </c>
     </row>
     <row r="59">
@@ -2086,22 +2086,22 @@
         </is>
       </c>
       <c r="B59" s="9" t="n">
-        <v>1909.8</v>
+        <v>1871.95</v>
       </c>
       <c r="C59" s="11" t="n">
-        <v>1891</v>
+        <v>1835.3</v>
       </c>
       <c r="D59" s="14" t="n">
-        <v>1892.4</v>
+        <v>1838.55</v>
       </c>
       <c r="E59" s="6" t="n">
-        <v>1893.55</v>
+        <v>1839.5</v>
       </c>
       <c r="F59" s="17" t="n">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="G59" s="6" t="n">
-        <v>1894.65</v>
+        <v>1846.2</v>
       </c>
     </row>
     <row r="60">
@@ -2111,22 +2111,22 @@
         </is>
       </c>
       <c r="B60" s="9" t="n">
-        <v>1360.95</v>
+        <v>1439.75</v>
       </c>
       <c r="C60" s="11" t="n">
-        <v>1346.95</v>
+        <v>1424.4</v>
       </c>
       <c r="D60" s="14" t="n">
-        <v>1347.95</v>
+        <v>1431.2</v>
       </c>
       <c r="E60" s="6" t="n">
-        <v>1353.1</v>
+        <v>1431.05</v>
       </c>
       <c r="F60" s="17" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G60" s="6" t="n">
-        <v>1360.6</v>
+        <v>1435.55</v>
       </c>
     </row>
     <row r="61">
@@ -2136,22 +2136,22 @@
         </is>
       </c>
       <c r="B61" s="9" t="n">
-        <v>3975</v>
+        <v>4025</v>
       </c>
       <c r="C61" s="11" t="n">
-        <v>3880.55</v>
+        <v>3955.05</v>
       </c>
       <c r="D61" s="14" t="n">
-        <v>3893.95</v>
+        <v>4019</v>
       </c>
       <c r="E61" s="6" t="n">
-        <v>3893.45</v>
+        <v>4014.4</v>
       </c>
       <c r="F61" s="17" t="n">
         <v>3</v>
       </c>
       <c r="G61" s="6" t="n">
-        <v>3962</v>
+        <v>3999.9</v>
       </c>
     </row>
     <row r="62">
@@ -2161,22 +2161,22 @@
         </is>
       </c>
       <c r="B62" s="9" t="n">
-        <v>573.4</v>
+        <v>601.8</v>
       </c>
       <c r="C62" s="11" t="n">
-        <v>560.9</v>
+        <v>594.05</v>
       </c>
       <c r="D62" s="14" t="n">
-        <v>561.7</v>
+        <v>596.85</v>
       </c>
       <c r="E62" s="6" t="n">
-        <v>561.85</v>
+        <v>598.35</v>
       </c>
       <c r="F62" s="17" t="n">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="G62" s="6" t="n">
-        <v>573.4</v>
+        <v>595.5</v>
       </c>
     </row>
     <row r="63">
@@ -2186,22 +2186,22 @@
         </is>
       </c>
       <c r="B63" s="9" t="n">
-        <v>713.5</v>
+        <v>686.5</v>
       </c>
       <c r="C63" s="11" t="n">
-        <v>684.4</v>
+        <v>678.9</v>
       </c>
       <c r="D63" s="14" t="n">
-        <v>705.3</v>
+        <v>682.1</v>
       </c>
       <c r="E63" s="6" t="n">
-        <v>705.3</v>
+        <v>683.6</v>
       </c>
       <c r="F63" s="17" t="n">
-        <v>226</v>
+        <v>83</v>
       </c>
       <c r="G63" s="6" t="n">
-        <v>689.2</v>
+        <v>679.9</v>
       </c>
     </row>
     <row r="64">
@@ -2211,22 +2211,22 @@
         </is>
       </c>
       <c r="B64" s="9" t="n">
-        <v>381</v>
+        <v>341.6</v>
       </c>
       <c r="C64" s="11" t="n">
-        <v>372.4</v>
+        <v>333.2</v>
       </c>
       <c r="D64" s="14" t="n">
-        <v>376.5</v>
+        <v>336.6</v>
       </c>
       <c r="E64" s="6" t="n">
-        <v>377.05</v>
+        <v>336.9</v>
       </c>
       <c r="F64" s="17" t="n">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="G64" s="6" t="n">
-        <v>374.2</v>
+        <v>334.9</v>
       </c>
     </row>
     <row r="65">
@@ -2236,22 +2236,22 @@
         </is>
       </c>
       <c r="B65" s="9" t="n">
-        <v>1634.95</v>
+        <v>1766.95</v>
       </c>
       <c r="C65" s="11" t="n">
-        <v>1588.35</v>
+        <v>1698.65</v>
       </c>
       <c r="D65" s="14" t="n">
-        <v>1591</v>
+        <v>1730.2</v>
       </c>
       <c r="E65" s="6" t="n">
-        <v>1596.85</v>
+        <v>1730.9</v>
       </c>
       <c r="F65" s="17" t="n">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="G65" s="6" t="n">
-        <v>1628</v>
+        <v>1715.7</v>
       </c>
     </row>
     <row r="66">
@@ -2261,22 +2261,22 @@
         </is>
       </c>
       <c r="B66" s="9" t="n">
-        <v>575.15</v>
+        <v>622</v>
       </c>
       <c r="C66" s="11" t="n">
-        <v>553.6</v>
+        <v>598.55</v>
       </c>
       <c r="D66" s="14" t="n">
-        <v>558.7</v>
+        <v>612.85</v>
       </c>
       <c r="E66" s="6" t="n">
-        <v>556.2</v>
+        <v>613.7</v>
       </c>
       <c r="F66" s="17" t="n">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="G66" s="6" t="n">
-        <v>573.45</v>
+        <v>602.8</v>
       </c>
     </row>
     <row r="67">
@@ -2286,22 +2286,22 @@
         </is>
       </c>
       <c r="B67" s="9" t="n">
-        <v>158.3</v>
+        <v>182.55</v>
       </c>
       <c r="C67" s="11" t="n">
-        <v>155.8</v>
+        <v>176</v>
       </c>
       <c r="D67" s="14" t="n">
-        <v>156.5</v>
+        <v>179.35</v>
       </c>
       <c r="E67" s="6" t="n">
-        <v>156.8</v>
+        <v>179.67</v>
       </c>
       <c r="F67" s="17" t="n">
-        <v>55</v>
+        <v>205</v>
       </c>
       <c r="G67" s="6" t="n">
-        <v>156.2</v>
+        <v>176.29</v>
       </c>
     </row>
     <row r="68">
@@ -2311,22 +2311,22 @@
         </is>
       </c>
       <c r="B68" s="9" t="n">
-        <v>471.75</v>
+        <v>488.9</v>
       </c>
       <c r="C68" s="11" t="n">
-        <v>458.2</v>
+        <v>481</v>
       </c>
       <c r="D68" s="14" t="n">
-        <v>461.8</v>
+        <v>481.5</v>
       </c>
       <c r="E68" s="6" t="n">
-        <v>461.5</v>
+        <v>482.6</v>
       </c>
       <c r="F68" s="17" t="n">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="G68" s="6" t="n">
-        <v>469.95</v>
+        <v>483.65</v>
       </c>
     </row>
     <row r="69">
@@ -2336,22 +2336,22 @@
         </is>
       </c>
       <c r="B69" s="9" t="n">
-        <v>573.05</v>
+        <v>615.6</v>
       </c>
       <c r="C69" s="11" t="n">
-        <v>565.05</v>
+        <v>597.05</v>
       </c>
       <c r="D69" s="14" t="n">
-        <v>566.3</v>
+        <v>612</v>
       </c>
       <c r="E69" s="6" t="n">
-        <v>565.85</v>
+        <v>613.85</v>
       </c>
       <c r="F69" s="17" t="n">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="G69" s="6" t="n">
-        <v>570.7</v>
+        <v>598.35</v>
       </c>
     </row>
     <row r="70">
@@ -2361,22 +2361,22 @@
         </is>
       </c>
       <c r="B70" s="9" t="n">
+        <v>224.25</v>
+      </c>
+      <c r="C70" s="11" t="n">
         <v>219.5</v>
       </c>
-      <c r="C70" s="11" t="n">
-        <v>212.75</v>
-      </c>
       <c r="D70" s="14" t="n">
-        <v>213</v>
+        <v>221.4</v>
       </c>
       <c r="E70" s="6" t="n">
-        <v>213.05</v>
+        <v>221.42</v>
       </c>
       <c r="F70" s="17" t="n">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G70" s="6" t="n">
-        <v>214.8</v>
+        <v>219.98</v>
       </c>
     </row>
     <row r="71">
@@ -2386,22 +2386,22 @@
         </is>
       </c>
       <c r="B71" s="9" t="n">
-        <v>2534.55</v>
+        <v>2585.95</v>
       </c>
       <c r="C71" s="11" t="n">
-        <v>2501</v>
+        <v>2556.4</v>
       </c>
       <c r="D71" s="14" t="n">
-        <v>2508.9</v>
+        <v>2580</v>
       </c>
       <c r="E71" s="6" t="n">
-        <v>2509.25</v>
+        <v>2577.55</v>
       </c>
       <c r="F71" s="17" t="n">
         <v>0</v>
       </c>
       <c r="G71" s="6" t="n">
-        <v>2523.75</v>
+        <v>2584.45</v>
       </c>
     </row>
     <row r="72">
@@ -2411,22 +2411,22 @@
         </is>
       </c>
       <c r="B72" s="9" t="n">
-        <v>4162.1</v>
+        <v>4297.45</v>
       </c>
       <c r="C72" s="11" t="n">
-        <v>4005.3</v>
+        <v>4260.25</v>
       </c>
       <c r="D72" s="14" t="n">
-        <v>4052</v>
+        <v>4271.4</v>
       </c>
       <c r="E72" s="6" t="n">
-        <v>4027.55</v>
+        <v>4270.4</v>
       </c>
       <c r="F72" s="17" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G72" s="6" t="n">
-        <v>4160</v>
+        <v>4265</v>
       </c>
     </row>
     <row r="73">
@@ -2436,22 +2436,22 @@
         </is>
       </c>
       <c r="B73" s="9" t="n">
-        <v>1470.55</v>
+        <v>1515.9</v>
       </c>
       <c r="C73" s="11" t="n">
-        <v>1439.25</v>
+        <v>1495.95</v>
       </c>
       <c r="D73" s="14" t="n">
-        <v>1463.45</v>
+        <v>1498.5</v>
       </c>
       <c r="E73" s="6" t="n">
-        <v>1460.25</v>
+        <v>1502.35</v>
       </c>
       <c r="F73" s="17" t="n">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="G73" s="6" t="n">
-        <v>1444.9</v>
+        <v>1498.4</v>
       </c>
     </row>
     <row r="74">
@@ -2461,22 +2461,22 @@
         </is>
       </c>
       <c r="B74" s="9" t="n">
-        <v>345.3</v>
+        <v>346.8</v>
       </c>
       <c r="C74" s="11" t="n">
-        <v>340.25</v>
+        <v>338.5</v>
       </c>
       <c r="D74" s="14" t="n">
-        <v>341.25</v>
+        <v>339.95</v>
       </c>
       <c r="E74" s="6" t="n">
-        <v>340.95</v>
+        <v>340.75</v>
       </c>
       <c r="F74" s="17" t="n">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="G74" s="6" t="n">
-        <v>344</v>
+        <v>341.4</v>
       </c>
     </row>
     <row r="75">
@@ -2486,22 +2486,22 @@
         </is>
       </c>
       <c r="B75" s="9" t="n">
-        <v>902.4</v>
+        <v>1093</v>
       </c>
       <c r="C75" s="11" t="n">
-        <v>888.2</v>
+        <v>1060.55</v>
       </c>
       <c r="D75" s="14" t="n">
-        <v>895</v>
+        <v>1070</v>
       </c>
       <c r="E75" s="6" t="n">
-        <v>894.95</v>
+        <v>1075.4</v>
       </c>
       <c r="F75" s="17" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G75" s="6" t="n">
-        <v>895.85</v>
+        <v>1063.95</v>
       </c>
     </row>
     <row r="76">
@@ -2511,22 +2511,22 @@
         </is>
       </c>
       <c r="B76" s="9" t="n">
-        <v>1354.5</v>
+        <v>1213.7</v>
       </c>
       <c r="C76" s="11" t="n">
-        <v>1276.1</v>
+        <v>1175.75</v>
       </c>
       <c r="D76" s="14" t="n">
-        <v>1286</v>
+        <v>1179.9</v>
       </c>
       <c r="E76" s="6" t="n">
-        <v>1294</v>
+        <v>1181.35</v>
       </c>
       <c r="F76" s="17" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G76" s="6" t="n">
-        <v>1333</v>
+        <v>1199.3</v>
       </c>
     </row>
     <row r="77">
@@ -2536,22 +2536,22 @@
         </is>
       </c>
       <c r="B77" s="9" t="n">
-        <v>1051.15</v>
+        <v>1059.25</v>
       </c>
       <c r="C77" s="11" t="n">
-        <v>1030.25</v>
+        <v>1036</v>
       </c>
       <c r="D77" s="14" t="n">
-        <v>1037.75</v>
+        <v>1052</v>
       </c>
       <c r="E77" s="6" t="n">
-        <v>1038.55</v>
+        <v>1052.45</v>
       </c>
       <c r="F77" s="17" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G77" s="6" t="n">
-        <v>1048.7</v>
+        <v>1038.2</v>
       </c>
     </row>
     <row r="78">
@@ -2561,22 +2561,22 @@
         </is>
       </c>
       <c r="B78" s="9" t="n">
-        <v>4002.95</v>
+        <v>4365</v>
       </c>
       <c r="C78" s="11" t="n">
-        <v>3926.1</v>
+        <v>4255.55</v>
       </c>
       <c r="D78" s="14" t="n">
-        <v>3944</v>
+        <v>4317.9</v>
       </c>
       <c r="E78" s="6" t="n">
-        <v>3939.3</v>
+        <v>4326.7</v>
       </c>
       <c r="F78" s="17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G78" s="6" t="n">
-        <v>3987.65</v>
+        <v>4259.45</v>
       </c>
     </row>
     <row r="79">
@@ -2586,22 +2586,22 @@
         </is>
       </c>
       <c r="B79" s="9" t="n">
-        <v>910</v>
+        <v>923.5</v>
       </c>
       <c r="C79" s="11" t="n">
-        <v>897.6</v>
+        <v>903.6</v>
       </c>
       <c r="D79" s="14" t="n">
-        <v>901</v>
+        <v>919</v>
       </c>
       <c r="E79" s="6" t="n">
-        <v>901.9</v>
+        <v>921.15</v>
       </c>
       <c r="F79" s="17" t="n">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="G79" s="6" t="n">
-        <v>900.85</v>
+        <v>907.5</v>
       </c>
     </row>
     <row r="80">
@@ -2611,22 +2611,22 @@
         </is>
       </c>
       <c r="B80" s="9" t="n">
-        <v>520.45</v>
+        <v>537.15</v>
       </c>
       <c r="C80" s="11" t="n">
-        <v>506.7</v>
+        <v>528.5</v>
       </c>
       <c r="D80" s="14" t="n">
-        <v>512</v>
+        <v>529.15</v>
       </c>
       <c r="E80" s="6" t="n">
-        <v>512.8</v>
+        <v>530.65</v>
       </c>
       <c r="F80" s="17" t="n">
-        <v>102</v>
+        <v>11</v>
       </c>
       <c r="G80" s="6" t="n">
-        <v>508.7</v>
+        <v>536.1</v>
       </c>
     </row>
     <row r="81">
@@ -2636,22 +2636,22 @@
         </is>
       </c>
       <c r="B81" s="9" t="n">
+        <v>1725.05</v>
+      </c>
+      <c r="C81" s="11" t="n">
         <v>1710.4</v>
       </c>
-      <c r="C81" s="11" t="n">
-        <v>1682.2</v>
-      </c>
       <c r="D81" s="14" t="n">
-        <v>1694.9</v>
+        <v>1721</v>
       </c>
       <c r="E81" s="6" t="n">
-        <v>1687.85</v>
+        <v>1717.2</v>
       </c>
       <c r="F81" s="17" t="n">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="G81" s="6" t="n">
-        <v>1710.1</v>
+        <v>1716.7</v>
       </c>
     </row>
     <row r="82">
@@ -2661,22 +2661,22 @@
         </is>
       </c>
       <c r="B82" s="9" t="n">
-        <v>2660</v>
+        <v>2776.3</v>
       </c>
       <c r="C82" s="11" t="n">
-        <v>2577.55</v>
+        <v>2716.6</v>
       </c>
       <c r="D82" s="14" t="n">
-        <v>2646</v>
+        <v>2755</v>
       </c>
       <c r="E82" s="6" t="n">
-        <v>2654.05</v>
+        <v>2750.2</v>
       </c>
       <c r="F82" s="17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G82" s="6" t="n">
-        <v>2584.15</v>
+        <v>2771.05</v>
       </c>
     </row>
     <row r="83">
@@ -2686,22 +2686,22 @@
         </is>
       </c>
       <c r="B83" s="9" t="n">
-        <v>445.5</v>
+        <v>441.5</v>
       </c>
       <c r="C83" s="11" t="n">
-        <v>439.1</v>
+        <v>434.05</v>
       </c>
       <c r="D83" s="14" t="n">
-        <v>441.55</v>
+        <v>434.6</v>
       </c>
       <c r="E83" s="6" t="n">
-        <v>440.5</v>
+        <v>434.9</v>
       </c>
       <c r="F83" s="17" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G83" s="6" t="n">
-        <v>444.9</v>
+        <v>441.2</v>
       </c>
     </row>
     <row r="84">
@@ -2711,22 +2711,22 @@
         </is>
       </c>
       <c r="B84" s="9" t="n">
-        <v>653.85</v>
+        <v>734.7</v>
       </c>
       <c r="C84" s="11" t="n">
-        <v>642.45</v>
+        <v>717.2</v>
       </c>
       <c r="D84" s="14" t="n">
-        <v>645</v>
+        <v>734</v>
       </c>
       <c r="E84" s="6" t="n">
-        <v>646.8</v>
+        <v>731.65</v>
       </c>
       <c r="F84" s="17" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G84" s="6" t="n">
-        <v>643.3</v>
+        <v>718.55</v>
       </c>
     </row>
     <row r="85">
@@ -2736,22 +2736,22 @@
         </is>
       </c>
       <c r="B85" s="9" t="n">
-        <v>4892.9</v>
+        <v>5070.2</v>
       </c>
       <c r="C85" s="11" t="n">
-        <v>4847.35</v>
+        <v>4995.25</v>
       </c>
       <c r="D85" s="14" t="n">
-        <v>4881</v>
+        <v>5025.6</v>
       </c>
       <c r="E85" s="6" t="n">
-        <v>4880.8</v>
+        <v>5032.55</v>
       </c>
       <c r="F85" s="17" t="n">
         <v>2</v>
       </c>
       <c r="G85" s="6" t="n">
-        <v>4858.25</v>
+        <v>5005</v>
       </c>
     </row>
     <row r="86">
@@ -2761,22 +2761,22 @@
         </is>
       </c>
       <c r="B86" s="9" t="n">
-        <v>4699</v>
+        <v>4870.4</v>
       </c>
       <c r="C86" s="11" t="n">
-        <v>4604</v>
+        <v>4830.2</v>
       </c>
       <c r="D86" s="14" t="n">
-        <v>4648.2</v>
+        <v>4848</v>
       </c>
       <c r="E86" s="6" t="n">
-        <v>4668.15</v>
+        <v>4845.8</v>
       </c>
       <c r="F86" s="17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G86" s="6" t="n">
-        <v>4612.1</v>
+        <v>4850.2</v>
       </c>
     </row>
     <row r="87">
@@ -2786,22 +2786,22 @@
         </is>
       </c>
       <c r="B87" s="9" t="n">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="C87" s="11" t="n">
-        <v>1586.2</v>
+        <v>1596.55</v>
       </c>
       <c r="D87" s="14" t="n">
-        <v>1598.5</v>
+        <v>1603.5</v>
       </c>
       <c r="E87" s="6" t="n">
-        <v>1601.45</v>
+        <v>1604.1</v>
       </c>
       <c r="F87" s="17" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G87" s="6" t="n">
-        <v>1589.55</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="88">
@@ -2811,22 +2811,22 @@
         </is>
       </c>
       <c r="B88" s="9" t="n">
-        <v>270.6</v>
+        <v>300</v>
       </c>
       <c r="C88" s="11" t="n">
-        <v>267.25</v>
+        <v>293.2</v>
       </c>
       <c r="D88" s="14" t="n">
-        <v>267.65</v>
+        <v>298.95</v>
       </c>
       <c r="E88" s="6" t="n">
-        <v>268.45</v>
+        <v>298.95</v>
       </c>
       <c r="F88" s="17" t="n">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="G88" s="6" t="n">
-        <v>268.55</v>
+        <v>293.85</v>
       </c>
     </row>
     <row r="89">
@@ -2836,22 +2836,22 @@
         </is>
       </c>
       <c r="B89" s="9" t="n">
-        <v>175.25</v>
+        <v>187.5</v>
       </c>
       <c r="C89" s="11" t="n">
-        <v>171.25</v>
+        <v>184.85</v>
       </c>
       <c r="D89" s="14" t="n">
-        <v>172.1</v>
+        <v>185.17</v>
       </c>
       <c r="E89" s="6" t="n">
-        <v>171.8</v>
+        <v>185.37</v>
       </c>
       <c r="F89" s="17" t="n">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="G89" s="6" t="n">
-        <v>171.5</v>
+        <v>186.8</v>
       </c>
     </row>
     <row r="90">
@@ -2861,22 +2861,22 @@
         </is>
       </c>
       <c r="B90" s="9" t="n">
-        <v>615</v>
+        <v>621.95</v>
       </c>
       <c r="C90" s="11" t="n">
-        <v>601.75</v>
+        <v>614</v>
       </c>
       <c r="D90" s="14" t="n">
-        <v>604</v>
+        <v>618.15</v>
       </c>
       <c r="E90" s="6" t="n">
-        <v>605.45</v>
+        <v>619.35</v>
       </c>
       <c r="F90" s="17" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G90" s="6" t="n">
-        <v>610.15</v>
+        <v>616.7</v>
       </c>
     </row>
     <row r="91">
@@ -2886,22 +2886,22 @@
         </is>
       </c>
       <c r="B91" s="9" t="n">
-        <v>1186.45</v>
+        <v>1278.4</v>
       </c>
       <c r="C91" s="11" t="n">
-        <v>1169.6</v>
+        <v>1258.2</v>
       </c>
       <c r="D91" s="14" t="n">
-        <v>1177.8</v>
+        <v>1270</v>
       </c>
       <c r="E91" s="6" t="n">
-        <v>1180.15</v>
+        <v>1269</v>
       </c>
       <c r="F91" s="17" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G91" s="6" t="n">
-        <v>1182</v>
+        <v>1277.65</v>
       </c>
     </row>
     <row r="92">
@@ -2911,22 +2911,22 @@
         </is>
       </c>
       <c r="B92" s="9" t="n">
-        <v>3809</v>
+        <v>3956</v>
       </c>
       <c r="C92" s="11" t="n">
-        <v>3728.7</v>
+        <v>3832.95</v>
       </c>
       <c r="D92" s="14" t="n">
-        <v>3738.95</v>
+        <v>3901.35</v>
       </c>
       <c r="E92" s="6" t="n">
-        <v>3748.7</v>
+        <v>3909.9</v>
       </c>
       <c r="F92" s="17" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G92" s="6" t="n">
-        <v>3751</v>
+        <v>3840</v>
       </c>
     </row>
     <row r="93">
@@ -2936,22 +2936,22 @@
         </is>
       </c>
       <c r="B93" s="9" t="n">
-        <v>1984.5</v>
+        <v>1981.1</v>
       </c>
       <c r="C93" s="11" t="n">
-        <v>1954.25</v>
+        <v>1953.1</v>
       </c>
       <c r="D93" s="14" t="n">
-        <v>1970.05</v>
+        <v>1957</v>
       </c>
       <c r="E93" s="6" t="n">
-        <v>1971.15</v>
+        <v>1958.2</v>
       </c>
       <c r="F93" s="17" t="n">
         <v>1</v>
       </c>
       <c r="G93" s="6" t="n">
-        <v>1971</v>
+        <v>1979.45</v>
       </c>
     </row>
     <row r="94">
@@ -2961,22 +2961,22 @@
         </is>
       </c>
       <c r="B94" s="9" t="n">
-        <v>983.25</v>
+        <v>999.65</v>
       </c>
       <c r="C94" s="11" t="n">
-        <v>963.1</v>
+        <v>983.3</v>
       </c>
       <c r="D94" s="14" t="n">
-        <v>969.8</v>
+        <v>992.9</v>
       </c>
       <c r="E94" s="6" t="n">
-        <v>971.75</v>
+        <v>993.5</v>
       </c>
       <c r="F94" s="17" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G94" s="6" t="n">
-        <v>974.95</v>
+        <v>988.6</v>
       </c>
     </row>
     <row r="95">
@@ -2986,22 +2986,22 @@
         </is>
       </c>
       <c r="B95" s="9" t="n">
-        <v>1305.15</v>
+        <v>1479</v>
       </c>
       <c r="C95" s="11" t="n">
-        <v>1287.05</v>
+        <v>1455</v>
       </c>
       <c r="D95" s="14" t="n">
-        <v>1304.9</v>
+        <v>1459.5</v>
       </c>
       <c r="E95" s="6" t="n">
-        <v>1303.8</v>
+        <v>1465.85</v>
       </c>
       <c r="F95" s="17" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G95" s="6" t="n">
-        <v>1290.4</v>
+        <v>1457.6</v>
       </c>
     </row>
     <row r="96">
@@ -3011,22 +3011,22 @@
         </is>
       </c>
       <c r="B96" s="9" t="n">
-        <v>2419</v>
+        <v>2428.9</v>
       </c>
       <c r="C96" s="11" t="n">
-        <v>2358.05</v>
+        <v>2395.55</v>
       </c>
       <c r="D96" s="14" t="n">
-        <v>2375</v>
+        <v>2406</v>
       </c>
       <c r="E96" s="6" t="n">
-        <v>2364.25</v>
+        <v>2408.85</v>
       </c>
       <c r="F96" s="17" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G96" s="6" t="n">
-        <v>2391.8</v>
+        <v>2426.75</v>
       </c>
     </row>
     <row r="97">
@@ -3036,22 +3036,22 @@
         </is>
       </c>
       <c r="B97" s="9" t="n">
-        <v>1753.35</v>
+        <v>1800.7</v>
       </c>
       <c r="C97" s="11" t="n">
-        <v>1729.15</v>
+        <v>1764.25</v>
       </c>
       <c r="D97" s="14" t="n">
-        <v>1739</v>
+        <v>1768</v>
       </c>
       <c r="E97" s="6" t="n">
-        <v>1738.9</v>
+        <v>1770</v>
       </c>
       <c r="F97" s="17" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G97" s="6" t="n">
-        <v>1737.45</v>
+        <v>1796.05</v>
       </c>
     </row>
     <row r="98">
@@ -3061,22 +3061,22 @@
         </is>
       </c>
       <c r="B98" s="9" t="n">
-        <v>616</v>
+        <v>656</v>
       </c>
       <c r="C98" s="11" t="n">
-        <v>604.45</v>
+        <v>642.25</v>
       </c>
       <c r="D98" s="14" t="n">
-        <v>609.3</v>
+        <v>646.95</v>
       </c>
       <c r="E98" s="6" t="n">
-        <v>611.1</v>
+        <v>646.5</v>
       </c>
       <c r="F98" s="17" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G98" s="6" t="n">
-        <v>608</v>
+        <v>649.9</v>
       </c>
     </row>
     <row r="99">
@@ -3086,22 +3086,22 @@
         </is>
       </c>
       <c r="B99" s="9" t="n">
-        <v>5984.9</v>
+        <v>6302</v>
       </c>
       <c r="C99" s="11" t="n">
-        <v>5907.5</v>
+        <v>6172</v>
       </c>
       <c r="D99" s="14" t="n">
-        <v>5939.4</v>
+        <v>6250</v>
       </c>
       <c r="E99" s="6" t="n">
-        <v>5921.2</v>
+        <v>6242.95</v>
       </c>
       <c r="F99" s="17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G99" s="6" t="n">
-        <v>5949.05</v>
+        <v>6220.75</v>
       </c>
     </row>
     <row r="100">
@@ -3111,22 +3111,22 @@
         </is>
       </c>
       <c r="B100" s="9" t="n">
-        <v>3348.95</v>
+        <v>3606</v>
       </c>
       <c r="C100" s="11" t="n">
-        <v>3300.05</v>
+        <v>3533</v>
       </c>
       <c r="D100" s="14" t="n">
-        <v>3305</v>
+        <v>3539.15</v>
       </c>
       <c r="E100" s="6" t="n">
-        <v>3314.2</v>
+        <v>3545.25</v>
       </c>
       <c r="F100" s="17" t="n">
         <v>1</v>
       </c>
       <c r="G100" s="6" t="n">
-        <v>3326.5</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="101">
@@ -3136,22 +3136,22 @@
         </is>
       </c>
       <c r="B101" s="9" t="n">
-        <v>260.15</v>
+        <v>268.7</v>
       </c>
       <c r="C101" s="11" t="n">
-        <v>254.35</v>
+        <v>263.1</v>
       </c>
       <c r="D101" s="14" t="n">
-        <v>257.9</v>
+        <v>266.85</v>
       </c>
       <c r="E101" s="6" t="n">
-        <v>258.15</v>
+        <v>267.4</v>
       </c>
       <c r="F101" s="17" t="n">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="G101" s="6" t="n">
-        <v>258.7</v>
+        <v>263.5</v>
       </c>
     </row>
     <row r="102">
@@ -3161,22 +3161,22 @@
         </is>
       </c>
       <c r="B102" s="9" t="n">
-        <v>366.35</v>
+        <v>369.45</v>
       </c>
       <c r="C102" s="11" t="n">
-        <v>361.5</v>
+        <v>366.1</v>
       </c>
       <c r="D102" s="14" t="n">
-        <v>365</v>
+        <v>368.5</v>
       </c>
       <c r="E102" s="6" t="n">
-        <v>364.6</v>
+        <v>368.45</v>
       </c>
       <c r="F102" s="17" t="n">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="G102" s="6" t="n">
-        <v>362.5</v>
+        <v>366.5</v>
       </c>
     </row>
     <row r="103">
@@ -3186,22 +3186,22 @@
         </is>
       </c>
       <c r="B103" s="9" t="n">
-        <v>1848.75</v>
+        <v>1937</v>
       </c>
       <c r="C103" s="11" t="n">
-        <v>1820</v>
+        <v>1893</v>
       </c>
       <c r="D103" s="14" t="n">
-        <v>1822.3</v>
+        <v>1902.4</v>
       </c>
       <c r="E103" s="6" t="n">
-        <v>1832.75</v>
+        <v>1907.8</v>
       </c>
       <c r="F103" s="17" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G103" s="6" t="n">
-        <v>1831.15</v>
+        <v>1922.1</v>
       </c>
     </row>
     <row r="104">
@@ -3211,22 +3211,22 @@
         </is>
       </c>
       <c r="B104" s="9" t="n">
-        <v>838.2</v>
+        <v>899.9</v>
       </c>
       <c r="C104" s="11" t="n">
-        <v>814.9</v>
+        <v>878.35</v>
       </c>
       <c r="D104" s="14" t="n">
-        <v>828.9</v>
+        <v>881.1</v>
       </c>
       <c r="E104" s="6" t="n">
-        <v>830.1</v>
+        <v>882.5</v>
       </c>
       <c r="F104" s="17" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G104" s="6" t="n">
-        <v>816.8</v>
+        <v>880.55</v>
       </c>
     </row>
     <row r="105">
@@ -3236,22 +3236,22 @@
         </is>
       </c>
       <c r="B105" s="9" t="n">
-        <v>3673.95</v>
+        <v>3800</v>
       </c>
       <c r="C105" s="11" t="n">
-        <v>3622.75</v>
+        <v>3736.6</v>
       </c>
       <c r="D105" s="14" t="n">
-        <v>3648</v>
+        <v>3769.7</v>
       </c>
       <c r="E105" s="6" t="n">
-        <v>3649.85</v>
+        <v>3772.8</v>
       </c>
       <c r="F105" s="17" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G105" s="6" t="n">
-        <v>3648.9</v>
+        <v>3746.6</v>
       </c>
     </row>
     <row r="106">
@@ -3261,22 +3261,22 @@
         </is>
       </c>
       <c r="B106" s="9" t="n">
-        <v>299.85</v>
+        <v>327.85</v>
       </c>
       <c r="C106" s="11" t="n">
-        <v>295.75</v>
+        <v>321.55</v>
       </c>
       <c r="D106" s="14" t="n">
-        <v>298</v>
+        <v>323</v>
       </c>
       <c r="E106" s="6" t="n">
-        <v>297.15</v>
+        <v>323.9</v>
       </c>
       <c r="F106" s="17" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G106" s="6" t="n">
-        <v>297.95</v>
+        <v>322.15</v>
       </c>
     </row>
     <row r="107">
@@ -3286,22 +3286,22 @@
         </is>
       </c>
       <c r="B107" s="9" t="n">
-        <v>3045</v>
+        <v>3124.85</v>
       </c>
       <c r="C107" s="11" t="n">
-        <v>3015</v>
+        <v>3091.6</v>
       </c>
       <c r="D107" s="14" t="n">
-        <v>3025</v>
+        <v>3109.5</v>
       </c>
       <c r="E107" s="6" t="n">
-        <v>3037</v>
+        <v>3109.8</v>
       </c>
       <c r="F107" s="17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G107" s="6" t="n">
-        <v>3036.3</v>
+        <v>3105.7</v>
       </c>
     </row>
     <row r="108">
@@ -3311,22 +3311,22 @@
         </is>
       </c>
       <c r="B108" s="9" t="n">
-        <v>6778.95</v>
+        <v>7140</v>
       </c>
       <c r="C108" s="11" t="n">
-        <v>6675</v>
+        <v>7000.25</v>
       </c>
       <c r="D108" s="14" t="n">
-        <v>6737</v>
+        <v>7080</v>
       </c>
       <c r="E108" s="6" t="n">
-        <v>6747.75</v>
+        <v>7079.9</v>
       </c>
       <c r="F108" s="17" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G108" s="6" t="n">
-        <v>6697.6</v>
+        <v>7044.3</v>
       </c>
     </row>
     <row r="109">
@@ -3336,22 +3336,22 @@
         </is>
       </c>
       <c r="B109" s="9" t="n">
-        <v>318.7</v>
+        <v>323.25</v>
       </c>
       <c r="C109" s="11" t="n">
-        <v>311.15</v>
+        <v>319.35</v>
       </c>
       <c r="D109" s="14" t="n">
-        <v>316.85</v>
+        <v>321.5</v>
       </c>
       <c r="E109" s="6" t="n">
-        <v>317.7</v>
+        <v>321.5</v>
       </c>
       <c r="F109" s="17" t="n">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="G109" s="6" t="n">
-        <v>311.55</v>
+        <v>320.65</v>
       </c>
     </row>
     <row r="110">
@@ -3361,22 +3361,22 @@
         </is>
       </c>
       <c r="B110" s="9" t="n">
-        <v>171.65</v>
+        <v>167.48</v>
       </c>
       <c r="C110" s="11" t="n">
-        <v>166.3</v>
+        <v>164.1</v>
       </c>
       <c r="D110" s="14" t="n">
-        <v>167.75</v>
+        <v>164.47</v>
       </c>
       <c r="E110" s="6" t="n">
-        <v>167.7</v>
+        <v>164.54</v>
       </c>
       <c r="F110" s="17" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G110" s="6" t="n">
-        <v>167.05</v>
+        <v>166.21</v>
       </c>
     </row>
     <row r="111">
@@ -3386,22 +3386,22 @@
         </is>
       </c>
       <c r="B111" s="9" t="n">
-        <v>762.3</v>
+        <v>878.3</v>
       </c>
       <c r="C111" s="11" t="n">
-        <v>748.25</v>
+        <v>853.05</v>
       </c>
       <c r="D111" s="14" t="n">
-        <v>750</v>
+        <v>866.5</v>
       </c>
       <c r="E111" s="6" t="n">
-        <v>752.35</v>
+        <v>869.35</v>
       </c>
       <c r="F111" s="17" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G111" s="6" t="n">
-        <v>758.1</v>
+        <v>855.05</v>
       </c>
     </row>
     <row r="112">
@@ -3411,22 +3411,22 @@
         </is>
       </c>
       <c r="B112" s="9" t="n">
-        <v>252.5</v>
+        <v>261.4</v>
       </c>
       <c r="C112" s="11" t="n">
-        <v>247.8</v>
+        <v>256.85</v>
       </c>
       <c r="D112" s="14" t="n">
-        <v>247.9</v>
+        <v>257.45</v>
       </c>
       <c r="E112" s="6" t="n">
-        <v>248.45</v>
+        <v>257.63</v>
       </c>
       <c r="F112" s="17" t="n">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="G112" s="6" t="n">
-        <v>250</v>
+        <v>258.83</v>
       </c>
     </row>
     <row r="113">
@@ -3436,22 +3436,22 @@
         </is>
       </c>
       <c r="B113" s="9" t="n">
-        <v>582.75</v>
+        <v>536.9</v>
       </c>
       <c r="C113" s="11" t="n">
-        <v>567</v>
+        <v>519.5</v>
       </c>
       <c r="D113" s="14" t="n">
-        <v>567.25</v>
+        <v>531</v>
       </c>
       <c r="E113" s="6" t="n">
-        <v>568.75</v>
+        <v>532.65</v>
       </c>
       <c r="F113" s="17" t="n">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="G113" s="6" t="n">
-        <v>572.1</v>
+        <v>520</v>
       </c>
     </row>
     <row r="114">
@@ -3461,22 +3461,22 @@
         </is>
       </c>
       <c r="B114" s="9" t="n">
-        <v>705</v>
+        <v>733.25</v>
       </c>
       <c r="C114" s="11" t="n">
-        <v>696.1</v>
+        <v>720.8</v>
       </c>
       <c r="D114" s="14" t="n">
-        <v>697.3</v>
+        <v>728.5</v>
       </c>
       <c r="E114" s="6" t="n">
-        <v>697.3</v>
+        <v>728.35</v>
       </c>
       <c r="F114" s="17" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G114" s="6" t="n">
-        <v>702.85</v>
+        <v>723.35</v>
       </c>
     </row>
     <row r="115">
@@ -3486,22 +3486,22 @@
         </is>
       </c>
       <c r="B115" s="9" t="n">
-        <v>1429.95</v>
+        <v>1473.75</v>
       </c>
       <c r="C115" s="11" t="n">
-        <v>1406.6</v>
+        <v>1445</v>
       </c>
       <c r="D115" s="14" t="n">
-        <v>1414</v>
+        <v>1467</v>
       </c>
       <c r="E115" s="6" t="n">
-        <v>1412.8</v>
+        <v>1469.9</v>
       </c>
       <c r="F115" s="17" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G115" s="6" t="n">
-        <v>1426.55</v>
+        <v>1450.1</v>
       </c>
     </row>
     <row r="116">
@@ -3511,22 +3511,22 @@
         </is>
       </c>
       <c r="B116" s="9" t="n">
-        <v>7123.6</v>
+        <v>7913.05</v>
       </c>
       <c r="C116" s="11" t="n">
-        <v>7000</v>
+        <v>7420</v>
       </c>
       <c r="D116" s="14" t="n">
-        <v>7005</v>
+        <v>7786</v>
       </c>
       <c r="E116" s="6" t="n">
-        <v>7016.8</v>
+        <v>7790.2</v>
       </c>
       <c r="F116" s="17" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="G116" s="6" t="n">
-        <v>7092.75</v>
+        <v>7440.8</v>
       </c>
     </row>
     <row r="117">
@@ -3536,22 +3536,22 @@
         </is>
       </c>
       <c r="B117" s="9" t="n">
-        <v>2281.85</v>
+        <v>2413.95</v>
       </c>
       <c r="C117" s="11" t="n">
-        <v>2235</v>
+        <v>2390.05</v>
       </c>
       <c r="D117" s="14" t="n">
-        <v>2239</v>
+        <v>2396.65</v>
       </c>
       <c r="E117" s="6" t="n">
-        <v>2239</v>
+        <v>2402</v>
       </c>
       <c r="F117" s="17" t="n">
         <v>4</v>
       </c>
       <c r="G117" s="6" t="n">
-        <v>2278.2</v>
+        <v>2401.95</v>
       </c>
     </row>
     <row r="118">
@@ -3561,22 +3561,22 @@
         </is>
       </c>
       <c r="B118" s="9" t="n">
-        <v>851.6</v>
+        <v>990</v>
       </c>
       <c r="C118" s="11" t="n">
-        <v>828.65</v>
+        <v>944.3</v>
       </c>
       <c r="D118" s="14" t="n">
-        <v>841</v>
+        <v>975</v>
       </c>
       <c r="E118" s="6" t="n">
-        <v>845.1</v>
+        <v>978.7</v>
       </c>
       <c r="F118" s="17" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G118" s="6" t="n">
-        <v>830</v>
+        <v>945.45</v>
       </c>
     </row>
     <row r="119">
@@ -3586,22 +3586,22 @@
         </is>
       </c>
       <c r="B119" s="9" t="n">
-        <v>1495</v>
+        <v>1518</v>
       </c>
       <c r="C119" s="11" t="n">
-        <v>1465.65</v>
+        <v>1510</v>
       </c>
       <c r="D119" s="14" t="n">
-        <v>1473</v>
+        <v>1515</v>
       </c>
       <c r="E119" s="6" t="n">
-        <v>1478.95</v>
+        <v>1516</v>
       </c>
       <c r="F119" s="17" t="n">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G119" s="6" t="n">
-        <v>1468.95</v>
+        <v>1511.25</v>
       </c>
     </row>
     <row r="120">
@@ -3611,22 +3611,22 @@
         </is>
       </c>
       <c r="B120" s="9" t="n">
-        <v>693.25</v>
+        <v>709.3</v>
       </c>
       <c r="C120" s="11" t="n">
-        <v>680.95</v>
+        <v>701</v>
       </c>
       <c r="D120" s="14" t="n">
-        <v>689.6</v>
+        <v>706</v>
       </c>
       <c r="E120" s="6" t="n">
-        <v>690.65</v>
+        <v>707.05</v>
       </c>
       <c r="F120" s="17" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G120" s="6" t="n">
-        <v>687.45</v>
+        <v>702</v>
       </c>
     </row>
     <row r="121">
@@ -3636,22 +3636,22 @@
         </is>
       </c>
       <c r="B121" s="9" t="n">
-        <v>1808.8</v>
+        <v>1880.95</v>
       </c>
       <c r="C121" s="11" t="n">
-        <v>1786.8</v>
+        <v>1860.55</v>
       </c>
       <c r="D121" s="14" t="n">
-        <v>1786.8</v>
+        <v>1866.05</v>
       </c>
       <c r="E121" s="6" t="n">
-        <v>1790.45</v>
+        <v>1868.4</v>
       </c>
       <c r="F121" s="17" t="n">
         <v>2</v>
       </c>
       <c r="G121" s="6" t="n">
-        <v>1799.95</v>
+        <v>1872.5</v>
       </c>
     </row>
     <row r="122">
@@ -3661,22 +3661,22 @@
         </is>
       </c>
       <c r="B122" s="9" t="n">
-        <v>950.5</v>
+        <v>997.25</v>
       </c>
       <c r="C122" s="11" t="n">
-        <v>939.8</v>
+        <v>981.4</v>
       </c>
       <c r="D122" s="14" t="n">
-        <v>943.5</v>
+        <v>992</v>
       </c>
       <c r="E122" s="6" t="n">
-        <v>943.6</v>
+        <v>993.4</v>
       </c>
       <c r="F122" s="17" t="n">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="G122" s="6" t="n">
-        <v>941.85</v>
+        <v>982.3</v>
       </c>
     </row>
     <row r="123">
@@ -3686,22 +3686,22 @@
         </is>
       </c>
       <c r="B123" s="9" t="n">
-        <v>1307.35</v>
+        <v>1379.2</v>
       </c>
       <c r="C123" s="11" t="n">
-        <v>1284.1</v>
+        <v>1364.1</v>
       </c>
       <c r="D123" s="14" t="n">
-        <v>1285.3</v>
+        <v>1372</v>
       </c>
       <c r="E123" s="6" t="n">
-        <v>1286.45</v>
+        <v>1371.45</v>
       </c>
       <c r="F123" s="17" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G123" s="6" t="n">
-        <v>1305.25</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="124">
@@ -3711,22 +3711,22 @@
         </is>
       </c>
       <c r="B124" s="9" t="n">
-        <v>2735</v>
+        <v>2919.3</v>
       </c>
       <c r="C124" s="11" t="n">
-        <v>2648</v>
+        <v>2860</v>
       </c>
       <c r="D124" s="14" t="n">
-        <v>2724</v>
+        <v>2863.15</v>
       </c>
       <c r="E124" s="6" t="n">
-        <v>2714.2</v>
+        <v>2882.1</v>
       </c>
       <c r="F124" s="17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G124" s="6" t="n">
-        <v>2680</v>
+        <v>2880.15</v>
       </c>
     </row>
     <row r="125">
@@ -3736,22 +3736,22 @@
         </is>
       </c>
       <c r="B125" s="9" t="n">
-        <v>1472.05</v>
+        <v>1604</v>
       </c>
       <c r="C125" s="11" t="n">
-        <v>1424</v>
+        <v>1576</v>
       </c>
       <c r="D125" s="14" t="n">
-        <v>1439</v>
+        <v>1602</v>
       </c>
       <c r="E125" s="6" t="n">
-        <v>1456.2</v>
+        <v>1599.1</v>
       </c>
       <c r="F125" s="17" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="G125" s="6" t="n">
-        <v>1465.75</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="126">
@@ -3761,22 +3761,22 @@
         </is>
       </c>
       <c r="B126" s="9" t="n">
-        <v>4719.5</v>
+        <v>5294</v>
       </c>
       <c r="C126" s="11" t="n">
-        <v>4646.5</v>
+        <v>5137.15</v>
       </c>
       <c r="D126" s="14" t="n">
-        <v>4662</v>
+        <v>5255</v>
       </c>
       <c r="E126" s="6" t="n">
-        <v>4672.05</v>
+        <v>5245.55</v>
       </c>
       <c r="F126" s="17" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G126" s="6" t="n">
-        <v>4684.15</v>
+        <v>5160.75</v>
       </c>
     </row>
     <row r="127">
@@ -3786,22 +3786,22 @@
         </is>
       </c>
       <c r="B127" s="9" t="n">
-        <v>2265.1</v>
+        <v>2519</v>
       </c>
       <c r="C127" s="11" t="n">
-        <v>2219.25</v>
+        <v>2441.65</v>
       </c>
       <c r="D127" s="14" t="n">
-        <v>2253.95</v>
+        <v>2496.3</v>
       </c>
       <c r="E127" s="6" t="n">
-        <v>2253.85</v>
+        <v>2503.85</v>
       </c>
       <c r="F127" s="17" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G127" s="6" t="n">
-        <v>2226.25</v>
+        <v>2449.6</v>
       </c>
     </row>
     <row r="128">
@@ -3811,22 +3811,22 @@
         </is>
       </c>
       <c r="B128" s="9" t="n">
-        <v>1883</v>
+        <v>2125.8</v>
       </c>
       <c r="C128" s="11" t="n">
-        <v>1851.6</v>
+        <v>2097.35</v>
       </c>
       <c r="D128" s="14" t="n">
-        <v>1869.95</v>
+        <v>2108</v>
       </c>
       <c r="E128" s="6" t="n">
-        <v>1877.75</v>
+        <v>2109.1</v>
       </c>
       <c r="F128" s="17" t="n">
         <v>1</v>
       </c>
       <c r="G128" s="6" t="n">
-        <v>1865.3</v>
+        <v>2120.3</v>
       </c>
     </row>
     <row r="129">
@@ -3836,22 +3836,22 @@
         </is>
       </c>
       <c r="B129" s="9" t="n">
-        <v>10169.95</v>
+        <v>11271</v>
       </c>
       <c r="C129" s="11" t="n">
-        <v>9961</v>
+        <v>11167.6</v>
       </c>
       <c r="D129" s="14" t="n">
-        <v>10031</v>
+        <v>11250</v>
       </c>
       <c r="E129" s="6" t="n">
-        <v>10023.4</v>
+        <v>11242.8</v>
       </c>
       <c r="F129" s="17" t="n">
         <v>3</v>
       </c>
       <c r="G129" s="6" t="n">
-        <v>10141.95</v>
+        <v>11175</v>
       </c>
     </row>
     <row r="130">
@@ -3861,22 +3861,22 @@
         </is>
       </c>
       <c r="B130" s="9" t="n">
-        <v>522.6</v>
+        <v>556.45</v>
       </c>
       <c r="C130" s="11" t="n">
-        <v>515.75</v>
+        <v>549.7</v>
       </c>
       <c r="D130" s="14" t="n">
-        <v>517</v>
+        <v>549.75</v>
       </c>
       <c r="E130" s="6" t="n">
-        <v>517.25</v>
+        <v>551.7</v>
       </c>
       <c r="F130" s="17" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G130" s="6" t="n">
-        <v>519.1</v>
+        <v>554.5</v>
       </c>
     </row>
     <row r="131">
@@ -3886,22 +3886,22 @@
         </is>
       </c>
       <c r="B131" s="9" t="n">
-        <v>462.3</v>
+        <v>451.9</v>
       </c>
       <c r="C131" s="11" t="n">
-        <v>451.15</v>
+        <v>442</v>
       </c>
       <c r="D131" s="14" t="n">
-        <v>453.9</v>
+        <v>446.7</v>
       </c>
       <c r="E131" s="6" t="n">
-        <v>454.25</v>
+        <v>447.6</v>
       </c>
       <c r="F131" s="17" t="n">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="G131" s="6" t="n">
-        <v>457.1</v>
+        <v>442.85</v>
       </c>
     </row>
     <row r="132">
@@ -3911,22 +3911,22 @@
         </is>
       </c>
       <c r="B132" s="9" t="n">
-        <v>1402.8</v>
+        <v>1511.95</v>
       </c>
       <c r="C132" s="11" t="n">
-        <v>1372</v>
+        <v>1470.05</v>
       </c>
       <c r="D132" s="14" t="n">
-        <v>1372.5</v>
+        <v>1496</v>
       </c>
       <c r="E132" s="6" t="n">
-        <v>1375.3</v>
+        <v>1498.5</v>
       </c>
       <c r="F132" s="17" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G132" s="6" t="n">
-        <v>1390.4</v>
+        <v>1477.05</v>
       </c>
     </row>
     <row r="133">
@@ -3936,22 +3936,22 @@
         </is>
       </c>
       <c r="B133" s="9" t="n">
-        <v>154.5</v>
+        <v>165.2</v>
       </c>
       <c r="C133" s="11" t="n">
-        <v>150.3</v>
+        <v>162.6</v>
       </c>
       <c r="D133" s="14" t="n">
-        <v>150.9</v>
+        <v>164.26</v>
       </c>
       <c r="E133" s="6" t="n">
-        <v>150.95</v>
+        <v>163.98</v>
       </c>
       <c r="F133" s="17" t="n">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="G133" s="6" t="n">
-        <v>151</v>
+        <v>163.9</v>
       </c>
     </row>
     <row r="134" ht="15.75" customHeight="1" thickBot="1">
@@ -3961,22 +3961,22 @@
         </is>
       </c>
       <c r="B134" s="19" t="n">
-        <v>1049.55</v>
+        <v>1111.8</v>
       </c>
       <c r="C134" s="12" t="n">
-        <v>1035.9</v>
+        <v>1093.9</v>
       </c>
       <c r="D134" s="15" t="n">
-        <v>1044.2</v>
+        <v>1110.5</v>
       </c>
       <c r="E134" s="7" t="n">
-        <v>1044.75</v>
+        <v>1109.55</v>
       </c>
       <c r="F134" s="18" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G134" s="7" t="n">
-        <v>1038.55</v>
+        <v>1097.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added IGL, ESCORTS, VEDL to 30 min, modified fo.py to work with new md file format
</commit_message>
<xml_diff>
--- a/algo high low.xlsx
+++ b/algo high low.xlsx
@@ -610,8 +610,10 @@
   </sheetPr>
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K94" sqref="K94"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="735" topLeftCell="A104" activePane="bottomLeft" state="split"/>
+      <selection activeCell="B16" sqref="B16:B52"/>
+      <selection pane="bottomLeft" activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -661,22 +663,22 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>679.4</v>
+        <v>720.35</v>
       </c>
       <c r="C2" s="10" t="n">
-        <v>671.45</v>
+        <v>703.8</v>
       </c>
       <c r="D2" s="13" t="n">
-        <v>675.5</v>
+        <v>708.1</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>675.75</v>
+        <v>708.4</v>
       </c>
       <c r="F2" s="16" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>673.95</v>
+        <v>719.2</v>
       </c>
     </row>
     <row r="3">
@@ -686,22 +688,22 @@
         </is>
       </c>
       <c r="B3" s="9" t="n">
-        <v>9145</v>
+        <v>8680.200000000001</v>
       </c>
       <c r="C3" s="11" t="n">
-        <v>8491.049999999999</v>
+        <v>8492</v>
       </c>
       <c r="D3" s="14" t="n">
-        <v>9031</v>
+        <v>8568.4</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>9020</v>
+        <v>8559.549999999999</v>
       </c>
       <c r="F3" s="17" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G3" s="6" t="n">
-        <v>8496.950000000001</v>
+        <v>8651.75</v>
       </c>
     </row>
     <row r="4">
@@ -711,22 +713,22 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>243.3</v>
+        <v>235.45</v>
       </c>
       <c r="C4" s="11" t="n">
-        <v>238.69</v>
+        <v>230.42</v>
       </c>
       <c r="D4" s="14" t="n">
-        <v>239.55</v>
+        <v>230.9</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>239.96</v>
+        <v>230.93</v>
       </c>
       <c r="F4" s="17" t="n">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="G4" s="6" t="n">
-        <v>239.9</v>
+        <v>235.25</v>
       </c>
     </row>
     <row r="5">
@@ -736,22 +738,22 @@
         </is>
       </c>
       <c r="B5" s="9" t="n">
-        <v>332.85</v>
+        <v>328.6</v>
       </c>
       <c r="C5" s="11" t="n">
-        <v>326.75</v>
+        <v>321.3</v>
       </c>
       <c r="D5" s="14" t="n">
-        <v>328.95</v>
+        <v>323</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>328.6</v>
+        <v>322.25</v>
       </c>
       <c r="F5" s="17" t="n">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>327.2</v>
+        <v>328.3</v>
       </c>
     </row>
     <row r="6">
@@ -761,22 +763,22 @@
         </is>
       </c>
       <c r="B6" s="9" t="n">
-        <v>3275</v>
+        <v>3143.55</v>
       </c>
       <c r="C6" s="11" t="n">
-        <v>3225</v>
+        <v>3075</v>
       </c>
       <c r="D6" s="14" t="n">
-        <v>3269</v>
+        <v>3112</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>3261.75</v>
+        <v>3113.6</v>
       </c>
       <c r="F6" s="17" t="n">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>3227.8</v>
+        <v>3139.4</v>
       </c>
     </row>
     <row r="7">
@@ -786,22 +788,22 @@
         </is>
       </c>
       <c r="B7" s="9" t="n">
-        <v>1442</v>
+        <v>1490.3</v>
       </c>
       <c r="C7" s="11" t="n">
-        <v>1395.45</v>
+        <v>1469</v>
       </c>
       <c r="D7" s="14" t="n">
-        <v>1429.7</v>
+        <v>1477</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>1430.7</v>
+        <v>1475.3</v>
       </c>
       <c r="F7" s="17" t="n">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>1397.45</v>
+        <v>1488.55</v>
       </c>
     </row>
     <row r="8">
@@ -811,22 +813,22 @@
         </is>
       </c>
       <c r="B8" s="9" t="n">
-        <v>5114.95</v>
+        <v>5243.7</v>
       </c>
       <c r="C8" s="11" t="n">
-        <v>5056.75</v>
+        <v>5063</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>5095.1</v>
+        <v>5230</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>5101.95</v>
+        <v>5221.85</v>
       </c>
       <c r="F8" s="17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v>5077.95</v>
+        <v>5106.7</v>
       </c>
     </row>
     <row r="9">
@@ -836,22 +838,22 @@
         </is>
       </c>
       <c r="B9" s="9" t="n">
-        <v>681.7</v>
+        <v>685.65</v>
       </c>
       <c r="C9" s="11" t="n">
-        <v>672.2</v>
+        <v>679.2</v>
       </c>
       <c r="D9" s="14" t="n">
-        <v>673.6</v>
+        <v>682.8</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>677.2</v>
+        <v>683.55</v>
       </c>
       <c r="F9" s="17" t="n">
-        <v>156</v>
+        <v>20</v>
       </c>
       <c r="G9" s="6" t="n">
-        <v>675.4</v>
+        <v>684</v>
       </c>
     </row>
     <row r="10">
@@ -861,22 +863,22 @@
         </is>
       </c>
       <c r="B10" s="9" t="n">
-        <v>6218</v>
+        <v>6349</v>
       </c>
       <c r="C10" s="11" t="n">
-        <v>6175</v>
+        <v>6292.8</v>
       </c>
       <c r="D10" s="14" t="n">
-        <v>6181.3</v>
+        <v>6300.75</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>6207.6</v>
+        <v>6317.45</v>
       </c>
       <c r="F10" s="17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10" s="6" t="n">
-        <v>6183.9</v>
+        <v>6344.35</v>
       </c>
     </row>
     <row r="11">
@@ -886,22 +888,22 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>478</v>
+        <v>533.5</v>
       </c>
       <c r="C11" s="11" t="n">
-        <v>472.1</v>
+        <v>520</v>
       </c>
       <c r="D11" s="14" t="n">
-        <v>476.6</v>
+        <v>523.7</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>476.45</v>
+        <v>522.35</v>
       </c>
       <c r="F11" s="17" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G11" s="6" t="n">
-        <v>474.4</v>
+        <v>527.95</v>
       </c>
     </row>
     <row r="12">
@@ -911,22 +913,22 @@
         </is>
       </c>
       <c r="B12" s="9" t="n">
-        <v>242.69</v>
+        <v>231.05</v>
       </c>
       <c r="C12" s="11" t="n">
-        <v>235.89</v>
+        <v>224.85</v>
       </c>
       <c r="D12" s="14" t="n">
-        <v>239.05</v>
+        <v>226.35</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>239.84</v>
+        <v>226.05</v>
       </c>
       <c r="F12" s="17" t="n">
-        <v>170</v>
+        <v>117</v>
       </c>
       <c r="G12" s="6" t="n">
-        <v>237.69</v>
+        <v>231.04</v>
       </c>
     </row>
     <row r="13">
@@ -936,22 +938,22 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>2291.95</v>
+        <v>2411.8</v>
       </c>
       <c r="C13" s="11" t="n">
-        <v>2252.95</v>
+        <v>2307.85</v>
       </c>
       <c r="D13" s="14" t="n">
-        <v>2271</v>
+        <v>2342.4</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>2269.45</v>
+        <v>2330.45</v>
       </c>
       <c r="F13" s="17" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G13" s="6" t="n">
-        <v>2254.15</v>
+        <v>2407.45</v>
       </c>
     </row>
     <row r="14">
@@ -961,22 +963,22 @@
         </is>
       </c>
       <c r="B14" s="9" t="n">
-        <v>6280.95</v>
+        <v>6840</v>
       </c>
       <c r="C14" s="11" t="n">
-        <v>6200</v>
+        <v>6710.3</v>
       </c>
       <c r="D14" s="14" t="n">
-        <v>6225.05</v>
+        <v>6800</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>6261.65</v>
+        <v>6824.5</v>
       </c>
       <c r="F14" s="17" t="n">
         <v>0</v>
       </c>
       <c r="G14" s="6" t="n">
-        <v>6213.8</v>
+        <v>6722.25</v>
       </c>
     </row>
     <row r="15">
@@ -986,22 +988,22 @@
         </is>
       </c>
       <c r="B15" s="9" t="n">
-        <v>669.95</v>
+        <v>665</v>
       </c>
       <c r="C15" s="11" t="n">
-        <v>658</v>
+        <v>639.1</v>
       </c>
       <c r="D15" s="14" t="n">
-        <v>661.2</v>
+        <v>645</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>661.25</v>
+        <v>642.7</v>
       </c>
       <c r="F15" s="17" t="n">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="G15" s="6" t="n">
-        <v>669.7</v>
+        <v>664.75</v>
       </c>
     </row>
     <row r="16">
@@ -1011,22 +1013,22 @@
         </is>
       </c>
       <c r="B16" s="9" t="n">
-        <v>1264.65</v>
+        <v>1320</v>
       </c>
       <c r="C16" s="11" t="n">
-        <v>1238.1</v>
+        <v>1285.75</v>
       </c>
       <c r="D16" s="14" t="n">
-        <v>1258.4</v>
+        <v>1308.45</v>
       </c>
       <c r="E16" s="6" t="n">
-        <v>1259</v>
+        <v>1305.4</v>
       </c>
       <c r="F16" s="17" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G16" s="6" t="n">
-        <v>1241.9</v>
+        <v>1317.35</v>
       </c>
     </row>
     <row r="17">
@@ -1036,22 +1038,22 @@
         </is>
       </c>
       <c r="B17" s="9" t="n">
-        <v>1596</v>
+        <v>1574.5</v>
       </c>
       <c r="C17" s="11" t="n">
-        <v>1575.35</v>
+        <v>1562</v>
       </c>
       <c r="D17" s="14" t="n">
-        <v>1587.05</v>
+        <v>1568</v>
       </c>
       <c r="E17" s="6" t="n">
-        <v>1591.75</v>
+        <v>1570.1</v>
       </c>
       <c r="F17" s="17" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G17" s="6" t="n">
-        <v>1582.6</v>
+        <v>1573.35</v>
       </c>
     </row>
     <row r="18">
@@ -1061,22 +1063,22 @@
         </is>
       </c>
       <c r="B18" s="9" t="n">
-        <v>7370</v>
+        <v>7108</v>
       </c>
       <c r="C18" s="11" t="n">
-        <v>7247</v>
+        <v>7047</v>
       </c>
       <c r="D18" s="14" t="n">
-        <v>7340.5</v>
+        <v>7099</v>
       </c>
       <c r="E18" s="6" t="n">
-        <v>7341.55</v>
+        <v>7098.25</v>
       </c>
       <c r="F18" s="17" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G18" s="6" t="n">
-        <v>7300</v>
+        <v>7100</v>
       </c>
     </row>
     <row r="19">
@@ -1086,22 +1088,22 @@
         </is>
       </c>
       <c r="B19" s="9" t="n">
-        <v>3256.65</v>
+        <v>3210</v>
       </c>
       <c r="C19" s="11" t="n">
-        <v>3178</v>
+        <v>3110</v>
       </c>
       <c r="D19" s="14" t="n">
-        <v>3245</v>
+        <v>3175.25</v>
       </c>
       <c r="E19" s="6" t="n">
-        <v>3240.6</v>
+        <v>3165.85</v>
       </c>
       <c r="F19" s="17" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G19" s="6" t="n">
-        <v>3183.55</v>
+        <v>3190.95</v>
       </c>
     </row>
     <row r="20">
@@ -1111,22 +1113,22 @@
         </is>
       </c>
       <c r="B20" s="9" t="n">
-        <v>443.05</v>
+        <v>431.7</v>
       </c>
       <c r="C20" s="11" t="n">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="D20" s="14" t="n">
-        <v>430</v>
+        <v>424.9</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>430.2</v>
+        <v>423.75</v>
       </c>
       <c r="F20" s="17" t="n">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="G20" s="6" t="n">
-        <v>442.95</v>
+        <v>425.25</v>
       </c>
     </row>
     <row r="21">
@@ -1136,22 +1138,22 @@
         </is>
       </c>
       <c r="B21" s="9" t="n">
-        <v>195.9</v>
+        <v>205.22</v>
       </c>
       <c r="C21" s="11" t="n">
-        <v>193.53</v>
+        <v>201.5</v>
       </c>
       <c r="D21" s="14" t="n">
-        <v>194.15</v>
+        <v>204</v>
       </c>
       <c r="E21" s="6" t="n">
-        <v>194.34</v>
+        <v>204.47</v>
       </c>
       <c r="F21" s="17" t="n">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="G21" s="6" t="n">
-        <v>195.6</v>
+        <v>202.85</v>
       </c>
     </row>
     <row r="22">
@@ -1161,22 +1163,22 @@
         </is>
       </c>
       <c r="B22" s="9" t="n">
-        <v>287.5</v>
+        <v>266.8</v>
       </c>
       <c r="C22" s="11" t="n">
-        <v>281.75</v>
+        <v>261.55</v>
       </c>
       <c r="D22" s="14" t="n">
-        <v>286</v>
+        <v>263</v>
       </c>
       <c r="E22" s="6" t="n">
-        <v>286.25</v>
+        <v>262.35</v>
       </c>
       <c r="F22" s="17" t="n">
-        <v>139</v>
+        <v>228</v>
       </c>
       <c r="G22" s="6" t="n">
-        <v>282.35</v>
+        <v>263.55</v>
       </c>
     </row>
     <row r="23">
@@ -1186,22 +1188,22 @@
         </is>
       </c>
       <c r="B23" s="9" t="n">
-        <v>1466.1</v>
+        <v>1536</v>
       </c>
       <c r="C23" s="11" t="n">
-        <v>1448</v>
+        <v>1490</v>
       </c>
       <c r="D23" s="14" t="n">
-        <v>1452.7</v>
+        <v>1532</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>1451.8</v>
+        <v>1531.9</v>
       </c>
       <c r="F23" s="17" t="n">
         <v>4</v>
       </c>
       <c r="G23" s="6" t="n">
-        <v>1463.75</v>
+        <v>1508.35</v>
       </c>
     </row>
     <row r="24">
@@ -1211,22 +1213,22 @@
         </is>
       </c>
       <c r="B24" s="9" t="n">
-        <v>310.5</v>
+        <v>335.8</v>
       </c>
       <c r="C24" s="11" t="n">
-        <v>301.5</v>
+        <v>327.7</v>
       </c>
       <c r="D24" s="14" t="n">
-        <v>309.7</v>
+        <v>335.5</v>
       </c>
       <c r="E24" s="6" t="n">
-        <v>309.6</v>
+        <v>334.6</v>
       </c>
       <c r="F24" s="17" t="n">
-        <v>673</v>
+        <v>709</v>
       </c>
       <c r="G24" s="6" t="n">
-        <v>302</v>
+        <v>328.85</v>
       </c>
     </row>
     <row r="25">
@@ -1236,22 +1238,22 @@
         </is>
       </c>
       <c r="B25" s="9" t="n">
-        <v>1739.45</v>
+        <v>1693.25</v>
       </c>
       <c r="C25" s="11" t="n">
-        <v>1627</v>
+        <v>1646.25</v>
       </c>
       <c r="D25" s="14" t="n">
-        <v>1714.2</v>
+        <v>1675.1</v>
       </c>
       <c r="E25" s="6" t="n">
-        <v>1717.3</v>
+        <v>1674.1</v>
       </c>
       <c r="F25" s="17" t="n">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G25" s="6" t="n">
-        <v>1629.25</v>
+        <v>1686.35</v>
       </c>
     </row>
     <row r="26">
@@ -1261,22 +1263,22 @@
         </is>
       </c>
       <c r="B26" s="9" t="n">
-        <v>339.7</v>
+        <v>373.85</v>
       </c>
       <c r="C26" s="11" t="n">
-        <v>334.15</v>
+        <v>365.4</v>
       </c>
       <c r="D26" s="14" t="n">
-        <v>334.25</v>
+        <v>366.5</v>
       </c>
       <c r="E26" s="6" t="n">
-        <v>334.8</v>
+        <v>366.65</v>
       </c>
       <c r="F26" s="17" t="n">
         <v>50</v>
       </c>
       <c r="G26" s="6" t="n">
-        <v>334.65</v>
+        <v>369.8</v>
       </c>
     </row>
     <row r="27">
@@ -1286,22 +1288,22 @@
         </is>
       </c>
       <c r="B27" s="9" t="n">
-        <v>5432.3</v>
+        <v>5615.95</v>
       </c>
       <c r="C27" s="11" t="n">
-        <v>5375.6</v>
+        <v>5534.05</v>
       </c>
       <c r="D27" s="14" t="n">
-        <v>5391.8</v>
+        <v>5556.45</v>
       </c>
       <c r="E27" s="6" t="n">
-        <v>5393.65</v>
+        <v>5568.55</v>
       </c>
       <c r="F27" s="17" t="n">
         <v>1</v>
       </c>
       <c r="G27" s="6" t="n">
-        <v>5421.85</v>
+        <v>5550</v>
       </c>
     </row>
     <row r="28">
@@ -1311,22 +1313,22 @@
         </is>
       </c>
       <c r="B28" s="9" t="n">
-        <v>685</v>
+        <v>721</v>
       </c>
       <c r="C28" s="11" t="n">
-        <v>670.2</v>
+        <v>702</v>
       </c>
       <c r="D28" s="14" t="n">
-        <v>678</v>
+        <v>708</v>
       </c>
       <c r="E28" s="6" t="n">
-        <v>677.95</v>
+        <v>707.75</v>
       </c>
       <c r="F28" s="17" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G28" s="6" t="n">
-        <v>671.2</v>
+        <v>717</v>
       </c>
     </row>
     <row r="29">
@@ -1336,22 +1338,22 @@
         </is>
       </c>
       <c r="B29" s="9" t="n">
-        <v>120.99</v>
+        <v>118.08</v>
       </c>
       <c r="C29" s="11" t="n">
-        <v>119.3</v>
+        <v>114.66</v>
       </c>
       <c r="D29" s="14" t="n">
-        <v>120.9</v>
+        <v>114.99</v>
       </c>
       <c r="E29" s="6" t="n">
-        <v>120.81</v>
+        <v>114.89</v>
       </c>
       <c r="F29" s="17" t="n">
-        <v>325</v>
+        <v>340</v>
       </c>
       <c r="G29" s="6" t="n">
-        <v>119.57</v>
+        <v>117.13</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -1361,22 +1363,22 @@
         </is>
       </c>
       <c r="B30" s="9" t="n">
-        <v>837.45</v>
+        <v>898</v>
       </c>
       <c r="C30" s="11" t="n">
-        <v>816.5</v>
+        <v>875</v>
       </c>
       <c r="D30" s="14" t="n">
-        <v>832.55</v>
+        <v>887.45</v>
       </c>
       <c r="E30" s="6" t="n">
-        <v>834.9</v>
+        <v>886.85</v>
       </c>
       <c r="F30" s="17" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G30" s="6" t="n">
-        <v>816.75</v>
+        <v>887.4</v>
       </c>
     </row>
     <row r="31">
@@ -1386,22 +1388,22 @@
         </is>
       </c>
       <c r="B31" s="9" t="n">
-        <v>436</v>
+        <v>535.85</v>
       </c>
       <c r="C31" s="11" t="n">
-        <v>426</v>
+        <v>519</v>
       </c>
       <c r="D31" s="14" t="n">
-        <v>427</v>
+        <v>535.3</v>
       </c>
       <c r="E31" s="6" t="n">
-        <v>426.7</v>
+        <v>534.3</v>
       </c>
       <c r="F31" s="17" t="n">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="G31" s="6" t="n">
-        <v>431.75</v>
+        <v>524</v>
       </c>
     </row>
     <row r="32">
@@ -1411,22 +1413,22 @@
         </is>
       </c>
       <c r="B32" s="9" t="n">
-        <v>1455.85</v>
+        <v>1430.9</v>
       </c>
       <c r="C32" s="11" t="n">
-        <v>1438.3</v>
+        <v>1395</v>
       </c>
       <c r="D32" s="14" t="n">
-        <v>1442.5</v>
+        <v>1416.5</v>
       </c>
       <c r="E32" s="6" t="n">
-        <v>1447</v>
+        <v>1412.15</v>
       </c>
       <c r="F32" s="17" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G32" s="6" t="n">
-        <v>1446.45</v>
+        <v>1427.9</v>
       </c>
     </row>
     <row r="33">
@@ -1436,22 +1438,22 @@
         </is>
       </c>
       <c r="B33" s="9" t="n">
-        <v>1567</v>
+        <v>1520</v>
       </c>
       <c r="C33" s="11" t="n">
-        <v>1549.05</v>
+        <v>1483.2</v>
       </c>
       <c r="D33" s="14" t="n">
-        <v>1566</v>
+        <v>1491</v>
       </c>
       <c r="E33" s="6" t="n">
-        <v>1564.75</v>
+        <v>1487.05</v>
       </c>
       <c r="F33" s="17" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G33" s="6" t="n">
-        <v>1551.3</v>
+        <v>1517.7</v>
       </c>
     </row>
     <row r="34">
@@ -1461,22 +1463,22 @@
         </is>
       </c>
       <c r="B34" s="9" t="n">
-        <v>5230.45</v>
+        <v>5975.35</v>
       </c>
       <c r="C34" s="11" t="n">
-        <v>5178.7</v>
+        <v>5752.65</v>
       </c>
       <c r="D34" s="14" t="n">
-        <v>5192.9</v>
+        <v>5868</v>
       </c>
       <c r="E34" s="6" t="n">
-        <v>5201.75</v>
+        <v>5855.45</v>
       </c>
       <c r="F34" s="17" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G34" s="6" t="n">
-        <v>5200.7</v>
+        <v>5913</v>
       </c>
     </row>
     <row r="35">
@@ -1486,22 +1488,22 @@
         </is>
       </c>
       <c r="B35" s="9" t="n">
-        <v>1146.65</v>
+        <v>1064</v>
       </c>
       <c r="C35" s="11" t="n">
-        <v>1124.5</v>
+        <v>1033.8</v>
       </c>
       <c r="D35" s="14" t="n">
-        <v>1134.8</v>
+        <v>1043.75</v>
       </c>
       <c r="E35" s="6" t="n">
-        <v>1139.85</v>
+        <v>1043.15</v>
       </c>
       <c r="F35" s="17" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G35" s="6" t="n">
-        <v>1134.05</v>
+        <v>1059.4</v>
       </c>
     </row>
     <row r="36">
@@ -1511,22 +1513,22 @@
         </is>
       </c>
       <c r="B36" s="9" t="n">
-        <v>1534.75</v>
+        <v>1637.5</v>
       </c>
       <c r="C36" s="11" t="n">
-        <v>1482.1</v>
+        <v>1582.3</v>
       </c>
       <c r="D36" s="14" t="n">
-        <v>1505.5</v>
+        <v>1610.5</v>
       </c>
       <c r="E36" s="6" t="n">
-        <v>1508.8</v>
+        <v>1615.75</v>
       </c>
       <c r="F36" s="17" t="n">
         <v>5</v>
       </c>
       <c r="G36" s="6" t="n">
-        <v>1485.7</v>
+        <v>1595.6</v>
       </c>
     </row>
     <row r="37">
@@ -1536,22 +1538,22 @@
         </is>
       </c>
       <c r="B37" s="9" t="n">
-        <v>429</v>
+        <v>423.45</v>
       </c>
       <c r="C37" s="11" t="n">
-        <v>421.2</v>
+        <v>411.7</v>
       </c>
       <c r="D37" s="14" t="n">
-        <v>425.1</v>
+        <v>421</v>
       </c>
       <c r="E37" s="6" t="n">
-        <v>426.55</v>
+        <v>420.6</v>
       </c>
       <c r="F37" s="17" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G37" s="6" t="n">
-        <v>421.75</v>
+        <v>412.8</v>
       </c>
     </row>
     <row r="38">
@@ -1561,22 +1563,22 @@
         </is>
       </c>
       <c r="B38" s="9" t="n">
-        <v>3871.8</v>
+        <v>4149.55</v>
       </c>
       <c r="C38" s="11" t="n">
-        <v>3723.9</v>
+        <v>3960.8</v>
       </c>
       <c r="D38" s="14" t="n">
-        <v>3817</v>
+        <v>4000.6</v>
       </c>
       <c r="E38" s="6" t="n">
-        <v>3825.6</v>
+        <v>4000.85</v>
       </c>
       <c r="F38" s="17" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G38" s="6" t="n">
-        <v>3734.35</v>
+        <v>4145</v>
       </c>
     </row>
     <row r="39">
@@ -1586,22 +1588,22 @@
         </is>
       </c>
       <c r="B39" s="9" t="n">
-        <v>616</v>
+        <v>633</v>
       </c>
       <c r="C39" s="11" t="n">
-        <v>607.5</v>
+        <v>613.45</v>
       </c>
       <c r="D39" s="14" t="n">
-        <v>609</v>
+        <v>624.3</v>
       </c>
       <c r="E39" s="6" t="n">
-        <v>608.65</v>
+        <v>623.45</v>
       </c>
       <c r="F39" s="17" t="n">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="G39" s="6" t="n">
-        <v>614.05</v>
+        <v>616.2</v>
       </c>
     </row>
     <row r="40">
@@ -1611,22 +1613,22 @@
         </is>
       </c>
       <c r="B40" s="9" t="n">
-        <v>1888.5</v>
+        <v>1861.25</v>
       </c>
       <c r="C40" s="11" t="n">
-        <v>1863.55</v>
+        <v>1843.6</v>
       </c>
       <c r="D40" s="14" t="n">
-        <v>1886.9</v>
+        <v>1858</v>
       </c>
       <c r="E40" s="6" t="n">
-        <v>1882.35</v>
+        <v>1855.85</v>
       </c>
       <c r="F40" s="17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G40" s="6" t="n">
-        <v>1870.95</v>
+        <v>1857.4</v>
       </c>
     </row>
     <row r="41">
@@ -1636,22 +1638,22 @@
         </is>
       </c>
       <c r="B41" s="9" t="n">
-        <v>609.8</v>
+        <v>774.95</v>
       </c>
       <c r="C41" s="11" t="n">
-        <v>579.3</v>
+        <v>747.55</v>
       </c>
       <c r="D41" s="14" t="n">
-        <v>595</v>
+        <v>768.1</v>
       </c>
       <c r="E41" s="6" t="n">
-        <v>593.6</v>
+        <v>770.7</v>
       </c>
       <c r="F41" s="17" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G41" s="6" t="n">
-        <v>597.3</v>
+        <v>751.6</v>
       </c>
     </row>
     <row r="42">
@@ -1661,22 +1663,22 @@
         </is>
       </c>
       <c r="B42" s="9" t="n">
-        <v>2441.4</v>
+        <v>2726.1</v>
       </c>
       <c r="C42" s="11" t="n">
-        <v>2400.35</v>
+        <v>2670.05</v>
       </c>
       <c r="D42" s="14" t="n">
-        <v>2416.6</v>
+        <v>2695</v>
       </c>
       <c r="E42" s="6" t="n">
-        <v>2413.7</v>
+        <v>2694.15</v>
       </c>
       <c r="F42" s="17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G42" s="6" t="n">
-        <v>2406.9</v>
+        <v>2699.8</v>
       </c>
     </row>
     <row r="43">
@@ -1686,22 +1688,22 @@
         </is>
       </c>
       <c r="B43" s="9" t="n">
-        <v>138.8</v>
+        <v>147.95</v>
       </c>
       <c r="C43" s="11" t="n">
-        <v>134.32</v>
+        <v>133.75</v>
       </c>
       <c r="D43" s="14" t="n">
-        <v>136</v>
+        <v>144.97</v>
       </c>
       <c r="E43" s="6" t="n">
-        <v>136.16</v>
+        <v>144.68</v>
       </c>
       <c r="F43" s="17" t="n">
-        <v>98</v>
+        <v>152</v>
       </c>
       <c r="G43" s="6" t="n">
-        <v>134.33</v>
+        <v>135.15</v>
       </c>
     </row>
     <row r="44">
@@ -1711,22 +1713,22 @@
         </is>
       </c>
       <c r="B44" s="9" t="n">
-        <v>4609.65</v>
+        <v>4579.95</v>
       </c>
       <c r="C44" s="11" t="n">
-        <v>4559.1</v>
+        <v>4445</v>
       </c>
       <c r="D44" s="14" t="n">
-        <v>4585</v>
+        <v>4480</v>
       </c>
       <c r="E44" s="6" t="n">
-        <v>4588.6</v>
+        <v>4464.2</v>
       </c>
       <c r="F44" s="17" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G44" s="6" t="n">
-        <v>4605</v>
+        <v>4569.35</v>
       </c>
     </row>
     <row r="45">
@@ -1736,22 +1738,22 @@
         </is>
       </c>
       <c r="B45" s="9" t="n">
-        <v>11458.9</v>
+        <v>12638.95</v>
       </c>
       <c r="C45" s="11" t="n">
-        <v>10864.85</v>
+        <v>12381.2</v>
       </c>
       <c r="D45" s="14" t="n">
-        <v>11240</v>
+        <v>12498</v>
       </c>
       <c r="E45" s="6" t="n">
-        <v>11242.85</v>
+        <v>12482.5</v>
       </c>
       <c r="F45" s="17" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G45" s="6" t="n">
-        <v>10896</v>
+        <v>12528.5</v>
       </c>
     </row>
     <row r="46">
@@ -1761,22 +1763,22 @@
         </is>
       </c>
       <c r="B46" s="9" t="n">
-        <v>883.65</v>
+        <v>839.1</v>
       </c>
       <c r="C46" s="11" t="n">
-        <v>871.9</v>
+        <v>828.05</v>
       </c>
       <c r="D46" s="14" t="n">
-        <v>877.25</v>
+        <v>834.2</v>
       </c>
       <c r="E46" s="6" t="n">
-        <v>878.6</v>
+        <v>835.7</v>
       </c>
       <c r="F46" s="17" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G46" s="6" t="n">
-        <v>872.85</v>
+        <v>838.5</v>
       </c>
     </row>
     <row r="47">
@@ -1786,22 +1788,22 @@
         </is>
       </c>
       <c r="B47" s="9" t="n">
-        <v>6090.5</v>
+        <v>6564</v>
       </c>
       <c r="C47" s="11" t="n">
-        <v>6035.1</v>
+        <v>6486</v>
       </c>
       <c r="D47" s="14" t="n">
-        <v>6085</v>
+        <v>6550</v>
       </c>
       <c r="E47" s="6" t="n">
-        <v>6085.25</v>
+        <v>6534.15</v>
       </c>
       <c r="F47" s="17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G47" s="6" t="n">
-        <v>6062.5</v>
+        <v>6535.95</v>
       </c>
     </row>
     <row r="48">
@@ -1811,22 +1813,22 @@
         </is>
       </c>
       <c r="B48" s="9" t="n">
-        <v>4309.95</v>
+        <v>4124.9</v>
       </c>
       <c r="C48" s="11" t="n">
-        <v>4209</v>
+        <v>4024</v>
       </c>
       <c r="D48" s="14" t="n">
-        <v>4290</v>
+        <v>4095</v>
       </c>
       <c r="E48" s="6" t="n">
-        <v>4292.1</v>
+        <v>4105.05</v>
       </c>
       <c r="F48" s="17" t="n">
         <v>2</v>
       </c>
       <c r="G48" s="6" t="n">
-        <v>4224.95</v>
+        <v>4099.75</v>
       </c>
     </row>
     <row r="49">
@@ -1836,22 +1838,22 @@
         </is>
       </c>
       <c r="B49" s="9" t="n">
-        <v>547.9</v>
+        <v>574</v>
       </c>
       <c r="C49" s="11" t="n">
-        <v>539.2</v>
+        <v>565.1</v>
       </c>
       <c r="D49" s="14" t="n">
-        <v>542.2</v>
+        <v>572.2</v>
       </c>
       <c r="E49" s="6" t="n">
-        <v>542.25</v>
+        <v>571.45</v>
       </c>
       <c r="F49" s="17" t="n">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="G49" s="6" t="n">
-        <v>540.85</v>
+        <v>571.25</v>
       </c>
     </row>
     <row r="50">
@@ -1861,22 +1863,22 @@
         </is>
       </c>
       <c r="B50" s="9" t="n">
-        <v>1240.75</v>
+        <v>1366.95</v>
       </c>
       <c r="C50" s="11" t="n">
-        <v>1221.8</v>
+        <v>1343</v>
       </c>
       <c r="D50" s="14" t="n">
-        <v>1236</v>
+        <v>1351.6</v>
       </c>
       <c r="E50" s="6" t="n">
-        <v>1237.15</v>
+        <v>1356.35</v>
       </c>
       <c r="F50" s="17" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G50" s="6" t="n">
-        <v>1229</v>
+        <v>1352.95</v>
       </c>
     </row>
     <row r="51">
@@ -1886,22 +1888,22 @@
         </is>
       </c>
       <c r="B51" s="9" t="n">
-        <v>871</v>
+        <v>914.95</v>
       </c>
       <c r="C51" s="11" t="n">
-        <v>850</v>
+        <v>880.05</v>
       </c>
       <c r="D51" s="14" t="n">
-        <v>854.3</v>
+        <v>888</v>
       </c>
       <c r="E51" s="6" t="n">
-        <v>853.35</v>
+        <v>886.35</v>
       </c>
       <c r="F51" s="17" t="n">
         <v>0</v>
       </c>
       <c r="G51" s="6" t="n">
-        <v>856.05</v>
+        <v>904.5</v>
       </c>
     </row>
     <row r="52">
@@ -1911,22 +1913,22 @@
         </is>
       </c>
       <c r="B52" s="9" t="n">
-        <v>688.15</v>
+        <v>722.4</v>
       </c>
       <c r="C52" s="11" t="n">
-        <v>680.8</v>
+        <v>706.5</v>
       </c>
       <c r="D52" s="14" t="n">
-        <v>683.05</v>
+        <v>714</v>
       </c>
       <c r="E52" s="6" t="n">
-        <v>683.8</v>
+        <v>713.95</v>
       </c>
       <c r="F52" s="17" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G52" s="6" t="n">
-        <v>685.05</v>
+        <v>714.35</v>
       </c>
     </row>
     <row r="53">
@@ -1936,22 +1938,22 @@
         </is>
       </c>
       <c r="B53" s="9" t="n">
-        <v>1412</v>
+        <v>1439.7</v>
       </c>
       <c r="C53" s="11" t="n">
-        <v>1389.8</v>
+        <v>1379.25</v>
       </c>
       <c r="D53" s="14" t="n">
-        <v>1391.5</v>
+        <v>1425</v>
       </c>
       <c r="E53" s="6" t="n">
-        <v>1392.95</v>
+        <v>1426</v>
       </c>
       <c r="F53" s="17" t="n">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="G53" s="6" t="n">
-        <v>1410.3</v>
+        <v>1384.5</v>
       </c>
     </row>
     <row r="54">
@@ -1961,22 +1963,22 @@
         </is>
       </c>
       <c r="B54" s="9" t="n">
-        <v>3052</v>
+        <v>3322.95</v>
       </c>
       <c r="C54" s="11" t="n">
-        <v>2975.65</v>
+        <v>3254.8</v>
       </c>
       <c r="D54" s="14" t="n">
-        <v>3005</v>
+        <v>3305.35</v>
       </c>
       <c r="E54" s="6" t="n">
-        <v>2998.5</v>
+        <v>3312</v>
       </c>
       <c r="F54" s="17" t="n">
         <v>6</v>
       </c>
       <c r="G54" s="6" t="n">
-        <v>3030.6</v>
+        <v>3305</v>
       </c>
     </row>
     <row r="55">
@@ -1986,22 +1988,22 @@
         </is>
       </c>
       <c r="B55" s="9" t="n">
-        <v>465.9</v>
+        <v>525.5</v>
       </c>
       <c r="C55" s="11" t="n">
-        <v>460.15</v>
+        <v>517</v>
       </c>
       <c r="D55" s="14" t="n">
-        <v>461</v>
+        <v>521.45</v>
       </c>
       <c r="E55" s="6" t="n">
-        <v>461.75</v>
+        <v>518.6</v>
       </c>
       <c r="F55" s="17" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G55" s="6" t="n">
-        <v>461.35</v>
+        <v>523.75</v>
       </c>
     </row>
     <row r="56">
@@ -2011,22 +2013,22 @@
         </is>
       </c>
       <c r="B56" s="9" t="n">
-        <v>2523.7</v>
+        <v>2748</v>
       </c>
       <c r="C56" s="11" t="n">
-        <v>2463.4</v>
+        <v>2713.85</v>
       </c>
       <c r="D56" s="14" t="n">
-        <v>2469</v>
+        <v>2734.4</v>
       </c>
       <c r="E56" s="6" t="n">
-        <v>2471.2</v>
+        <v>2742.15</v>
       </c>
       <c r="F56" s="17" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G56" s="6" t="n">
-        <v>2486.95</v>
+        <v>2737.3</v>
       </c>
     </row>
     <row r="57">
@@ -2036,22 +2038,22 @@
         </is>
       </c>
       <c r="B57" s="9" t="n">
-        <v>640.65</v>
+        <v>655.55</v>
       </c>
       <c r="C57" s="11" t="n">
-        <v>626.85</v>
+        <v>639</v>
       </c>
       <c r="D57" s="14" t="n">
-        <v>629.95</v>
+        <v>652</v>
       </c>
       <c r="E57" s="6" t="n">
-        <v>632.05</v>
+        <v>653.35</v>
       </c>
       <c r="F57" s="17" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G57" s="6" t="n">
-        <v>636.5</v>
+        <v>647.65</v>
       </c>
     </row>
     <row r="58">
@@ -2061,22 +2063,22 @@
         </is>
       </c>
       <c r="B58" s="9" t="n">
-        <v>5260</v>
+        <v>5662.45</v>
       </c>
       <c r="C58" s="11" t="n">
-        <v>5103.75</v>
+        <v>5561.2</v>
       </c>
       <c r="D58" s="14" t="n">
-        <v>5188</v>
+        <v>5628</v>
       </c>
       <c r="E58" s="6" t="n">
-        <v>5200.55</v>
+        <v>5621.95</v>
       </c>
       <c r="F58" s="17" t="n">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="G58" s="6" t="n">
-        <v>5125</v>
+        <v>5618.1</v>
       </c>
     </row>
     <row r="59">
@@ -2086,22 +2088,22 @@
         </is>
       </c>
       <c r="B59" s="9" t="n">
-        <v>1871.95</v>
+        <v>1899</v>
       </c>
       <c r="C59" s="11" t="n">
-        <v>1835.3</v>
+        <v>1866.65</v>
       </c>
       <c r="D59" s="14" t="n">
-        <v>1838.55</v>
+        <v>1886.85</v>
       </c>
       <c r="E59" s="6" t="n">
-        <v>1839.5</v>
+        <v>1886.2</v>
       </c>
       <c r="F59" s="17" t="n">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="G59" s="6" t="n">
-        <v>1846.2</v>
+        <v>1892.45</v>
       </c>
     </row>
     <row r="60">
@@ -2111,22 +2113,22 @@
         </is>
       </c>
       <c r="B60" s="9" t="n">
-        <v>1439.75</v>
+        <v>1540</v>
       </c>
       <c r="C60" s="11" t="n">
-        <v>1424.4</v>
+        <v>1506.2</v>
       </c>
       <c r="D60" s="14" t="n">
-        <v>1431.2</v>
+        <v>1537.95</v>
       </c>
       <c r="E60" s="6" t="n">
-        <v>1431.05</v>
+        <v>1533.4</v>
       </c>
       <c r="F60" s="17" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G60" s="6" t="n">
-        <v>1435.55</v>
+        <v>1524.6</v>
       </c>
     </row>
     <row r="61">
@@ -2136,22 +2138,22 @@
         </is>
       </c>
       <c r="B61" s="9" t="n">
-        <v>4025</v>
+        <v>4250.3</v>
       </c>
       <c r="C61" s="11" t="n">
-        <v>3955.05</v>
+        <v>4103.65</v>
       </c>
       <c r="D61" s="14" t="n">
-        <v>4019</v>
+        <v>4169.45</v>
       </c>
       <c r="E61" s="6" t="n">
-        <v>4014.4</v>
+        <v>4159.05</v>
       </c>
       <c r="F61" s="17" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G61" s="6" t="n">
-        <v>3999.9</v>
+        <v>4245.1</v>
       </c>
     </row>
     <row r="62">
@@ -2161,22 +2163,22 @@
         </is>
       </c>
       <c r="B62" s="9" t="n">
-        <v>601.8</v>
+        <v>622.05</v>
       </c>
       <c r="C62" s="11" t="n">
-        <v>594.05</v>
+        <v>608.6</v>
       </c>
       <c r="D62" s="14" t="n">
-        <v>596.85</v>
+        <v>621</v>
       </c>
       <c r="E62" s="6" t="n">
-        <v>598.35</v>
+        <v>620.9</v>
       </c>
       <c r="F62" s="17" t="n">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G62" s="6" t="n">
-        <v>595.5</v>
+        <v>611.45</v>
       </c>
     </row>
     <row r="63">
@@ -2186,22 +2188,22 @@
         </is>
       </c>
       <c r="B63" s="9" t="n">
-        <v>686.5</v>
+        <v>705.9</v>
       </c>
       <c r="C63" s="11" t="n">
-        <v>678.9</v>
+        <v>691.65</v>
       </c>
       <c r="D63" s="14" t="n">
-        <v>682.1</v>
+        <v>697.6</v>
       </c>
       <c r="E63" s="6" t="n">
-        <v>683.6</v>
+        <v>697.2</v>
       </c>
       <c r="F63" s="17" t="n">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="G63" s="6" t="n">
-        <v>679.9</v>
+        <v>700.8</v>
       </c>
     </row>
     <row r="64">
@@ -2211,22 +2213,22 @@
         </is>
       </c>
       <c r="B64" s="9" t="n">
-        <v>341.6</v>
+        <v>343.75</v>
       </c>
       <c r="C64" s="11" t="n">
-        <v>333.2</v>
+        <v>331.15</v>
       </c>
       <c r="D64" s="14" t="n">
-        <v>336.6</v>
+        <v>342.85</v>
       </c>
       <c r="E64" s="6" t="n">
-        <v>336.9</v>
+        <v>342.25</v>
       </c>
       <c r="F64" s="17" t="n">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="G64" s="6" t="n">
-        <v>334.9</v>
+        <v>331.9</v>
       </c>
     </row>
     <row r="65">
@@ -2236,22 +2238,22 @@
         </is>
       </c>
       <c r="B65" s="9" t="n">
-        <v>1766.95</v>
+        <v>1853.6</v>
       </c>
       <c r="C65" s="11" t="n">
-        <v>1698.65</v>
+        <v>1831.5</v>
       </c>
       <c r="D65" s="14" t="n">
-        <v>1730.2</v>
+        <v>1841.4</v>
       </c>
       <c r="E65" s="6" t="n">
-        <v>1730.9</v>
+        <v>1838.95</v>
       </c>
       <c r="F65" s="17" t="n">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="G65" s="6" t="n">
-        <v>1715.7</v>
+        <v>1847.75</v>
       </c>
     </row>
     <row r="66">
@@ -2261,22 +2263,22 @@
         </is>
       </c>
       <c r="B66" s="9" t="n">
-        <v>622</v>
+        <v>642.5</v>
       </c>
       <c r="C66" s="11" t="n">
-        <v>598.55</v>
+        <v>628.6</v>
       </c>
       <c r="D66" s="14" t="n">
-        <v>612.85</v>
+        <v>639</v>
       </c>
       <c r="E66" s="6" t="n">
-        <v>613.7</v>
+        <v>636.35</v>
       </c>
       <c r="F66" s="17" t="n">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="G66" s="6" t="n">
-        <v>602.8</v>
+        <v>638.1</v>
       </c>
     </row>
     <row r="67">
@@ -2286,22 +2288,22 @@
         </is>
       </c>
       <c r="B67" s="9" t="n">
-        <v>182.55</v>
+        <v>185.25</v>
       </c>
       <c r="C67" s="11" t="n">
-        <v>176</v>
+        <v>180.36</v>
       </c>
       <c r="D67" s="14" t="n">
-        <v>179.35</v>
+        <v>182</v>
       </c>
       <c r="E67" s="6" t="n">
-        <v>179.67</v>
+        <v>181.65</v>
       </c>
       <c r="F67" s="17" t="n">
-        <v>205</v>
+        <v>87</v>
       </c>
       <c r="G67" s="6" t="n">
-        <v>176.29</v>
+        <v>184.75</v>
       </c>
     </row>
     <row r="68">
@@ -2311,22 +2313,22 @@
         </is>
       </c>
       <c r="B68" s="9" t="n">
-        <v>488.9</v>
+        <v>526.25</v>
       </c>
       <c r="C68" s="11" t="n">
-        <v>481</v>
+        <v>516.85</v>
       </c>
       <c r="D68" s="14" t="n">
-        <v>481.5</v>
+        <v>525.5</v>
       </c>
       <c r="E68" s="6" t="n">
-        <v>482.6</v>
+        <v>525</v>
       </c>
       <c r="F68" s="17" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G68" s="6" t="n">
-        <v>483.65</v>
+        <v>521.75</v>
       </c>
     </row>
     <row r="69">
@@ -2336,22 +2338,22 @@
         </is>
       </c>
       <c r="B69" s="9" t="n">
-        <v>615.6</v>
+        <v>614.8</v>
       </c>
       <c r="C69" s="11" t="n">
-        <v>597.05</v>
+        <v>604.1</v>
       </c>
       <c r="D69" s="14" t="n">
-        <v>612</v>
+        <v>608.55</v>
       </c>
       <c r="E69" s="6" t="n">
-        <v>613.85</v>
+        <v>608.7</v>
       </c>
       <c r="F69" s="17" t="n">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="G69" s="6" t="n">
-        <v>598.35</v>
+        <v>613.65</v>
       </c>
     </row>
     <row r="70">
@@ -2361,22 +2363,22 @@
         </is>
       </c>
       <c r="B70" s="9" t="n">
-        <v>224.25</v>
+        <v>282.7</v>
       </c>
       <c r="C70" s="11" t="n">
-        <v>219.5</v>
+        <v>276.05</v>
       </c>
       <c r="D70" s="14" t="n">
-        <v>221.4</v>
+        <v>276.75</v>
       </c>
       <c r="E70" s="6" t="n">
-        <v>221.42</v>
+        <v>277</v>
       </c>
       <c r="F70" s="17" t="n">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="G70" s="6" t="n">
-        <v>219.98</v>
+        <v>281.9</v>
       </c>
     </row>
     <row r="71">
@@ -2386,22 +2388,22 @@
         </is>
       </c>
       <c r="B71" s="9" t="n">
-        <v>2585.95</v>
+        <v>2692</v>
       </c>
       <c r="C71" s="11" t="n">
-        <v>2556.4</v>
+        <v>2631.45</v>
       </c>
       <c r="D71" s="14" t="n">
-        <v>2580</v>
+        <v>2653.35</v>
       </c>
       <c r="E71" s="6" t="n">
-        <v>2577.55</v>
+        <v>2646.4</v>
       </c>
       <c r="F71" s="17" t="n">
         <v>0</v>
       </c>
       <c r="G71" s="6" t="n">
-        <v>2584.45</v>
+        <v>2686.45</v>
       </c>
     </row>
     <row r="72">
@@ -2411,22 +2413,22 @@
         </is>
       </c>
       <c r="B72" s="9" t="n">
-        <v>4297.45</v>
+        <v>4310.75</v>
       </c>
       <c r="C72" s="11" t="n">
-        <v>4260.25</v>
+        <v>4228.6</v>
       </c>
       <c r="D72" s="14" t="n">
-        <v>4271.4</v>
+        <v>4234</v>
       </c>
       <c r="E72" s="6" t="n">
-        <v>4270.4</v>
+        <v>4237.95</v>
       </c>
       <c r="F72" s="17" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G72" s="6" t="n">
-        <v>4265</v>
+        <v>4303</v>
       </c>
     </row>
     <row r="73">
@@ -2436,22 +2438,22 @@
         </is>
       </c>
       <c r="B73" s="9" t="n">
-        <v>1515.9</v>
+        <v>1441.7</v>
       </c>
       <c r="C73" s="11" t="n">
-        <v>1495.95</v>
+        <v>1426.3</v>
       </c>
       <c r="D73" s="14" t="n">
-        <v>1498.5</v>
+        <v>1439</v>
       </c>
       <c r="E73" s="6" t="n">
-        <v>1502.35</v>
+        <v>1438.05</v>
       </c>
       <c r="F73" s="17" t="n">
         <v>27</v>
       </c>
       <c r="G73" s="6" t="n">
-        <v>1498.4</v>
+        <v>1435.6</v>
       </c>
     </row>
     <row r="74">
@@ -2461,22 +2463,22 @@
         </is>
       </c>
       <c r="B74" s="9" t="n">
-        <v>346.8</v>
+        <v>398.85</v>
       </c>
       <c r="C74" s="11" t="n">
-        <v>338.5</v>
+        <v>384.2</v>
       </c>
       <c r="D74" s="14" t="n">
-        <v>339.95</v>
+        <v>386.5</v>
       </c>
       <c r="E74" s="6" t="n">
-        <v>340.75</v>
+        <v>385.75</v>
       </c>
       <c r="F74" s="17" t="n">
-        <v>123</v>
+        <v>173</v>
       </c>
       <c r="G74" s="6" t="n">
-        <v>341.4</v>
+        <v>395.4</v>
       </c>
     </row>
     <row r="75">
@@ -2486,22 +2488,22 @@
         </is>
       </c>
       <c r="B75" s="9" t="n">
-        <v>1093</v>
+        <v>1097.35</v>
       </c>
       <c r="C75" s="11" t="n">
-        <v>1060.55</v>
+        <v>1072.3</v>
       </c>
       <c r="D75" s="14" t="n">
-        <v>1070</v>
+        <v>1082.55</v>
       </c>
       <c r="E75" s="6" t="n">
-        <v>1075.4</v>
+        <v>1081.7</v>
       </c>
       <c r="F75" s="17" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G75" s="6" t="n">
-        <v>1063.95</v>
+        <v>1082.85</v>
       </c>
     </row>
     <row r="76">
@@ -2511,22 +2513,22 @@
         </is>
       </c>
       <c r="B76" s="9" t="n">
-        <v>1213.7</v>
+        <v>1196.75</v>
       </c>
       <c r="C76" s="11" t="n">
-        <v>1175.75</v>
+        <v>1181.65</v>
       </c>
       <c r="D76" s="14" t="n">
-        <v>1179.9</v>
+        <v>1190</v>
       </c>
       <c r="E76" s="6" t="n">
-        <v>1181.35</v>
+        <v>1188.15</v>
       </c>
       <c r="F76" s="17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G76" s="6" t="n">
-        <v>1199.3</v>
+        <v>1192.8</v>
       </c>
     </row>
     <row r="77">
@@ -2536,22 +2538,22 @@
         </is>
       </c>
       <c r="B77" s="9" t="n">
-        <v>1059.25</v>
+        <v>1050.4</v>
       </c>
       <c r="C77" s="11" t="n">
-        <v>1036</v>
+        <v>1023.5</v>
       </c>
       <c r="D77" s="14" t="n">
-        <v>1052</v>
+        <v>1027</v>
       </c>
       <c r="E77" s="6" t="n">
-        <v>1052.45</v>
+        <v>1025.95</v>
       </c>
       <c r="F77" s="17" t="n">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="G77" s="6" t="n">
-        <v>1038.2</v>
+        <v>1048.5</v>
       </c>
     </row>
     <row r="78">
@@ -2561,22 +2563,22 @@
         </is>
       </c>
       <c r="B78" s="9" t="n">
-        <v>4365</v>
+        <v>4223.9</v>
       </c>
       <c r="C78" s="11" t="n">
-        <v>4255.55</v>
+        <v>4175.1</v>
       </c>
       <c r="D78" s="14" t="n">
-        <v>4317.9</v>
+        <v>4213.1</v>
       </c>
       <c r="E78" s="6" t="n">
-        <v>4326.7</v>
+        <v>4216.75</v>
       </c>
       <c r="F78" s="17" t="n">
         <v>1</v>
       </c>
       <c r="G78" s="6" t="n">
-        <v>4259.45</v>
+        <v>4213.7</v>
       </c>
     </row>
     <row r="79">
@@ -2586,22 +2588,22 @@
         </is>
       </c>
       <c r="B79" s="9" t="n">
-        <v>923.5</v>
+        <v>951.9</v>
       </c>
       <c r="C79" s="11" t="n">
-        <v>903.6</v>
+        <v>934.05</v>
       </c>
       <c r="D79" s="14" t="n">
-        <v>919</v>
+        <v>942.85</v>
       </c>
       <c r="E79" s="6" t="n">
-        <v>921.15</v>
+        <v>939.2</v>
       </c>
       <c r="F79" s="17" t="n">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="G79" s="6" t="n">
-        <v>907.5</v>
+        <v>949.6</v>
       </c>
     </row>
     <row r="80">
@@ -2611,22 +2613,22 @@
         </is>
       </c>
       <c r="B80" s="9" t="n">
-        <v>537.15</v>
+        <v>577</v>
       </c>
       <c r="C80" s="11" t="n">
-        <v>528.5</v>
+        <v>564.1</v>
       </c>
       <c r="D80" s="14" t="n">
-        <v>529.15</v>
+        <v>571.9</v>
       </c>
       <c r="E80" s="6" t="n">
-        <v>530.65</v>
+        <v>574.15</v>
       </c>
       <c r="F80" s="17" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G80" s="6" t="n">
-        <v>536.1</v>
+        <v>573.35</v>
       </c>
     </row>
     <row r="81">
@@ -2636,22 +2638,22 @@
         </is>
       </c>
       <c r="B81" s="9" t="n">
-        <v>1725.05</v>
+        <v>1856.3</v>
       </c>
       <c r="C81" s="11" t="n">
-        <v>1710.4</v>
+        <v>1835.45</v>
       </c>
       <c r="D81" s="14" t="n">
-        <v>1721</v>
+        <v>1855.8</v>
       </c>
       <c r="E81" s="6" t="n">
-        <v>1717.2</v>
+        <v>1853.2</v>
       </c>
       <c r="F81" s="17" t="n">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G81" s="6" t="n">
-        <v>1716.7</v>
+        <v>1846.35</v>
       </c>
     </row>
     <row r="82">
@@ -2661,22 +2663,22 @@
         </is>
       </c>
       <c r="B82" s="9" t="n">
-        <v>2776.3</v>
+        <v>2939.1</v>
       </c>
       <c r="C82" s="11" t="n">
-        <v>2716.6</v>
+        <v>2868</v>
       </c>
       <c r="D82" s="14" t="n">
-        <v>2755</v>
+        <v>2918</v>
       </c>
       <c r="E82" s="6" t="n">
-        <v>2750.2</v>
+        <v>2906.4</v>
       </c>
       <c r="F82" s="17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G82" s="6" t="n">
-        <v>2771.05</v>
+        <v>2883.95</v>
       </c>
     </row>
     <row r="83">
@@ -2686,22 +2688,22 @@
         </is>
       </c>
       <c r="B83" s="9" t="n">
-        <v>441.5</v>
+        <v>477.65</v>
       </c>
       <c r="C83" s="11" t="n">
-        <v>434.05</v>
+        <v>464.15</v>
       </c>
       <c r="D83" s="14" t="n">
-        <v>434.6</v>
+        <v>475.55</v>
       </c>
       <c r="E83" s="6" t="n">
-        <v>434.9</v>
+        <v>474.45</v>
       </c>
       <c r="F83" s="17" t="n">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="G83" s="6" t="n">
-        <v>441.2</v>
+        <v>472.5</v>
       </c>
     </row>
     <row r="84">
@@ -2711,22 +2713,22 @@
         </is>
       </c>
       <c r="B84" s="9" t="n">
-        <v>734.7</v>
+        <v>792.05</v>
       </c>
       <c r="C84" s="11" t="n">
-        <v>717.2</v>
+        <v>780.2</v>
       </c>
       <c r="D84" s="14" t="n">
-        <v>734</v>
+        <v>783.8</v>
       </c>
       <c r="E84" s="6" t="n">
-        <v>731.65</v>
+        <v>782.15</v>
       </c>
       <c r="F84" s="17" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G84" s="6" t="n">
-        <v>718.55</v>
+        <v>787.6</v>
       </c>
     </row>
     <row r="85">
@@ -2736,22 +2738,22 @@
         </is>
       </c>
       <c r="B85" s="9" t="n">
-        <v>5070.2</v>
+        <v>5459.65</v>
       </c>
       <c r="C85" s="11" t="n">
-        <v>4995.25</v>
+        <v>5347.25</v>
       </c>
       <c r="D85" s="14" t="n">
-        <v>5025.6</v>
+        <v>5402.05</v>
       </c>
       <c r="E85" s="6" t="n">
-        <v>5032.55</v>
+        <v>5389.7</v>
       </c>
       <c r="F85" s="17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G85" s="6" t="n">
-        <v>5005</v>
+        <v>5455.25</v>
       </c>
     </row>
     <row r="86">
@@ -2761,22 +2763,22 @@
         </is>
       </c>
       <c r="B86" s="9" t="n">
-        <v>4870.4</v>
+        <v>5137.65</v>
       </c>
       <c r="C86" s="11" t="n">
-        <v>4830.2</v>
+        <v>5067.05</v>
       </c>
       <c r="D86" s="14" t="n">
-        <v>4848</v>
+        <v>5117.4</v>
       </c>
       <c r="E86" s="6" t="n">
-        <v>4845.8</v>
+        <v>5109.05</v>
       </c>
       <c r="F86" s="17" t="n">
         <v>1</v>
       </c>
       <c r="G86" s="6" t="n">
-        <v>4850.2</v>
+        <v>5120.6</v>
       </c>
     </row>
     <row r="87">
@@ -2786,22 +2788,22 @@
         </is>
       </c>
       <c r="B87" s="9" t="n">
-        <v>1611</v>
+        <v>1782.45</v>
       </c>
       <c r="C87" s="11" t="n">
-        <v>1596.55</v>
+        <v>1760.25</v>
       </c>
       <c r="D87" s="14" t="n">
-        <v>1603.5</v>
+        <v>1781.5</v>
       </c>
       <c r="E87" s="6" t="n">
-        <v>1604.1</v>
+        <v>1778.9</v>
       </c>
       <c r="F87" s="17" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G87" s="6" t="n">
-        <v>1609</v>
+        <v>1776.8</v>
       </c>
     </row>
     <row r="88">
@@ -2811,22 +2813,22 @@
         </is>
       </c>
       <c r="B88" s="9" t="n">
-        <v>300</v>
+        <v>305.35</v>
       </c>
       <c r="C88" s="11" t="n">
-        <v>293.2</v>
+        <v>298</v>
       </c>
       <c r="D88" s="14" t="n">
-        <v>298.95</v>
+        <v>303.5</v>
       </c>
       <c r="E88" s="6" t="n">
-        <v>298.95</v>
+        <v>302.8</v>
       </c>
       <c r="F88" s="17" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="G88" s="6" t="n">
-        <v>293.85</v>
+        <v>299.65</v>
       </c>
     </row>
     <row r="89">
@@ -2836,22 +2838,22 @@
         </is>
       </c>
       <c r="B89" s="9" t="n">
-        <v>187.5</v>
+        <v>208.87</v>
       </c>
       <c r="C89" s="11" t="n">
-        <v>184.85</v>
+        <v>205.8</v>
       </c>
       <c r="D89" s="14" t="n">
-        <v>185.17</v>
+        <v>207</v>
       </c>
       <c r="E89" s="6" t="n">
-        <v>185.37</v>
+        <v>206.65</v>
       </c>
       <c r="F89" s="17" t="n">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G89" s="6" t="n">
-        <v>186.8</v>
+        <v>208.6</v>
       </c>
     </row>
     <row r="90">
@@ -2861,22 +2863,22 @@
         </is>
       </c>
       <c r="B90" s="9" t="n">
-        <v>621.95</v>
+        <v>655.8</v>
       </c>
       <c r="C90" s="11" t="n">
-        <v>614</v>
+        <v>630.5</v>
       </c>
       <c r="D90" s="14" t="n">
-        <v>618.15</v>
+        <v>640.05</v>
       </c>
       <c r="E90" s="6" t="n">
-        <v>619.35</v>
+        <v>641.3</v>
       </c>
       <c r="F90" s="17" t="n">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="G90" s="6" t="n">
-        <v>616.7</v>
+        <v>633.75</v>
       </c>
     </row>
     <row r="91">
@@ -2886,22 +2888,22 @@
         </is>
       </c>
       <c r="B91" s="9" t="n">
-        <v>1278.4</v>
+        <v>1279</v>
       </c>
       <c r="C91" s="11" t="n">
-        <v>1258.2</v>
+        <v>1259</v>
       </c>
       <c r="D91" s="14" t="n">
-        <v>1270</v>
+        <v>1277.3</v>
       </c>
       <c r="E91" s="6" t="n">
-        <v>1269</v>
+        <v>1272.1</v>
       </c>
       <c r="F91" s="17" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G91" s="6" t="n">
-        <v>1277.65</v>
+        <v>1263.05</v>
       </c>
     </row>
     <row r="92">
@@ -2911,22 +2913,22 @@
         </is>
       </c>
       <c r="B92" s="9" t="n">
-        <v>3956</v>
+        <v>3984.5</v>
       </c>
       <c r="C92" s="11" t="n">
-        <v>3832.95</v>
+        <v>3900.3</v>
       </c>
       <c r="D92" s="14" t="n">
-        <v>3901.35</v>
+        <v>3955</v>
       </c>
       <c r="E92" s="6" t="n">
-        <v>3909.9</v>
+        <v>3946.9</v>
       </c>
       <c r="F92" s="17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G92" s="6" t="n">
-        <v>3840</v>
+        <v>3958.85</v>
       </c>
     </row>
     <row r="93">
@@ -2936,22 +2938,22 @@
         </is>
       </c>
       <c r="B93" s="9" t="n">
-        <v>1981.1</v>
+        <v>2047.35</v>
       </c>
       <c r="C93" s="11" t="n">
-        <v>1953.1</v>
+        <v>1990</v>
       </c>
       <c r="D93" s="14" t="n">
-        <v>1957</v>
+        <v>2042</v>
       </c>
       <c r="E93" s="6" t="n">
-        <v>1958.2</v>
+        <v>2042.25</v>
       </c>
       <c r="F93" s="17" t="n">
         <v>1</v>
       </c>
       <c r="G93" s="6" t="n">
-        <v>1979.45</v>
+        <v>2026.3</v>
       </c>
     </row>
     <row r="94">
@@ -2961,22 +2963,22 @@
         </is>
       </c>
       <c r="B94" s="9" t="n">
-        <v>999.65</v>
+        <v>1006.7</v>
       </c>
       <c r="C94" s="11" t="n">
-        <v>983.3</v>
+        <v>989.1</v>
       </c>
       <c r="D94" s="14" t="n">
-        <v>992.9</v>
+        <v>992.25</v>
       </c>
       <c r="E94" s="6" t="n">
-        <v>993.5</v>
+        <v>992.85</v>
       </c>
       <c r="F94" s="17" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G94" s="6" t="n">
-        <v>988.6</v>
+        <v>993.35</v>
       </c>
     </row>
     <row r="95">
@@ -2986,22 +2988,22 @@
         </is>
       </c>
       <c r="B95" s="9" t="n">
-        <v>1479</v>
+        <v>1696</v>
       </c>
       <c r="C95" s="11" t="n">
-        <v>1455</v>
+        <v>1641.55</v>
       </c>
       <c r="D95" s="14" t="n">
-        <v>1459.5</v>
+        <v>1666</v>
       </c>
       <c r="E95" s="6" t="n">
-        <v>1465.85</v>
+        <v>1669</v>
       </c>
       <c r="F95" s="17" t="n">
         <v>4</v>
       </c>
       <c r="G95" s="6" t="n">
-        <v>1457.6</v>
+        <v>1689.1</v>
       </c>
     </row>
     <row r="96">
@@ -3011,22 +3013,22 @@
         </is>
       </c>
       <c r="B96" s="9" t="n">
-        <v>2428.9</v>
+        <v>2652</v>
       </c>
       <c r="C96" s="11" t="n">
-        <v>2395.55</v>
+        <v>2589.85</v>
       </c>
       <c r="D96" s="14" t="n">
-        <v>2406</v>
+        <v>2611.5</v>
       </c>
       <c r="E96" s="6" t="n">
-        <v>2408.85</v>
+        <v>2609.55</v>
       </c>
       <c r="F96" s="17" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G96" s="6" t="n">
-        <v>2426.75</v>
+        <v>2645.5</v>
       </c>
     </row>
     <row r="97">
@@ -3036,22 +3038,22 @@
         </is>
       </c>
       <c r="B97" s="9" t="n">
-        <v>1800.7</v>
+        <v>1807.8</v>
       </c>
       <c r="C97" s="11" t="n">
-        <v>1764.25</v>
+        <v>1770</v>
       </c>
       <c r="D97" s="14" t="n">
-        <v>1768</v>
+        <v>1783</v>
       </c>
       <c r="E97" s="6" t="n">
-        <v>1770</v>
+        <v>1784.4</v>
       </c>
       <c r="F97" s="17" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G97" s="6" t="n">
-        <v>1796.05</v>
+        <v>1807.8</v>
       </c>
     </row>
     <row r="98">
@@ -3061,22 +3063,22 @@
         </is>
       </c>
       <c r="B98" s="9" t="n">
-        <v>656</v>
+        <v>675</v>
       </c>
       <c r="C98" s="11" t="n">
-        <v>642.25</v>
+        <v>658.2</v>
       </c>
       <c r="D98" s="14" t="n">
-        <v>646.95</v>
+        <v>667.1</v>
       </c>
       <c r="E98" s="6" t="n">
-        <v>646.5</v>
+        <v>667.45</v>
       </c>
       <c r="F98" s="17" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G98" s="6" t="n">
-        <v>649.9</v>
+        <v>658.2</v>
       </c>
     </row>
     <row r="99">
@@ -3086,22 +3088,22 @@
         </is>
       </c>
       <c r="B99" s="9" t="n">
-        <v>6302</v>
+        <v>6879.65</v>
       </c>
       <c r="C99" s="11" t="n">
-        <v>6172</v>
+        <v>6818.8</v>
       </c>
       <c r="D99" s="14" t="n">
-        <v>6250</v>
+        <v>6870</v>
       </c>
       <c r="E99" s="6" t="n">
-        <v>6242.95</v>
+        <v>6857.45</v>
       </c>
       <c r="F99" s="17" t="n">
         <v>2</v>
       </c>
       <c r="G99" s="6" t="n">
-        <v>6220.75</v>
+        <v>6849.8</v>
       </c>
     </row>
     <row r="100">
@@ -3111,22 +3113,22 @@
         </is>
       </c>
       <c r="B100" s="9" t="n">
-        <v>3606</v>
+        <v>3715.8</v>
       </c>
       <c r="C100" s="11" t="n">
-        <v>3533</v>
+        <v>3621.1</v>
       </c>
       <c r="D100" s="14" t="n">
-        <v>3539.15</v>
+        <v>3672</v>
       </c>
       <c r="E100" s="6" t="n">
-        <v>3545.25</v>
+        <v>3663.55</v>
       </c>
       <c r="F100" s="17" t="n">
         <v>1</v>
       </c>
       <c r="G100" s="6" t="n">
-        <v>3600</v>
+        <v>3649.95</v>
       </c>
     </row>
     <row r="101">
@@ -3136,22 +3138,22 @@
         </is>
       </c>
       <c r="B101" s="9" t="n">
-        <v>268.7</v>
+        <v>253.4</v>
       </c>
       <c r="C101" s="11" t="n">
-        <v>263.1</v>
+        <v>249.5</v>
       </c>
       <c r="D101" s="14" t="n">
-        <v>266.85</v>
+        <v>250.31</v>
       </c>
       <c r="E101" s="6" t="n">
-        <v>267.4</v>
+        <v>250.13</v>
       </c>
       <c r="F101" s="17" t="n">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="G101" s="6" t="n">
-        <v>263.5</v>
+        <v>251.78</v>
       </c>
     </row>
     <row r="102">
@@ -3161,22 +3163,22 @@
         </is>
       </c>
       <c r="B102" s="9" t="n">
-        <v>369.45</v>
+        <v>380.7</v>
       </c>
       <c r="C102" s="11" t="n">
-        <v>366.1</v>
+        <v>376.15</v>
       </c>
       <c r="D102" s="14" t="n">
-        <v>368.5</v>
+        <v>378.1</v>
       </c>
       <c r="E102" s="6" t="n">
-        <v>368.45</v>
+        <v>377.45</v>
       </c>
       <c r="F102" s="17" t="n">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="G102" s="6" t="n">
-        <v>366.5</v>
+        <v>378.7</v>
       </c>
     </row>
     <row r="103">
@@ -3186,22 +3188,22 @@
         </is>
       </c>
       <c r="B103" s="9" t="n">
-        <v>1937</v>
+        <v>1778.75</v>
       </c>
       <c r="C103" s="11" t="n">
-        <v>1893</v>
+        <v>1715</v>
       </c>
       <c r="D103" s="14" t="n">
-        <v>1902.4</v>
+        <v>1719.85</v>
       </c>
       <c r="E103" s="6" t="n">
-        <v>1907.8</v>
+        <v>1723.25</v>
       </c>
       <c r="F103" s="17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G103" s="6" t="n">
-        <v>1922.1</v>
+        <v>1776.95</v>
       </c>
     </row>
     <row r="104">
@@ -3211,22 +3213,22 @@
         </is>
       </c>
       <c r="B104" s="9" t="n">
-        <v>899.9</v>
+        <v>932.8</v>
       </c>
       <c r="C104" s="11" t="n">
-        <v>878.35</v>
+        <v>920.5</v>
       </c>
       <c r="D104" s="14" t="n">
-        <v>881.1</v>
+        <v>930</v>
       </c>
       <c r="E104" s="6" t="n">
-        <v>882.5</v>
+        <v>930.1</v>
       </c>
       <c r="F104" s="17" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G104" s="6" t="n">
-        <v>880.55</v>
+        <v>927.45</v>
       </c>
     </row>
     <row r="105">
@@ -3236,22 +3238,22 @@
         </is>
       </c>
       <c r="B105" s="9" t="n">
-        <v>3800</v>
+        <v>4775</v>
       </c>
       <c r="C105" s="11" t="n">
-        <v>3736.6</v>
+        <v>4566.25</v>
       </c>
       <c r="D105" s="14" t="n">
-        <v>3769.7</v>
+        <v>4599.25</v>
       </c>
       <c r="E105" s="6" t="n">
-        <v>3772.8</v>
+        <v>4586.3</v>
       </c>
       <c r="F105" s="17" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G105" s="6" t="n">
-        <v>3746.6</v>
+        <v>4770.5</v>
       </c>
     </row>
     <row r="106">
@@ -3261,22 +3263,22 @@
         </is>
       </c>
       <c r="B106" s="9" t="n">
-        <v>327.85</v>
+        <v>339.5</v>
       </c>
       <c r="C106" s="11" t="n">
-        <v>321.55</v>
+        <v>333.1</v>
       </c>
       <c r="D106" s="14" t="n">
-        <v>323</v>
+        <v>337.7</v>
       </c>
       <c r="E106" s="6" t="n">
-        <v>323.9</v>
+        <v>337.15</v>
       </c>
       <c r="F106" s="17" t="n">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G106" s="6" t="n">
-        <v>322.15</v>
+        <v>337.8</v>
       </c>
     </row>
     <row r="107">
@@ -3286,22 +3288,22 @@
         </is>
       </c>
       <c r="B107" s="9" t="n">
-        <v>3124.85</v>
+        <v>3100.45</v>
       </c>
       <c r="C107" s="11" t="n">
-        <v>3091.6</v>
+        <v>3056</v>
       </c>
       <c r="D107" s="14" t="n">
-        <v>3109.5</v>
+        <v>3070</v>
       </c>
       <c r="E107" s="6" t="n">
-        <v>3109.8</v>
+        <v>3069</v>
       </c>
       <c r="F107" s="17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G107" s="6" t="n">
-        <v>3105.7</v>
+        <v>3098.8</v>
       </c>
     </row>
     <row r="108">
@@ -3311,22 +3313,22 @@
         </is>
       </c>
       <c r="B108" s="9" t="n">
-        <v>7140</v>
+        <v>6675</v>
       </c>
       <c r="C108" s="11" t="n">
-        <v>7000.25</v>
+        <v>6535</v>
       </c>
       <c r="D108" s="14" t="n">
-        <v>7080</v>
+        <v>6549.8</v>
       </c>
       <c r="E108" s="6" t="n">
-        <v>7079.9</v>
+        <v>6546.6</v>
       </c>
       <c r="F108" s="17" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G108" s="6" t="n">
-        <v>7044.3</v>
+        <v>6646.2</v>
       </c>
     </row>
     <row r="109">
@@ -3336,22 +3338,22 @@
         </is>
       </c>
       <c r="B109" s="9" t="n">
-        <v>323.25</v>
+        <v>340.6</v>
       </c>
       <c r="C109" s="11" t="n">
-        <v>319.35</v>
+        <v>336.85</v>
       </c>
       <c r="D109" s="14" t="n">
-        <v>321.5</v>
+        <v>339.8</v>
       </c>
       <c r="E109" s="6" t="n">
-        <v>321.5</v>
+        <v>339.4</v>
       </c>
       <c r="F109" s="17" t="n">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="G109" s="6" t="n">
-        <v>320.65</v>
+        <v>338.15</v>
       </c>
     </row>
     <row r="110">
@@ -3361,22 +3363,22 @@
         </is>
       </c>
       <c r="B110" s="9" t="n">
-        <v>167.48</v>
+        <v>166.99</v>
       </c>
       <c r="C110" s="11" t="n">
-        <v>164.1</v>
+        <v>163.25</v>
       </c>
       <c r="D110" s="14" t="n">
-        <v>164.47</v>
+        <v>163.5</v>
       </c>
       <c r="E110" s="6" t="n">
-        <v>164.54</v>
+        <v>163.55</v>
       </c>
       <c r="F110" s="17" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G110" s="6" t="n">
-        <v>166.21</v>
+        <v>165.96</v>
       </c>
     </row>
     <row r="111">
@@ -3386,22 +3388,22 @@
         </is>
       </c>
       <c r="B111" s="9" t="n">
-        <v>878.3</v>
+        <v>807.95</v>
       </c>
       <c r="C111" s="11" t="n">
-        <v>853.05</v>
+        <v>790.5</v>
       </c>
       <c r="D111" s="14" t="n">
-        <v>866.5</v>
+        <v>798.45</v>
       </c>
       <c r="E111" s="6" t="n">
-        <v>869.35</v>
+        <v>794.8</v>
       </c>
       <c r="F111" s="17" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G111" s="6" t="n">
-        <v>855.05</v>
+        <v>805.05</v>
       </c>
     </row>
     <row r="112">
@@ -3411,22 +3413,22 @@
         </is>
       </c>
       <c r="B112" s="9" t="n">
-        <v>261.4</v>
+        <v>260.85</v>
       </c>
       <c r="C112" s="11" t="n">
-        <v>256.85</v>
+        <v>252.85</v>
       </c>
       <c r="D112" s="14" t="n">
-        <v>257.45</v>
+        <v>253.85</v>
       </c>
       <c r="E112" s="6" t="n">
-        <v>257.63</v>
+        <v>253.65</v>
       </c>
       <c r="F112" s="17" t="n">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="G112" s="6" t="n">
-        <v>258.83</v>
+        <v>260.35</v>
       </c>
     </row>
     <row r="113">
@@ -3436,22 +3438,22 @@
         </is>
       </c>
       <c r="B113" s="9" t="n">
-        <v>536.9</v>
+        <v>615.55</v>
       </c>
       <c r="C113" s="11" t="n">
-        <v>519.5</v>
+        <v>591.55</v>
       </c>
       <c r="D113" s="14" t="n">
-        <v>531</v>
+        <v>608.5</v>
       </c>
       <c r="E113" s="6" t="n">
-        <v>532.65</v>
+        <v>607.6</v>
       </c>
       <c r="F113" s="17" t="n">
-        <v>158</v>
+        <v>297</v>
       </c>
       <c r="G113" s="6" t="n">
-        <v>520</v>
+        <v>593.55</v>
       </c>
     </row>
     <row r="114">
@@ -3461,22 +3463,22 @@
         </is>
       </c>
       <c r="B114" s="9" t="n">
-        <v>733.25</v>
+        <v>740</v>
       </c>
       <c r="C114" s="11" t="n">
-        <v>720.8</v>
+        <v>714.35</v>
       </c>
       <c r="D114" s="14" t="n">
-        <v>728.5</v>
+        <v>735.5</v>
       </c>
       <c r="E114" s="6" t="n">
-        <v>728.35</v>
+        <v>735.65</v>
       </c>
       <c r="F114" s="17" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G114" s="6" t="n">
-        <v>723.35</v>
+        <v>722.65</v>
       </c>
     </row>
     <row r="115">
@@ -3486,22 +3488,22 @@
         </is>
       </c>
       <c r="B115" s="9" t="n">
-        <v>1473.75</v>
+        <v>1530.35</v>
       </c>
       <c r="C115" s="11" t="n">
-        <v>1445</v>
+        <v>1508.25</v>
       </c>
       <c r="D115" s="14" t="n">
-        <v>1467</v>
+        <v>1521.5</v>
       </c>
       <c r="E115" s="6" t="n">
-        <v>1469.9</v>
+        <v>1514.95</v>
       </c>
       <c r="F115" s="17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G115" s="6" t="n">
-        <v>1450.1</v>
+        <v>1518.65</v>
       </c>
     </row>
     <row r="116">
@@ -3511,22 +3513,22 @@
         </is>
       </c>
       <c r="B116" s="9" t="n">
-        <v>7913.05</v>
+        <v>7867</v>
       </c>
       <c r="C116" s="11" t="n">
-        <v>7420</v>
+        <v>7685.05</v>
       </c>
       <c r="D116" s="14" t="n">
-        <v>7786</v>
+        <v>7742</v>
       </c>
       <c r="E116" s="6" t="n">
-        <v>7790.2</v>
+        <v>7741.35</v>
       </c>
       <c r="F116" s="17" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G116" s="6" t="n">
-        <v>7440.8</v>
+        <v>7854.1</v>
       </c>
     </row>
     <row r="117">
@@ -3536,22 +3538,22 @@
         </is>
       </c>
       <c r="B117" s="9" t="n">
-        <v>2413.95</v>
+        <v>2419.7</v>
       </c>
       <c r="C117" s="11" t="n">
-        <v>2390.05</v>
+        <v>2357.05</v>
       </c>
       <c r="D117" s="14" t="n">
-        <v>2396.65</v>
+        <v>2369</v>
       </c>
       <c r="E117" s="6" t="n">
-        <v>2402</v>
+        <v>2368.3</v>
       </c>
       <c r="F117" s="17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G117" s="6" t="n">
-        <v>2401.95</v>
+        <v>2404.4</v>
       </c>
     </row>
     <row r="118">
@@ -3561,22 +3563,22 @@
         </is>
       </c>
       <c r="B118" s="9" t="n">
-        <v>990</v>
+        <v>942.65</v>
       </c>
       <c r="C118" s="11" t="n">
-        <v>944.3</v>
+        <v>923.05</v>
       </c>
       <c r="D118" s="14" t="n">
-        <v>975</v>
+        <v>933</v>
       </c>
       <c r="E118" s="6" t="n">
-        <v>978.7</v>
+        <v>931.95</v>
       </c>
       <c r="F118" s="17" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G118" s="6" t="n">
-        <v>945.45</v>
+        <v>928</v>
       </c>
     </row>
     <row r="119">
@@ -3586,22 +3588,22 @@
         </is>
       </c>
       <c r="B119" s="9" t="n">
-        <v>1518</v>
+        <v>1573.05</v>
       </c>
       <c r="C119" s="11" t="n">
-        <v>1510</v>
+        <v>1550.95</v>
       </c>
       <c r="D119" s="14" t="n">
-        <v>1515</v>
+        <v>1554.25</v>
       </c>
       <c r="E119" s="6" t="n">
-        <v>1516</v>
+        <v>1556.4</v>
       </c>
       <c r="F119" s="17" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G119" s="6" t="n">
-        <v>1511.25</v>
+        <v>1571.55</v>
       </c>
     </row>
     <row r="120">
@@ -3611,22 +3613,22 @@
         </is>
       </c>
       <c r="B120" s="9" t="n">
-        <v>709.3</v>
+        <v>735</v>
       </c>
       <c r="C120" s="11" t="n">
-        <v>701</v>
+        <v>723.7</v>
       </c>
       <c r="D120" s="14" t="n">
-        <v>706</v>
+        <v>733.7</v>
       </c>
       <c r="E120" s="6" t="n">
-        <v>707.05</v>
+        <v>731.7</v>
       </c>
       <c r="F120" s="17" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G120" s="6" t="n">
-        <v>702</v>
+        <v>726.35</v>
       </c>
     </row>
     <row r="121">
@@ -3636,22 +3638,22 @@
         </is>
       </c>
       <c r="B121" s="9" t="n">
-        <v>1880.95</v>
+        <v>1887.4</v>
       </c>
       <c r="C121" s="11" t="n">
-        <v>1860.55</v>
+        <v>1840</v>
       </c>
       <c r="D121" s="14" t="n">
-        <v>1866.05</v>
+        <v>1850</v>
       </c>
       <c r="E121" s="6" t="n">
-        <v>1868.4</v>
+        <v>1857.2</v>
       </c>
       <c r="F121" s="17" t="n">
         <v>2</v>
       </c>
       <c r="G121" s="6" t="n">
-        <v>1872.5</v>
+        <v>1877.65</v>
       </c>
     </row>
     <row r="122">
@@ -3661,22 +3663,22 @@
         </is>
       </c>
       <c r="B122" s="9" t="n">
-        <v>997.25</v>
+        <v>1016.6</v>
       </c>
       <c r="C122" s="11" t="n">
-        <v>981.4</v>
+        <v>996.2</v>
       </c>
       <c r="D122" s="14" t="n">
-        <v>992</v>
+        <v>1002.9</v>
       </c>
       <c r="E122" s="6" t="n">
-        <v>993.4</v>
+        <v>1002.6</v>
       </c>
       <c r="F122" s="17" t="n">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="G122" s="6" t="n">
-        <v>982.3</v>
+        <v>1010.7</v>
       </c>
     </row>
     <row r="123">
@@ -3686,22 +3688,22 @@
         </is>
       </c>
       <c r="B123" s="9" t="n">
-        <v>1379.2</v>
+        <v>1478.95</v>
       </c>
       <c r="C123" s="11" t="n">
-        <v>1364.1</v>
+        <v>1460.15</v>
       </c>
       <c r="D123" s="14" t="n">
-        <v>1372</v>
+        <v>1465.2</v>
       </c>
       <c r="E123" s="6" t="n">
-        <v>1371.45</v>
+        <v>1467.6</v>
       </c>
       <c r="F123" s="17" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G123" s="6" t="n">
-        <v>1369</v>
+        <v>1475.75</v>
       </c>
     </row>
     <row r="124">
@@ -3711,22 +3713,22 @@
         </is>
       </c>
       <c r="B124" s="9" t="n">
-        <v>2919.3</v>
+        <v>2908.55</v>
       </c>
       <c r="C124" s="11" t="n">
-        <v>2860</v>
+        <v>2846.65</v>
       </c>
       <c r="D124" s="14" t="n">
-        <v>2863.15</v>
+        <v>2880.15</v>
       </c>
       <c r="E124" s="6" t="n">
-        <v>2882.1</v>
+        <v>2882.75</v>
       </c>
       <c r="F124" s="17" t="n">
         <v>1</v>
       </c>
       <c r="G124" s="6" t="n">
-        <v>2880.15</v>
+        <v>2902</v>
       </c>
     </row>
     <row r="125">
@@ -3736,22 +3738,22 @@
         </is>
       </c>
       <c r="B125" s="9" t="n">
-        <v>1604</v>
+        <v>1476.3</v>
       </c>
       <c r="C125" s="11" t="n">
-        <v>1576</v>
+        <v>1458</v>
       </c>
       <c r="D125" s="14" t="n">
-        <v>1602</v>
+        <v>1471.1</v>
       </c>
       <c r="E125" s="6" t="n">
-        <v>1599.1</v>
+        <v>1473.3</v>
       </c>
       <c r="F125" s="17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G125" s="6" t="n">
-        <v>1578</v>
+        <v>1462.55</v>
       </c>
     </row>
     <row r="126">
@@ -3761,22 +3763,22 @@
         </is>
       </c>
       <c r="B126" s="9" t="n">
-        <v>5294</v>
+        <v>5656.55</v>
       </c>
       <c r="C126" s="11" t="n">
-        <v>5137.15</v>
+        <v>5572</v>
       </c>
       <c r="D126" s="14" t="n">
-        <v>5255</v>
+        <v>5595</v>
       </c>
       <c r="E126" s="6" t="n">
-        <v>5245.55</v>
+        <v>5594.25</v>
       </c>
       <c r="F126" s="17" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G126" s="6" t="n">
-        <v>5160.75</v>
+        <v>5635.05</v>
       </c>
     </row>
     <row r="127">
@@ -3786,22 +3788,22 @@
         </is>
       </c>
       <c r="B127" s="9" t="n">
-        <v>2519</v>
+        <v>2441.95</v>
       </c>
       <c r="C127" s="11" t="n">
-        <v>2441.65</v>
+        <v>2381.4</v>
       </c>
       <c r="D127" s="14" t="n">
-        <v>2496.3</v>
+        <v>2400.5</v>
       </c>
       <c r="E127" s="6" t="n">
-        <v>2503.85</v>
+        <v>2398.25</v>
       </c>
       <c r="F127" s="17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G127" s="6" t="n">
-        <v>2449.6</v>
+        <v>2434.8</v>
       </c>
     </row>
     <row r="128">
@@ -3811,22 +3813,22 @@
         </is>
       </c>
       <c r="B128" s="9" t="n">
-        <v>2125.8</v>
+        <v>2133.7</v>
       </c>
       <c r="C128" s="11" t="n">
-        <v>2097.35</v>
+        <v>2070</v>
       </c>
       <c r="D128" s="14" t="n">
-        <v>2108</v>
+        <v>2115.95</v>
       </c>
       <c r="E128" s="6" t="n">
-        <v>2109.1</v>
+        <v>2110.95</v>
       </c>
       <c r="F128" s="17" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G128" s="6" t="n">
-        <v>2120.3</v>
+        <v>2076.25</v>
       </c>
     </row>
     <row r="129">
@@ -3836,22 +3838,22 @@
         </is>
       </c>
       <c r="B129" s="9" t="n">
-        <v>11271</v>
+        <v>11645</v>
       </c>
       <c r="C129" s="11" t="n">
-        <v>11167.6</v>
+        <v>11530</v>
       </c>
       <c r="D129" s="14" t="n">
-        <v>11250</v>
+        <v>11579</v>
       </c>
       <c r="E129" s="6" t="n">
-        <v>11242.8</v>
+        <v>11582.9</v>
       </c>
       <c r="F129" s="17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G129" s="6" t="n">
-        <v>11175</v>
+        <v>11627.45</v>
       </c>
     </row>
     <row r="130">
@@ -3861,22 +3863,22 @@
         </is>
       </c>
       <c r="B130" s="9" t="n">
-        <v>556.45</v>
+        <v>574</v>
       </c>
       <c r="C130" s="11" t="n">
-        <v>549.7</v>
+        <v>562.15</v>
       </c>
       <c r="D130" s="14" t="n">
-        <v>549.75</v>
+        <v>568.8</v>
       </c>
       <c r="E130" s="6" t="n">
-        <v>551.7</v>
+        <v>567.4</v>
       </c>
       <c r="F130" s="17" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G130" s="6" t="n">
-        <v>554.5</v>
+        <v>573.7</v>
       </c>
     </row>
     <row r="131">
@@ -3886,22 +3888,22 @@
         </is>
       </c>
       <c r="B131" s="9" t="n">
-        <v>451.9</v>
+        <v>477.5</v>
       </c>
       <c r="C131" s="11" t="n">
-        <v>442</v>
+        <v>464.8</v>
       </c>
       <c r="D131" s="14" t="n">
-        <v>446.7</v>
+        <v>466.1</v>
       </c>
       <c r="E131" s="6" t="n">
-        <v>447.6</v>
+        <v>465.65</v>
       </c>
       <c r="F131" s="17" t="n">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="G131" s="6" t="n">
-        <v>442.85</v>
+        <v>474.5</v>
       </c>
     </row>
     <row r="132">
@@ -3911,22 +3913,22 @@
         </is>
       </c>
       <c r="B132" s="9" t="n">
-        <v>1511.95</v>
+        <v>1479</v>
       </c>
       <c r="C132" s="11" t="n">
-        <v>1470.05</v>
+        <v>1439.05</v>
       </c>
       <c r="D132" s="14" t="n">
-        <v>1496</v>
+        <v>1462.95</v>
       </c>
       <c r="E132" s="6" t="n">
-        <v>1498.5</v>
+        <v>1459.65</v>
       </c>
       <c r="F132" s="17" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G132" s="6" t="n">
-        <v>1477.05</v>
+        <v>1449.7</v>
       </c>
     </row>
     <row r="133">
@@ -3936,22 +3938,22 @@
         </is>
       </c>
       <c r="B133" s="9" t="n">
-        <v>165.2</v>
+        <v>151.83</v>
       </c>
       <c r="C133" s="11" t="n">
-        <v>162.6</v>
+        <v>148.5</v>
       </c>
       <c r="D133" s="14" t="n">
-        <v>164.26</v>
+        <v>151</v>
       </c>
       <c r="E133" s="6" t="n">
-        <v>163.98</v>
+        <v>150.67</v>
       </c>
       <c r="F133" s="17" t="n">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="G133" s="6" t="n">
-        <v>163.9</v>
+        <v>151.5</v>
       </c>
     </row>
     <row r="134" ht="15.75" customHeight="1" thickBot="1">
@@ -3961,22 +3963,22 @@
         </is>
       </c>
       <c r="B134" s="19" t="n">
-        <v>1111.8</v>
+        <v>1184.15</v>
       </c>
       <c r="C134" s="12" t="n">
-        <v>1093.9</v>
+        <v>1154.45</v>
       </c>
       <c r="D134" s="15" t="n">
-        <v>1110.5</v>
+        <v>1159.55</v>
       </c>
       <c r="E134" s="7" t="n">
-        <v>1109.55</v>
+        <v>1157.8</v>
       </c>
       <c r="F134" s="18" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G134" s="7" t="n">
-        <v>1097.8</v>
+        <v>1177.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new algo path to MWCL creation updation.py
</commit_message>
<xml_diff>
--- a/algo high low.xlsx
+++ b/algo high low.xlsx
@@ -662,22 +662,22 @@
         </is>
       </c>
       <c r="B2" s="7" t="n">
-        <v>541.65</v>
+        <v>526.45</v>
       </c>
       <c r="C2" s="9" t="n">
-        <v>534.95</v>
+        <v>509.05</v>
       </c>
       <c r="D2" s="12" t="n">
-        <v>539</v>
+        <v>523</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>539</v>
+        <v>524.25</v>
       </c>
       <c r="F2" s="15" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>536.65</v>
+        <v>516.3</v>
       </c>
     </row>
     <row r="3">
@@ -687,22 +687,22 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>8678</v>
+        <v>8850</v>
       </c>
       <c r="C3" s="10" t="n">
-        <v>8545</v>
+        <v>8565.1</v>
       </c>
       <c r="D3" s="13" t="n">
-        <v>8631</v>
+        <v>8778</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>8648.299999999999</v>
+        <v>8783</v>
       </c>
       <c r="F3" s="16" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>8616</v>
+        <v>8569</v>
       </c>
     </row>
     <row r="4">
@@ -712,22 +712,22 @@
         </is>
       </c>
       <c r="B4" s="8" t="n">
-        <v>228.1</v>
+        <v>223.02</v>
       </c>
       <c r="C4" s="10" t="n">
-        <v>223.02</v>
+        <v>213.35</v>
       </c>
       <c r="D4" s="13" t="n">
-        <v>225.3</v>
+        <v>222.21</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>225.85</v>
+        <v>222.08</v>
       </c>
       <c r="F4" s="16" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>225.75</v>
+        <v>214.75</v>
       </c>
     </row>
     <row r="5">
@@ -737,22 +737,22 @@
         </is>
       </c>
       <c r="B5" s="8" t="n">
-        <v>353.55</v>
+        <v>335.85</v>
       </c>
       <c r="C5" s="10" t="n">
-        <v>343.05</v>
+        <v>323.05</v>
       </c>
       <c r="D5" s="13" t="n">
-        <v>349.1</v>
+        <v>335</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>348.7</v>
+        <v>334.05</v>
       </c>
       <c r="F5" s="16" t="n">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>347.5</v>
+        <v>326.35</v>
       </c>
     </row>
     <row r="6">
@@ -762,22 +762,22 @@
         </is>
       </c>
       <c r="B6" s="8" t="n">
-        <v>3128</v>
+        <v>3031.7</v>
       </c>
       <c r="C6" s="10" t="n">
-        <v>3091.5</v>
+        <v>2974.05</v>
       </c>
       <c r="D6" s="13" t="n">
-        <v>3103.25</v>
+        <v>2999.95</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>3104.7</v>
+        <v>3002</v>
       </c>
       <c r="F6" s="16" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>3116.25</v>
+        <v>2979</v>
       </c>
     </row>
     <row r="7">
@@ -787,22 +787,22 @@
         </is>
       </c>
       <c r="B7" s="8" t="n">
-        <v>1424.7</v>
+        <v>1410.55</v>
       </c>
       <c r="C7" s="10" t="n">
-        <v>1407</v>
+        <v>1376</v>
       </c>
       <c r="D7" s="13" t="n">
-        <v>1419.3</v>
+        <v>1405.1</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>1420.3</v>
+        <v>1405.6</v>
       </c>
       <c r="F7" s="16" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>1420.45</v>
+        <v>1380.3</v>
       </c>
     </row>
     <row r="8">
@@ -812,22 +812,22 @@
         </is>
       </c>
       <c r="B8" s="8" t="n">
-        <v>6318.55</v>
+        <v>6158</v>
       </c>
       <c r="C8" s="10" t="n">
-        <v>6230.7</v>
+        <v>6032</v>
       </c>
       <c r="D8" s="13" t="n">
-        <v>6251.05</v>
+        <v>6154</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>6265.5</v>
+        <v>6132.75</v>
       </c>
       <c r="F8" s="16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>6278.7</v>
+        <v>6104.3</v>
       </c>
     </row>
     <row r="9">
@@ -837,22 +837,22 @@
         </is>
       </c>
       <c r="B9" s="8" t="n">
-        <v>595.9</v>
+        <v>577.4</v>
       </c>
       <c r="C9" s="10" t="n">
-        <v>586.55</v>
+        <v>558.95</v>
       </c>
       <c r="D9" s="13" t="n">
-        <v>590</v>
+        <v>571.1</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>590.35</v>
+        <v>573.95</v>
       </c>
       <c r="F9" s="16" t="n">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="G9" s="5" t="n">
-        <v>595.2</v>
+        <v>559.55</v>
       </c>
     </row>
     <row r="10">
@@ -862,22 +862,22 @@
         </is>
       </c>
       <c r="B10" s="8" t="n">
-        <v>7150.35</v>
+        <v>7041.65</v>
       </c>
       <c r="C10" s="10" t="n">
-        <v>7040</v>
+        <v>6957.75</v>
       </c>
       <c r="D10" s="13" t="n">
-        <v>7130.55</v>
+        <v>6970.2</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>7140.15</v>
+        <v>6982.9</v>
       </c>
       <c r="F10" s="16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>7048.15</v>
+        <v>6963.25</v>
       </c>
     </row>
     <row r="11">
@@ -887,22 +887,22 @@
         </is>
       </c>
       <c r="B11" s="8" t="n">
-        <v>518.7</v>
+        <v>510.9</v>
       </c>
       <c r="C11" s="10" t="n">
-        <v>508.05</v>
+        <v>498.2</v>
       </c>
       <c r="D11" s="13" t="n">
-        <v>516</v>
+        <v>505.55</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>515</v>
+        <v>505.75</v>
       </c>
       <c r="F11" s="16" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>508.2</v>
+        <v>499.15</v>
       </c>
     </row>
     <row r="12">
@@ -912,22 +912,22 @@
         </is>
       </c>
       <c r="B12" s="8" t="n">
-        <v>228.46</v>
+        <v>223.9</v>
       </c>
       <c r="C12" s="10" t="n">
-        <v>223.9</v>
+        <v>217.8</v>
       </c>
       <c r="D12" s="13" t="n">
-        <v>225.38</v>
+        <v>223.4</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>226.3</v>
+        <v>223.28</v>
       </c>
       <c r="F12" s="16" t="n">
-        <v>106</v>
+        <v>47</v>
       </c>
       <c r="G12" s="5" t="n">
-        <v>228.1</v>
+        <v>218.27</v>
       </c>
     </row>
     <row r="13">
@@ -937,22 +937,22 @@
         </is>
       </c>
       <c r="B13" s="8" t="n">
-        <v>1917.55</v>
+        <v>1879</v>
       </c>
       <c r="C13" s="10" t="n">
-        <v>1893.15</v>
+        <v>1843.35</v>
       </c>
       <c r="D13" s="13" t="n">
-        <v>1902.55</v>
+        <v>1877</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>1904.5</v>
+        <v>1871.7</v>
       </c>
       <c r="F13" s="16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>1909.75</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="14">
@@ -962,22 +962,22 @@
         </is>
       </c>
       <c r="B14" s="8" t="n">
-        <v>8045.7</v>
+        <v>7810.35</v>
       </c>
       <c r="C14" s="10" t="n">
-        <v>7614.35</v>
+        <v>7700.1</v>
       </c>
       <c r="D14" s="13" t="n">
-        <v>7829.95</v>
+        <v>7765</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>7836.5</v>
+        <v>7774.5</v>
       </c>
       <c r="F14" s="16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>7958.35</v>
+        <v>7717.45</v>
       </c>
     </row>
     <row r="15">
@@ -987,22 +987,22 @@
         </is>
       </c>
       <c r="B15" s="8" t="n">
-        <v>702.5</v>
+        <v>687.5</v>
       </c>
       <c r="C15" s="10" t="n">
-        <v>690.65</v>
+        <v>677.55</v>
       </c>
       <c r="D15" s="13" t="n">
-        <v>696.25</v>
+        <v>683.4</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>695.8</v>
+        <v>683.65</v>
       </c>
       <c r="F15" s="16" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>702.45</v>
+        <v>677.95</v>
       </c>
     </row>
     <row r="16">
@@ -1012,22 +1012,22 @@
         </is>
       </c>
       <c r="B16" s="8" t="n">
-        <v>1499</v>
+        <v>1481.55</v>
       </c>
       <c r="C16" s="10" t="n">
-        <v>1466.55</v>
+        <v>1450</v>
       </c>
       <c r="D16" s="13" t="n">
-        <v>1480</v>
+        <v>1470.5</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>1480.05</v>
+        <v>1472.7</v>
       </c>
       <c r="F16" s="16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>1493.4</v>
+        <v>1452.75</v>
       </c>
     </row>
     <row r="17">
@@ -1037,22 +1037,22 @@
         </is>
       </c>
       <c r="B17" s="8" t="n">
-        <v>1895.75</v>
+        <v>1833.3</v>
       </c>
       <c r="C17" s="10" t="n">
-        <v>1842</v>
+        <v>1800</v>
       </c>
       <c r="D17" s="13" t="n">
-        <v>1856.95</v>
+        <v>1821.5</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>1853.95</v>
+        <v>1819.9</v>
       </c>
       <c r="F17" s="16" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>1881.2</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="18">
@@ -1062,22 +1062,22 @@
         </is>
       </c>
       <c r="B18" s="8" t="n">
-        <v>7252.85</v>
+        <v>6938.65</v>
       </c>
       <c r="C18" s="10" t="n">
-        <v>6979</v>
+        <v>6820.7</v>
       </c>
       <c r="D18" s="13" t="n">
-        <v>7029.8</v>
+        <v>6910.05</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>7016.9</v>
+        <v>6899.55</v>
       </c>
       <c r="F18" s="16" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>7244.65</v>
+        <v>6844.25</v>
       </c>
     </row>
     <row r="19">
@@ -1087,22 +1087,22 @@
         </is>
       </c>
       <c r="B19" s="8" t="n">
-        <v>3034.25</v>
+        <v>3013.1</v>
       </c>
       <c r="C19" s="10" t="n">
-        <v>2973.2</v>
+        <v>2930</v>
       </c>
       <c r="D19" s="13" t="n">
-        <v>3013.1</v>
+        <v>3000</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>3028.2</v>
+        <v>2998.65</v>
       </c>
       <c r="F19" s="16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>2998.9</v>
+        <v>2931.2</v>
       </c>
     </row>
     <row r="20">
@@ -1112,22 +1112,22 @@
         </is>
       </c>
       <c r="B20" s="8" t="n">
-        <v>674</v>
+        <v>646.3</v>
       </c>
       <c r="C20" s="10" t="n">
-        <v>649.9</v>
+        <v>632.2</v>
       </c>
       <c r="D20" s="13" t="n">
-        <v>666</v>
+        <v>639.45</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>666.45</v>
+        <v>638.25</v>
       </c>
       <c r="F20" s="16" t="n">
         <v>10</v>
       </c>
       <c r="G20" s="5" t="n">
-        <v>650.5</v>
+        <v>633.1</v>
       </c>
     </row>
     <row r="21">
@@ -1137,22 +1137,22 @@
         </is>
       </c>
       <c r="B21" s="8" t="n">
-        <v>199.94</v>
+        <v>192.68</v>
       </c>
       <c r="C21" s="10" t="n">
-        <v>193.81</v>
+        <v>188.68</v>
       </c>
       <c r="D21" s="13" t="n">
-        <v>194.39</v>
+        <v>191.96</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>194.35</v>
+        <v>191.96</v>
       </c>
       <c r="F21" s="16" t="n">
-        <v>216</v>
+        <v>98</v>
       </c>
       <c r="G21" s="5" t="n">
-        <v>199.93</v>
+        <v>188.9</v>
       </c>
     </row>
     <row r="22">
@@ -1162,22 +1162,22 @@
         </is>
       </c>
       <c r="B22" s="8" t="n">
-        <v>248.14</v>
+        <v>248.75</v>
       </c>
       <c r="C22" s="10" t="n">
-        <v>242.18</v>
+        <v>237.85</v>
       </c>
       <c r="D22" s="13" t="n">
-        <v>244.3</v>
+        <v>247.5</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>243.81</v>
+        <v>247.97</v>
       </c>
       <c r="F22" s="16" t="n">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>247.7</v>
+        <v>238.2</v>
       </c>
     </row>
     <row r="23">
@@ -1187,22 +1187,22 @@
         </is>
       </c>
       <c r="B23" s="8" t="n">
-        <v>1454.9</v>
+        <v>1468.8</v>
       </c>
       <c r="C23" s="10" t="n">
-        <v>1416</v>
+        <v>1417.8</v>
       </c>
       <c r="D23" s="13" t="n">
-        <v>1454</v>
+        <v>1464</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>1450.65</v>
+        <v>1464.95</v>
       </c>
       <c r="F23" s="16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G23" s="5" t="n">
-        <v>1422.5</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="24">
@@ -1212,22 +1212,22 @@
         </is>
       </c>
       <c r="B24" s="8" t="n">
-        <v>289.45</v>
+        <v>287.8</v>
       </c>
       <c r="C24" s="10" t="n">
-        <v>286.3</v>
+        <v>277.8</v>
       </c>
       <c r="D24" s="13" t="n">
-        <v>288.7</v>
+        <v>287</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>288.85</v>
+        <v>287.15</v>
       </c>
       <c r="F24" s="16" t="n">
-        <v>147</v>
+        <v>100</v>
       </c>
       <c r="G24" s="5" t="n">
-        <v>287.1</v>
+        <v>279.05</v>
       </c>
     </row>
     <row r="25">
@@ -1237,22 +1237,22 @@
         </is>
       </c>
       <c r="B25" s="8" t="n">
-        <v>1498.35</v>
+        <v>1485</v>
       </c>
       <c r="C25" s="10" t="n">
-        <v>1475.85</v>
+        <v>1454.8</v>
       </c>
       <c r="D25" s="13" t="n">
-        <v>1480</v>
+        <v>1473.5</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>1480.45</v>
+        <v>1474.75</v>
       </c>
       <c r="F25" s="16" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G25" s="5" t="n">
-        <v>1496.8</v>
+        <v>1458.25</v>
       </c>
     </row>
     <row r="26">
@@ -1262,22 +1262,22 @@
         </is>
       </c>
       <c r="B26" s="8" t="n">
-        <v>272.6</v>
+        <v>255.8</v>
       </c>
       <c r="C26" s="10" t="n">
-        <v>267.75</v>
+        <v>246.5</v>
       </c>
       <c r="D26" s="13" t="n">
-        <v>271.5</v>
+        <v>253.85</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>271.6</v>
+        <v>253.85</v>
       </c>
       <c r="F26" s="16" t="n">
-        <v>56</v>
+        <v>182</v>
       </c>
       <c r="G26" s="5" t="n">
-        <v>270.2</v>
+        <v>249.35</v>
       </c>
     </row>
     <row r="27">
@@ -1287,22 +1287,22 @@
         </is>
       </c>
       <c r="B27" s="8" t="n">
-        <v>353.35</v>
+        <v>342.55</v>
       </c>
       <c r="C27" s="10" t="n">
-        <v>346.95</v>
+        <v>332.5</v>
       </c>
       <c r="D27" s="13" t="n">
-        <v>352.6</v>
+        <v>339.85</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>352.2</v>
+        <v>339.95</v>
       </c>
       <c r="F27" s="16" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G27" s="5" t="n">
-        <v>348.35</v>
+        <v>334.4</v>
       </c>
     </row>
     <row r="28">
@@ -1312,22 +1312,22 @@
         </is>
       </c>
       <c r="B28" s="8" t="n">
-        <v>6082.95</v>
+        <v>5974.45</v>
       </c>
       <c r="C28" s="10" t="n">
-        <v>5986.95</v>
+        <v>5870</v>
       </c>
       <c r="D28" s="13" t="n">
-        <v>6051.05</v>
+        <v>5870</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>6068.7</v>
+        <v>5887.2</v>
       </c>
       <c r="F28" s="16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G28" s="5" t="n">
-        <v>6032.55</v>
+        <v>5908</v>
       </c>
     </row>
     <row r="29">
@@ -1337,22 +1337,22 @@
         </is>
       </c>
       <c r="B29" s="8" t="n">
-        <v>606</v>
+        <v>597.6</v>
       </c>
       <c r="C29" s="10" t="n">
-        <v>589.45</v>
+        <v>576</v>
       </c>
       <c r="D29" s="13" t="n">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>593.2</v>
+        <v>594.85</v>
       </c>
       <c r="F29" s="16" t="n">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G29" s="5" t="n">
-        <v>605.2</v>
+        <v>585.05</v>
       </c>
     </row>
     <row r="30">
@@ -1362,22 +1362,22 @@
         </is>
       </c>
       <c r="B30" s="8" t="n">
-        <v>105.3</v>
+        <v>104.99</v>
       </c>
       <c r="C30" s="10" t="n">
-        <v>104</v>
+        <v>100.94</v>
       </c>
       <c r="D30" s="13" t="n">
-        <v>104.43</v>
+        <v>104.6</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>104.43</v>
+        <v>104.67</v>
       </c>
       <c r="F30" s="16" t="n">
-        <v>84</v>
+        <v>199</v>
       </c>
       <c r="G30" s="5" t="n">
-        <v>105.14</v>
+        <v>100.97</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
@@ -1387,22 +1387,22 @@
         </is>
       </c>
       <c r="B31" s="8" t="n">
-        <v>897</v>
+        <v>865</v>
       </c>
       <c r="C31" s="10" t="n">
-        <v>877.1</v>
+        <v>842.1</v>
       </c>
       <c r="D31" s="13" t="n">
-        <v>890</v>
+        <v>860</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>890.8</v>
+        <v>861.1</v>
       </c>
       <c r="F31" s="16" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G31" s="5" t="n">
-        <v>878.9</v>
+        <v>845.15</v>
       </c>
     </row>
     <row r="32">
@@ -1412,22 +1412,22 @@
         </is>
       </c>
       <c r="B32" s="8" t="n">
-        <v>505</v>
+        <v>495.85</v>
       </c>
       <c r="C32" s="10" t="n">
-        <v>499.4</v>
+        <v>486.15</v>
       </c>
       <c r="D32" s="13" t="n">
-        <v>504</v>
+        <v>493.5</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>504.1</v>
+        <v>493.05</v>
       </c>
       <c r="F32" s="16" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G32" s="5" t="n">
-        <v>501.3</v>
+        <v>488.1</v>
       </c>
     </row>
     <row r="33">
@@ -1437,22 +1437,22 @@
         </is>
       </c>
       <c r="B33" s="8" t="n">
-        <v>1511.7</v>
+        <v>1468.25</v>
       </c>
       <c r="C33" s="10" t="n">
-        <v>1491.15</v>
+        <v>1431.2</v>
       </c>
       <c r="D33" s="13" t="n">
-        <v>1503.15</v>
+        <v>1463</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>1503.05</v>
+        <v>1460.3</v>
       </c>
       <c r="F33" s="16" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G33" s="5" t="n">
-        <v>1510.75</v>
+        <v>1442.9</v>
       </c>
     </row>
     <row r="34">
@@ -1462,22 +1462,22 @@
         </is>
       </c>
       <c r="B34" s="8" t="n">
-        <v>1600.9</v>
+        <v>1562.05</v>
       </c>
       <c r="C34" s="10" t="n">
-        <v>1568</v>
+        <v>1536.35</v>
       </c>
       <c r="D34" s="13" t="n">
-        <v>1569.8</v>
+        <v>1552</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>1571.75</v>
+        <v>1551.7</v>
       </c>
       <c r="F34" s="16" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G34" s="5" t="n">
-        <v>1597</v>
+        <v>1543.25</v>
       </c>
     </row>
     <row r="35">
@@ -1487,22 +1487,22 @@
         </is>
       </c>
       <c r="B35" s="8" t="n">
-        <v>7585</v>
+        <v>7233.95</v>
       </c>
       <c r="C35" s="10" t="n">
-        <v>7436</v>
+        <v>7130.05</v>
       </c>
       <c r="D35" s="13" t="n">
-        <v>7466.25</v>
+        <v>7219.3</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>7469.95</v>
+        <v>7210.4</v>
       </c>
       <c r="F35" s="16" t="n">
         <v>2</v>
       </c>
       <c r="G35" s="5" t="n">
-        <v>7526.85</v>
+        <v>7173.05</v>
       </c>
     </row>
     <row r="36">
@@ -1512,22 +1512,22 @@
         </is>
       </c>
       <c r="B36" s="8" t="n">
-        <v>889.9</v>
+        <v>876</v>
       </c>
       <c r="C36" s="10" t="n">
-        <v>875.5</v>
+        <v>854.75</v>
       </c>
       <c r="D36" s="13" t="n">
-        <v>887</v>
+        <v>874</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>888.95</v>
+        <v>872.6</v>
       </c>
       <c r="F36" s="16" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G36" s="5" t="n">
-        <v>881.25</v>
+        <v>857.7</v>
       </c>
     </row>
     <row r="37">
@@ -1537,22 +1537,22 @@
         </is>
       </c>
       <c r="B37" s="8" t="n">
-        <v>1635.45</v>
+        <v>1626.25</v>
       </c>
       <c r="C37" s="10" t="n">
-        <v>1614.2</v>
+        <v>1576.15</v>
       </c>
       <c r="D37" s="13" t="n">
-        <v>1628.05</v>
+        <v>1615</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>1631.4</v>
+        <v>1621.1</v>
       </c>
       <c r="F37" s="16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="5" t="n">
-        <v>1630</v>
+        <v>1576.95</v>
       </c>
     </row>
     <row r="38">
@@ -1562,22 +1562,22 @@
         </is>
       </c>
       <c r="B38" s="8" t="n">
-        <v>431.3</v>
+        <v>414.95</v>
       </c>
       <c r="C38" s="10" t="n">
-        <v>424.25</v>
+        <v>406.1</v>
       </c>
       <c r="D38" s="13" t="n">
-        <v>430.1</v>
+        <v>409.85</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>430.05</v>
+        <v>409.05</v>
       </c>
       <c r="F38" s="16" t="n">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="G38" s="5" t="n">
-        <v>427.35</v>
+        <v>410.1</v>
       </c>
     </row>
     <row r="39">
@@ -1587,22 +1587,22 @@
         </is>
       </c>
       <c r="B39" s="8" t="n">
-        <v>3709</v>
+        <v>3715.5</v>
       </c>
       <c r="C39" s="10" t="n">
-        <v>3648.6</v>
+        <v>3640</v>
       </c>
       <c r="D39" s="13" t="n">
-        <v>3658.15</v>
+        <v>3711.8</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>3669.05</v>
+        <v>3710.1</v>
       </c>
       <c r="F39" s="16" t="n">
         <v>2</v>
       </c>
       <c r="G39" s="5" t="n">
-        <v>3692.9</v>
+        <v>3656</v>
       </c>
     </row>
     <row r="40">
@@ -1612,22 +1612,22 @@
         </is>
       </c>
       <c r="B40" s="8" t="n">
-        <v>572.9</v>
+        <v>572.1</v>
       </c>
       <c r="C40" s="10" t="n">
-        <v>567.55</v>
+        <v>564.95</v>
       </c>
       <c r="D40" s="13" t="n">
-        <v>570.4</v>
+        <v>571.2</v>
       </c>
       <c r="E40" s="5" t="n">
-        <v>571</v>
+        <v>571.4</v>
       </c>
       <c r="F40" s="16" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G40" s="5" t="n">
-        <v>568.4</v>
+        <v>567.25</v>
       </c>
     </row>
     <row r="41">
@@ -1637,22 +1637,22 @@
         </is>
       </c>
       <c r="B41" s="8" t="n">
-        <v>1894.65</v>
+        <v>1859.8</v>
       </c>
       <c r="C41" s="10" t="n">
-        <v>1853.7</v>
+        <v>1815</v>
       </c>
       <c r="D41" s="13" t="n">
-        <v>1880</v>
+        <v>1840</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>1885.95</v>
+        <v>1852.15</v>
       </c>
       <c r="F41" s="16" t="n">
         <v>1</v>
       </c>
       <c r="G41" s="5" t="n">
-        <v>1889.2</v>
+        <v>1816.5</v>
       </c>
     </row>
     <row r="42">
@@ -1662,22 +1662,22 @@
         </is>
       </c>
       <c r="B42" s="8" t="n">
-        <v>1059.6</v>
+        <v>1032.4</v>
       </c>
       <c r="C42" s="10" t="n">
-        <v>1043.4</v>
+        <v>1000.9</v>
       </c>
       <c r="D42" s="13" t="n">
-        <v>1044.5</v>
+        <v>1020</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>1046.35</v>
+        <v>1019.8</v>
       </c>
       <c r="F42" s="16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G42" s="5" t="n">
-        <v>1057</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="43">
@@ -1687,22 +1687,22 @@
         </is>
       </c>
       <c r="B43" s="8" t="n">
-        <v>2944</v>
+        <v>2857.65</v>
       </c>
       <c r="C43" s="10" t="n">
-        <v>2870.3</v>
+        <v>2822.1</v>
       </c>
       <c r="D43" s="13" t="n">
-        <v>2935.55</v>
+        <v>2830</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>2932.6</v>
+        <v>2839.4</v>
       </c>
       <c r="F43" s="16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G43" s="5" t="n">
-        <v>2898.85</v>
+        <v>2830.55</v>
       </c>
     </row>
     <row r="44">
@@ -1712,22 +1712,22 @@
         </is>
       </c>
       <c r="B44" s="8" t="n">
-        <v>124</v>
+        <v>121.99</v>
       </c>
       <c r="C44" s="10" t="n">
-        <v>122</v>
+        <v>119.69</v>
       </c>
       <c r="D44" s="13" t="n">
-        <v>122.4</v>
+        <v>121.7</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>122.32</v>
+        <v>121.43</v>
       </c>
       <c r="F44" s="16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G44" s="5" t="n">
-        <v>123.77</v>
+        <v>119.8</v>
       </c>
     </row>
     <row r="45">
@@ -1737,22 +1737,22 @@
         </is>
       </c>
       <c r="B45" s="8" t="n">
-        <v>6275.85</v>
+        <v>6091.9</v>
       </c>
       <c r="C45" s="10" t="n">
-        <v>6020.35</v>
+        <v>6004.65</v>
       </c>
       <c r="D45" s="13" t="n">
-        <v>6103.85</v>
+        <v>6033.5</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>6106.7</v>
+        <v>6022.25</v>
       </c>
       <c r="F45" s="16" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="G45" s="5" t="n">
-        <v>6219.55</v>
+        <v>6040.6</v>
       </c>
     </row>
     <row r="46">
@@ -1762,22 +1762,22 @@
         </is>
       </c>
       <c r="B46" s="8" t="n">
-        <v>15423.95</v>
+        <v>15453.1</v>
       </c>
       <c r="C46" s="10" t="n">
-        <v>15275</v>
+        <v>14921.65</v>
       </c>
       <c r="D46" s="13" t="n">
-        <v>15394.9</v>
+        <v>15370</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>15404.45</v>
+        <v>15381.8</v>
       </c>
       <c r="F46" s="16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G46" s="5" t="n">
-        <v>15335.05</v>
+        <v>14949.95</v>
       </c>
     </row>
     <row r="47">
@@ -1787,22 +1787,22 @@
         </is>
       </c>
       <c r="B47" s="8" t="n">
-        <v>877.25</v>
+        <v>880.35</v>
       </c>
       <c r="C47" s="10" t="n">
-        <v>857.05</v>
+        <v>848.7</v>
       </c>
       <c r="D47" s="13" t="n">
-        <v>875.05</v>
+        <v>874</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>875.45</v>
+        <v>875.15</v>
       </c>
       <c r="F47" s="16" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G47" s="5" t="n">
-        <v>861.95</v>
+        <v>851.25</v>
       </c>
     </row>
     <row r="48">
@@ -1812,22 +1812,22 @@
         </is>
       </c>
       <c r="B48" s="8" t="n">
-        <v>6679.4</v>
+        <v>6774</v>
       </c>
       <c r="C48" s="10" t="n">
-        <v>6605.2</v>
+        <v>6662.4</v>
       </c>
       <c r="D48" s="13" t="n">
-        <v>6620</v>
+        <v>6736.5</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>6611.65</v>
+        <v>6741.1</v>
       </c>
       <c r="F48" s="16" t="n">
         <v>2</v>
       </c>
       <c r="G48" s="5" t="n">
-        <v>6663</v>
+        <v>6671.8</v>
       </c>
     </row>
     <row r="49">
@@ -1837,22 +1837,22 @@
         </is>
       </c>
       <c r="B49" s="8" t="n">
-        <v>3987.15</v>
+        <v>3835.25</v>
       </c>
       <c r="C49" s="10" t="n">
-        <v>3881.6</v>
+        <v>3701</v>
       </c>
       <c r="D49" s="13" t="n">
-        <v>3932</v>
+        <v>3791.6</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>3932</v>
+        <v>3815.4</v>
       </c>
       <c r="F49" s="16" t="n">
         <v>1</v>
       </c>
       <c r="G49" s="5" t="n">
-        <v>3975.6</v>
+        <v>3757.6</v>
       </c>
     </row>
     <row r="50">
@@ -1862,22 +1862,22 @@
         </is>
       </c>
       <c r="B50" s="8" t="n">
-        <v>531.65</v>
+        <v>500.5</v>
       </c>
       <c r="C50" s="10" t="n">
-        <v>519.2</v>
+        <v>486.25</v>
       </c>
       <c r="D50" s="13" t="n">
-        <v>522.3</v>
+        <v>495.25</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>522.15</v>
+        <v>495.8</v>
       </c>
       <c r="F50" s="16" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G50" s="5" t="n">
-        <v>530.8</v>
+        <v>486.5</v>
       </c>
     </row>
     <row r="51">
@@ -1887,22 +1887,22 @@
         </is>
       </c>
       <c r="B51" s="8" t="n">
-        <v>1830</v>
+        <v>1747.2</v>
       </c>
       <c r="C51" s="10" t="n">
-        <v>1794.15</v>
+        <v>1717.5</v>
       </c>
       <c r="D51" s="13" t="n">
-        <v>1803.6</v>
+        <v>1735.5</v>
       </c>
       <c r="E51" s="5" t="n">
-        <v>1804.9</v>
+        <v>1738.45</v>
       </c>
       <c r="F51" s="16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G51" s="5" t="n">
-        <v>1813.95</v>
+        <v>1727.4</v>
       </c>
     </row>
     <row r="52">
@@ -1912,22 +1912,22 @@
         </is>
       </c>
       <c r="B52" s="8" t="n">
-        <v>1219.9</v>
+        <v>1143.7</v>
       </c>
       <c r="C52" s="10" t="n">
-        <v>1161.2</v>
+        <v>1092.05</v>
       </c>
       <c r="D52" s="13" t="n">
-        <v>1197.5</v>
+        <v>1126.15</v>
       </c>
       <c r="E52" s="5" t="n">
-        <v>1202.7</v>
+        <v>1130</v>
       </c>
       <c r="F52" s="16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G52" s="5" t="n">
-        <v>1172.9</v>
+        <v>1094.65</v>
       </c>
     </row>
     <row r="53">
@@ -1937,22 +1937,22 @@
         </is>
       </c>
       <c r="B53" s="8" t="n">
-        <v>650</v>
+        <v>644.7</v>
       </c>
       <c r="C53" s="10" t="n">
-        <v>640.25</v>
+        <v>627.1</v>
       </c>
       <c r="D53" s="13" t="n">
-        <v>645.6</v>
+        <v>642.05</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>645.65</v>
+        <v>641.6</v>
       </c>
       <c r="F53" s="16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G53" s="5" t="n">
-        <v>647.35</v>
+        <v>628</v>
       </c>
     </row>
     <row r="54">
@@ -1962,22 +1962,22 @@
         </is>
       </c>
       <c r="B54" s="8" t="n">
-        <v>1346.15</v>
+        <v>1348</v>
       </c>
       <c r="C54" s="10" t="n">
-        <v>1320.2</v>
+        <v>1333</v>
       </c>
       <c r="D54" s="13" t="n">
-        <v>1343.1</v>
+        <v>1333</v>
       </c>
       <c r="E54" s="5" t="n">
-        <v>1342.45</v>
+        <v>1336.15</v>
       </c>
       <c r="F54" s="16" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G54" s="5" t="n">
-        <v>1321.45</v>
+        <v>1341.05</v>
       </c>
     </row>
     <row r="55">
@@ -1987,22 +1987,22 @@
         </is>
       </c>
       <c r="B55" s="8" t="n">
-        <v>3165</v>
+        <v>3150</v>
       </c>
       <c r="C55" s="10" t="n">
-        <v>3037</v>
+        <v>3001</v>
       </c>
       <c r="D55" s="13" t="n">
-        <v>3161.7</v>
+        <v>3125</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>3146.65</v>
+        <v>3133.65</v>
       </c>
       <c r="F55" s="16" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G55" s="5" t="n">
-        <v>3087.2</v>
+        <v>3029</v>
       </c>
     </row>
     <row r="56">
@@ -2012,22 +2012,22 @@
         </is>
       </c>
       <c r="B56" s="8" t="n">
-        <v>607.65</v>
+        <v>601.95</v>
       </c>
       <c r="C56" s="10" t="n">
-        <v>595.05</v>
+        <v>579.5</v>
       </c>
       <c r="D56" s="13" t="n">
-        <v>600.1</v>
+        <v>595.1</v>
       </c>
       <c r="E56" s="5" t="n">
-        <v>599.65</v>
+        <v>597.25</v>
       </c>
       <c r="F56" s="16" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G56" s="5" t="n">
-        <v>606.45</v>
+        <v>580.25</v>
       </c>
     </row>
     <row r="57">
@@ -2037,22 +2037,22 @@
         </is>
       </c>
       <c r="B57" s="8" t="n">
-        <v>2747.95</v>
+        <v>2766</v>
       </c>
       <c r="C57" s="10" t="n">
-        <v>2700.7</v>
+        <v>2674.65</v>
       </c>
       <c r="D57" s="13" t="n">
-        <v>2727.55</v>
+        <v>2746</v>
       </c>
       <c r="E57" s="5" t="n">
-        <v>2735.8</v>
+        <v>2760.95</v>
       </c>
       <c r="F57" s="16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G57" s="5" t="n">
-        <v>2739.75</v>
+        <v>2682.05</v>
       </c>
     </row>
     <row r="58">
@@ -2062,22 +2062,22 @@
         </is>
       </c>
       <c r="B58" s="8" t="n">
-        <v>594.95</v>
+        <v>566.55</v>
       </c>
       <c r="C58" s="10" t="n">
-        <v>584.3</v>
+        <v>543.35</v>
       </c>
       <c r="D58" s="13" t="n">
-        <v>588</v>
+        <v>563.4</v>
       </c>
       <c r="E58" s="5" t="n">
-        <v>585.9</v>
+        <v>563</v>
       </c>
       <c r="F58" s="16" t="n">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G58" s="5" t="n">
-        <v>591.5</v>
+        <v>545</v>
       </c>
     </row>
     <row r="59">
@@ -2087,22 +2087,22 @@
         </is>
       </c>
       <c r="B59" s="8" t="n">
-        <v>4597.9</v>
+        <v>4559</v>
       </c>
       <c r="C59" s="10" t="n">
-        <v>4505.75</v>
+        <v>4423.25</v>
       </c>
       <c r="D59" s="13" t="n">
-        <v>4574.05</v>
+        <v>4528</v>
       </c>
       <c r="E59" s="5" t="n">
-        <v>4575.4</v>
+        <v>4524.7</v>
       </c>
       <c r="F59" s="16" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G59" s="5" t="n">
-        <v>4523.25</v>
+        <v>4430.75</v>
       </c>
     </row>
     <row r="60">
@@ -2112,22 +2112,22 @@
         </is>
       </c>
       <c r="B60" s="8" t="n">
-        <v>1943.5</v>
+        <v>1865</v>
       </c>
       <c r="C60" s="10" t="n">
-        <v>1921.6</v>
+        <v>1772.4</v>
       </c>
       <c r="D60" s="13" t="n">
-        <v>1932.9</v>
+        <v>1845.05</v>
       </c>
       <c r="E60" s="5" t="n">
-        <v>1934.7</v>
+        <v>1849.7</v>
       </c>
       <c r="F60" s="16" t="n">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="G60" s="5" t="n">
-        <v>1941.65</v>
+        <v>1786.6</v>
       </c>
     </row>
     <row r="61">
@@ -2137,22 +2137,22 @@
         </is>
       </c>
       <c r="B61" s="8" t="n">
-        <v>1882.75</v>
+        <v>1870.5</v>
       </c>
       <c r="C61" s="10" t="n">
-        <v>1852.5</v>
+        <v>1843</v>
       </c>
       <c r="D61" s="13" t="n">
-        <v>1866</v>
+        <v>1856.55</v>
       </c>
       <c r="E61" s="5" t="n">
-        <v>1870.1</v>
+        <v>1857.7</v>
       </c>
       <c r="F61" s="16" t="n">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="G61" s="5" t="n">
-        <v>1873.1</v>
+        <v>1862.95</v>
       </c>
     </row>
     <row r="62">
@@ -2162,22 +2162,22 @@
         </is>
       </c>
       <c r="B62" s="8" t="n">
-        <v>4604.25</v>
+        <v>4750.2</v>
       </c>
       <c r="C62" s="10" t="n">
-        <v>4465.15</v>
+        <v>4605</v>
       </c>
       <c r="D62" s="13" t="n">
-        <v>4560</v>
+        <v>4708.9</v>
       </c>
       <c r="E62" s="5" t="n">
-        <v>4555.1</v>
+        <v>4709.75</v>
       </c>
       <c r="F62" s="16" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G62" s="5" t="n">
-        <v>4496.5</v>
+        <v>4610.7</v>
       </c>
     </row>
     <row r="63">
@@ -2187,22 +2187,22 @@
         </is>
       </c>
       <c r="B63" s="8" t="n">
-        <v>746.45</v>
+        <v>744</v>
       </c>
       <c r="C63" s="10" t="n">
-        <v>711.3</v>
+        <v>721.45</v>
       </c>
       <c r="D63" s="13" t="n">
-        <v>714.05</v>
+        <v>743.55</v>
       </c>
       <c r="E63" s="5" t="n">
-        <v>714.25</v>
+        <v>742.45</v>
       </c>
       <c r="F63" s="16" t="n">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="G63" s="5" t="n">
-        <v>742.45</v>
+        <v>722.05</v>
       </c>
     </row>
     <row r="64">
@@ -2212,22 +2212,22 @@
         </is>
       </c>
       <c r="B64" s="8" t="n">
-        <v>738.9</v>
+        <v>756.45</v>
       </c>
       <c r="C64" s="10" t="n">
-        <v>720.65</v>
+        <v>725.5</v>
       </c>
       <c r="D64" s="13" t="n">
-        <v>726.75</v>
+        <v>753.2</v>
       </c>
       <c r="E64" s="5" t="n">
-        <v>726.95</v>
+        <v>753.5</v>
       </c>
       <c r="F64" s="16" t="n">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="G64" s="5" t="n">
-        <v>738.3</v>
+        <v>725.6</v>
       </c>
     </row>
     <row r="65">
@@ -2237,22 +2237,22 @@
         </is>
       </c>
       <c r="B65" s="8" t="n">
-        <v>325.45</v>
+        <v>326.5</v>
       </c>
       <c r="C65" s="10" t="n">
-        <v>316.9</v>
+        <v>306.9</v>
       </c>
       <c r="D65" s="13" t="n">
-        <v>317.95</v>
+        <v>321</v>
       </c>
       <c r="E65" s="5" t="n">
-        <v>320.9</v>
+        <v>323</v>
       </c>
       <c r="F65" s="16" t="n">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="G65" s="5" t="n">
-        <v>323.6</v>
+        <v>310</v>
       </c>
     </row>
     <row r="66">
@@ -2262,22 +2262,22 @@
         </is>
       </c>
       <c r="B66" s="8" t="n">
-        <v>2134.25</v>
+        <v>2041</v>
       </c>
       <c r="C66" s="10" t="n">
-        <v>2083.05</v>
+        <v>2001.05</v>
       </c>
       <c r="D66" s="13" t="n">
-        <v>2100.2</v>
+        <v>2011</v>
       </c>
       <c r="E66" s="5" t="n">
-        <v>2103.2</v>
+        <v>2020.95</v>
       </c>
       <c r="F66" s="16" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G66" s="5" t="n">
-        <v>2088.2</v>
+        <v>2017.85</v>
       </c>
     </row>
     <row r="67">
@@ -2287,22 +2287,22 @@
         </is>
       </c>
       <c r="B67" s="8" t="n">
-        <v>759.45</v>
+        <v>748.6</v>
       </c>
       <c r="C67" s="10" t="n">
-        <v>728.05</v>
+        <v>724.75</v>
       </c>
       <c r="D67" s="13" t="n">
-        <v>734.8</v>
+        <v>745.05</v>
       </c>
       <c r="E67" s="5" t="n">
-        <v>733.75</v>
+        <v>745.35</v>
       </c>
       <c r="F67" s="16" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G67" s="5" t="n">
-        <v>743.15</v>
+        <v>725.15</v>
       </c>
     </row>
     <row r="68">
@@ -2312,22 +2312,22 @@
         </is>
       </c>
       <c r="B68" s="8" t="n">
-        <v>194.26</v>
+        <v>192.5</v>
       </c>
       <c r="C68" s="10" t="n">
-        <v>189.3</v>
+        <v>186.71</v>
       </c>
       <c r="D68" s="13" t="n">
-        <v>191.87</v>
+        <v>190.92</v>
       </c>
       <c r="E68" s="5" t="n">
-        <v>191.6</v>
+        <v>190.96</v>
       </c>
       <c r="F68" s="16" t="n">
-        <v>162</v>
+        <v>52</v>
       </c>
       <c r="G68" s="5" t="n">
-        <v>192.91</v>
+        <v>186.9</v>
       </c>
     </row>
     <row r="69">
@@ -2337,22 +2337,22 @@
         </is>
       </c>
       <c r="B69" s="8" t="n">
-        <v>527.95</v>
+        <v>466.25</v>
       </c>
       <c r="C69" s="10" t="n">
-        <v>516</v>
+        <v>439.35</v>
       </c>
       <c r="D69" s="13" t="n">
-        <v>524.2</v>
+        <v>452.8</v>
       </c>
       <c r="E69" s="5" t="n">
-        <v>524.65</v>
+        <v>451.7</v>
       </c>
       <c r="F69" s="16" t="n">
-        <v>19</v>
+        <v>183</v>
       </c>
       <c r="G69" s="5" t="n">
-        <v>520</v>
+        <v>455.75</v>
       </c>
     </row>
     <row r="70">
@@ -2362,22 +2362,22 @@
         </is>
       </c>
       <c r="B70" s="8" t="n">
-        <v>713.95</v>
+        <v>693</v>
       </c>
       <c r="C70" s="10" t="n">
-        <v>702.6</v>
+        <v>680.4</v>
       </c>
       <c r="D70" s="13" t="n">
-        <v>712.1</v>
+        <v>686.55</v>
       </c>
       <c r="E70" s="5" t="n">
-        <v>712.6</v>
+        <v>686.7</v>
       </c>
       <c r="F70" s="16" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="G70" s="5" t="n">
-        <v>708.5</v>
+        <v>681.35</v>
       </c>
     </row>
     <row r="71">
@@ -2390,19 +2390,19 @@
         <v>362.9</v>
       </c>
       <c r="C71" s="10" t="n">
-        <v>361.8</v>
+        <v>358.1</v>
       </c>
       <c r="D71" s="13" t="n">
-        <v>362.5</v>
+        <v>361.6</v>
       </c>
       <c r="E71" s="5" t="n">
-        <v>362.5</v>
+        <v>362</v>
       </c>
       <c r="F71" s="16" t="n">
         <v>5</v>
       </c>
       <c r="G71" s="5" t="n">
-        <v>362.25</v>
+        <v>358.1</v>
       </c>
     </row>
     <row r="72">
@@ -2412,22 +2412,22 @@
         </is>
       </c>
       <c r="B72" s="8" t="n">
-        <v>3117.1</v>
+        <v>3066.6</v>
       </c>
       <c r="C72" s="10" t="n">
-        <v>3030</v>
+        <v>2969.05</v>
       </c>
       <c r="D72" s="13" t="n">
-        <v>3040</v>
+        <v>2983</v>
       </c>
       <c r="E72" s="5" t="n">
-        <v>3040.55</v>
+        <v>3013.15</v>
       </c>
       <c r="F72" s="16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G72" s="5" t="n">
-        <v>3115.1</v>
+        <v>3000.3</v>
       </c>
     </row>
     <row r="73">
@@ -2437,22 +2437,22 @@
         </is>
       </c>
       <c r="B73" s="8" t="n">
-        <v>4777.7</v>
+        <v>4697</v>
       </c>
       <c r="C73" s="10" t="n">
-        <v>4701</v>
+        <v>4581.85</v>
       </c>
       <c r="D73" s="13" t="n">
-        <v>4745</v>
+        <v>4647.8</v>
       </c>
       <c r="E73" s="5" t="n">
-        <v>4756.45</v>
+        <v>4663.05</v>
       </c>
       <c r="F73" s="16" t="n">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="G73" s="5" t="n">
-        <v>4771.15</v>
+        <v>4581.9</v>
       </c>
     </row>
     <row r="74">
@@ -2462,22 +2462,22 @@
         </is>
       </c>
       <c r="B74" s="8" t="n">
-        <v>1372</v>
+        <v>1354.95</v>
       </c>
       <c r="C74" s="10" t="n">
-        <v>1349.45</v>
+        <v>1331.5</v>
       </c>
       <c r="D74" s="13" t="n">
-        <v>1360.95</v>
+        <v>1347.95</v>
       </c>
       <c r="E74" s="5" t="n">
-        <v>1360.9</v>
+        <v>1347.25</v>
       </c>
       <c r="F74" s="16" t="n">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="G74" s="5" t="n">
-        <v>1370.1</v>
+        <v>1333.85</v>
       </c>
     </row>
     <row r="75">
@@ -2487,22 +2487,22 @@
         </is>
       </c>
       <c r="B75" s="8" t="n">
-        <v>388.95</v>
+        <v>386.35</v>
       </c>
       <c r="C75" s="10" t="n">
-        <v>381.55</v>
+        <v>378.25</v>
       </c>
       <c r="D75" s="13" t="n">
-        <v>385.15</v>
+        <v>384.4</v>
       </c>
       <c r="E75" s="5" t="n">
-        <v>385.9</v>
+        <v>384.55</v>
       </c>
       <c r="F75" s="16" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G75" s="5" t="n">
-        <v>385.75</v>
+        <v>378.75</v>
       </c>
     </row>
     <row r="76">
@@ -2512,22 +2512,22 @@
         </is>
       </c>
       <c r="B76" s="8" t="n">
-        <v>897.05</v>
+        <v>867.5</v>
       </c>
       <c r="C76" s="10" t="n">
-        <v>874</v>
+        <v>854</v>
       </c>
       <c r="D76" s="13" t="n">
-        <v>890.65</v>
+        <v>855</v>
       </c>
       <c r="E76" s="5" t="n">
-        <v>894.2</v>
+        <v>858.75</v>
       </c>
       <c r="F76" s="16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G76" s="5" t="n">
-        <v>884.95</v>
+        <v>860.1</v>
       </c>
     </row>
     <row r="77">
@@ -2537,22 +2537,22 @@
         </is>
       </c>
       <c r="B77" s="8" t="n">
-        <v>1708.65</v>
+        <v>1673.55</v>
       </c>
       <c r="C77" s="10" t="n">
-        <v>1676.4</v>
+        <v>1631.35</v>
       </c>
       <c r="D77" s="13" t="n">
-        <v>1702</v>
+        <v>1647</v>
       </c>
       <c r="E77" s="5" t="n">
-        <v>1703.25</v>
+        <v>1649.85</v>
       </c>
       <c r="F77" s="16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G77" s="5" t="n">
-        <v>1681.45</v>
+        <v>1634.1</v>
       </c>
     </row>
     <row r="78">
@@ -2562,22 +2562,22 @@
         </is>
       </c>
       <c r="B78" s="8" t="n">
-        <v>987.6</v>
+        <v>973.2</v>
       </c>
       <c r="C78" s="10" t="n">
+        <v>923.7</v>
+      </c>
+      <c r="D78" s="13" t="n">
         <v>965</v>
       </c>
-      <c r="D78" s="13" t="n">
-        <v>968</v>
-      </c>
       <c r="E78" s="5" t="n">
-        <v>968.7</v>
+        <v>964.5</v>
       </c>
       <c r="F78" s="16" t="n">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="G78" s="5" t="n">
-        <v>983</v>
+        <v>924</v>
       </c>
     </row>
     <row r="79">
@@ -2587,22 +2587,22 @@
         </is>
       </c>
       <c r="B79" s="8" t="n">
-        <v>4335</v>
+        <v>4319</v>
       </c>
       <c r="C79" s="10" t="n">
-        <v>4253.5</v>
+        <v>4227.55</v>
       </c>
       <c r="D79" s="13" t="n">
-        <v>4330.9</v>
+        <v>4299</v>
       </c>
       <c r="E79" s="5" t="n">
-        <v>4323.65</v>
+        <v>4302.7</v>
       </c>
       <c r="F79" s="16" t="n">
         <v>0</v>
       </c>
       <c r="G79" s="5" t="n">
-        <v>4305.25</v>
+        <v>4227.85</v>
       </c>
     </row>
     <row r="80">
@@ -2612,22 +2612,22 @@
         </is>
       </c>
       <c r="B80" s="8" t="n">
-        <v>1010.35</v>
+        <v>998.25</v>
       </c>
       <c r="C80" s="10" t="n">
-        <v>992</v>
+        <v>973.1</v>
       </c>
       <c r="D80" s="13" t="n">
-        <v>1001.8</v>
+        <v>995</v>
       </c>
       <c r="E80" s="5" t="n">
-        <v>1000.85</v>
+        <v>992.6</v>
       </c>
       <c r="F80" s="16" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G80" s="5" t="n">
-        <v>1009.85</v>
+        <v>974.25</v>
       </c>
     </row>
     <row r="81">
@@ -2637,22 +2637,22 @@
         </is>
       </c>
       <c r="B81" s="8" t="n">
-        <v>627.95</v>
+        <v>628.55</v>
       </c>
       <c r="C81" s="10" t="n">
-        <v>617.2</v>
+        <v>605.35</v>
       </c>
       <c r="D81" s="13" t="n">
-        <v>627.95</v>
+        <v>623.45</v>
       </c>
       <c r="E81" s="5" t="n">
-        <v>626.6</v>
+        <v>625</v>
       </c>
       <c r="F81" s="16" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G81" s="5" t="n">
-        <v>622</v>
+        <v>607.3</v>
       </c>
     </row>
     <row r="82">
@@ -2662,22 +2662,22 @@
         </is>
       </c>
       <c r="B82" s="8" t="n">
-        <v>1911.1</v>
+        <v>1878.5</v>
       </c>
       <c r="C82" s="10" t="n">
-        <v>1887.45</v>
+        <v>1851</v>
       </c>
       <c r="D82" s="13" t="n">
-        <v>1895.4</v>
+        <v>1871.85</v>
       </c>
       <c r="E82" s="5" t="n">
-        <v>1895.2</v>
+        <v>1871.05</v>
       </c>
       <c r="F82" s="16" t="n">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G82" s="5" t="n">
-        <v>1905.75</v>
+        <v>1852.9</v>
       </c>
     </row>
     <row r="83">
@@ -2687,22 +2687,22 @@
         </is>
       </c>
       <c r="B83" s="8" t="n">
-        <v>3425.95</v>
+        <v>3382.75</v>
       </c>
       <c r="C83" s="10" t="n">
-        <v>3366.95</v>
+        <v>3334.05</v>
       </c>
       <c r="D83" s="13" t="n">
-        <v>3404.5</v>
+        <v>3355</v>
       </c>
       <c r="E83" s="5" t="n">
-        <v>3391.35</v>
+        <v>3356.1</v>
       </c>
       <c r="F83" s="16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G83" s="5" t="n">
-        <v>3421.35</v>
+        <v>3348.35</v>
       </c>
     </row>
     <row r="84">
@@ -2712,22 +2712,22 @@
         </is>
       </c>
       <c r="B84" s="8" t="n">
-        <v>486.5</v>
+        <v>482.25</v>
       </c>
       <c r="C84" s="10" t="n">
-        <v>474.3</v>
+        <v>461.7</v>
       </c>
       <c r="D84" s="13" t="n">
-        <v>482.5</v>
+        <v>475.45</v>
       </c>
       <c r="E84" s="5" t="n">
-        <v>482</v>
+        <v>475.15</v>
       </c>
       <c r="F84" s="16" t="n">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="G84" s="5" t="n">
-        <v>480.7</v>
+        <v>462.75</v>
       </c>
     </row>
     <row r="85">
@@ -2737,22 +2737,22 @@
         </is>
       </c>
       <c r="B85" s="8" t="n">
-        <v>627.9</v>
+        <v>619.9</v>
       </c>
       <c r="C85" s="10" t="n">
-        <v>621.1</v>
+        <v>602.25</v>
       </c>
       <c r="D85" s="13" t="n">
-        <v>627.15</v>
+        <v>619.6</v>
       </c>
       <c r="E85" s="5" t="n">
-        <v>625.95</v>
+        <v>618.6</v>
       </c>
       <c r="F85" s="16" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G85" s="5" t="n">
-        <v>623.8</v>
+        <v>602.55</v>
       </c>
     </row>
     <row r="86">
@@ -2762,22 +2762,22 @@
         </is>
       </c>
       <c r="B86" s="8" t="n">
-        <v>6551.7</v>
+        <v>6240.45</v>
       </c>
       <c r="C86" s="10" t="n">
-        <v>6440.05</v>
+        <v>5960</v>
       </c>
       <c r="D86" s="13" t="n">
-        <v>6450</v>
+        <v>6007</v>
       </c>
       <c r="E86" s="5" t="n">
-        <v>6460.8</v>
+        <v>5991.7</v>
       </c>
       <c r="F86" s="16" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G86" s="5" t="n">
-        <v>6540</v>
+        <v>6204.1</v>
       </c>
     </row>
     <row r="87">
@@ -2787,22 +2787,22 @@
         </is>
       </c>
       <c r="B87" s="8" t="n">
-        <v>5327.05</v>
+        <v>5284</v>
       </c>
       <c r="C87" s="10" t="n">
-        <v>5252</v>
+        <v>5118.05</v>
       </c>
       <c r="D87" s="13" t="n">
-        <v>5320</v>
+        <v>5151.2</v>
       </c>
       <c r="E87" s="5" t="n">
-        <v>5318.6</v>
+        <v>5132.1</v>
       </c>
       <c r="F87" s="16" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G87" s="5" t="n">
-        <v>5323</v>
+        <v>5256.45</v>
       </c>
     </row>
     <row r="88">
@@ -2812,22 +2812,22 @@
         </is>
       </c>
       <c r="B88" s="8" t="n">
-        <v>2272.9</v>
+        <v>2196.7</v>
       </c>
       <c r="C88" s="10" t="n">
-        <v>2242.45</v>
+        <v>2153.65</v>
       </c>
       <c r="D88" s="13" t="n">
-        <v>2248.55</v>
+        <v>2180.5</v>
       </c>
       <c r="E88" s="5" t="n">
-        <v>2250.9</v>
+        <v>2179.7</v>
       </c>
       <c r="F88" s="16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G88" s="5" t="n">
-        <v>2254.35</v>
+        <v>2158.5</v>
       </c>
     </row>
     <row r="89">
@@ -2837,22 +2837,22 @@
         </is>
       </c>
       <c r="B89" s="8" t="n">
-        <v>288.3</v>
+        <v>293.4</v>
       </c>
       <c r="C89" s="10" t="n">
-        <v>283.1</v>
+        <v>280</v>
       </c>
       <c r="D89" s="13" t="n">
-        <v>288</v>
+        <v>291.1</v>
       </c>
       <c r="E89" s="5" t="n">
-        <v>286.4</v>
+        <v>291</v>
       </c>
       <c r="F89" s="16" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="G89" s="5" t="n">
-        <v>285.95</v>
+        <v>280.5</v>
       </c>
     </row>
     <row r="90">
@@ -2862,22 +2862,22 @@
         </is>
       </c>
       <c r="B90" s="8" t="n">
-        <v>186.95</v>
+        <v>159.59</v>
       </c>
       <c r="C90" s="10" t="n">
-        <v>181.5</v>
+        <v>145.42</v>
       </c>
       <c r="D90" s="13" t="n">
-        <v>183.59</v>
+        <v>154.3</v>
       </c>
       <c r="E90" s="5" t="n">
-        <v>183.2</v>
+        <v>153.27</v>
       </c>
       <c r="F90" s="16" t="n">
-        <v>48</v>
+        <v>807</v>
       </c>
       <c r="G90" s="5" t="n">
-        <v>185.51</v>
+        <v>159.59</v>
       </c>
     </row>
     <row r="91">
@@ -2887,22 +2887,22 @@
         </is>
       </c>
       <c r="B91" s="8" t="n">
-        <v>692.5</v>
+        <v>673.8</v>
       </c>
       <c r="C91" s="10" t="n">
-        <v>680.75</v>
+        <v>654.6</v>
       </c>
       <c r="D91" s="13" t="n">
-        <v>685</v>
+        <v>667.45</v>
       </c>
       <c r="E91" s="5" t="n">
-        <v>685.7</v>
+        <v>669.3</v>
       </c>
       <c r="F91" s="16" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G91" s="5" t="n">
-        <v>686.8</v>
+        <v>657.1</v>
       </c>
     </row>
     <row r="92">
@@ -2912,22 +2912,22 @@
         </is>
       </c>
       <c r="B92" s="8" t="n">
-        <v>1552.3</v>
+        <v>1526.95</v>
       </c>
       <c r="C92" s="10" t="n">
-        <v>1521.35</v>
+        <v>1502</v>
       </c>
       <c r="D92" s="13" t="n">
-        <v>1550</v>
+        <v>1515</v>
       </c>
       <c r="E92" s="5" t="n">
-        <v>1547.8</v>
+        <v>1519.25</v>
       </c>
       <c r="F92" s="16" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G92" s="5" t="n">
-        <v>1531</v>
+        <v>1509.95</v>
       </c>
     </row>
     <row r="93">
@@ -2937,22 +2937,22 @@
         </is>
       </c>
       <c r="B93" s="8" t="n">
-        <v>6547.75</v>
+        <v>6605.95</v>
       </c>
       <c r="C93" s="10" t="n">
-        <v>6424.4</v>
+        <v>6285.35</v>
       </c>
       <c r="D93" s="13" t="n">
-        <v>6535</v>
+        <v>6575</v>
       </c>
       <c r="E93" s="5" t="n">
-        <v>6511</v>
+        <v>6561.15</v>
       </c>
       <c r="F93" s="16" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G93" s="5" t="n">
-        <v>6467</v>
+        <v>6290.35</v>
       </c>
     </row>
     <row r="94">
@@ -2962,22 +2962,22 @@
         </is>
       </c>
       <c r="B94" s="8" t="n">
-        <v>2272</v>
+        <v>2218</v>
       </c>
       <c r="C94" s="10" t="n">
-        <v>2235.1</v>
+        <v>2190.55</v>
       </c>
       <c r="D94" s="13" t="n">
-        <v>2258</v>
+        <v>2192</v>
       </c>
       <c r="E94" s="5" t="n">
-        <v>2259.55</v>
+        <v>2205.65</v>
       </c>
       <c r="F94" s="16" t="n">
         <v>0</v>
       </c>
       <c r="G94" s="5" t="n">
-        <v>2267.55</v>
+        <v>2190.55</v>
       </c>
     </row>
     <row r="95">
@@ -2987,22 +2987,22 @@
         </is>
       </c>
       <c r="B95" s="8" t="n">
-        <v>1205.5</v>
+        <v>1202.5</v>
       </c>
       <c r="C95" s="10" t="n">
-        <v>1173.7</v>
+        <v>1162.85</v>
       </c>
       <c r="D95" s="13" t="n">
-        <v>1189</v>
+        <v>1195</v>
       </c>
       <c r="E95" s="5" t="n">
-        <v>1183.85</v>
+        <v>1196.65</v>
       </c>
       <c r="F95" s="16" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G95" s="5" t="n">
-        <v>1201.8</v>
+        <v>1164.25</v>
       </c>
     </row>
     <row r="96">
@@ -3012,22 +3012,22 @@
         </is>
       </c>
       <c r="B96" s="8" t="n">
-        <v>1857</v>
+        <v>1637.2</v>
       </c>
       <c r="C96" s="10" t="n">
-        <v>1802.55</v>
+        <v>1503.75</v>
       </c>
       <c r="D96" s="13" t="n">
-        <v>1832</v>
+        <v>1587</v>
       </c>
       <c r="E96" s="5" t="n">
-        <v>1833.4</v>
+        <v>1582.25</v>
       </c>
       <c r="F96" s="16" t="n">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="G96" s="5" t="n">
-        <v>1807.7</v>
+        <v>1590.65</v>
       </c>
     </row>
     <row r="97">
@@ -3037,22 +3037,22 @@
         </is>
       </c>
       <c r="B97" s="8" t="n">
-        <v>3012.9</v>
+        <v>3108.9</v>
       </c>
       <c r="C97" s="10" t="n">
-        <v>2890</v>
+        <v>3002.4</v>
       </c>
       <c r="D97" s="13" t="n">
-        <v>2933</v>
+        <v>3096</v>
       </c>
       <c r="E97" s="5" t="n">
-        <v>2929.8</v>
+        <v>3095.75</v>
       </c>
       <c r="F97" s="16" t="n">
         <v>9</v>
       </c>
       <c r="G97" s="5" t="n">
-        <v>2996</v>
+        <v>3064.3</v>
       </c>
     </row>
     <row r="98">
@@ -3062,22 +3062,22 @@
         </is>
       </c>
       <c r="B98" s="8" t="n">
-        <v>1974</v>
+        <v>1983.95</v>
       </c>
       <c r="C98" s="10" t="n">
-        <v>1943.6</v>
+        <v>1923.7</v>
       </c>
       <c r="D98" s="13" t="n">
-        <v>1963</v>
+        <v>1965</v>
       </c>
       <c r="E98" s="5" t="n">
-        <v>1956.95</v>
+        <v>1968.75</v>
       </c>
       <c r="F98" s="16" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G98" s="5" t="n">
-        <v>1954.4</v>
+        <v>1938.5</v>
       </c>
     </row>
     <row r="99">
@@ -3087,22 +3087,22 @@
         </is>
       </c>
       <c r="B99" s="8" t="n">
-        <v>715</v>
+        <v>715.9</v>
       </c>
       <c r="C99" s="10" t="n">
-        <v>697.2</v>
+        <v>690</v>
       </c>
       <c r="D99" s="13" t="n">
-        <v>708</v>
+        <v>702</v>
       </c>
       <c r="E99" s="5" t="n">
-        <v>707.05</v>
+        <v>703.4</v>
       </c>
       <c r="F99" s="16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G99" s="5" t="n">
-        <v>708.4</v>
+        <v>690</v>
       </c>
     </row>
     <row r="100">
@@ -3112,22 +3112,22 @@
         </is>
       </c>
       <c r="B100" s="8" t="n">
-        <v>8362.299999999999</v>
+        <v>8110.2</v>
       </c>
       <c r="C100" s="10" t="n">
-        <v>8229.85</v>
+        <v>7951</v>
       </c>
       <c r="D100" s="13" t="n">
-        <v>8265</v>
+        <v>8110.2</v>
       </c>
       <c r="E100" s="5" t="n">
-        <v>8288.4</v>
+        <v>8088.85</v>
       </c>
       <c r="F100" s="16" t="n">
         <v>1</v>
       </c>
       <c r="G100" s="5" t="n">
-        <v>8350.049999999999</v>
+        <v>8008.55</v>
       </c>
     </row>
     <row r="101">
@@ -3137,22 +3137,22 @@
         </is>
       </c>
       <c r="B101" s="8" t="n">
-        <v>3385.25</v>
+        <v>3384</v>
       </c>
       <c r="C101" s="10" t="n">
-        <v>3319.5</v>
+        <v>3288.05</v>
       </c>
       <c r="D101" s="13" t="n">
-        <v>3362</v>
+        <v>3360.1</v>
       </c>
       <c r="E101" s="5" t="n">
-        <v>3359.3</v>
+        <v>3375.65</v>
       </c>
       <c r="F101" s="16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G101" s="5" t="n">
-        <v>3350.3</v>
+        <v>3291.55</v>
       </c>
     </row>
     <row r="102">
@@ -3162,22 +3162,22 @@
         </is>
       </c>
       <c r="B102" s="8" t="n">
-        <v>235.83</v>
+        <v>232.4</v>
       </c>
       <c r="C102" s="10" t="n">
-        <v>231.17</v>
+        <v>219.65</v>
       </c>
       <c r="D102" s="13" t="n">
-        <v>231.75</v>
+        <v>231.5</v>
       </c>
       <c r="E102" s="5" t="n">
-        <v>232.08</v>
+        <v>231.44</v>
       </c>
       <c r="F102" s="16" t="n">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="G102" s="5" t="n">
-        <v>234.89</v>
+        <v>220.77</v>
       </c>
     </row>
     <row r="103">
@@ -3187,22 +3187,22 @@
         </is>
       </c>
       <c r="B103" s="8" t="n">
-        <v>427.2</v>
+        <v>425.95</v>
       </c>
       <c r="C103" s="10" t="n">
-        <v>423.9</v>
+        <v>414.85</v>
       </c>
       <c r="D103" s="13" t="n">
-        <v>425.8</v>
+        <v>425.1</v>
       </c>
       <c r="E103" s="5" t="n">
-        <v>426.6</v>
+        <v>424.95</v>
       </c>
       <c r="F103" s="16" t="n">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G103" s="5" t="n">
-        <v>424.15</v>
+        <v>414.95</v>
       </c>
     </row>
     <row r="104">
@@ -3212,22 +3212,22 @@
         </is>
       </c>
       <c r="B104" s="8" t="n">
-        <v>2040.5</v>
+        <v>1942</v>
       </c>
       <c r="C104" s="10" t="n">
-        <v>1971</v>
+        <v>1884.35</v>
       </c>
       <c r="D104" s="13" t="n">
-        <v>2037.95</v>
+        <v>1930.95</v>
       </c>
       <c r="E104" s="5" t="n">
-        <v>2028.9</v>
+        <v>1931.5</v>
       </c>
       <c r="F104" s="16" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G104" s="5" t="n">
-        <v>1977.4</v>
+        <v>1893.5</v>
       </c>
     </row>
     <row r="105">
@@ -3237,22 +3237,22 @@
         </is>
       </c>
       <c r="B105" s="8" t="n">
-        <v>284</v>
+        <v>284.5</v>
       </c>
       <c r="C105" s="10" t="n">
-        <v>281.55</v>
+        <v>279.2</v>
       </c>
       <c r="D105" s="13" t="n">
-        <v>283.55</v>
+        <v>282.6</v>
       </c>
       <c r="E105" s="5" t="n">
-        <v>283.7</v>
+        <v>283.3</v>
       </c>
       <c r="F105" s="16" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="G105" s="5" t="n">
-        <v>282.9</v>
+        <v>279.65</v>
       </c>
     </row>
     <row r="106">
@@ -3262,22 +3262,22 @@
         </is>
       </c>
       <c r="B106" s="8" t="n">
-        <v>1104.6</v>
+        <v>1063.95</v>
       </c>
       <c r="C106" s="10" t="n">
-        <v>1081.45</v>
+        <v>1022.35</v>
       </c>
       <c r="D106" s="13" t="n">
-        <v>1096.05</v>
+        <v>1043.95</v>
       </c>
       <c r="E106" s="5" t="n">
-        <v>1095.85</v>
+        <v>1035.95</v>
       </c>
       <c r="F106" s="16" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G106" s="5" t="n">
-        <v>1102.3</v>
+        <v>1025.7</v>
       </c>
     </row>
     <row r="107">
@@ -3287,22 +3287,22 @@
         </is>
       </c>
       <c r="B107" s="8" t="n">
-        <v>5689.95</v>
+        <v>5534.1</v>
       </c>
       <c r="C107" s="10" t="n">
-        <v>5591</v>
+        <v>5403.1</v>
       </c>
       <c r="D107" s="13" t="n">
-        <v>5629</v>
+        <v>5527</v>
       </c>
       <c r="E107" s="5" t="n">
-        <v>5630.9</v>
+        <v>5506.15</v>
       </c>
       <c r="F107" s="16" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G107" s="5" t="n">
-        <v>5681.45</v>
+        <v>5480</v>
       </c>
     </row>
     <row r="108">
@@ -3312,22 +3312,22 @@
         </is>
       </c>
       <c r="B108" s="8" t="n">
-        <v>357.3</v>
+        <v>350.6</v>
       </c>
       <c r="C108" s="10" t="n">
-        <v>352.2</v>
+        <v>342.85</v>
       </c>
       <c r="D108" s="13" t="n">
-        <v>355.6</v>
+        <v>348</v>
       </c>
       <c r="E108" s="5" t="n">
-        <v>356.25</v>
+        <v>349.45</v>
       </c>
       <c r="F108" s="16" t="n">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G108" s="5" t="n">
-        <v>354</v>
+        <v>344.3</v>
       </c>
     </row>
     <row r="109">
@@ -3337,22 +3337,22 @@
         </is>
       </c>
       <c r="B109" s="8" t="n">
-        <v>3207.85</v>
+        <v>3304.4</v>
       </c>
       <c r="C109" s="10" t="n">
-        <v>3140.5</v>
+        <v>3171</v>
       </c>
       <c r="D109" s="13" t="n">
-        <v>3174.25</v>
+        <v>3184</v>
       </c>
       <c r="E109" s="5" t="n">
-        <v>3163.75</v>
+        <v>3184</v>
       </c>
       <c r="F109" s="16" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G109" s="5" t="n">
-        <v>3201.55</v>
+        <v>3227.45</v>
       </c>
     </row>
     <row r="110">
@@ -3362,22 +3362,22 @@
         </is>
       </c>
       <c r="B110" s="8" t="n">
-        <v>7588</v>
+        <v>7170</v>
       </c>
       <c r="C110" s="10" t="n">
-        <v>7393.5</v>
+        <v>6612</v>
       </c>
       <c r="D110" s="13" t="n">
-        <v>7504.2</v>
+        <v>7107</v>
       </c>
       <c r="E110" s="5" t="n">
-        <v>7489.3</v>
+        <v>7120.4</v>
       </c>
       <c r="F110" s="16" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="G110" s="5" t="n">
-        <v>7558</v>
+        <v>6754</v>
       </c>
     </row>
     <row r="111">
@@ -3387,19 +3387,19 @@
         </is>
       </c>
       <c r="B111" s="8" t="n">
-        <v>331.25</v>
+        <v>333.85</v>
       </c>
       <c r="C111" s="10" t="n">
-        <v>327.5</v>
+        <v>328.25</v>
       </c>
       <c r="D111" s="13" t="n">
-        <v>329.35</v>
+        <v>331</v>
       </c>
       <c r="E111" s="5" t="n">
-        <v>329.85</v>
+        <v>332.05</v>
       </c>
       <c r="F111" s="16" t="n">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="G111" s="5" t="n">
         <v>329</v>
@@ -3412,22 +3412,22 @@
         </is>
       </c>
       <c r="B112" s="8" t="n">
-        <v>177.65</v>
+        <v>179.7</v>
       </c>
       <c r="C112" s="10" t="n">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D112" s="13" t="n">
-        <v>173.88</v>
+        <v>177.98</v>
       </c>
       <c r="E112" s="5" t="n">
-        <v>174.43</v>
+        <v>177.82</v>
       </c>
       <c r="F112" s="16" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G112" s="5" t="n">
-        <v>172.07</v>
+        <v>174.49</v>
       </c>
     </row>
     <row r="113">
@@ -3437,22 +3437,22 @@
         </is>
       </c>
       <c r="B113" s="8" t="n">
-        <v>872</v>
+        <v>861.8</v>
       </c>
       <c r="C113" s="10" t="n">
-        <v>860.8</v>
+        <v>839.95</v>
       </c>
       <c r="D113" s="13" t="n">
-        <v>870</v>
+        <v>850</v>
       </c>
       <c r="E113" s="5" t="n">
-        <v>870.1</v>
+        <v>851.3</v>
       </c>
       <c r="F113" s="16" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G113" s="5" t="n">
-        <v>867.4</v>
+        <v>841.05</v>
       </c>
     </row>
     <row r="114">
@@ -3462,22 +3462,22 @@
         </is>
       </c>
       <c r="B114" s="8" t="n">
-        <v>209.55</v>
+        <v>208.15</v>
       </c>
       <c r="C114" s="10" t="n">
-        <v>204.63</v>
+        <v>200.67</v>
       </c>
       <c r="D114" s="13" t="n">
-        <v>209.5</v>
+        <v>205</v>
       </c>
       <c r="E114" s="5" t="n">
-        <v>208.72</v>
+        <v>205.26</v>
       </c>
       <c r="F114" s="16" t="n">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G114" s="5" t="n">
-        <v>205.75</v>
+        <v>201.18</v>
       </c>
     </row>
     <row r="115">
@@ -3487,22 +3487,22 @@
         </is>
       </c>
       <c r="B115" s="8" t="n">
-        <v>548.45</v>
+        <v>548.5</v>
       </c>
       <c r="C115" s="10" t="n">
-        <v>541.65</v>
+        <v>532.05</v>
       </c>
       <c r="D115" s="13" t="n">
-        <v>548.2</v>
+        <v>544.85</v>
       </c>
       <c r="E115" s="5" t="n">
-        <v>547.3</v>
+        <v>546.25</v>
       </c>
       <c r="F115" s="16" t="n">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="G115" s="5" t="n">
-        <v>546.3</v>
+        <v>532.75</v>
       </c>
     </row>
     <row r="116">
@@ -3512,22 +3512,22 @@
         </is>
       </c>
       <c r="B116" s="8" t="n">
-        <v>740.95</v>
+        <v>743.2</v>
       </c>
       <c r="C116" s="10" t="n">
-        <v>730.55</v>
+        <v>731.2</v>
       </c>
       <c r="D116" s="13" t="n">
-        <v>740</v>
+        <v>741.5</v>
       </c>
       <c r="E116" s="5" t="n">
-        <v>739.05</v>
+        <v>740.15</v>
       </c>
       <c r="F116" s="16" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G116" s="5" t="n">
-        <v>738.4</v>
+        <v>732</v>
       </c>
     </row>
     <row r="117">
@@ -3537,22 +3537,22 @@
         </is>
       </c>
       <c r="B117" s="8" t="n">
-        <v>1754.95</v>
+        <v>1717.45</v>
       </c>
       <c r="C117" s="10" t="n">
-        <v>1718.5</v>
+        <v>1681.15</v>
       </c>
       <c r="D117" s="13" t="n">
-        <v>1729</v>
+        <v>1704.5</v>
       </c>
       <c r="E117" s="5" t="n">
-        <v>1723.75</v>
+        <v>1706.05</v>
       </c>
       <c r="F117" s="16" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G117" s="5" t="n">
-        <v>1752.45</v>
+        <v>1685.4</v>
       </c>
     </row>
     <row r="118">
@@ -3562,22 +3562,22 @@
         </is>
       </c>
       <c r="B118" s="8" t="n">
-        <v>7880.1</v>
+        <v>7854.6</v>
       </c>
       <c r="C118" s="10" t="n">
-        <v>7703.75</v>
+        <v>7565</v>
       </c>
       <c r="D118" s="13" t="n">
-        <v>7875</v>
+        <v>7795</v>
       </c>
       <c r="E118" s="5" t="n">
-        <v>7870.05</v>
+        <v>7803</v>
       </c>
       <c r="F118" s="16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G118" s="5" t="n">
-        <v>7822.5</v>
+        <v>7599.4</v>
       </c>
     </row>
     <row r="119">
@@ -3587,22 +3587,22 @@
         </is>
       </c>
       <c r="B119" s="8" t="n">
-        <v>2355</v>
+        <v>2333.35</v>
       </c>
       <c r="C119" s="10" t="n">
-        <v>2334.8</v>
+        <v>2266.45</v>
       </c>
       <c r="D119" s="13" t="n">
-        <v>2351.05</v>
+        <v>2325</v>
       </c>
       <c r="E119" s="5" t="n">
-        <v>2351.4</v>
+        <v>2325.7</v>
       </c>
       <c r="F119" s="16" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G119" s="5" t="n">
-        <v>2353.85</v>
+        <v>2272.95</v>
       </c>
     </row>
     <row r="120">
@@ -3612,22 +3612,22 @@
         </is>
       </c>
       <c r="B120" s="8" t="n">
-        <v>1588.9</v>
+        <v>1654.95</v>
       </c>
       <c r="C120" s="10" t="n">
-        <v>1514.7</v>
+        <v>1597</v>
       </c>
       <c r="D120" s="13" t="n">
-        <v>1565</v>
+        <v>1628.5</v>
       </c>
       <c r="E120" s="5" t="n">
-        <v>1565.95</v>
+        <v>1628.9</v>
       </c>
       <c r="F120" s="16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G120" s="5" t="n">
-        <v>1545.9</v>
+        <v>1599.35</v>
       </c>
     </row>
     <row r="121">
@@ -3637,22 +3637,22 @@
         </is>
       </c>
       <c r="B121" s="8" t="n">
-        <v>1919.6</v>
+        <v>1917.9</v>
       </c>
       <c r="C121" s="10" t="n">
-        <v>1894.65</v>
+        <v>1872.7</v>
       </c>
       <c r="D121" s="13" t="n">
-        <v>1899.5</v>
+        <v>1907.1</v>
       </c>
       <c r="E121" s="5" t="n">
-        <v>1898.45</v>
+        <v>1910.35</v>
       </c>
       <c r="F121" s="16" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G121" s="5" t="n">
-        <v>1919.4</v>
+        <v>1881.4</v>
       </c>
     </row>
     <row r="122">
@@ -3662,22 +3662,22 @@
         </is>
       </c>
       <c r="B122" s="8" t="n">
-        <v>893.95</v>
+        <v>885.55</v>
       </c>
       <c r="C122" s="10" t="n">
-        <v>881.55</v>
+        <v>873.75</v>
       </c>
       <c r="D122" s="13" t="n">
-        <v>884.6</v>
+        <v>876.85</v>
       </c>
       <c r="E122" s="5" t="n">
-        <v>886.85</v>
+        <v>877.4</v>
       </c>
       <c r="F122" s="16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G122" s="5" t="n">
-        <v>890.1</v>
+        <v>874.8</v>
       </c>
     </row>
     <row r="123">
@@ -3687,22 +3687,22 @@
         </is>
       </c>
       <c r="B123" s="8" t="n">
-        <v>1945.4</v>
+        <v>1880.7</v>
       </c>
       <c r="C123" s="10" t="n">
-        <v>1910.2</v>
+        <v>1808.1</v>
       </c>
       <c r="D123" s="13" t="n">
-        <v>1931.5</v>
+        <v>1873.45</v>
       </c>
       <c r="E123" s="5" t="n">
-        <v>1931.3</v>
+        <v>1873</v>
       </c>
       <c r="F123" s="16" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G123" s="5" t="n">
-        <v>1944</v>
+        <v>1822.1</v>
       </c>
     </row>
     <row r="124">
@@ -3712,22 +3712,22 @@
         </is>
       </c>
       <c r="B124" s="8" t="n">
-        <v>931.8</v>
+        <v>917.7</v>
       </c>
       <c r="C124" s="10" t="n">
-        <v>913</v>
+        <v>889.2</v>
       </c>
       <c r="D124" s="13" t="n">
-        <v>918.9</v>
+        <v>911</v>
       </c>
       <c r="E124" s="5" t="n">
-        <v>917.3</v>
+        <v>910.15</v>
       </c>
       <c r="F124" s="16" t="n">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="G124" s="5" t="n">
-        <v>929.3</v>
+        <v>890.5</v>
       </c>
     </row>
     <row r="125">
@@ -3737,22 +3737,22 @@
         </is>
       </c>
       <c r="B125" s="8" t="n">
-        <v>1701.75</v>
+        <v>1702.4</v>
       </c>
       <c r="C125" s="10" t="n">
-        <v>1663.5</v>
+        <v>1645.6</v>
       </c>
       <c r="D125" s="13" t="n">
-        <v>1674.15</v>
+        <v>1685.15</v>
       </c>
       <c r="E125" s="5" t="n">
-        <v>1675.35</v>
+        <v>1687.9</v>
       </c>
       <c r="F125" s="16" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G125" s="5" t="n">
-        <v>1698.5</v>
+        <v>1682.9</v>
       </c>
     </row>
     <row r="126">
@@ -3762,22 +3762,22 @@
         </is>
       </c>
       <c r="B126" s="8" t="n">
-        <v>3531.75</v>
+        <v>3482.65</v>
       </c>
       <c r="C126" s="10" t="n">
-        <v>3477.55</v>
+        <v>3390.95</v>
       </c>
       <c r="D126" s="13" t="n">
-        <v>3510</v>
+        <v>3435.1</v>
       </c>
       <c r="E126" s="5" t="n">
-        <v>3497.6</v>
+        <v>3449.5</v>
       </c>
       <c r="F126" s="16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G126" s="5" t="n">
-        <v>3514.55</v>
+        <v>3395.45</v>
       </c>
     </row>
     <row r="127">
@@ -3787,22 +3787,22 @@
         </is>
       </c>
       <c r="B127" s="8" t="n">
-        <v>1961.45</v>
+        <v>1993</v>
       </c>
       <c r="C127" s="10" t="n">
-        <v>1939.65</v>
+        <v>1912.9</v>
       </c>
       <c r="D127" s="13" t="n">
-        <v>1950</v>
+        <v>1972</v>
       </c>
       <c r="E127" s="5" t="n">
-        <v>1953.2</v>
+        <v>1973.65</v>
       </c>
       <c r="F127" s="16" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G127" s="5" t="n">
-        <v>1952.6</v>
+        <v>1913.95</v>
       </c>
     </row>
     <row r="128">
@@ -3812,22 +3812,22 @@
         </is>
       </c>
       <c r="B128" s="8" t="n">
-        <v>8225</v>
+        <v>7800</v>
       </c>
       <c r="C128" s="10" t="n">
-        <v>8090</v>
+        <v>7650.9</v>
       </c>
       <c r="D128" s="13" t="n">
-        <v>8125</v>
+        <v>7765.8</v>
       </c>
       <c r="E128" s="5" t="n">
-        <v>8124.25</v>
+        <v>7768.05</v>
       </c>
       <c r="F128" s="16" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G128" s="5" t="n">
-        <v>8204.450000000001</v>
+        <v>7668.35</v>
       </c>
     </row>
     <row r="129">
@@ -3837,22 +3837,22 @@
         </is>
       </c>
       <c r="B129" s="8" t="n">
-        <v>2844.8</v>
+        <v>2753.8</v>
       </c>
       <c r="C129" s="10" t="n">
-        <v>2800.65</v>
+        <v>2669.7</v>
       </c>
       <c r="D129" s="13" t="n">
-        <v>2833</v>
+        <v>2718</v>
       </c>
       <c r="E129" s="5" t="n">
-        <v>2833.6</v>
+        <v>2715.9</v>
       </c>
       <c r="F129" s="16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G129" s="5" t="n">
-        <v>2824</v>
+        <v>2682.25</v>
       </c>
     </row>
     <row r="130">
@@ -3862,22 +3862,22 @@
         </is>
       </c>
       <c r="B130" s="8" t="n">
-        <v>2102.5</v>
+        <v>1982.7</v>
       </c>
       <c r="C130" s="10" t="n">
-        <v>2055.4</v>
+        <v>1961.1</v>
       </c>
       <c r="D130" s="13" t="n">
-        <v>2071.65</v>
+        <v>1975</v>
       </c>
       <c r="E130" s="5" t="n">
-        <v>2069.35</v>
+        <v>1976.55</v>
       </c>
       <c r="F130" s="16" t="n">
         <v>1</v>
       </c>
       <c r="G130" s="5" t="n">
-        <v>2078.7</v>
+        <v>1965.95</v>
       </c>
     </row>
     <row r="131">
@@ -3887,22 +3887,22 @@
         </is>
       </c>
       <c r="B131" s="8" t="n">
-        <v>11432.95</v>
+        <v>11139.95</v>
       </c>
       <c r="C131" s="10" t="n">
-        <v>11290</v>
+        <v>10901</v>
       </c>
       <c r="D131" s="13" t="n">
-        <v>11425</v>
+        <v>11084</v>
       </c>
       <c r="E131" s="5" t="n">
-        <v>11416.9</v>
+        <v>11069.3</v>
       </c>
       <c r="F131" s="16" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G131" s="5" t="n">
-        <v>11389.95</v>
+        <v>10915.35</v>
       </c>
     </row>
     <row r="132">
@@ -3912,22 +3912,22 @@
         </is>
       </c>
       <c r="B132" s="8" t="n">
-        <v>576.8</v>
+        <v>557.75</v>
       </c>
       <c r="C132" s="10" t="n">
-        <v>569.15</v>
+        <v>542.6</v>
       </c>
       <c r="D132" s="13" t="n">
-        <v>573.9</v>
+        <v>557</v>
       </c>
       <c r="E132" s="5" t="n">
-        <v>574.1</v>
+        <v>555.25</v>
       </c>
       <c r="F132" s="16" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G132" s="5" t="n">
-        <v>576.05</v>
+        <v>545.4</v>
       </c>
     </row>
     <row r="133">
@@ -3937,22 +3937,22 @@
         </is>
       </c>
       <c r="B133" s="8" t="n">
-        <v>495.7</v>
+        <v>483.65</v>
       </c>
       <c r="C133" s="10" t="n">
-        <v>486.4</v>
+        <v>464</v>
       </c>
       <c r="D133" s="13" t="n">
-        <v>490</v>
+        <v>480.4</v>
       </c>
       <c r="E133" s="5" t="n">
-        <v>489.85</v>
+        <v>480.85</v>
       </c>
       <c r="F133" s="16" t="n">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="G133" s="5" t="n">
-        <v>494.55</v>
+        <v>466.85</v>
       </c>
     </row>
     <row r="134">
@@ -3962,22 +3962,22 @@
         </is>
       </c>
       <c r="B134" s="8" t="n">
-        <v>1816.8</v>
+        <v>1870</v>
       </c>
       <c r="C134" s="10" t="n">
-        <v>1784.45</v>
+        <v>1815.25</v>
       </c>
       <c r="D134" s="13" t="n">
-        <v>1814</v>
+        <v>1868</v>
       </c>
       <c r="E134" s="5" t="n">
-        <v>1811.1</v>
+        <v>1865.3</v>
       </c>
       <c r="F134" s="16" t="n">
         <v>16</v>
       </c>
       <c r="G134" s="5" t="n">
-        <v>1807.2</v>
+        <v>1817.2</v>
       </c>
     </row>
     <row r="135">
@@ -3987,22 +3987,22 @@
         </is>
       </c>
       <c r="B135" s="8" t="n">
-        <v>131.2</v>
+        <v>134.11</v>
       </c>
       <c r="C135" s="10" t="n">
-        <v>128.75</v>
+        <v>125.33</v>
       </c>
       <c r="D135" s="13" t="n">
-        <v>129.9</v>
+        <v>130.5</v>
       </c>
       <c r="E135" s="5" t="n">
-        <v>129.3</v>
+        <v>132.46</v>
       </c>
       <c r="F135" s="16" t="n">
-        <v>74</v>
+        <v>411</v>
       </c>
       <c r="G135" s="5" t="n">
-        <v>131.2</v>
+        <v>125.4</v>
       </c>
     </row>
     <row r="136" ht="15.75" customHeight="1" thickBot="1">
@@ -4012,22 +4012,22 @@
         </is>
       </c>
       <c r="B136" s="18" t="n">
-        <v>1071.75</v>
+        <v>1029.85</v>
       </c>
       <c r="C136" s="11" t="n">
-        <v>1054.35</v>
+        <v>1013.9</v>
       </c>
       <c r="D136" s="14" t="n">
-        <v>1056.2</v>
+        <v>1021</v>
       </c>
       <c r="E136" s="6" t="n">
-        <v>1058.15</v>
+        <v>1022.45</v>
       </c>
       <c r="F136" s="17" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G136" s="6" t="n">
-        <v>1065.9</v>
+        <v>1016.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>